<commit_message>
Updating Project Plan to Resolve review points on CYRS, HSI and SRS documents
Signed-off-by: May Alaa <mayelfkiy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
   <si>
     <t>HELP</t>
   </si>
@@ -242,9 +242,6 @@
     <t>Ali</t>
   </si>
   <si>
-    <t>21/1/20</t>
-  </si>
-  <si>
     <t>Type</t>
   </si>
   <si>
@@ -254,13 +251,31 @@
     <t>Amira, Ali</t>
   </si>
   <si>
-    <t>28/1/20</t>
-  </si>
-  <si>
-    <t>22/1/20</t>
-  </si>
-  <si>
-    <t>24/1/20</t>
+    <t>CYRS Resolve</t>
+  </si>
+  <si>
+    <t>Ibrahim</t>
+  </si>
+  <si>
+    <t>SRS Resolve</t>
+  </si>
+  <si>
+    <t>HSI Resolve</t>
+  </si>
+  <si>
+    <t>CYRS Cross Review</t>
+  </si>
+  <si>
+    <t>SRS Cross Review</t>
+  </si>
+  <si>
+    <t>HSI Cross Review</t>
+  </si>
+  <si>
+    <t>Farag</t>
+  </si>
+  <si>
+    <t>Update RTM</t>
   </si>
 </sst>
 </file>
@@ -1209,7 +1224,7 @@
                   <a14:compatExt spid="_x0000_s6145"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001180000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1259,7 +1274,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1314,7 +1329,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1615,10 +1630,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO37"/>
+  <dimension ref="A1:BO43"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2276,7 +2291,7 @@
         <v>34</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E8" s="13" t="s">
         <v>31</v>
@@ -2611,8 +2626,8 @@
         <f>IF(OR(ISBLANK(F10),ISBLANK(G10)),"",G10-F10+1)</f>
         <v>4</v>
       </c>
-      <c r="I10" s="56" t="s">
-        <v>66</v>
+      <c r="I10" s="56">
+        <v>43851</v>
       </c>
       <c r="J10" s="57"/>
       <c r="K10" s="57"/>
@@ -2684,9 +2699,11 @@
         <v>60</v>
       </c>
       <c r="D11" s="75" t="s">
-        <v>68</v>
-      </c>
-      <c r="E11" s="51"/>
+        <v>67</v>
+      </c>
+      <c r="E11" s="51">
+        <v>1</v>
+      </c>
       <c r="F11" s="54">
         <v>43852</v>
       </c>
@@ -2694,16 +2711,16 @@
         <v>43853</v>
       </c>
       <c r="H11" s="62">
-        <f t="shared" ref="H11:H17" si="3">IF(OR(ISBLANK(F11),ISBLANK(G11)),"",G11-F11+1)</f>
+        <f t="shared" ref="H11:H23" si="3">IF(OR(ISBLANK(F11),ISBLANK(G11)),"",G11-F11+1)</f>
         <v>2</v>
       </c>
-      <c r="I11" s="54" t="s">
-        <v>71</v>
+      <c r="I11" s="54">
+        <v>43852</v>
       </c>
       <c r="J11" s="55"/>
       <c r="K11" s="55"/>
       <c r="L11" s="62" t="str">
-        <f t="shared" ref="L11:L34" si="4">IF(OR(ISBLANK(I11),ISBLANK(J11)),"",J11-I11+1)</f>
+        <f t="shared" ref="L11:L40" si="4">IF(OR(ISBLANK(I11),ISBLANK(J11)),"",J11-I11+1)</f>
         <v/>
       </c>
       <c r="M11" s="16"/>
@@ -2770,9 +2787,11 @@
         <v>61</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="E12" s="51"/>
+        <v>67</v>
+      </c>
+      <c r="E12" s="51">
+        <v>1</v>
+      </c>
       <c r="F12" s="54">
         <v>43854</v>
       </c>
@@ -2783,8 +2802,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="I12" s="54" t="s">
-        <v>72</v>
+      <c r="I12" s="54">
+        <v>43854</v>
       </c>
       <c r="J12" s="55"/>
       <c r="K12" s="55"/>
@@ -2853,12 +2872,14 @@
         <v>59</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D13" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="E13" s="51"/>
+        <v>67</v>
+      </c>
+      <c r="E13" s="51">
+        <v>1</v>
+      </c>
       <c r="F13" s="54">
         <v>43854</v>
       </c>
@@ -2869,8 +2890,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="I13" s="54" t="s">
-        <v>72</v>
+      <c r="I13" s="54">
+        <v>43854</v>
       </c>
       <c r="J13" s="55"/>
       <c r="K13" s="55"/>
@@ -2942,9 +2963,11 @@
         <v>65</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="E14" s="51"/>
+        <v>67</v>
+      </c>
+      <c r="E14" s="51">
+        <v>1</v>
+      </c>
       <c r="F14" s="54">
         <v>43853</v>
       </c>
@@ -2955,8 +2978,8 @@
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
-      <c r="I14" s="54" t="s">
-        <v>71</v>
+      <c r="I14" s="54">
+        <v>43852</v>
       </c>
       <c r="J14" s="55"/>
       <c r="K14" s="55"/>
@@ -3028,21 +3051,23 @@
         <v>64</v>
       </c>
       <c r="D15" s="41" t="s">
-        <v>68</v>
-      </c>
-      <c r="E15" s="51"/>
+        <v>67</v>
+      </c>
+      <c r="E15" s="51">
+        <v>1</v>
+      </c>
       <c r="F15" s="54">
-        <v>43853</v>
+        <v>43857</v>
       </c>
       <c r="G15" s="55">
-        <v>43853</v>
+        <v>43868</v>
       </c>
       <c r="H15" s="62">
         <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-      <c r="I15" s="54" t="s">
-        <v>70</v>
+        <v>12</v>
+      </c>
+      <c r="I15" s="54">
+        <v>43858</v>
       </c>
       <c r="J15" s="55"/>
       <c r="K15" s="55"/>
@@ -3108,24 +3133,29 @@
     <row r="16" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
+        <v>69</v>
+      </c>
+      <c r="C16" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D16" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="E16" s="51"/>
-      <c r="F16" s="54"/>
-      <c r="G16" s="55"/>
-      <c r="H16" s="62" t="str">
+      <c r="F16" s="54">
+        <v>43862</v>
+      </c>
+      <c r="G16" s="55">
+        <v>43863</v>
+      </c>
+      <c r="H16" s="62">
         <f t="shared" si="3"/>
-        <v/>
+        <v>2</v>
       </c>
       <c r="I16" s="54"/>
       <c r="J16" s="55"/>
       <c r="K16" s="55"/>
-      <c r="L16" s="62" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="L16" s="62"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
@@ -3184,24 +3214,29 @@
     <row r="17" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="47"/>
       <c r="B17" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
+        <v>71</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="E17" s="51"/>
-      <c r="F17" s="54"/>
-      <c r="G17" s="55"/>
-      <c r="H17" s="62" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="F17" s="54">
+        <v>43865</v>
+      </c>
+      <c r="G17" s="55">
+        <v>43866</v>
+      </c>
+      <c r="H17" s="62">
+        <f>IF(OR(ISBLANK(F17),ISBLANK(G17)),"",G17-F17+1)</f>
+        <v>2</v>
       </c>
       <c r="I17" s="54"/>
       <c r="J17" s="55"/>
       <c r="K17" s="55"/>
-      <c r="L17" s="62" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="L17" s="62"/>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
@@ -3214,10 +3249,10 @@
       <c r="V17" s="16"/>
       <c r="W17" s="16"/>
       <c r="X17" s="16"/>
-      <c r="Y17" s="17"/>
+      <c r="Y17" s="16"/>
       <c r="Z17" s="16"/>
       <c r="AA17" s="16"/>
-      <c r="AB17" s="17"/>
+      <c r="AB17" s="16"/>
       <c r="AC17" s="16"/>
       <c r="AD17" s="16"/>
       <c r="AE17" s="16"/>
@@ -3258,23 +3293,31 @@
       <c r="BN17" s="16"/>
     </row>
     <row r="18" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="48"/>
-      <c r="B18" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="52"/>
-      <c r="F18" s="56"/>
-      <c r="G18" s="57"/>
-      <c r="H18" s="63" t="str">
-        <f t="shared" ref="H18:H34" si="5">IF(OR(ISBLANK(F18),ISBLANK(G18)),"",G18-F18+1)</f>
-        <v/>
-      </c>
-      <c r="I18" s="56"/>
-      <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="63" t="str">
+      <c r="A18" s="47"/>
+      <c r="B18" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="C18" s="41" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E18" s="51"/>
+      <c r="F18" s="54">
+        <v>43862</v>
+      </c>
+      <c r="G18" s="55">
+        <v>43864</v>
+      </c>
+      <c r="H18" s="62">
+        <f>IF(OR(ISBLANK(F18),ISBLANK(G18)),"",G18-F18+1)</f>
+        <v>3</v>
+      </c>
+      <c r="I18" s="54"/>
+      <c r="J18" s="55"/>
+      <c r="K18" s="55"/>
+      <c r="L18" s="62" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
@@ -3336,14 +3379,25 @@
     <row r="19" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
+        <v>73</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D19" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="E19" s="51"/>
-      <c r="F19" s="54"/>
-      <c r="G19" s="55"/>
-      <c r="H19" s="62"/>
+      <c r="F19" s="54">
+        <v>43864</v>
+      </c>
+      <c r="G19" s="55">
+        <v>43865</v>
+      </c>
+      <c r="H19" s="62">
+        <f>IF(OR(ISBLANK(F19),ISBLANK(G19)),"",G19-F19+1)</f>
+        <v>2</v>
+      </c>
       <c r="I19" s="54"/>
       <c r="J19" s="55"/>
       <c r="K19" s="55"/>
@@ -3406,14 +3460,25 @@
     <row r="20" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
+        <v>74</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="E20" s="51"/>
-      <c r="F20" s="54"/>
-      <c r="G20" s="55"/>
-      <c r="H20" s="62"/>
+      <c r="F20" s="54">
+        <v>43866</v>
+      </c>
+      <c r="G20" s="55">
+        <v>43867</v>
+      </c>
+      <c r="H20" s="62">
+        <f>IF(OR(ISBLANK(F20),ISBLANK(G20)),"",G20-F20+1)</f>
+        <v>2</v>
+      </c>
       <c r="I20" s="54"/>
       <c r="J20" s="55"/>
       <c r="K20" s="55"/>
@@ -3476,14 +3541,25 @@
     <row r="21" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
+        <v>75</v>
+      </c>
+      <c r="C21" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D21" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="E21" s="51"/>
-      <c r="F21" s="54"/>
-      <c r="G21" s="55"/>
-      <c r="H21" s="62"/>
+      <c r="F21" s="54">
+        <v>43864</v>
+      </c>
+      <c r="G21" s="55">
+        <v>43865</v>
+      </c>
+      <c r="H21" s="62">
+        <f>IF(OR(ISBLANK(F21),ISBLANK(G21)),"",G21-F21+1)</f>
+        <v>2</v>
+      </c>
       <c r="I21" s="54"/>
       <c r="J21" s="55"/>
       <c r="K21" s="55"/>
@@ -3546,14 +3622,25 @@
     <row r="22" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
       <c r="B22" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
+        <v>77</v>
+      </c>
+      <c r="C22" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D22" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="E22" s="51"/>
-      <c r="F22" s="54"/>
-      <c r="G22" s="55"/>
-      <c r="H22" s="62"/>
+      <c r="F22" s="54">
+        <v>43867</v>
+      </c>
+      <c r="G22" s="55">
+        <v>43868</v>
+      </c>
+      <c r="H22" s="62">
+        <f>IF(OR(ISBLANK(F22),ISBLANK(G22)),"",G22-F22+1)</f>
+        <v>2</v>
+      </c>
       <c r="I22" s="54"/>
       <c r="J22" s="55"/>
       <c r="K22" s="55"/>
@@ -3616,18 +3703,24 @@
     <row r="23" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
       <c r="B23" s="15" t="s">
-        <v>13</v>
+        <v>44</v>
       </c>
       <c r="C23" s="41"/>
       <c r="D23" s="41"/>
       <c r="E23" s="51"/>
       <c r="F23" s="54"/>
       <c r="G23" s="55"/>
-      <c r="H23" s="62"/>
+      <c r="H23" s="62" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="I23" s="54"/>
       <c r="J23" s="55"/>
       <c r="K23" s="55"/>
-      <c r="L23" s="62"/>
+      <c r="L23" s="62" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>
@@ -3640,10 +3733,10 @@
       <c r="V23" s="16"/>
       <c r="W23" s="16"/>
       <c r="X23" s="16"/>
-      <c r="Y23" s="16"/>
+      <c r="Y23" s="17"/>
       <c r="Z23" s="16"/>
       <c r="AA23" s="16"/>
-      <c r="AB23" s="16"/>
+      <c r="AB23" s="17"/>
       <c r="AC23" s="16"/>
       <c r="AD23" s="16"/>
       <c r="AE23" s="16"/>
@@ -3684,20 +3777,26 @@
       <c r="BN23" s="16"/>
     </row>
     <row r="24" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="47"/>
-      <c r="B24" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="54"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="54"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="62"/>
+      <c r="A24" s="48"/>
+      <c r="B24" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C24" s="42"/>
+      <c r="D24" s="42"/>
+      <c r="E24" s="52"/>
+      <c r="F24" s="56"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="63" t="str">
+        <f t="shared" ref="H24:H40" si="5">IF(OR(ISBLANK(F24),ISBLANK(G24)),"",G24-F24+1)</f>
+        <v/>
+      </c>
+      <c r="I24" s="56"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
@@ -3755,23 +3854,19 @@
     </row>
     <row r="25" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
-      <c r="B25" s="44"/>
+      <c r="B25" s="15" t="s">
+        <v>15</v>
+      </c>
       <c r="C25" s="41"/>
       <c r="D25" s="41"/>
       <c r="E25" s="51"/>
       <c r="F25" s="54"/>
       <c r="G25" s="55"/>
-      <c r="H25" s="62" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="H25" s="62"/>
       <c r="I25" s="54"/>
       <c r="J25" s="55"/>
       <c r="K25" s="55"/>
-      <c r="L25" s="62" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="L25" s="62"/>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
@@ -3829,23 +3924,19 @@
     </row>
     <row r="26" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="47"/>
-      <c r="B26" s="44"/>
+      <c r="B26" s="15" t="s">
+        <v>16</v>
+      </c>
       <c r="C26" s="41"/>
       <c r="D26" s="41"/>
       <c r="E26" s="51"/>
       <c r="F26" s="54"/>
       <c r="G26" s="55"/>
-      <c r="H26" s="62" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="H26" s="62"/>
       <c r="I26" s="54"/>
       <c r="J26" s="55"/>
       <c r="K26" s="55"/>
-      <c r="L26" s="62" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="L26" s="62"/>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
@@ -3903,23 +3994,19 @@
     </row>
     <row r="27" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
-      <c r="B27" s="44"/>
+      <c r="B27" s="15" t="s">
+        <v>11</v>
+      </c>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
       <c r="E27" s="51"/>
       <c r="F27" s="54"/>
       <c r="G27" s="55"/>
-      <c r="H27" s="62" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="H27" s="62"/>
       <c r="I27" s="54"/>
       <c r="J27" s="55"/>
       <c r="K27" s="55"/>
-      <c r="L27" s="62" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="L27" s="62"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
@@ -3977,7 +4064,9 @@
     </row>
     <row r="28" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
-      <c r="B28" s="44"/>
+      <c r="B28" s="15" t="s">
+        <v>12</v>
+      </c>
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
       <c r="E28" s="51"/>
@@ -4045,7 +4134,9 @@
     </row>
     <row r="29" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
-      <c r="B29" s="44"/>
+      <c r="B29" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="C29" s="41"/>
       <c r="D29" s="41"/>
       <c r="E29" s="51"/>
@@ -4113,7 +4204,9 @@
     </row>
     <row r="30" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="47"/>
-      <c r="B30" s="44"/>
+      <c r="B30" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="C30" s="41"/>
       <c r="D30" s="41"/>
       <c r="E30" s="51"/>
@@ -4187,11 +4280,17 @@
       <c r="E31" s="51"/>
       <c r="F31" s="54"/>
       <c r="G31" s="55"/>
-      <c r="H31" s="62"/>
+      <c r="H31" s="62" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="I31" s="54"/>
       <c r="J31" s="55"/>
       <c r="K31" s="55"/>
-      <c r="L31" s="62"/>
+      <c r="L31" s="62" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
       <c r="O31" s="16"/>
@@ -4255,11 +4354,17 @@
       <c r="E32" s="51"/>
       <c r="F32" s="54"/>
       <c r="G32" s="55"/>
-      <c r="H32" s="62"/>
+      <c r="H32" s="62" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
       <c r="I32" s="54"/>
       <c r="J32" s="55"/>
       <c r="K32" s="55"/>
-      <c r="L32" s="62"/>
+      <c r="L32" s="62" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
       <c r="O32" s="16"/>
@@ -4390,92 +4495,506 @@
       <c r="BN33" s="16"/>
     </row>
     <row r="34" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="49"/>
-      <c r="B34" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="C34" s="43"/>
-      <c r="D34" s="43"/>
-      <c r="E34" s="53"/>
-      <c r="F34" s="58"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="64" t="str">
+      <c r="A34" s="47"/>
+      <c r="B34" s="44"/>
+      <c r="C34" s="41"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="51"/>
+      <c r="F34" s="54"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="62"/>
+      <c r="I34" s="54"/>
+      <c r="J34" s="55"/>
+      <c r="K34" s="55"/>
+      <c r="L34" s="62"/>
+      <c r="M34" s="16"/>
+      <c r="N34" s="16"/>
+      <c r="O34" s="16"/>
+      <c r="P34" s="16"/>
+      <c r="Q34" s="16"/>
+      <c r="R34" s="16"/>
+      <c r="S34" s="16"/>
+      <c r="T34" s="16"/>
+      <c r="U34" s="16"/>
+      <c r="V34" s="16"/>
+      <c r="W34" s="16"/>
+      <c r="X34" s="16"/>
+      <c r="Y34" s="16"/>
+      <c r="Z34" s="16"/>
+      <c r="AA34" s="16"/>
+      <c r="AB34" s="16"/>
+      <c r="AC34" s="16"/>
+      <c r="AD34" s="16"/>
+      <c r="AE34" s="16"/>
+      <c r="AF34" s="16"/>
+      <c r="AG34" s="16"/>
+      <c r="AH34" s="16"/>
+      <c r="AI34" s="16"/>
+      <c r="AJ34" s="16"/>
+      <c r="AK34" s="16"/>
+      <c r="AL34" s="16"/>
+      <c r="AM34" s="16"/>
+      <c r="AN34" s="16"/>
+      <c r="AO34" s="16"/>
+      <c r="AP34" s="16"/>
+      <c r="AQ34" s="16"/>
+      <c r="AR34" s="16"/>
+      <c r="AS34" s="16"/>
+      <c r="AT34" s="16"/>
+      <c r="AU34" s="16"/>
+      <c r="AV34" s="16"/>
+      <c r="AW34" s="16"/>
+      <c r="AX34" s="16"/>
+      <c r="AY34" s="16"/>
+      <c r="AZ34" s="16"/>
+      <c r="BA34" s="16"/>
+      <c r="BB34" s="16"/>
+      <c r="BC34" s="16"/>
+      <c r="BD34" s="16"/>
+      <c r="BE34" s="16"/>
+      <c r="BF34" s="16"/>
+      <c r="BG34" s="16"/>
+      <c r="BH34" s="16"/>
+      <c r="BI34" s="16"/>
+      <c r="BJ34" s="16"/>
+      <c r="BK34" s="16"/>
+      <c r="BL34" s="16"/>
+      <c r="BM34" s="16"/>
+      <c r="BN34" s="16"/>
+    </row>
+    <row r="35" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="47"/>
+      <c r="B35" s="44"/>
+      <c r="C35" s="41"/>
+      <c r="D35" s="41"/>
+      <c r="E35" s="51"/>
+      <c r="F35" s="54"/>
+      <c r="G35" s="55"/>
+      <c r="H35" s="62"/>
+      <c r="I35" s="54"/>
+      <c r="J35" s="55"/>
+      <c r="K35" s="55"/>
+      <c r="L35" s="62"/>
+      <c r="M35" s="16"/>
+      <c r="N35" s="16"/>
+      <c r="O35" s="16"/>
+      <c r="P35" s="16"/>
+      <c r="Q35" s="16"/>
+      <c r="R35" s="16"/>
+      <c r="S35" s="16"/>
+      <c r="T35" s="16"/>
+      <c r="U35" s="16"/>
+      <c r="V35" s="16"/>
+      <c r="W35" s="16"/>
+      <c r="X35" s="16"/>
+      <c r="Y35" s="16"/>
+      <c r="Z35" s="16"/>
+      <c r="AA35" s="16"/>
+      <c r="AB35" s="16"/>
+      <c r="AC35" s="16"/>
+      <c r="AD35" s="16"/>
+      <c r="AE35" s="16"/>
+      <c r="AF35" s="16"/>
+      <c r="AG35" s="16"/>
+      <c r="AH35" s="16"/>
+      <c r="AI35" s="16"/>
+      <c r="AJ35" s="16"/>
+      <c r="AK35" s="16"/>
+      <c r="AL35" s="16"/>
+      <c r="AM35" s="16"/>
+      <c r="AN35" s="16"/>
+      <c r="AO35" s="16"/>
+      <c r="AP35" s="16"/>
+      <c r="AQ35" s="16"/>
+      <c r="AR35" s="16"/>
+      <c r="AS35" s="16"/>
+      <c r="AT35" s="16"/>
+      <c r="AU35" s="16"/>
+      <c r="AV35" s="16"/>
+      <c r="AW35" s="16"/>
+      <c r="AX35" s="16"/>
+      <c r="AY35" s="16"/>
+      <c r="AZ35" s="16"/>
+      <c r="BA35" s="16"/>
+      <c r="BB35" s="16"/>
+      <c r="BC35" s="16"/>
+      <c r="BD35" s="16"/>
+      <c r="BE35" s="16"/>
+      <c r="BF35" s="16"/>
+      <c r="BG35" s="16"/>
+      <c r="BH35" s="16"/>
+      <c r="BI35" s="16"/>
+      <c r="BJ35" s="16"/>
+      <c r="BK35" s="16"/>
+      <c r="BL35" s="16"/>
+      <c r="BM35" s="16"/>
+      <c r="BN35" s="16"/>
+    </row>
+    <row r="36" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="47"/>
+      <c r="B36" s="44"/>
+      <c r="C36" s="41"/>
+      <c r="D36" s="41"/>
+      <c r="E36" s="51"/>
+      <c r="F36" s="54"/>
+      <c r="G36" s="55"/>
+      <c r="H36" s="62"/>
+      <c r="I36" s="54"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="55"/>
+      <c r="L36" s="62"/>
+      <c r="M36" s="16"/>
+      <c r="N36" s="16"/>
+      <c r="O36" s="16"/>
+      <c r="P36" s="16"/>
+      <c r="Q36" s="16"/>
+      <c r="R36" s="16"/>
+      <c r="S36" s="16"/>
+      <c r="T36" s="16"/>
+      <c r="U36" s="16"/>
+      <c r="V36" s="16"/>
+      <c r="W36" s="16"/>
+      <c r="X36" s="16"/>
+      <c r="Y36" s="16"/>
+      <c r="Z36" s="16"/>
+      <c r="AA36" s="16"/>
+      <c r="AB36" s="16"/>
+      <c r="AC36" s="16"/>
+      <c r="AD36" s="16"/>
+      <c r="AE36" s="16"/>
+      <c r="AF36" s="16"/>
+      <c r="AG36" s="16"/>
+      <c r="AH36" s="16"/>
+      <c r="AI36" s="16"/>
+      <c r="AJ36" s="16"/>
+      <c r="AK36" s="16"/>
+      <c r="AL36" s="16"/>
+      <c r="AM36" s="16"/>
+      <c r="AN36" s="16"/>
+      <c r="AO36" s="16"/>
+      <c r="AP36" s="16"/>
+      <c r="AQ36" s="16"/>
+      <c r="AR36" s="16"/>
+      <c r="AS36" s="16"/>
+      <c r="AT36" s="16"/>
+      <c r="AU36" s="16"/>
+      <c r="AV36" s="16"/>
+      <c r="AW36" s="16"/>
+      <c r="AX36" s="16"/>
+      <c r="AY36" s="16"/>
+      <c r="AZ36" s="16"/>
+      <c r="BA36" s="16"/>
+      <c r="BB36" s="16"/>
+      <c r="BC36" s="16"/>
+      <c r="BD36" s="16"/>
+      <c r="BE36" s="16"/>
+      <c r="BF36" s="16"/>
+      <c r="BG36" s="16"/>
+      <c r="BH36" s="16"/>
+      <c r="BI36" s="16"/>
+      <c r="BJ36" s="16"/>
+      <c r="BK36" s="16"/>
+      <c r="BL36" s="16"/>
+      <c r="BM36" s="16"/>
+      <c r="BN36" s="16"/>
+    </row>
+    <row r="37" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="47"/>
+      <c r="B37" s="44"/>
+      <c r="C37" s="41"/>
+      <c r="D37" s="41"/>
+      <c r="E37" s="51"/>
+      <c r="F37" s="54"/>
+      <c r="G37" s="55"/>
+      <c r="H37" s="62"/>
+      <c r="I37" s="54"/>
+      <c r="J37" s="55"/>
+      <c r="K37" s="55"/>
+      <c r="L37" s="62"/>
+      <c r="M37" s="16"/>
+      <c r="N37" s="16"/>
+      <c r="O37" s="16"/>
+      <c r="P37" s="16"/>
+      <c r="Q37" s="16"/>
+      <c r="R37" s="16"/>
+      <c r="S37" s="16"/>
+      <c r="T37" s="16"/>
+      <c r="U37" s="16"/>
+      <c r="V37" s="16"/>
+      <c r="W37" s="16"/>
+      <c r="X37" s="16"/>
+      <c r="Y37" s="16"/>
+      <c r="Z37" s="16"/>
+      <c r="AA37" s="16"/>
+      <c r="AB37" s="16"/>
+      <c r="AC37" s="16"/>
+      <c r="AD37" s="16"/>
+      <c r="AE37" s="16"/>
+      <c r="AF37" s="16"/>
+      <c r="AG37" s="16"/>
+      <c r="AH37" s="16"/>
+      <c r="AI37" s="16"/>
+      <c r="AJ37" s="16"/>
+      <c r="AK37" s="16"/>
+      <c r="AL37" s="16"/>
+      <c r="AM37" s="16"/>
+      <c r="AN37" s="16"/>
+      <c r="AO37" s="16"/>
+      <c r="AP37" s="16"/>
+      <c r="AQ37" s="16"/>
+      <c r="AR37" s="16"/>
+      <c r="AS37" s="16"/>
+      <c r="AT37" s="16"/>
+      <c r="AU37" s="16"/>
+      <c r="AV37" s="16"/>
+      <c r="AW37" s="16"/>
+      <c r="AX37" s="16"/>
+      <c r="AY37" s="16"/>
+      <c r="AZ37" s="16"/>
+      <c r="BA37" s="16"/>
+      <c r="BB37" s="16"/>
+      <c r="BC37" s="16"/>
+      <c r="BD37" s="16"/>
+      <c r="BE37" s="16"/>
+      <c r="BF37" s="16"/>
+      <c r="BG37" s="16"/>
+      <c r="BH37" s="16"/>
+      <c r="BI37" s="16"/>
+      <c r="BJ37" s="16"/>
+      <c r="BK37" s="16"/>
+      <c r="BL37" s="16"/>
+      <c r="BM37" s="16"/>
+      <c r="BN37" s="16"/>
+    </row>
+    <row r="38" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="47"/>
+      <c r="B38" s="44"/>
+      <c r="C38" s="41"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="51"/>
+      <c r="F38" s="54"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="62"/>
+      <c r="I38" s="54"/>
+      <c r="J38" s="55"/>
+      <c r="K38" s="55"/>
+      <c r="L38" s="62"/>
+      <c r="M38" s="16"/>
+      <c r="N38" s="16"/>
+      <c r="O38" s="16"/>
+      <c r="P38" s="16"/>
+      <c r="Q38" s="16"/>
+      <c r="R38" s="16"/>
+      <c r="S38" s="16"/>
+      <c r="T38" s="16"/>
+      <c r="U38" s="16"/>
+      <c r="V38" s="16"/>
+      <c r="W38" s="16"/>
+      <c r="X38" s="16"/>
+      <c r="Y38" s="16"/>
+      <c r="Z38" s="16"/>
+      <c r="AA38" s="16"/>
+      <c r="AB38" s="16"/>
+      <c r="AC38" s="16"/>
+      <c r="AD38" s="16"/>
+      <c r="AE38" s="16"/>
+      <c r="AF38" s="16"/>
+      <c r="AG38" s="16"/>
+      <c r="AH38" s="16"/>
+      <c r="AI38" s="16"/>
+      <c r="AJ38" s="16"/>
+      <c r="AK38" s="16"/>
+      <c r="AL38" s="16"/>
+      <c r="AM38" s="16"/>
+      <c r="AN38" s="16"/>
+      <c r="AO38" s="16"/>
+      <c r="AP38" s="16"/>
+      <c r="AQ38" s="16"/>
+      <c r="AR38" s="16"/>
+      <c r="AS38" s="16"/>
+      <c r="AT38" s="16"/>
+      <c r="AU38" s="16"/>
+      <c r="AV38" s="16"/>
+      <c r="AW38" s="16"/>
+      <c r="AX38" s="16"/>
+      <c r="AY38" s="16"/>
+      <c r="AZ38" s="16"/>
+      <c r="BA38" s="16"/>
+      <c r="BB38" s="16"/>
+      <c r="BC38" s="16"/>
+      <c r="BD38" s="16"/>
+      <c r="BE38" s="16"/>
+      <c r="BF38" s="16"/>
+      <c r="BG38" s="16"/>
+      <c r="BH38" s="16"/>
+      <c r="BI38" s="16"/>
+      <c r="BJ38" s="16"/>
+      <c r="BK38" s="16"/>
+      <c r="BL38" s="16"/>
+      <c r="BM38" s="16"/>
+      <c r="BN38" s="16"/>
+    </row>
+    <row r="39" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="47"/>
+      <c r="B39" s="44"/>
+      <c r="C39" s="41"/>
+      <c r="D39" s="41"/>
+      <c r="E39" s="51"/>
+      <c r="F39" s="54"/>
+      <c r="G39" s="55"/>
+      <c r="H39" s="62" t="str">
         <f t="shared" si="5"/>
         <v/>
       </c>
-      <c r="I34" s="58"/>
-      <c r="J34" s="59"/>
-      <c r="K34" s="59"/>
-      <c r="L34" s="64" t="str">
+      <c r="I39" s="54"/>
+      <c r="J39" s="55"/>
+      <c r="K39" s="55"/>
+      <c r="L39" s="62" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="M34" s="18"/>
-      <c r="N34" s="18"/>
-      <c r="O34" s="18"/>
-      <c r="P34" s="18"/>
-      <c r="Q34" s="18"/>
-      <c r="R34" s="18"/>
-      <c r="S34" s="18"/>
-      <c r="T34" s="18"/>
-      <c r="U34" s="18"/>
-      <c r="V34" s="18"/>
-      <c r="W34" s="18"/>
-      <c r="X34" s="18"/>
-      <c r="Y34" s="18"/>
-      <c r="Z34" s="18"/>
-      <c r="AA34" s="18"/>
-      <c r="AB34" s="18"/>
-      <c r="AC34" s="18"/>
-      <c r="AD34" s="18"/>
-      <c r="AE34" s="18"/>
-      <c r="AF34" s="18"/>
-      <c r="AG34" s="18"/>
-      <c r="AH34" s="18"/>
-      <c r="AI34" s="18"/>
-      <c r="AJ34" s="18"/>
-      <c r="AK34" s="18"/>
-      <c r="AL34" s="18"/>
-      <c r="AM34" s="18"/>
-      <c r="AN34" s="18"/>
-      <c r="AO34" s="18"/>
-      <c r="AP34" s="18"/>
-      <c r="AQ34" s="18"/>
-      <c r="AR34" s="18"/>
-      <c r="AS34" s="18"/>
-      <c r="AT34" s="18"/>
-      <c r="AU34" s="18"/>
-      <c r="AV34" s="18"/>
-      <c r="AW34" s="18"/>
-      <c r="AX34" s="18"/>
-      <c r="AY34" s="18"/>
-      <c r="AZ34" s="18"/>
-      <c r="BA34" s="18"/>
-      <c r="BB34" s="18"/>
-      <c r="BC34" s="18"/>
-      <c r="BD34" s="18"/>
-      <c r="BE34" s="18"/>
-      <c r="BF34" s="18"/>
-      <c r="BG34" s="18"/>
-      <c r="BH34" s="18"/>
-      <c r="BI34" s="18"/>
-      <c r="BJ34" s="18"/>
-      <c r="BK34" s="18"/>
-      <c r="BL34" s="18"/>
-      <c r="BM34" s="18"/>
-      <c r="BN34" s="18"/>
-    </row>
-    <row r="36" spans="1:66" ht="15" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-    </row>
-    <row r="37" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A37" s="65"/>
+      <c r="M39" s="16"/>
+      <c r="N39" s="16"/>
+      <c r="O39" s="16"/>
+      <c r="P39" s="16"/>
+      <c r="Q39" s="16"/>
+      <c r="R39" s="16"/>
+      <c r="S39" s="16"/>
+      <c r="T39" s="16"/>
+      <c r="U39" s="16"/>
+      <c r="V39" s="16"/>
+      <c r="W39" s="16"/>
+      <c r="X39" s="16"/>
+      <c r="Y39" s="16"/>
+      <c r="Z39" s="16"/>
+      <c r="AA39" s="16"/>
+      <c r="AB39" s="16"/>
+      <c r="AC39" s="16"/>
+      <c r="AD39" s="16"/>
+      <c r="AE39" s="16"/>
+      <c r="AF39" s="16"/>
+      <c r="AG39" s="16"/>
+      <c r="AH39" s="16"/>
+      <c r="AI39" s="16"/>
+      <c r="AJ39" s="16"/>
+      <c r="AK39" s="16"/>
+      <c r="AL39" s="16"/>
+      <c r="AM39" s="16"/>
+      <c r="AN39" s="16"/>
+      <c r="AO39" s="16"/>
+      <c r="AP39" s="16"/>
+      <c r="AQ39" s="16"/>
+      <c r="AR39" s="16"/>
+      <c r="AS39" s="16"/>
+      <c r="AT39" s="16"/>
+      <c r="AU39" s="16"/>
+      <c r="AV39" s="16"/>
+      <c r="AW39" s="16"/>
+      <c r="AX39" s="16"/>
+      <c r="AY39" s="16"/>
+      <c r="AZ39" s="16"/>
+      <c r="BA39" s="16"/>
+      <c r="BB39" s="16"/>
+      <c r="BC39" s="16"/>
+      <c r="BD39" s="16"/>
+      <c r="BE39" s="16"/>
+      <c r="BF39" s="16"/>
+      <c r="BG39" s="16"/>
+      <c r="BH39" s="16"/>
+      <c r="BI39" s="16"/>
+      <c r="BJ39" s="16"/>
+      <c r="BK39" s="16"/>
+      <c r="BL39" s="16"/>
+      <c r="BM39" s="16"/>
+      <c r="BN39" s="16"/>
+    </row>
+    <row r="40" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="49"/>
+      <c r="B40" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="43"/>
+      <c r="D40" s="43"/>
+      <c r="E40" s="53"/>
+      <c r="F40" s="58"/>
+      <c r="G40" s="59"/>
+      <c r="H40" s="64" t="str">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+      <c r="I40" s="58"/>
+      <c r="J40" s="59"/>
+      <c r="K40" s="59"/>
+      <c r="L40" s="64" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M40" s="18"/>
+      <c r="N40" s="18"/>
+      <c r="O40" s="18"/>
+      <c r="P40" s="18"/>
+      <c r="Q40" s="18"/>
+      <c r="R40" s="18"/>
+      <c r="S40" s="18"/>
+      <c r="T40" s="18"/>
+      <c r="U40" s="18"/>
+      <c r="V40" s="18"/>
+      <c r="W40" s="18"/>
+      <c r="X40" s="18"/>
+      <c r="Y40" s="18"/>
+      <c r="Z40" s="18"/>
+      <c r="AA40" s="18"/>
+      <c r="AB40" s="18"/>
+      <c r="AC40" s="18"/>
+      <c r="AD40" s="18"/>
+      <c r="AE40" s="18"/>
+      <c r="AF40" s="18"/>
+      <c r="AG40" s="18"/>
+      <c r="AH40" s="18"/>
+      <c r="AI40" s="18"/>
+      <c r="AJ40" s="18"/>
+      <c r="AK40" s="18"/>
+      <c r="AL40" s="18"/>
+      <c r="AM40" s="18"/>
+      <c r="AN40" s="18"/>
+      <c r="AO40" s="18"/>
+      <c r="AP40" s="18"/>
+      <c r="AQ40" s="18"/>
+      <c r="AR40" s="18"/>
+      <c r="AS40" s="18"/>
+      <c r="AT40" s="18"/>
+      <c r="AU40" s="18"/>
+      <c r="AV40" s="18"/>
+      <c r="AW40" s="18"/>
+      <c r="AX40" s="18"/>
+      <c r="AY40" s="18"/>
+      <c r="AZ40" s="18"/>
+      <c r="BA40" s="18"/>
+      <c r="BB40" s="18"/>
+      <c r="BC40" s="18"/>
+      <c r="BD40" s="18"/>
+      <c r="BE40" s="18"/>
+      <c r="BF40" s="18"/>
+      <c r="BG40" s="18"/>
+      <c r="BH40" s="18"/>
+      <c r="BI40" s="18"/>
+      <c r="BJ40" s="18"/>
+      <c r="BK40" s="18"/>
+      <c r="BL40" s="18"/>
+      <c r="BM40" s="18"/>
+      <c r="BN40" s="18"/>
+    </row>
+    <row r="42" spans="1:66" ht="15" x14ac:dyDescent="0.25">
+      <c r="A42" s="19"/>
+    </row>
+    <row r="43" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A43" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F4:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E34">
+  <conditionalFormatting sqref="E9:E40">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -4489,7 +5008,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M9:BN34">
+  <conditionalFormatting sqref="M9:BN40">
     <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
       <formula>NOT(AND(MAX($J9,$G9)&gt;=M$6,MIN($I9,$F9)&lt;N$6))</formula>
     </cfRule>
@@ -4500,7 +5019,7 @@
       <formula>AND($J9&gt;=M$6,$I9&lt;N$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M7:BN34">
+  <conditionalFormatting sqref="M7:BN40">
     <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
     </cfRule>
@@ -4561,7 +5080,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E9:E34</xm:sqref>
+          <xm:sqref>E9:E40</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Project Plan Update Signed-off-by: May Alaa <mayelfkiy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
   <si>
     <t>HELP</t>
   </si>
@@ -276,6 +276,15 @@
   </si>
   <si>
     <t>Update RTM</t>
+  </si>
+  <si>
+    <t>Week 1</t>
+  </si>
+  <si>
+    <t>Week 2</t>
+  </si>
+  <si>
+    <t>Amira</t>
   </si>
 </sst>
 </file>
@@ -962,7 +971,77 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="21">
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <border>
         <left style="thin">
@@ -1094,15 +1173,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9">
-      <tableStyleElement type="wholeTable" dxfId="12"/>
-      <tableStyleElement type="headerRow" dxfId="11"/>
-      <tableStyleElement type="totalRow" dxfId="10"/>
-      <tableStyleElement type="firstColumn" dxfId="9"/>
-      <tableStyleElement type="lastColumn" dxfId="8"/>
-      <tableStyleElement type="firstRowStripe" dxfId="7"/>
-      <tableStyleElement type="secondRowStripe" dxfId="6"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="5"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="4"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstColumn" dxfId="17"/>
+      <tableStyleElement type="lastColumn" dxfId="16"/>
+      <tableStyleElement type="firstRowStripe" dxfId="15"/>
+      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="12"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1224,7 +1303,7 @@
                   <a14:compatExt spid="_x0000_s6145"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1274,7 +1353,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1329,7 +1408,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1630,10 +1709,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO43"/>
+  <dimension ref="A1:BO45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A9" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H23" sqref="H23"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2690,39 +2769,21 @@
       <c r="BM10" s="16"/>
       <c r="BN10" s="16"/>
     </row>
-    <row r="11" spans="1:67" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="47"/>
-      <c r="B11" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C11" s="75" t="s">
-        <v>60</v>
-      </c>
-      <c r="D11" s="75" t="s">
-        <v>67</v>
-      </c>
-      <c r="E11" s="51">
-        <v>1</v>
-      </c>
-      <c r="F11" s="54">
-        <v>43852</v>
-      </c>
-      <c r="G11" s="55">
-        <v>43853</v>
-      </c>
-      <c r="H11" s="62">
-        <f t="shared" ref="H11:H23" si="3">IF(OR(ISBLANK(F11),ISBLANK(G11)),"",G11-F11+1)</f>
-        <v>2</v>
-      </c>
-      <c r="I11" s="54">
-        <v>43852</v>
-      </c>
-      <c r="J11" s="55"/>
-      <c r="K11" s="55"/>
-      <c r="L11" s="62" t="str">
-        <f t="shared" ref="L11:L40" si="4">IF(OR(ISBLANK(I11),ISBLANK(J11)),"",J11-I11+1)</f>
-        <v/>
-      </c>
+    <row r="11" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="48"/>
+      <c r="B11" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="56"/>
+      <c r="G11" s="57"/>
+      <c r="H11" s="63"/>
+      <c r="I11" s="56"/>
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="63"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
@@ -2778,37 +2839,37 @@
       <c r="BM11" s="16"/>
       <c r="BN11" s="16"/>
     </row>
-    <row r="12" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:67" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C12" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D12" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="75" t="s">
+        <v>60</v>
+      </c>
+      <c r="D12" s="75" t="s">
         <v>67</v>
       </c>
       <c r="E12" s="51">
         <v>1</v>
       </c>
       <c r="F12" s="54">
-        <v>43854</v>
+        <v>43852</v>
       </c>
       <c r="G12" s="55">
-        <v>43854</v>
+        <v>43853</v>
       </c>
       <c r="H12" s="62">
-        <f t="shared" si="3"/>
-        <v>1</v>
+        <f t="shared" ref="H12:H25" si="3">IF(OR(ISBLANK(F12),ISBLANK(G12)),"",G12-F12+1)</f>
+        <v>2</v>
       </c>
       <c r="I12" s="54">
-        <v>43854</v>
+        <v>43852</v>
       </c>
       <c r="J12" s="55"/>
       <c r="K12" s="55"/>
       <c r="L12" s="62" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="L12:L42" si="4">IF(OR(ISBLANK(I12),ISBLANK(J12)),"",J12-I12+1)</f>
         <v/>
       </c>
       <c r="M12" s="16"/>
@@ -2823,8 +2884,8 @@
       <c r="V12" s="16"/>
       <c r="W12" s="16"/>
       <c r="X12" s="16"/>
-      <c r="Y12" s="17"/>
-      <c r="Z12" s="17"/>
+      <c r="Y12" s="16"/>
+      <c r="Z12" s="16"/>
       <c r="AA12" s="16"/>
       <c r="AB12" s="16"/>
       <c r="AC12" s="16"/>
@@ -2869,10 +2930,10 @@
     <row r="13" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C13" s="41" t="s">
-        <v>68</v>
+        <v>61</v>
       </c>
       <c r="D13" s="41" t="s">
         <v>67</v>
@@ -2911,8 +2972,8 @@
       <c r="V13" s="16"/>
       <c r="W13" s="16"/>
       <c r="X13" s="16"/>
-      <c r="Y13" s="16"/>
-      <c r="Z13" s="16"/>
+      <c r="Y13" s="17"/>
+      <c r="Z13" s="17"/>
       <c r="AA13" s="16"/>
       <c r="AB13" s="16"/>
       <c r="AC13" s="16"/>
@@ -2957,10 +3018,10 @@
     <row r="14" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="15" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C14" s="41" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="D14" s="41" t="s">
         <v>67</v>
@@ -2969,17 +3030,17 @@
         <v>1</v>
       </c>
       <c r="F14" s="54">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="G14" s="55">
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="H14" s="62">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
       <c r="I14" s="54">
-        <v>43852</v>
+        <v>43854</v>
       </c>
       <c r="J14" s="55"/>
       <c r="K14" s="55"/>
@@ -3003,7 +3064,7 @@
       <c r="Z14" s="16"/>
       <c r="AA14" s="16"/>
       <c r="AB14" s="16"/>
-      <c r="AC14" s="17"/>
+      <c r="AC14" s="16"/>
       <c r="AD14" s="16"/>
       <c r="AE14" s="16"/>
       <c r="AF14" s="16"/>
@@ -3045,10 +3106,10 @@
     <row r="15" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
       <c r="B15" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C15" s="41" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D15" s="41" t="s">
         <v>67</v>
@@ -3057,17 +3118,17 @@
         <v>1</v>
       </c>
       <c r="F15" s="54">
-        <v>43857</v>
+        <v>43853</v>
       </c>
       <c r="G15" s="55">
-        <v>43868</v>
+        <v>43853</v>
       </c>
       <c r="H15" s="62">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I15" s="54">
-        <v>43858</v>
+        <v>43852</v>
       </c>
       <c r="J15" s="55"/>
       <c r="K15" s="55"/>
@@ -3091,7 +3152,7 @@
       <c r="Z15" s="16"/>
       <c r="AA15" s="16"/>
       <c r="AB15" s="16"/>
-      <c r="AC15" s="16"/>
+      <c r="AC15" s="17"/>
       <c r="AD15" s="16"/>
       <c r="AE15" s="16"/>
       <c r="AF15" s="16"/>
@@ -3133,29 +3194,36 @@
     <row r="16" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="15" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="C16" s="41" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="D16" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="51"/>
+      <c r="E16" s="51">
+        <v>1</v>
+      </c>
       <c r="F16" s="54">
-        <v>43862</v>
+        <v>43857</v>
       </c>
       <c r="G16" s="55">
-        <v>43863</v>
+        <v>43868</v>
       </c>
       <c r="H16" s="62">
         <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-      <c r="I16" s="54"/>
+        <v>12</v>
+      </c>
+      <c r="I16" s="54">
+        <v>43858</v>
+      </c>
       <c r="J16" s="55"/>
       <c r="K16" s="55"/>
-      <c r="L16" s="62"/>
+      <c r="L16" s="62" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
@@ -3212,31 +3280,20 @@
       <c r="BN16" s="16"/>
     </row>
     <row r="17" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="47"/>
-      <c r="B17" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="41" t="s">
-        <v>61</v>
-      </c>
-      <c r="D17" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E17" s="51"/>
-      <c r="F17" s="54">
-        <v>43865</v>
-      </c>
-      <c r="G17" s="55">
-        <v>43866</v>
-      </c>
-      <c r="H17" s="62">
-        <f>IF(OR(ISBLANK(F17),ISBLANK(G17)),"",G17-F17+1)</f>
-        <v>2</v>
-      </c>
-      <c r="I17" s="54"/>
-      <c r="J17" s="55"/>
-      <c r="K17" s="55"/>
-      <c r="L17" s="62"/>
+      <c r="A17" s="48"/>
+      <c r="B17" s="45" t="s">
+        <v>79</v>
+      </c>
+      <c r="C17" s="42"/>
+      <c r="D17" s="42"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="56"/>
+      <c r="G17" s="57"/>
+      <c r="H17" s="63"/>
+      <c r="I17" s="56"/>
+      <c r="J17" s="57"/>
+      <c r="K17" s="57"/>
+      <c r="L17" s="63"/>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
       <c r="O17" s="16"/>
@@ -3295,10 +3352,10 @@
     <row r="18" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="15" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C18" s="41" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D18" s="41" t="s">
         <v>67</v>
@@ -3308,19 +3365,16 @@
         <v>43862</v>
       </c>
       <c r="G18" s="55">
-        <v>43864</v>
+        <v>43863</v>
       </c>
       <c r="H18" s="62">
-        <f>IF(OR(ISBLANK(F18),ISBLANK(G18)),"",G18-F18+1)</f>
-        <v>3</v>
+        <f t="shared" si="3"/>
+        <v>2</v>
       </c>
       <c r="I18" s="54"/>
       <c r="J18" s="55"/>
       <c r="K18" s="55"/>
-      <c r="L18" s="62" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="L18" s="62"/>
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
@@ -3379,23 +3433,23 @@
     <row r="19" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="15" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C19" s="41" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D19" s="41" t="s">
         <v>67</v>
       </c>
       <c r="E19" s="51"/>
       <c r="F19" s="54">
-        <v>43864</v>
+        <v>43865</v>
       </c>
       <c r="G19" s="55">
-        <v>43865</v>
+        <v>43866</v>
       </c>
       <c r="H19" s="62">
-        <f>IF(OR(ISBLANK(F19),ISBLANK(G19)),"",G19-F19+1)</f>
+        <f t="shared" ref="H19:H24" si="5">IF(OR(ISBLANK(F19),ISBLANK(G19)),"",G19-F19+1)</f>
         <v>2</v>
       </c>
       <c r="I19" s="54"/>
@@ -3460,29 +3514,32 @@
     <row r="20" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="15" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="C20" s="41" t="s">
-        <v>70</v>
+        <v>80</v>
       </c>
       <c r="D20" s="41" t="s">
         <v>67</v>
       </c>
       <c r="E20" s="51"/>
       <c r="F20" s="54">
-        <v>43866</v>
+        <v>43862</v>
       </c>
       <c r="G20" s="55">
-        <v>43867</v>
+        <v>43864</v>
       </c>
       <c r="H20" s="62">
-        <f>IF(OR(ISBLANK(F20),ISBLANK(G20)),"",G20-F20+1)</f>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>3</v>
       </c>
       <c r="I20" s="54"/>
       <c r="J20" s="55"/>
       <c r="K20" s="55"/>
-      <c r="L20" s="62"/>
+      <c r="L20" s="62" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
@@ -3541,10 +3598,10 @@
     <row r="21" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="15" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C21" s="41" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
       <c r="D21" s="41" t="s">
         <v>67</v>
@@ -3557,7 +3614,7 @@
         <v>43865</v>
       </c>
       <c r="H21" s="62">
-        <f>IF(OR(ISBLANK(F21),ISBLANK(G21)),"",G21-F21+1)</f>
+        <f t="shared" si="5"/>
         <v>2</v>
       </c>
       <c r="I21" s="54"/>
@@ -3622,24 +3679,24 @@
     <row r="22" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
       <c r="B22" s="15" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="C22" s="41" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="D22" s="41" t="s">
         <v>67</v>
       </c>
       <c r="E22" s="51"/>
       <c r="F22" s="54">
-        <v>43867</v>
+        <v>43866</v>
       </c>
       <c r="G22" s="55">
-        <v>43868</v>
+        <v>43866</v>
       </c>
       <c r="H22" s="62">
-        <f>IF(OR(ISBLANK(F22),ISBLANK(G22)),"",G22-F22+1)</f>
-        <v>2</v>
+        <f t="shared" si="5"/>
+        <v>1</v>
       </c>
       <c r="I22" s="54"/>
       <c r="J22" s="55"/>
@@ -3703,24 +3760,29 @@
     <row r="23" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
       <c r="B23" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
+        <v>75</v>
+      </c>
+      <c r="C23" s="41" t="s">
+        <v>76</v>
+      </c>
+      <c r="D23" s="41" t="s">
+        <v>67</v>
+      </c>
       <c r="E23" s="51"/>
-      <c r="F23" s="54"/>
-      <c r="G23" s="55"/>
-      <c r="H23" s="62" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="F23" s="54">
+        <v>43864</v>
+      </c>
+      <c r="G23" s="55">
+        <v>43865</v>
+      </c>
+      <c r="H23" s="62">
+        <f t="shared" si="5"/>
+        <v>2</v>
       </c>
       <c r="I23" s="54"/>
       <c r="J23" s="55"/>
       <c r="K23" s="55"/>
-      <c r="L23" s="62" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="L23" s="62"/>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>
@@ -3733,10 +3795,10 @@
       <c r="V23" s="16"/>
       <c r="W23" s="16"/>
       <c r="X23" s="16"/>
-      <c r="Y23" s="17"/>
+      <c r="Y23" s="16"/>
       <c r="Z23" s="16"/>
       <c r="AA23" s="16"/>
-      <c r="AB23" s="17"/>
+      <c r="AB23" s="16"/>
       <c r="AC23" s="16"/>
       <c r="AD23" s="16"/>
       <c r="AE23" s="16"/>
@@ -3777,26 +3839,31 @@
       <c r="BN23" s="16"/>
     </row>
     <row r="24" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="48"/>
-      <c r="B24" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="52"/>
-      <c r="F24" s="56"/>
-      <c r="G24" s="57"/>
-      <c r="H24" s="63" t="str">
-        <f t="shared" ref="H24:H40" si="5">IF(OR(ISBLANK(F24),ISBLANK(G24)),"",G24-F24+1)</f>
-        <v/>
-      </c>
-      <c r="I24" s="56"/>
-      <c r="J24" s="57"/>
-      <c r="K24" s="57"/>
-      <c r="L24" s="63" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="A24" s="47"/>
+      <c r="B24" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="C24" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="D24" s="41" t="s">
+        <v>67</v>
+      </c>
+      <c r="E24" s="51"/>
+      <c r="F24" s="54">
+        <v>43867</v>
+      </c>
+      <c r="G24" s="55">
+        <v>43868</v>
+      </c>
+      <c r="H24" s="62">
+        <f t="shared" si="5"/>
+        <v>2</v>
+      </c>
+      <c r="I24" s="54"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="62"/>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
@@ -3855,18 +3922,24 @@
     <row r="25" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
       <c r="B25" s="15" t="s">
-        <v>15</v>
+        <v>44</v>
       </c>
       <c r="C25" s="41"/>
       <c r="D25" s="41"/>
       <c r="E25" s="51"/>
       <c r="F25" s="54"/>
       <c r="G25" s="55"/>
-      <c r="H25" s="62"/>
+      <c r="H25" s="62" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
       <c r="I25" s="54"/>
       <c r="J25" s="55"/>
       <c r="K25" s="55"/>
-      <c r="L25" s="62"/>
+      <c r="L25" s="62" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
@@ -3879,10 +3952,10 @@
       <c r="V25" s="16"/>
       <c r="W25" s="16"/>
       <c r="X25" s="16"/>
-      <c r="Y25" s="16"/>
+      <c r="Y25" s="17"/>
       <c r="Z25" s="16"/>
       <c r="AA25" s="16"/>
-      <c r="AB25" s="16"/>
+      <c r="AB25" s="17"/>
       <c r="AC25" s="16"/>
       <c r="AD25" s="16"/>
       <c r="AE25" s="16"/>
@@ -3923,20 +3996,26 @@
       <c r="BN25" s="16"/>
     </row>
     <row r="26" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="47"/>
-      <c r="B26" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="54"/>
-      <c r="G26" s="55"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="54"/>
-      <c r="J26" s="55"/>
-      <c r="K26" s="55"/>
-      <c r="L26" s="62"/>
+      <c r="A26" s="48"/>
+      <c r="B26" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="42"/>
+      <c r="D26" s="42"/>
+      <c r="E26" s="52"/>
+      <c r="F26" s="56"/>
+      <c r="G26" s="57"/>
+      <c r="H26" s="63" t="str">
+        <f t="shared" ref="H26:H42" si="6">IF(OR(ISBLANK(F26),ISBLANK(G26)),"",G26-F26+1)</f>
+        <v/>
+      </c>
+      <c r="I26" s="56"/>
+      <c r="J26" s="57"/>
+      <c r="K26" s="57"/>
+      <c r="L26" s="63" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
       <c r="O26" s="16"/>
@@ -3995,7 +4074,7 @@
     <row r="27" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
       <c r="B27" s="15" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C27" s="41"/>
       <c r="D27" s="41"/>
@@ -4065,7 +4144,7 @@
     <row r="28" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
       <c r="B28" s="15" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="C28" s="41"/>
       <c r="D28" s="41"/>
@@ -4135,7 +4214,7 @@
     <row r="29" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
       <c r="B29" s="15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C29" s="41"/>
       <c r="D29" s="41"/>
@@ -4205,7 +4284,7 @@
     <row r="30" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="47"/>
       <c r="B30" s="15" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="C30" s="41"/>
       <c r="D30" s="41"/>
@@ -4274,23 +4353,19 @@
     </row>
     <row r="31" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="47"/>
-      <c r="B31" s="44"/>
+      <c r="B31" s="15" t="s">
+        <v>13</v>
+      </c>
       <c r="C31" s="41"/>
       <c r="D31" s="41"/>
       <c r="E31" s="51"/>
       <c r="F31" s="54"/>
       <c r="G31" s="55"/>
-      <c r="H31" s="62" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="H31" s="62"/>
       <c r="I31" s="54"/>
       <c r="J31" s="55"/>
       <c r="K31" s="55"/>
-      <c r="L31" s="62" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="L31" s="62"/>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
       <c r="O31" s="16"/>
@@ -4348,23 +4423,19 @@
     </row>
     <row r="32" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="47"/>
-      <c r="B32" s="44"/>
+      <c r="B32" s="15" t="s">
+        <v>17</v>
+      </c>
       <c r="C32" s="41"/>
       <c r="D32" s="41"/>
       <c r="E32" s="51"/>
       <c r="F32" s="54"/>
       <c r="G32" s="55"/>
-      <c r="H32" s="62" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="H32" s="62"/>
       <c r="I32" s="54"/>
       <c r="J32" s="55"/>
       <c r="K32" s="55"/>
-      <c r="L32" s="62" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="L32" s="62"/>
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
       <c r="O32" s="16"/>
@@ -4429,7 +4500,7 @@
       <c r="F33" s="54"/>
       <c r="G33" s="55"/>
       <c r="H33" s="62" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I33" s="54"/>
@@ -4502,11 +4573,17 @@
       <c r="E34" s="51"/>
       <c r="F34" s="54"/>
       <c r="G34" s="55"/>
-      <c r="H34" s="62"/>
+      <c r="H34" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
       <c r="I34" s="54"/>
       <c r="J34" s="55"/>
       <c r="K34" s="55"/>
-      <c r="L34" s="62"/>
+      <c r="L34" s="62" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="M34" s="16"/>
       <c r="N34" s="16"/>
       <c r="O34" s="16"/>
@@ -4570,11 +4647,17 @@
       <c r="E35" s="51"/>
       <c r="F35" s="54"/>
       <c r="G35" s="55"/>
-      <c r="H35" s="62"/>
+      <c r="H35" s="62" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
       <c r="I35" s="54"/>
       <c r="J35" s="55"/>
       <c r="K35" s="55"/>
-      <c r="L35" s="62"/>
+      <c r="L35" s="62" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
       <c r="O35" s="16"/>
@@ -4842,17 +4925,11 @@
       <c r="E39" s="51"/>
       <c r="F39" s="54"/>
       <c r="G39" s="55"/>
-      <c r="H39" s="62" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="H39" s="62"/>
       <c r="I39" s="54"/>
       <c r="J39" s="55"/>
       <c r="K39" s="55"/>
-      <c r="L39" s="62" t="str">
-        <f t="shared" si="4"/>
-        <v/>
-      </c>
+      <c r="L39" s="62"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
@@ -4909,93 +4986,235 @@
       <c r="BN39" s="16"/>
     </row>
     <row r="40" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="49"/>
-      <c r="B40" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="C40" s="43"/>
-      <c r="D40" s="43"/>
-      <c r="E40" s="53"/>
-      <c r="F40" s="58"/>
-      <c r="G40" s="59"/>
-      <c r="H40" s="64" t="str">
-        <f t="shared" si="5"/>
+      <c r="A40" s="47"/>
+      <c r="B40" s="44"/>
+      <c r="C40" s="41"/>
+      <c r="D40" s="41"/>
+      <c r="E40" s="51"/>
+      <c r="F40" s="54"/>
+      <c r="G40" s="55"/>
+      <c r="H40" s="62"/>
+      <c r="I40" s="54"/>
+      <c r="J40" s="55"/>
+      <c r="K40" s="55"/>
+      <c r="L40" s="62"/>
+      <c r="M40" s="16"/>
+      <c r="N40" s="16"/>
+      <c r="O40" s="16"/>
+      <c r="P40" s="16"/>
+      <c r="Q40" s="16"/>
+      <c r="R40" s="16"/>
+      <c r="S40" s="16"/>
+      <c r="T40" s="16"/>
+      <c r="U40" s="16"/>
+      <c r="V40" s="16"/>
+      <c r="W40" s="16"/>
+      <c r="X40" s="16"/>
+      <c r="Y40" s="16"/>
+      <c r="Z40" s="16"/>
+      <c r="AA40" s="16"/>
+      <c r="AB40" s="16"/>
+      <c r="AC40" s="16"/>
+      <c r="AD40" s="16"/>
+      <c r="AE40" s="16"/>
+      <c r="AF40" s="16"/>
+      <c r="AG40" s="16"/>
+      <c r="AH40" s="16"/>
+      <c r="AI40" s="16"/>
+      <c r="AJ40" s="16"/>
+      <c r="AK40" s="16"/>
+      <c r="AL40" s="16"/>
+      <c r="AM40" s="16"/>
+      <c r="AN40" s="16"/>
+      <c r="AO40" s="16"/>
+      <c r="AP40" s="16"/>
+      <c r="AQ40" s="16"/>
+      <c r="AR40" s="16"/>
+      <c r="AS40" s="16"/>
+      <c r="AT40" s="16"/>
+      <c r="AU40" s="16"/>
+      <c r="AV40" s="16"/>
+      <c r="AW40" s="16"/>
+      <c r="AX40" s="16"/>
+      <c r="AY40" s="16"/>
+      <c r="AZ40" s="16"/>
+      <c r="BA40" s="16"/>
+      <c r="BB40" s="16"/>
+      <c r="BC40" s="16"/>
+      <c r="BD40" s="16"/>
+      <c r="BE40" s="16"/>
+      <c r="BF40" s="16"/>
+      <c r="BG40" s="16"/>
+      <c r="BH40" s="16"/>
+      <c r="BI40" s="16"/>
+      <c r="BJ40" s="16"/>
+      <c r="BK40" s="16"/>
+      <c r="BL40" s="16"/>
+      <c r="BM40" s="16"/>
+      <c r="BN40" s="16"/>
+    </row>
+    <row r="41" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="47"/>
+      <c r="B41" s="44"/>
+      <c r="C41" s="41"/>
+      <c r="D41" s="41"/>
+      <c r="E41" s="51"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="55"/>
+      <c r="H41" s="62" t="str">
+        <f t="shared" si="6"/>
         <v/>
       </c>
-      <c r="I40" s="58"/>
-      <c r="J40" s="59"/>
-      <c r="K40" s="59"/>
-      <c r="L40" s="64" t="str">
+      <c r="I41" s="54"/>
+      <c r="J41" s="55"/>
+      <c r="K41" s="55"/>
+      <c r="L41" s="62" t="str">
         <f t="shared" si="4"/>
         <v/>
       </c>
-      <c r="M40" s="18"/>
-      <c r="N40" s="18"/>
-      <c r="O40" s="18"/>
-      <c r="P40" s="18"/>
-      <c r="Q40" s="18"/>
-      <c r="R40" s="18"/>
-      <c r="S40" s="18"/>
-      <c r="T40" s="18"/>
-      <c r="U40" s="18"/>
-      <c r="V40" s="18"/>
-      <c r="W40" s="18"/>
-      <c r="X40" s="18"/>
-      <c r="Y40" s="18"/>
-      <c r="Z40" s="18"/>
-      <c r="AA40" s="18"/>
-      <c r="AB40" s="18"/>
-      <c r="AC40" s="18"/>
-      <c r="AD40" s="18"/>
-      <c r="AE40" s="18"/>
-      <c r="AF40" s="18"/>
-      <c r="AG40" s="18"/>
-      <c r="AH40" s="18"/>
-      <c r="AI40" s="18"/>
-      <c r="AJ40" s="18"/>
-      <c r="AK40" s="18"/>
-      <c r="AL40" s="18"/>
-      <c r="AM40" s="18"/>
-      <c r="AN40" s="18"/>
-      <c r="AO40" s="18"/>
-      <c r="AP40" s="18"/>
-      <c r="AQ40" s="18"/>
-      <c r="AR40" s="18"/>
-      <c r="AS40" s="18"/>
-      <c r="AT40" s="18"/>
-      <c r="AU40" s="18"/>
-      <c r="AV40" s="18"/>
-      <c r="AW40" s="18"/>
-      <c r="AX40" s="18"/>
-      <c r="AY40" s="18"/>
-      <c r="AZ40" s="18"/>
-      <c r="BA40" s="18"/>
-      <c r="BB40" s="18"/>
-      <c r="BC40" s="18"/>
-      <c r="BD40" s="18"/>
-      <c r="BE40" s="18"/>
-      <c r="BF40" s="18"/>
-      <c r="BG40" s="18"/>
-      <c r="BH40" s="18"/>
-      <c r="BI40" s="18"/>
-      <c r="BJ40" s="18"/>
-      <c r="BK40" s="18"/>
-      <c r="BL40" s="18"/>
-      <c r="BM40" s="18"/>
-      <c r="BN40" s="18"/>
-    </row>
-    <row r="42" spans="1:66" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="19"/>
-    </row>
-    <row r="43" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A43" s="65"/>
+      <c r="M41" s="16"/>
+      <c r="N41" s="16"/>
+      <c r="O41" s="16"/>
+      <c r="P41" s="16"/>
+      <c r="Q41" s="16"/>
+      <c r="R41" s="16"/>
+      <c r="S41" s="16"/>
+      <c r="T41" s="16"/>
+      <c r="U41" s="16"/>
+      <c r="V41" s="16"/>
+      <c r="W41" s="16"/>
+      <c r="X41" s="16"/>
+      <c r="Y41" s="16"/>
+      <c r="Z41" s="16"/>
+      <c r="AA41" s="16"/>
+      <c r="AB41" s="16"/>
+      <c r="AC41" s="16"/>
+      <c r="AD41" s="16"/>
+      <c r="AE41" s="16"/>
+      <c r="AF41" s="16"/>
+      <c r="AG41" s="16"/>
+      <c r="AH41" s="16"/>
+      <c r="AI41" s="16"/>
+      <c r="AJ41" s="16"/>
+      <c r="AK41" s="16"/>
+      <c r="AL41" s="16"/>
+      <c r="AM41" s="16"/>
+      <c r="AN41" s="16"/>
+      <c r="AO41" s="16"/>
+      <c r="AP41" s="16"/>
+      <c r="AQ41" s="16"/>
+      <c r="AR41" s="16"/>
+      <c r="AS41" s="16"/>
+      <c r="AT41" s="16"/>
+      <c r="AU41" s="16"/>
+      <c r="AV41" s="16"/>
+      <c r="AW41" s="16"/>
+      <c r="AX41" s="16"/>
+      <c r="AY41" s="16"/>
+      <c r="AZ41" s="16"/>
+      <c r="BA41" s="16"/>
+      <c r="BB41" s="16"/>
+      <c r="BC41" s="16"/>
+      <c r="BD41" s="16"/>
+      <c r="BE41" s="16"/>
+      <c r="BF41" s="16"/>
+      <c r="BG41" s="16"/>
+      <c r="BH41" s="16"/>
+      <c r="BI41" s="16"/>
+      <c r="BJ41" s="16"/>
+      <c r="BK41" s="16"/>
+      <c r="BL41" s="16"/>
+      <c r="BM41" s="16"/>
+      <c r="BN41" s="16"/>
+    </row>
+    <row r="42" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="49"/>
+      <c r="B42" s="46" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="43"/>
+      <c r="D42" s="43"/>
+      <c r="E42" s="53"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="59"/>
+      <c r="H42" s="64" t="str">
+        <f t="shared" si="6"/>
+        <v/>
+      </c>
+      <c r="I42" s="58"/>
+      <c r="J42" s="59"/>
+      <c r="K42" s="59"/>
+      <c r="L42" s="64" t="str">
+        <f t="shared" si="4"/>
+        <v/>
+      </c>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
+      <c r="T42" s="18"/>
+      <c r="U42" s="18"/>
+      <c r="V42" s="18"/>
+      <c r="W42" s="18"/>
+      <c r="X42" s="18"/>
+      <c r="Y42" s="18"/>
+      <c r="Z42" s="18"/>
+      <c r="AA42" s="18"/>
+      <c r="AB42" s="18"/>
+      <c r="AC42" s="18"/>
+      <c r="AD42" s="18"/>
+      <c r="AE42" s="18"/>
+      <c r="AF42" s="18"/>
+      <c r="AG42" s="18"/>
+      <c r="AH42" s="18"/>
+      <c r="AI42" s="18"/>
+      <c r="AJ42" s="18"/>
+      <c r="AK42" s="18"/>
+      <c r="AL42" s="18"/>
+      <c r="AM42" s="18"/>
+      <c r="AN42" s="18"/>
+      <c r="AO42" s="18"/>
+      <c r="AP42" s="18"/>
+      <c r="AQ42" s="18"/>
+      <c r="AR42" s="18"/>
+      <c r="AS42" s="18"/>
+      <c r="AT42" s="18"/>
+      <c r="AU42" s="18"/>
+      <c r="AV42" s="18"/>
+      <c r="AW42" s="18"/>
+      <c r="AX42" s="18"/>
+      <c r="AY42" s="18"/>
+      <c r="AZ42" s="18"/>
+      <c r="BA42" s="18"/>
+      <c r="BB42" s="18"/>
+      <c r="BC42" s="18"/>
+      <c r="BD42" s="18"/>
+      <c r="BE42" s="18"/>
+      <c r="BF42" s="18"/>
+      <c r="BG42" s="18"/>
+      <c r="BH42" s="18"/>
+      <c r="BI42" s="18"/>
+      <c r="BJ42" s="18"/>
+      <c r="BK42" s="18"/>
+      <c r="BL42" s="18"/>
+      <c r="BM42" s="18"/>
+      <c r="BN42" s="18"/>
+    </row>
+    <row r="44" spans="1:66" ht="15" x14ac:dyDescent="0.25">
+      <c r="A44" s="19"/>
+    </row>
+    <row r="45" spans="1:66" x14ac:dyDescent="0.2">
+      <c r="A45" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="F4:G4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E40">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="E9:E16 E18:E42">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5008,19 +5227,49 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M9:BN40">
-    <cfRule type="expression" dxfId="3" priority="5" stopIfTrue="1">
+  <conditionalFormatting sqref="M9:BN16 M18:BN42">
+    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
       <formula>NOT(AND(MAX($J9,$G9)&gt;=M$6,MIN($I9,$F9)&lt;N$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="6">
+    <cfRule type="expression" dxfId="10" priority="11">
       <formula>AND($G9&gt;=M$6,$F9&lt;N$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="8" stopIfTrue="1">
+    <cfRule type="expression" dxfId="9" priority="13" stopIfTrue="1">
       <formula>AND($J9&gt;=M$6,$I9&lt;N$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M7:BN40">
-    <cfRule type="expression" dxfId="0" priority="1">
+  <conditionalFormatting sqref="M7:BN16 M18:BN42">
+    <cfRule type="expression" dxfId="8" priority="6">
+      <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="7" tint="0.59999389629810485"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{35B0E45D-0F80-4816-B43B-129D908BE9C3}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17:BN17">
+    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J17,$G17)&gt;=M$6,MIN($I17,$F17)&lt;N$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="4">
+      <formula>AND($G17&gt;=M$6,$F17&lt;N$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+      <formula>AND($J17&gt;=M$6,$I17&lt;N$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M17:BN17">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5080,7 +5329,22 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E9:E40</xm:sqref>
+          <xm:sqref>E9:E16 E18:E42</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{35B0E45D-0F80-4816-B43B-129D908BE9C3}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>E17</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Update the project plan
Signed-off-by: Mohammmedibra96 <mohammedibra96@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\SOFTWARE_ENG_ELECTRIC_BLENDER\SW deliveries log\Project_Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\software\project\SW deliveries log\Project_Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectPlan" sheetId="11" r:id="rId1"/>
@@ -26,7 +26,7 @@
     <definedName name="vertex42_id" hidden="1">"project-planner.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Project Planner Template"</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -290,12 +290,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
   </numFmts>
-  <fonts count="34" x14ac:knownFonts="1">
+  <fonts count="34">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -971,7 +971,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="17">
     <dxf>
       <border>
         <left style="thin">
@@ -979,41 +979,6 @@
         </left>
         <right style="thin">
           <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
         </right>
         <vertical/>
         <horizontal/>
@@ -1173,15 +1138,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="totalRow" dxfId="18"/>
-      <tableStyleElement type="firstColumn" dxfId="17"/>
-      <tableStyleElement type="lastColumn" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="16"/>
+      <tableStyleElement type="headerRow" dxfId="15"/>
+      <tableStyleElement type="totalRow" dxfId="14"/>
+      <tableStyleElement type="firstColumn" dxfId="13"/>
+      <tableStyleElement type="lastColumn" dxfId="12"/>
+      <tableStyleElement type="firstRowStripe" dxfId="11"/>
+      <tableStyleElement type="secondRowStripe" dxfId="10"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="8"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1293,7 +1258,7 @@
           <xdr:col>28</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>180975</xdr:rowOff>
+          <xdr:rowOff>184150</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1303,7 +1268,7 @@
                   <a14:compatExt spid="_x0000_s6145"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1353,7 +1318,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1408,7 +1373,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1711,29 +1676,29 @@
   </sheetPr>
   <dimension ref="A1:BO45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A11" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="5.375" customWidth="1"/>
+    <col min="1" max="1" width="5.33203125" customWidth="1"/>
     <col min="2" max="2" width="19.75" customWidth="1"/>
     <col min="3" max="3" width="13.25" customWidth="1"/>
     <col min="4" max="4" width="13.25" style="72" customWidth="1"/>
-    <col min="5" max="5" width="10.625" customWidth="1"/>
+    <col min="5" max="5" width="10.58203125" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="10" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
-    <col min="8" max="8" width="7.375" customWidth="1"/>
+    <col min="8" max="8" width="7.33203125" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="10" customWidth="1"/>
     <col min="10" max="10" width="9.5" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="72" customWidth="1"/>
     <col min="12" max="12" width="13.75" customWidth="1"/>
-    <col min="13" max="66" width="3.125" customWidth="1"/>
+    <col min="13" max="66" width="3.08203125" customWidth="1"/>
     <col min="67" max="67" width="3.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:67" ht="25">
       <c r="A1" s="60" t="s">
         <v>48</v>
       </c>
@@ -1753,7 +1718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:67" ht="19.5" customHeight="1">
       <c r="A2" s="14" t="s">
         <v>49</v>
       </c>
@@ -1762,7 +1727,7 @@
       <c r="D2" s="14"/>
       <c r="M2" s="69"/>
     </row>
-    <row r="3" spans="1:67" s="72" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:67" s="72" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="71" t="s">
         <v>52</v>
       </c>
@@ -1773,7 +1738,7 @@
       <c r="I3" s="73"/>
       <c r="M3" s="69"/>
     </row>
-    <row r="4" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:67" ht="19.5" customHeight="1">
       <c r="A4" s="71" t="s">
         <v>53</v>
       </c>
@@ -1786,7 +1751,7 @@
       </c>
       <c r="G4" s="77"/>
     </row>
-    <row r="5" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:67" ht="19.5" customHeight="1">
       <c r="A5" s="35"/>
       <c r="E5" s="35" t="s">
         <v>32</v>
@@ -1795,7 +1760,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:67" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:67" ht="18" hidden="1" customHeight="1">
       <c r="A6" s="35"/>
       <c r="E6" s="35" t="s">
         <v>33</v>
@@ -2024,7 +1989,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="7" spans="1:67" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:67" ht="47.25" customHeight="1">
       <c r="A7" s="74" t="s">
         <v>56</v>
       </c>
@@ -2359,7 +2324,7 @@
 '20</v>
       </c>
     </row>
-    <row r="8" spans="1:67" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:67" ht="29.25" customHeight="1" thickBot="1">
       <c r="A8" s="50" t="s">
         <v>27</v>
       </c>
@@ -2613,7 +2578,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:67" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:67" s="8" customFormat="1" ht="14.5" thickBot="1">
       <c r="A9" s="47"/>
       <c r="B9" s="44"/>
       <c r="C9" s="41"/>
@@ -2687,7 +2652,7 @@
       <c r="BM9" s="16"/>
       <c r="BN9" s="16"/>
     </row>
-    <row r="10" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A10" s="48"/>
       <c r="B10" s="45" t="s">
         <v>50</v>
@@ -2769,7 +2734,7 @@
       <c r="BM10" s="16"/>
       <c r="BN10" s="16"/>
     </row>
-    <row r="11" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A11" s="48"/>
       <c r="B11" s="45" t="s">
         <v>78</v>
@@ -2839,7 +2804,7 @@
       <c r="BM11" s="16"/>
       <c r="BN11" s="16"/>
     </row>
-    <row r="12" spans="1:67" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:67" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
       <c r="A12" s="47"/>
       <c r="B12" s="15" t="s">
         <v>57</v>
@@ -2927,7 +2892,7 @@
       <c r="BM12" s="16"/>
       <c r="BN12" s="16"/>
     </row>
-    <row r="13" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A13" s="47"/>
       <c r="B13" s="15" t="s">
         <v>58</v>
@@ -3015,7 +2980,7 @@
       <c r="BM13" s="16"/>
       <c r="BN13" s="16"/>
     </row>
-    <row r="14" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A14" s="47"/>
       <c r="B14" s="15" t="s">
         <v>59</v>
@@ -3103,7 +3068,7 @@
       <c r="BM14" s="16"/>
       <c r="BN14" s="16"/>
     </row>
-    <row r="15" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A15" s="47"/>
       <c r="B15" s="15" t="s">
         <v>62</v>
@@ -3191,7 +3156,7 @@
       <c r="BM15" s="16"/>
       <c r="BN15" s="16"/>
     </row>
-    <row r="16" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A16" s="47"/>
       <c r="B16" s="15" t="s">
         <v>63</v>
@@ -3279,7 +3244,7 @@
       <c r="BM16" s="16"/>
       <c r="BN16" s="16"/>
     </row>
-    <row r="17" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A17" s="48"/>
       <c r="B17" s="45" t="s">
         <v>79</v>
@@ -3349,7 +3314,7 @@
       <c r="BM17" s="16"/>
       <c r="BN17" s="16"/>
     </row>
-    <row r="18" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A18" s="47"/>
       <c r="B18" s="15" t="s">
         <v>69</v>
@@ -3360,7 +3325,9 @@
       <c r="D18" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E18" s="51"/>
+      <c r="E18" s="51">
+        <v>1</v>
+      </c>
       <c r="F18" s="54">
         <v>43862</v>
       </c>
@@ -3371,8 +3338,12 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="I18" s="54"/>
-      <c r="J18" s="55"/>
+      <c r="I18" s="54">
+        <v>43862</v>
+      </c>
+      <c r="J18" s="55">
+        <v>43864</v>
+      </c>
       <c r="K18" s="55"/>
       <c r="L18" s="62"/>
       <c r="M18" s="16"/>
@@ -3430,7 +3401,7 @@
       <c r="BM18" s="16"/>
       <c r="BN18" s="16"/>
     </row>
-    <row r="19" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A19" s="47"/>
       <c r="B19" s="15" t="s">
         <v>71</v>
@@ -3511,7 +3482,7 @@
       <c r="BM19" s="16"/>
       <c r="BN19" s="16"/>
     </row>
-    <row r="20" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A20" s="47"/>
       <c r="B20" s="15" t="s">
         <v>72</v>
@@ -3595,7 +3566,7 @@
       <c r="BM20" s="16"/>
       <c r="BN20" s="16"/>
     </row>
-    <row r="21" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A21" s="47"/>
       <c r="B21" s="15" t="s">
         <v>73</v>
@@ -3676,7 +3647,7 @@
       <c r="BM21" s="16"/>
       <c r="BN21" s="16"/>
     </row>
-    <row r="22" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A22" s="47"/>
       <c r="B22" s="15" t="s">
         <v>74</v>
@@ -3757,7 +3728,7 @@
       <c r="BM22" s="16"/>
       <c r="BN22" s="16"/>
     </row>
-    <row r="23" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A23" s="47"/>
       <c r="B23" s="15" t="s">
         <v>75</v>
@@ -3838,7 +3809,7 @@
       <c r="BM23" s="16"/>
       <c r="BN23" s="16"/>
     </row>
-    <row r="24" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A24" s="47"/>
       <c r="B24" s="15" t="s">
         <v>77</v>
@@ -3919,7 +3890,7 @@
       <c r="BM24" s="16"/>
       <c r="BN24" s="16"/>
     </row>
-    <row r="25" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A25" s="47"/>
       <c r="B25" s="15" t="s">
         <v>44</v>
@@ -3995,7 +3966,7 @@
       <c r="BM25" s="16"/>
       <c r="BN25" s="16"/>
     </row>
-    <row r="26" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A26" s="48"/>
       <c r="B26" s="45" t="s">
         <v>14</v>
@@ -4071,7 +4042,7 @@
       <c r="BM26" s="16"/>
       <c r="BN26" s="16"/>
     </row>
-    <row r="27" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A27" s="47"/>
       <c r="B27" s="15" t="s">
         <v>15</v>
@@ -4141,7 +4112,7 @@
       <c r="BM27" s="16"/>
       <c r="BN27" s="16"/>
     </row>
-    <row r="28" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A28" s="47"/>
       <c r="B28" s="15" t="s">
         <v>16</v>
@@ -4211,7 +4182,7 @@
       <c r="BM28" s="16"/>
       <c r="BN28" s="16"/>
     </row>
-    <row r="29" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A29" s="47"/>
       <c r="B29" s="15" t="s">
         <v>11</v>
@@ -4281,7 +4252,7 @@
       <c r="BM29" s="16"/>
       <c r="BN29" s="16"/>
     </row>
-    <row r="30" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A30" s="47"/>
       <c r="B30" s="15" t="s">
         <v>12</v>
@@ -4351,7 +4322,7 @@
       <c r="BM30" s="16"/>
       <c r="BN30" s="16"/>
     </row>
-    <row r="31" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A31" s="47"/>
       <c r="B31" s="15" t="s">
         <v>13</v>
@@ -4421,7 +4392,7 @@
       <c r="BM31" s="16"/>
       <c r="BN31" s="16"/>
     </row>
-    <row r="32" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A32" s="47"/>
       <c r="B32" s="15" t="s">
         <v>17</v>
@@ -4491,7 +4462,7 @@
       <c r="BM32" s="16"/>
       <c r="BN32" s="16"/>
     </row>
-    <row r="33" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A33" s="47"/>
       <c r="B33" s="44"/>
       <c r="C33" s="41"/>
@@ -4565,7 +4536,7 @@
       <c r="BM33" s="16"/>
       <c r="BN33" s="16"/>
     </row>
-    <row r="34" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A34" s="47"/>
       <c r="B34" s="44"/>
       <c r="C34" s="41"/>
@@ -4639,7 +4610,7 @@
       <c r="BM34" s="16"/>
       <c r="BN34" s="16"/>
     </row>
-    <row r="35" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A35" s="47"/>
       <c r="B35" s="44"/>
       <c r="C35" s="41"/>
@@ -4713,7 +4684,7 @@
       <c r="BM35" s="16"/>
       <c r="BN35" s="16"/>
     </row>
-    <row r="36" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A36" s="47"/>
       <c r="B36" s="44"/>
       <c r="C36" s="41"/>
@@ -4781,7 +4752,7 @@
       <c r="BM36" s="16"/>
       <c r="BN36" s="16"/>
     </row>
-    <row r="37" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A37" s="47"/>
       <c r="B37" s="44"/>
       <c r="C37" s="41"/>
@@ -4849,7 +4820,7 @@
       <c r="BM37" s="16"/>
       <c r="BN37" s="16"/>
     </row>
-    <row r="38" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A38" s="47"/>
       <c r="B38" s="44"/>
       <c r="C38" s="41"/>
@@ -4917,7 +4888,7 @@
       <c r="BM38" s="16"/>
       <c r="BN38" s="16"/>
     </row>
-    <row r="39" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A39" s="47"/>
       <c r="B39" s="44"/>
       <c r="C39" s="41"/>
@@ -4985,7 +4956,7 @@
       <c r="BM39" s="16"/>
       <c r="BN39" s="16"/>
     </row>
-    <row r="40" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A40" s="47"/>
       <c r="B40" s="44"/>
       <c r="C40" s="41"/>
@@ -5053,7 +5024,7 @@
       <c r="BM40" s="16"/>
       <c r="BN40" s="16"/>
     </row>
-    <row r="41" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A41" s="47"/>
       <c r="B41" s="44"/>
       <c r="C41" s="41"/>
@@ -5127,7 +5098,7 @@
       <c r="BM41" s="16"/>
       <c r="BN41" s="16"/>
     </row>
-    <row r="42" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
       <c r="A42" s="49"/>
       <c r="B42" s="46" t="s">
         <v>19</v>
@@ -5203,10 +5174,10 @@
       <c r="BM42" s="18"/>
       <c r="BN42" s="18"/>
     </row>
-    <row r="44" spans="1:66" ht="15" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:66">
       <c r="A44" s="19"/>
     </row>
-    <row r="45" spans="1:66" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:66">
       <c r="A45" s="65"/>
     </row>
   </sheetData>
@@ -5228,18 +5199,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M9:BN16 M18:BN42">
-    <cfRule type="expression" dxfId="11" priority="10" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
       <formula>NOT(AND(MAX($J9,$G9)&gt;=M$6,MIN($I9,$F9)&lt;N$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="11">
+    <cfRule type="expression" dxfId="6" priority="11">
       <formula>AND($G9&gt;=M$6,$F9&lt;N$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="13" stopIfTrue="1">
+    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
       <formula>AND($J9&gt;=M$6,$I9&lt;N$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M7:BN16 M18:BN42">
-    <cfRule type="expression" dxfId="8" priority="6">
+    <cfRule type="expression" dxfId="4" priority="6">
       <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5258,18 +5229,18 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17:BN17">
-    <cfRule type="expression" dxfId="7" priority="3" stopIfTrue="1">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
       <formula>NOT(AND(MAX($J17,$G17)&gt;=M$6,MIN($I17,$F17)&lt;N$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="4">
+    <cfRule type="expression" dxfId="2" priority="4">
       <formula>AND($G17&gt;=M$6,$F17&lt;N$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="5" priority="5" stopIfTrue="1">
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
       <formula>AND($J17&gt;=M$6,$I17&lt;N$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17:BN17">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5303,7 +5274,7 @@
                     <xdr:col>28</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>180975</xdr:rowOff>
+                    <xdr:rowOff>184150</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5360,155 +5331,155 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="68.5" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" ht="33" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4">
       <c r="B2" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="78"/>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4">
       <c r="C3" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" ht="56">
       <c r="B5" s="7" t="s">
         <v>47</v>
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4">
       <c r="B6" s="7"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4">
       <c r="B7" s="20"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" ht="15.5">
       <c r="B8" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" ht="15.5">
       <c r="B9" s="22" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4">
       <c r="B10" s="20"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4">
       <c r="B11" s="7"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="7"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" ht="28">
       <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4">
       <c r="B14" s="7"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="7"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" ht="28">
       <c r="B16" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4">
       <c r="B17" s="7"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="7"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" ht="28">
       <c r="B19" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4">
       <c r="B20" s="7"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4">
       <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="7"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" ht="42">
       <c r="B22" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:4">
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:4" ht="28">
       <c r="B24" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4">
       <c r="A26" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B26" s="7"/>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:4">
       <c r="B27" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:4">
       <c r="B28" s="68" t="s">
         <v>46</v>
       </c>
@@ -5533,166 +5504,166 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="2.625" style="32" customWidth="1"/>
+    <col min="1" max="1" width="2.58203125" style="32" customWidth="1"/>
     <col min="2" max="2" width="66.5" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" ht="35.25" customHeight="1">
       <c r="A1" s="24"/>
       <c r="B1" s="25" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="26"/>
     </row>
-    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" ht="15.5">
       <c r="A2" s="24"/>
       <c r="B2" s="27"/>
       <c r="C2" s="26"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3">
       <c r="A3" s="24"/>
       <c r="B3" s="28" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="26"/>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3">
       <c r="A4" s="24"/>
       <c r="B4" s="33" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="26"/>
     </row>
-    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" ht="15.5">
       <c r="A5" s="24"/>
       <c r="B5" s="29"/>
       <c r="C5" s="26"/>
     </row>
-    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.5">
       <c r="A6" s="24"/>
       <c r="B6" s="30" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="26"/>
     </row>
-    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" ht="15.5">
       <c r="A7" s="24"/>
       <c r="B7" s="29"/>
       <c r="C7" s="26"/>
     </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" ht="31">
       <c r="A8" s="24"/>
       <c r="B8" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="26"/>
     </row>
-    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" ht="15.5">
       <c r="A9" s="24"/>
       <c r="B9" s="29"/>
       <c r="C9" s="26"/>
     </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" ht="31">
       <c r="A10" s="24"/>
       <c r="B10" s="29" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="26"/>
     </row>
-    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" ht="15.5">
       <c r="A11" s="24"/>
       <c r="B11" s="29"/>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" ht="31">
       <c r="A12" s="24"/>
       <c r="B12" s="29" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="26"/>
     </row>
-    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" ht="15.5">
       <c r="A13" s="24"/>
       <c r="B13" s="29"/>
       <c r="C13" s="26"/>
     </row>
-    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:3" ht="15.5">
       <c r="A14" s="24"/>
       <c r="B14" s="34" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:3" ht="15.5">
       <c r="A15" s="24"/>
       <c r="B15" s="31"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.5">
       <c r="A16" s="24"/>
       <c r="B16" s="66" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="26"/>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:3">
       <c r="A17" s="24"/>
       <c r="B17" s="24"/>
       <c r="C17" s="26"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:3">
       <c r="A18" s="24"/>
       <c r="B18" s="24"/>
       <c r="C18" s="26"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:3">
       <c r="A19" s="24"/>
       <c r="B19" s="24"/>
       <c r="C19" s="26"/>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:3">
       <c r="A20" s="24"/>
       <c r="B20" s="24"/>
       <c r="C20" s="26"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:3">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="26"/>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:3">
       <c r="A22" s="24"/>
       <c r="B22" s="24"/>
       <c r="C22" s="26"/>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:3">
       <c r="A23" s="24"/>
       <c r="B23" s="24"/>
       <c r="C23" s="26"/>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:3">
       <c r="A24" s="24"/>
       <c r="B24" s="24"/>
       <c r="C24" s="26"/>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:3">
       <c r="A25" s="24"/>
       <c r="B25" s="24"/>
       <c r="C25" s="26"/>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:3">
       <c r="A26" s="24"/>
       <c r="B26" s="24"/>
       <c r="C26" s="26"/>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:3">
       <c r="A27" s="24"/>
       <c r="B27" s="24"/>
       <c r="C27" s="26"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:3">
       <c r="A28" s="24"/>
       <c r="B28" s="24"/>
       <c r="C28" s="26"/>

</xml_diff>

<commit_message>
Project Plan Progress Updated Signed-off-by: AmiraZaher <amirazaher96@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -5,11 +5,11 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ITI\software\project\SW deliveries log\Project_Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Software Engineering\Blender_Project\SW deliveries log\Project_Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7760"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="ProjectPlan" sheetId="11" r:id="rId1"/>
@@ -295,7 +295,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
   </numFmts>
-  <fonts count="34">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1258,7 +1258,7 @@
           <xdr:col>28</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>4</xdr:row>
-          <xdr:rowOff>184150</xdr:rowOff>
+          <xdr:rowOff>180975</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -1676,29 +1676,29 @@
   </sheetPr>
   <dimension ref="A1:BO45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A16" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="H18" sqref="H18"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A15" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5.33203125" customWidth="1"/>
+    <col min="1" max="1" width="5.375" customWidth="1"/>
     <col min="2" max="2" width="19.75" customWidth="1"/>
     <col min="3" max="3" width="13.25" customWidth="1"/>
     <col min="4" max="4" width="13.25" style="72" customWidth="1"/>
-    <col min="5" max="5" width="10.58203125" customWidth="1"/>
+    <col min="5" max="5" width="10.625" customWidth="1"/>
     <col min="6" max="6" width="9.5" style="10" customWidth="1"/>
     <col min="7" max="7" width="9.5" customWidth="1"/>
-    <col min="8" max="8" width="7.33203125" customWidth="1"/>
+    <col min="8" max="8" width="7.375" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="10" customWidth="1"/>
-    <col min="10" max="10" width="9.5" customWidth="1"/>
+    <col min="10" max="10" width="9.625" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="72" customWidth="1"/>
     <col min="12" max="12" width="13.75" customWidth="1"/>
-    <col min="13" max="66" width="3.08203125" customWidth="1"/>
+    <col min="13" max="66" width="3.125" customWidth="1"/>
     <col min="67" max="67" width="3.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="25">
+    <row r="1" spans="1:67" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="60" t="s">
         <v>48</v>
       </c>
@@ -1718,7 +1718,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:67" ht="19.5" customHeight="1">
+    <row r="2" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
         <v>49</v>
       </c>
@@ -1727,7 +1727,7 @@
       <c r="D2" s="14"/>
       <c r="M2" s="69"/>
     </row>
-    <row r="3" spans="1:67" s="72" customFormat="1" ht="19.5" customHeight="1">
+    <row r="3" spans="1:67" s="72" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="71" t="s">
         <v>52</v>
       </c>
@@ -1738,7 +1738,7 @@
       <c r="I3" s="73"/>
       <c r="M3" s="69"/>
     </row>
-    <row r="4" spans="1:67" ht="19.5" customHeight="1">
+    <row r="4" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>53</v>
       </c>
@@ -1751,7 +1751,7 @@
       </c>
       <c r="G4" s="77"/>
     </row>
-    <row r="5" spans="1:67" ht="19.5" customHeight="1">
+    <row r="5" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="35"/>
       <c r="E5" s="35" t="s">
         <v>32</v>
@@ -1760,7 +1760,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="6" spans="1:67" ht="18" hidden="1" customHeight="1">
+    <row r="6" spans="1:67" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="35"/>
       <c r="E6" s="35" t="s">
         <v>33</v>
@@ -1989,7 +1989,7 @@
         <v>43905</v>
       </c>
     </row>
-    <row r="7" spans="1:67" ht="47.25" customHeight="1">
+    <row r="7" spans="1:67" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="74" t="s">
         <v>56</v>
       </c>
@@ -2324,7 +2324,7 @@
 '20</v>
       </c>
     </row>
-    <row r="8" spans="1:67" ht="29.25" customHeight="1" thickBot="1">
+    <row r="8" spans="1:67" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
         <v>27</v>
       </c>
@@ -2578,7 +2578,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:67" s="8" customFormat="1" ht="14.5" thickBot="1">
+    <row r="9" spans="1:67" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="44"/>
       <c r="C9" s="41"/>
@@ -2652,7 +2652,7 @@
       <c r="BM9" s="16"/>
       <c r="BN9" s="16"/>
     </row>
-    <row r="10" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="10" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
       <c r="B10" s="45" t="s">
         <v>50</v>
@@ -2734,7 +2734,7 @@
       <c r="BM10" s="16"/>
       <c r="BN10" s="16"/>
     </row>
-    <row r="11" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="11" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="48"/>
       <c r="B11" s="45" t="s">
         <v>78</v>
@@ -2804,7 +2804,7 @@
       <c r="BM11" s="16"/>
       <c r="BN11" s="16"/>
     </row>
-    <row r="12" spans="1:67" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1">
+    <row r="12" spans="1:67" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="15" t="s">
         <v>57</v>
@@ -2834,7 +2834,7 @@
       <c r="J12" s="55"/>
       <c r="K12" s="55"/>
       <c r="L12" s="62" t="str">
-        <f t="shared" ref="L12:L42" si="4">IF(OR(ISBLANK(I12),ISBLANK(J12)),"",J12-I12+1)</f>
+        <f>IF(OR(ISBLANK(I12),ISBLANK(J12)),"",J12-I12+1)</f>
         <v/>
       </c>
       <c r="M12" s="16"/>
@@ -2892,7 +2892,7 @@
       <c r="BM12" s="16"/>
       <c r="BN12" s="16"/>
     </row>
-    <row r="13" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="13" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="15" t="s">
         <v>58</v>
@@ -2922,7 +2922,7 @@
       <c r="J13" s="55"/>
       <c r="K13" s="55"/>
       <c r="L13" s="62" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(ISBLANK(I13),ISBLANK(J13)),"",J13-I13+1)</f>
         <v/>
       </c>
       <c r="M13" s="16"/>
@@ -2980,7 +2980,7 @@
       <c r="BM13" s="16"/>
       <c r="BN13" s="16"/>
     </row>
-    <row r="14" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="14" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="15" t="s">
         <v>59</v>
@@ -3010,7 +3010,7 @@
       <c r="J14" s="55"/>
       <c r="K14" s="55"/>
       <c r="L14" s="62" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(ISBLANK(I14),ISBLANK(J14)),"",J14-I14+1)</f>
         <v/>
       </c>
       <c r="M14" s="16"/>
@@ -3068,7 +3068,7 @@
       <c r="BM14" s="16"/>
       <c r="BN14" s="16"/>
     </row>
-    <row r="15" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="15" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
       <c r="B15" s="15" t="s">
         <v>62</v>
@@ -3098,7 +3098,7 @@
       <c r="J15" s="55"/>
       <c r="K15" s="55"/>
       <c r="L15" s="62" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(ISBLANK(I15),ISBLANK(J15)),"",J15-I15+1)</f>
         <v/>
       </c>
       <c r="M15" s="16"/>
@@ -3156,7 +3156,7 @@
       <c r="BM15" s="16"/>
       <c r="BN15" s="16"/>
     </row>
-    <row r="16" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="16" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="15" t="s">
         <v>63</v>
@@ -3186,7 +3186,7 @@
       <c r="J16" s="55"/>
       <c r="K16" s="55"/>
       <c r="L16" s="62" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(ISBLANK(I16),ISBLANK(J16)),"",J16-I16+1)</f>
         <v/>
       </c>
       <c r="M16" s="16"/>
@@ -3244,7 +3244,7 @@
       <c r="BM16" s="16"/>
       <c r="BN16" s="16"/>
     </row>
-    <row r="17" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="17" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="48"/>
       <c r="B17" s="45" t="s">
         <v>79</v>
@@ -3314,7 +3314,7 @@
       <c r="BM17" s="16"/>
       <c r="BN17" s="16"/>
     </row>
-    <row r="18" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="18" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="47"/>
       <c r="B18" s="15" t="s">
         <v>69</v>
@@ -3400,7 +3400,7 @@
       <c r="BM18" s="16"/>
       <c r="BN18" s="16"/>
     </row>
-    <row r="19" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="19" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="15" t="s">
         <v>71</v>
@@ -3419,7 +3419,7 @@
         <v>43866</v>
       </c>
       <c r="H19" s="62">
-        <f t="shared" ref="H19:H24" si="5">IF(OR(ISBLANK(F19),ISBLANK(G19)),"",G19-F19+1)</f>
+        <f t="shared" ref="H19:H24" si="4">IF(OR(ISBLANK(F19),ISBLANK(G19)),"",G19-F19+1)</f>
         <v>2</v>
       </c>
       <c r="I19" s="54"/>
@@ -3481,7 +3481,7 @@
       <c r="BM19" s="16"/>
       <c r="BN19" s="16"/>
     </row>
-    <row r="20" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="20" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="15" t="s">
         <v>72</v>
@@ -3492,7 +3492,9 @@
       <c r="D20" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="51"/>
+      <c r="E20" s="51">
+        <v>1</v>
+      </c>
       <c r="F20" s="54">
         <v>43862</v>
       </c>
@@ -3500,15 +3502,19 @@
         <v>43864</v>
       </c>
       <c r="H20" s="62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>3</v>
       </c>
-      <c r="I20" s="54"/>
-      <c r="J20" s="55"/>
+      <c r="I20" s="54">
+        <v>43862</v>
+      </c>
+      <c r="J20" s="55">
+        <v>43867</v>
+      </c>
       <c r="K20" s="55"/>
-      <c r="L20" s="62" t="str">
-        <f t="shared" si="4"/>
-        <v/>
+      <c r="L20" s="62">
+        <f>IF(OR(ISBLANK(I20),ISBLANK(J20)),"",J20-I20+1)</f>
+        <v>6</v>
       </c>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
@@ -3565,7 +3571,7 @@
       <c r="BM20" s="16"/>
       <c r="BN20" s="16"/>
     </row>
-    <row r="21" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="21" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="15" t="s">
         <v>73</v>
@@ -3584,7 +3590,7 @@
         <v>43865</v>
       </c>
       <c r="H21" s="62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I21" s="54"/>
@@ -3646,7 +3652,7 @@
       <c r="BM21" s="16"/>
       <c r="BN21" s="16"/>
     </row>
-    <row r="22" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="22" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
       <c r="B22" s="15" t="s">
         <v>74</v>
@@ -3657,7 +3663,9 @@
       <c r="D22" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="51"/>
+      <c r="E22" s="51">
+        <v>1</v>
+      </c>
       <c r="F22" s="54">
         <v>43866</v>
       </c>
@@ -3665,11 +3673,15 @@
         <v>43866</v>
       </c>
       <c r="H22" s="62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>1</v>
       </c>
-      <c r="I22" s="54"/>
-      <c r="J22" s="55"/>
+      <c r="I22" s="54">
+        <v>43862</v>
+      </c>
+      <c r="J22" s="55">
+        <v>43867</v>
+      </c>
       <c r="K22" s="55"/>
       <c r="L22" s="62"/>
       <c r="M22" s="16"/>
@@ -3727,7 +3739,7 @@
       <c r="BM22" s="16"/>
       <c r="BN22" s="16"/>
     </row>
-    <row r="23" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="23" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
       <c r="B23" s="15" t="s">
         <v>75</v>
@@ -3746,7 +3758,7 @@
         <v>43865</v>
       </c>
       <c r="H23" s="62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I23" s="54"/>
@@ -3808,7 +3820,7 @@
       <c r="BM23" s="16"/>
       <c r="BN23" s="16"/>
     </row>
-    <row r="24" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="24" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47"/>
       <c r="B24" s="15" t="s">
         <v>77</v>
@@ -3827,7 +3839,7 @@
         <v>43868</v>
       </c>
       <c r="H24" s="62">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>2</v>
       </c>
       <c r="I24" s="54"/>
@@ -3889,7 +3901,7 @@
       <c r="BM24" s="16"/>
       <c r="BN24" s="16"/>
     </row>
-    <row r="25" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="25" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
       <c r="B25" s="15" t="s">
         <v>44</v>
@@ -3907,7 +3919,7 @@
       <c r="J25" s="55"/>
       <c r="K25" s="55"/>
       <c r="L25" s="62" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(ISBLANK(I25),ISBLANK(J25)),"",J25-I25+1)</f>
         <v/>
       </c>
       <c r="M25" s="16"/>
@@ -3965,7 +3977,7 @@
       <c r="BM25" s="16"/>
       <c r="BN25" s="16"/>
     </row>
-    <row r="26" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="26" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="48"/>
       <c r="B26" s="45" t="s">
         <v>14</v>
@@ -3976,14 +3988,14 @@
       <c r="F26" s="56"/>
       <c r="G26" s="57"/>
       <c r="H26" s="63" t="str">
-        <f t="shared" ref="H26:H42" si="6">IF(OR(ISBLANK(F26),ISBLANK(G26)),"",G26-F26+1)</f>
+        <f t="shared" ref="H26:H42" si="5">IF(OR(ISBLANK(F26),ISBLANK(G26)),"",G26-F26+1)</f>
         <v/>
       </c>
       <c r="I26" s="56"/>
       <c r="J26" s="57"/>
       <c r="K26" s="57"/>
       <c r="L26" s="63" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(ISBLANK(I26),ISBLANK(J26)),"",J26-I26+1)</f>
         <v/>
       </c>
       <c r="M26" s="16"/>
@@ -4041,7 +4053,7 @@
       <c r="BM26" s="16"/>
       <c r="BN26" s="16"/>
     </row>
-    <row r="27" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="27" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="47"/>
       <c r="B27" s="15" t="s">
         <v>15</v>
@@ -4111,7 +4123,7 @@
       <c r="BM27" s="16"/>
       <c r="BN27" s="16"/>
     </row>
-    <row r="28" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="28" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
       <c r="B28" s="15" t="s">
         <v>16</v>
@@ -4181,7 +4193,7 @@
       <c r="BM28" s="16"/>
       <c r="BN28" s="16"/>
     </row>
-    <row r="29" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="29" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
       <c r="B29" s="15" t="s">
         <v>11</v>
@@ -4251,7 +4263,7 @@
       <c r="BM29" s="16"/>
       <c r="BN29" s="16"/>
     </row>
-    <row r="30" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="30" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="47"/>
       <c r="B30" s="15" t="s">
         <v>12</v>
@@ -4321,7 +4333,7 @@
       <c r="BM30" s="16"/>
       <c r="BN30" s="16"/>
     </row>
-    <row r="31" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="31" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="47"/>
       <c r="B31" s="15" t="s">
         <v>13</v>
@@ -4391,7 +4403,7 @@
       <c r="BM31" s="16"/>
       <c r="BN31" s="16"/>
     </row>
-    <row r="32" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="32" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="47"/>
       <c r="B32" s="15" t="s">
         <v>17</v>
@@ -4461,7 +4473,7 @@
       <c r="BM32" s="16"/>
       <c r="BN32" s="16"/>
     </row>
-    <row r="33" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="33" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="47"/>
       <c r="B33" s="44"/>
       <c r="C33" s="41"/>
@@ -4470,14 +4482,14 @@
       <c r="F33" s="54"/>
       <c r="G33" s="55"/>
       <c r="H33" s="62" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I33" s="54"/>
       <c r="J33" s="55"/>
       <c r="K33" s="55"/>
       <c r="L33" s="62" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(ISBLANK(I33),ISBLANK(J33)),"",J33-I33+1)</f>
         <v/>
       </c>
       <c r="M33" s="16"/>
@@ -4535,7 +4547,7 @@
       <c r="BM33" s="16"/>
       <c r="BN33" s="16"/>
     </row>
-    <row r="34" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="34" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="47"/>
       <c r="B34" s="44"/>
       <c r="C34" s="41"/>
@@ -4544,14 +4556,14 @@
       <c r="F34" s="54"/>
       <c r="G34" s="55"/>
       <c r="H34" s="62" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I34" s="54"/>
       <c r="J34" s="55"/>
       <c r="K34" s="55"/>
       <c r="L34" s="62" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(ISBLANK(I34),ISBLANK(J34)),"",J34-I34+1)</f>
         <v/>
       </c>
       <c r="M34" s="16"/>
@@ -4609,7 +4621,7 @@
       <c r="BM34" s="16"/>
       <c r="BN34" s="16"/>
     </row>
-    <row r="35" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="35" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="47"/>
       <c r="B35" s="44"/>
       <c r="C35" s="41"/>
@@ -4618,14 +4630,14 @@
       <c r="F35" s="54"/>
       <c r="G35" s="55"/>
       <c r="H35" s="62" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I35" s="54"/>
       <c r="J35" s="55"/>
       <c r="K35" s="55"/>
       <c r="L35" s="62" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(ISBLANK(I35),ISBLANK(J35)),"",J35-I35+1)</f>
         <v/>
       </c>
       <c r="M35" s="16"/>
@@ -4683,7 +4695,7 @@
       <c r="BM35" s="16"/>
       <c r="BN35" s="16"/>
     </row>
-    <row r="36" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="36" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="47"/>
       <c r="B36" s="44"/>
       <c r="C36" s="41"/>
@@ -4751,7 +4763,7 @@
       <c r="BM36" s="16"/>
       <c r="BN36" s="16"/>
     </row>
-    <row r="37" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="37" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="47"/>
       <c r="B37" s="44"/>
       <c r="C37" s="41"/>
@@ -4819,7 +4831,7 @@
       <c r="BM37" s="16"/>
       <c r="BN37" s="16"/>
     </row>
-    <row r="38" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="38" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="47"/>
       <c r="B38" s="44"/>
       <c r="C38" s="41"/>
@@ -4887,7 +4899,7 @@
       <c r="BM38" s="16"/>
       <c r="BN38" s="16"/>
     </row>
-    <row r="39" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="39" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="47"/>
       <c r="B39" s="44"/>
       <c r="C39" s="41"/>
@@ -4955,7 +4967,7 @@
       <c r="BM39" s="16"/>
       <c r="BN39" s="16"/>
     </row>
-    <row r="40" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="40" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="47"/>
       <c r="B40" s="44"/>
       <c r="C40" s="41"/>
@@ -5023,7 +5035,7 @@
       <c r="BM40" s="16"/>
       <c r="BN40" s="16"/>
     </row>
-    <row r="41" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="41" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="47"/>
       <c r="B41" s="44"/>
       <c r="C41" s="41"/>
@@ -5032,14 +5044,14 @@
       <c r="F41" s="54"/>
       <c r="G41" s="55"/>
       <c r="H41" s="62" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I41" s="54"/>
       <c r="J41" s="55"/>
       <c r="K41" s="55"/>
       <c r="L41" s="62" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(ISBLANK(I41),ISBLANK(J41)),"",J41-I41+1)</f>
         <v/>
       </c>
       <c r="M41" s="16"/>
@@ -5097,7 +5109,7 @@
       <c r="BM41" s="16"/>
       <c r="BN41" s="16"/>
     </row>
-    <row r="42" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1">
+    <row r="42" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="49"/>
       <c r="B42" s="46" t="s">
         <v>19</v>
@@ -5108,14 +5120,14 @@
       <c r="F42" s="58"/>
       <c r="G42" s="59"/>
       <c r="H42" s="64" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v/>
       </c>
       <c r="I42" s="58"/>
       <c r="J42" s="59"/>
       <c r="K42" s="59"/>
       <c r="L42" s="64" t="str">
-        <f t="shared" si="4"/>
+        <f>IF(OR(ISBLANK(I42),ISBLANK(J42)),"",J42-I42+1)</f>
         <v/>
       </c>
       <c r="M42" s="18"/>
@@ -5173,10 +5185,10 @@
       <c r="BM42" s="18"/>
       <c r="BN42" s="18"/>
     </row>
-    <row r="44" spans="1:66">
+    <row r="44" spans="1:66" ht="15" x14ac:dyDescent="0.25">
       <c r="A44" s="19"/>
     </row>
-    <row r="45" spans="1:66">
+    <row r="45" spans="1:66" x14ac:dyDescent="0.2">
       <c r="A45" s="65"/>
     </row>
   </sheetData>
@@ -5243,7 +5255,7 @@
       <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="1">
+  <dataValidations disablePrompts="1" count="1">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5">
       <formula1>"Daily,Weekly,Monthly,Quarterly"</formula1>
     </dataValidation>
@@ -5273,7 +5285,7 @@
                     <xdr:col>28</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>4</xdr:row>
-                    <xdr:rowOff>184150</xdr:rowOff>
+                    <xdr:rowOff>180975</xdr:rowOff>
                   </to>
                 </anchor>
               </controlPr>
@@ -5330,155 +5342,155 @@
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="68.5" customWidth="1"/>
     <col min="3" max="3" width="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="33" customHeight="1">
+    <row r="1" spans="1:4" ht="33" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3"/>
       <c r="C1" s="4"/>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="78" t="s">
         <v>35</v>
       </c>
       <c r="C2" s="78"/>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3" s="23" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="5"/>
       <c r="D4" s="5"/>
     </row>
-    <row r="5" spans="1:4" ht="56">
+    <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
         <v>47</v>
       </c>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="1:4">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B6" s="7"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B7" s="20"/>
       <c r="D7" s="5"/>
     </row>
-    <row r="8" spans="1:4" ht="15.5">
+    <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="21" t="s">
         <v>21</v>
       </c>
       <c r="D8" s="5"/>
     </row>
-    <row r="9" spans="1:4" ht="15.5">
+    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="22" t="s">
         <v>45</v>
       </c>
       <c r="D9" s="5"/>
     </row>
-    <row r="10" spans="1:4">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B10" s="20"/>
       <c r="D10" s="5"/>
     </row>
-    <row r="11" spans="1:4">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B11" s="7"/>
       <c r="D11" s="5"/>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="7"/>
       <c r="D12" s="5"/>
     </row>
-    <row r="13" spans="1:4" ht="28">
+    <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
         <v>18</v>
       </c>
       <c r="D13" s="5"/>
     </row>
-    <row r="14" spans="1:4">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B14" s="7"/>
       <c r="D14" s="5"/>
     </row>
-    <row r="15" spans="1:4">
+    <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
         <v>36</v>
       </c>
       <c r="B15" s="7"/>
       <c r="D15" s="5"/>
     </row>
-    <row r="16" spans="1:4" ht="28">
+    <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
         <v>37</v>
       </c>
       <c r="D16" s="5"/>
     </row>
-    <row r="17" spans="1:4">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B17" s="7"/>
       <c r="D17" s="5"/>
     </row>
-    <row r="18" spans="1:4">
+    <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>20</v>
       </c>
       <c r="B18" s="7"/>
       <c r="D18" s="5"/>
     </row>
-    <row r="19" spans="1:4" ht="28">
+    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
         <v>38</v>
       </c>
       <c r="D19" s="5"/>
     </row>
-    <row r="20" spans="1:4">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B20" s="7"/>
       <c r="D20" s="5"/>
     </row>
-    <row r="21" spans="1:4">
+    <row r="21" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A21" s="6" t="s">
         <v>4</v>
       </c>
       <c r="B21" s="7"/>
       <c r="D21" s="5"/>
     </row>
-    <row r="22" spans="1:4" ht="42">
+    <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="23" spans="1:4">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B23" s="7"/>
     </row>
-    <row r="24" spans="1:4" ht="28">
+    <row r="24" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B24" s="7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4">
+    <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>40</v>
       </c>
       <c r="B26" s="7"/>
     </row>
-    <row r="27" spans="1:4">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="68" t="s">
         <v>46</v>
       </c>
@@ -5503,166 +5515,166 @@
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="2.58203125" style="32" customWidth="1"/>
+    <col min="1" max="1" width="2.625" style="32" customWidth="1"/>
     <col min="2" max="2" width="66.5" style="32" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="35.25" customHeight="1">
+    <row r="1" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24"/>
       <c r="B1" s="25" t="s">
         <v>42</v>
       </c>
       <c r="C1" s="26"/>
     </row>
-    <row r="2" spans="1:3" ht="15.5">
+    <row r="2" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A2" s="24"/>
       <c r="B2" s="27"/>
       <c r="C2" s="26"/>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="24"/>
       <c r="B3" s="28" t="s">
         <v>23</v>
       </c>
       <c r="C3" s="26"/>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="24"/>
       <c r="B4" s="33" t="s">
         <v>35</v>
       </c>
       <c r="C4" s="26"/>
     </row>
-    <row r="5" spans="1:3" ht="15.5">
+    <row r="5" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A5" s="24"/>
       <c r="B5" s="29"/>
       <c r="C5" s="26"/>
     </row>
-    <row r="6" spans="1:3" ht="15.5">
+    <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="30" t="s">
         <v>22</v>
       </c>
       <c r="C6" s="26"/>
     </row>
-    <row r="7" spans="1:3" ht="15.5">
+    <row r="7" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A7" s="24"/>
       <c r="B7" s="29"/>
       <c r="C7" s="26"/>
     </row>
-    <row r="8" spans="1:3" ht="31">
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="24"/>
       <c r="B8" s="29" t="s">
         <v>2</v>
       </c>
       <c r="C8" s="26"/>
     </row>
-    <row r="9" spans="1:3" ht="15.5">
+    <row r="9" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A9" s="24"/>
       <c r="B9" s="29"/>
       <c r="C9" s="26"/>
     </row>
-    <row r="10" spans="1:3" ht="31">
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="24"/>
       <c r="B10" s="29" t="s">
         <v>24</v>
       </c>
       <c r="C10" s="26"/>
     </row>
-    <row r="11" spans="1:3" ht="15.5">
+    <row r="11" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A11" s="24"/>
       <c r="B11" s="29"/>
       <c r="C11" s="26"/>
     </row>
-    <row r="12" spans="1:3" ht="31">
+    <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="24"/>
       <c r="B12" s="29" t="s">
         <v>25</v>
       </c>
       <c r="C12" s="26"/>
     </row>
-    <row r="13" spans="1:3" ht="15.5">
+    <row r="13" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="24"/>
       <c r="B13" s="29"/>
       <c r="C13" s="26"/>
     </row>
-    <row r="14" spans="1:3" ht="15.5">
+    <row r="14" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A14" s="24"/>
       <c r="B14" s="34" t="s">
         <v>3</v>
       </c>
       <c r="C14" s="26"/>
     </row>
-    <row r="15" spans="1:3" ht="15.5">
+    <row r="15" spans="1:3" ht="15" x14ac:dyDescent="0.2">
       <c r="A15" s="24"/>
       <c r="B15" s="31"/>
       <c r="C15" s="26"/>
     </row>
-    <row r="16" spans="1:3" ht="15.5">
+    <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="66" t="s">
         <v>43</v>
       </c>
       <c r="C16" s="26"/>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" s="24"/>
       <c r="B17" s="24"/>
       <c r="C17" s="26"/>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="24"/>
       <c r="B18" s="24"/>
       <c r="C18" s="26"/>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="24"/>
       <c r="B19" s="24"/>
       <c r="C19" s="26"/>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="24"/>
       <c r="B20" s="24"/>
       <c r="C20" s="26"/>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="24"/>
       <c r="B21" s="24"/>
       <c r="C21" s="26"/>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="24"/>
       <c r="B22" s="24"/>
       <c r="C22" s="26"/>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="24"/>
       <c r="B23" s="24"/>
       <c r="C23" s="26"/>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="24"/>
       <c r="B24" s="24"/>
       <c r="C24" s="26"/>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="24"/>
       <c r="B25" s="24"/>
       <c r="C25" s="26"/>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="24"/>
       <c r="B26" s="24"/>
       <c r="C26" s="26"/>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="24"/>
       <c r="B27" s="24"/>
       <c r="C27" s="26"/>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="24"/>
       <c r="B28" s="24"/>
       <c r="C28" s="26"/>

</xml_diff>

<commit_message>
Updating RTM to reflect modified requirements according to review Updating Project Plan with Actual end dates of tasks Signed-off-by: May Alaa <mayelfkiy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Software Engineering\Blender_Project\SW deliveries log\Project_Plan\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pc\Desktop\SOFTWARE_ENG_ELECTRIC_BLENDER\SW deliveries log\Project_Plan\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
     <definedName name="vertex42_id" hidden="1">"project-planner.xlsx"</definedName>
     <definedName name="vertex42_title" hidden="1">"Project Planner Template"</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -290,7 +290,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
@@ -1268,7 +1268,7 @@
                   <a14:compatExt spid="_x0000_s6145"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1318,7 +1318,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1373,7 +1373,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1676,8 +1676,8 @@
   </sheetPr>
   <dimension ref="A1:BO45"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A15" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2831,12 +2831,11 @@
       <c r="I12" s="54">
         <v>43852</v>
       </c>
-      <c r="J12" s="55"/>
+      <c r="J12" s="55">
+        <v>43853</v>
+      </c>
       <c r="K12" s="55"/>
-      <c r="L12" s="62" t="str">
-        <f>IF(OR(ISBLANK(I12),ISBLANK(J12)),"",J12-I12+1)</f>
-        <v/>
-      </c>
+      <c r="L12" s="62"/>
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
@@ -2919,12 +2918,11 @@
       <c r="I13" s="54">
         <v>43854</v>
       </c>
-      <c r="J13" s="55"/>
+      <c r="J13" s="55">
+        <v>43854</v>
+      </c>
       <c r="K13" s="55"/>
-      <c r="L13" s="62" t="str">
-        <f>IF(OR(ISBLANK(I13),ISBLANK(J13)),"",J13-I13+1)</f>
-        <v/>
-      </c>
+      <c r="L13" s="62"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
@@ -3007,12 +3005,11 @@
       <c r="I14" s="54">
         <v>43854</v>
       </c>
-      <c r="J14" s="55"/>
+      <c r="J14" s="55">
+        <v>43854</v>
+      </c>
       <c r="K14" s="55"/>
-      <c r="L14" s="62" t="str">
-        <f>IF(OR(ISBLANK(I14),ISBLANK(J14)),"",J14-I14+1)</f>
-        <v/>
-      </c>
+      <c r="L14" s="62"/>
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
@@ -3095,12 +3092,11 @@
       <c r="I15" s="54">
         <v>43852</v>
       </c>
-      <c r="J15" s="55"/>
+      <c r="J15" s="55">
+        <v>43853</v>
+      </c>
       <c r="K15" s="55"/>
-      <c r="L15" s="62" t="str">
-        <f>IF(OR(ISBLANK(I15),ISBLANK(J15)),"",J15-I15+1)</f>
-        <v/>
-      </c>
+      <c r="L15" s="62"/>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
@@ -3171,24 +3167,23 @@
         <v>1</v>
       </c>
       <c r="F16" s="54">
-        <v>43857</v>
+        <v>43867</v>
       </c>
       <c r="G16" s="55">
         <v>43868</v>
       </c>
       <c r="H16" s="62">
         <f t="shared" si="3"/>
-        <v>12</v>
+        <v>2</v>
       </c>
       <c r="I16" s="54">
-        <v>43858</v>
-      </c>
-      <c r="J16" s="55"/>
+        <v>43867</v>
+      </c>
+      <c r="J16" s="55">
+        <v>43868</v>
+      </c>
       <c r="K16" s="55"/>
-      <c r="L16" s="62" t="str">
-        <f>IF(OR(ISBLANK(I16),ISBLANK(J16)),"",J16-I16+1)</f>
-        <v/>
-      </c>
+      <c r="L16" s="62"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
@@ -3411,7 +3406,9 @@
       <c r="D19" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="51"/>
+      <c r="E19" s="51">
+        <v>1</v>
+      </c>
       <c r="F19" s="54">
         <v>43865</v>
       </c>
@@ -3422,8 +3419,12 @@
         <f t="shared" ref="H19:H24" si="4">IF(OR(ISBLANK(F19),ISBLANK(G19)),"",G19-F19+1)</f>
         <v>2</v>
       </c>
-      <c r="I19" s="54"/>
-      <c r="J19" s="55"/>
+      <c r="I19" s="54">
+        <v>43865</v>
+      </c>
+      <c r="J19" s="55">
+        <v>43867</v>
+      </c>
       <c r="K19" s="55"/>
       <c r="L19" s="62"/>
       <c r="M19" s="16"/>
@@ -3512,10 +3513,7 @@
         <v>43867</v>
       </c>
       <c r="K20" s="55"/>
-      <c r="L20" s="62">
-        <f>IF(OR(ISBLANK(I20),ISBLANK(J20)),"",J20-I20+1)</f>
-        <v>6</v>
-      </c>
+      <c r="L20" s="62"/>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
@@ -3582,7 +3580,9 @@
       <c r="D21" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E21" s="51"/>
+      <c r="E21" s="51">
+        <v>1</v>
+      </c>
       <c r="F21" s="54">
         <v>43864</v>
       </c>
@@ -3593,8 +3593,12 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="I21" s="54"/>
-      <c r="J21" s="55"/>
+      <c r="I21" s="54">
+        <v>43865</v>
+      </c>
+      <c r="J21" s="55">
+        <v>43865</v>
+      </c>
       <c r="K21" s="55"/>
       <c r="L21" s="62"/>
       <c r="M21" s="16"/>
@@ -3750,7 +3754,9 @@
       <c r="D23" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="51"/>
+      <c r="E23" s="51">
+        <v>1</v>
+      </c>
       <c r="F23" s="54">
         <v>43864</v>
       </c>
@@ -3761,8 +3767,12 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="I23" s="54"/>
-      <c r="J23" s="55"/>
+      <c r="I23" s="54">
+        <v>43868</v>
+      </c>
+      <c r="J23" s="55">
+        <v>43868</v>
+      </c>
       <c r="K23" s="55"/>
       <c r="L23" s="62"/>
       <c r="M23" s="16"/>
@@ -3831,7 +3841,9 @@
       <c r="D24" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="51"/>
+      <c r="E24" s="51">
+        <v>1</v>
+      </c>
       <c r="F24" s="54">
         <v>43867</v>
       </c>
@@ -3842,8 +3854,12 @@
         <f t="shared" si="4"/>
         <v>2</v>
       </c>
-      <c r="I24" s="54"/>
-      <c r="J24" s="55"/>
+      <c r="I24" s="54">
+        <v>43868</v>
+      </c>
+      <c r="J24" s="55">
+        <v>43868</v>
+      </c>
       <c r="K24" s="55"/>
       <c r="L24" s="62"/>
       <c r="M24" s="16"/>

</xml_diff>

<commit_message>
Updating the Project Plan assigning tasks to resolve Final issues in HSI, CYRS and SRS before release Signed-off-by: May Alaa <mayelfkiy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="89">
   <si>
     <t>HELP</t>
   </si>
@@ -132,10 +132,6 @@
 START</t>
   </si>
   <si>
-    <t>PLAN
-DAYS</t>
-  </si>
-  <si>
     <t>PROGRESS</t>
   </si>
   <si>
@@ -285,6 +281,33 @@
   </si>
   <si>
     <t>Amira</t>
+  </si>
+  <si>
+    <t>Week 3</t>
+  </si>
+  <si>
+    <t>Task Description</t>
+  </si>
+  <si>
+    <t>Solve issues described in point 9,10 and 11 in the review sheet</t>
+  </si>
+  <si>
+    <t>Solve issues described in point 7,8,9,10 in the review sheet</t>
+  </si>
+  <si>
+    <t>Solve issues described in point 1-6 in the review sheet</t>
+  </si>
+  <si>
+    <t>Cross review on the CYRS</t>
+  </si>
+  <si>
+    <t>Cross review on the SRS</t>
+  </si>
+  <si>
+    <t>Cross review on the HSI</t>
+  </si>
+  <si>
+    <t>Updating RTM to reflect modified requirements</t>
   </si>
 </sst>
 </file>
@@ -759,7 +782,7 @@
     </xf>
     <xf numFmtId="9" fontId="26" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="80">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -965,20 +988,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="17">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
         <right style="thin">
-          <color rgb="FFC00000"/>
+          <color theme="0" tint="-0.14996795556505021"/>
         </right>
         <vertical/>
         <horizontal/>
@@ -1020,23 +1057,60 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
         <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
         </right>
         <vertical/>
         <horizontal/>
@@ -1138,15 +1212,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9">
-      <tableStyleElement type="wholeTable" dxfId="16"/>
-      <tableStyleElement type="headerRow" dxfId="15"/>
-      <tableStyleElement type="totalRow" dxfId="14"/>
-      <tableStyleElement type="firstColumn" dxfId="13"/>
-      <tableStyleElement type="lastColumn" dxfId="12"/>
-      <tableStyleElement type="firstRowStripe" dxfId="11"/>
-      <tableStyleElement type="secondRowStripe" dxfId="10"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="9"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="8"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstColumn" dxfId="17"/>
+      <tableStyleElement type="lastColumn" dxfId="16"/>
+      <tableStyleElement type="firstRowStripe" dxfId="15"/>
+      <tableStyleElement type="secondRowStripe" dxfId="14"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="12"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1240,7 +1314,7 @@
 </file>
 
 <file path=xl/ctrlProps/ctrlProp1.xml><?xml version="1.0" encoding="utf-8"?>
-<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$F$6" horiz="1" max="100" min="1" page="4"/>
+<formControlPr xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" objectType="Scroll" dx="22" fmlaLink="$G$6" horiz="1" max="100" min="1" page="4"/>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1268,7 +1342,7 @@
                   <a14:compatExt spid="_x0000_s6145"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001180000}"/>
+                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1318,7 +1392,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1373,7 +1447,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1674,22 +1748,22 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO45"/>
+  <dimension ref="A1:BO55"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A8" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.375" customWidth="1"/>
     <col min="2" max="2" width="19.75" customWidth="1"/>
-    <col min="3" max="3" width="13.25" customWidth="1"/>
-    <col min="4" max="4" width="13.25" style="72" customWidth="1"/>
-    <col min="5" max="5" width="10.625" customWidth="1"/>
-    <col min="6" max="6" width="9.5" style="10" customWidth="1"/>
-    <col min="7" max="7" width="9.5" customWidth="1"/>
-    <col min="8" max="8" width="7.375" customWidth="1"/>
+    <col min="3" max="3" width="23.625" style="72" customWidth="1"/>
+    <col min="4" max="4" width="13.25" customWidth="1"/>
+    <col min="5" max="5" width="13.25" style="72" customWidth="1"/>
+    <col min="6" max="6" width="10.625" customWidth="1"/>
+    <col min="7" max="7" width="9.5" style="10" customWidth="1"/>
+    <col min="8" max="8" width="9.5" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="10" customWidth="1"/>
     <col min="10" max="10" width="9.625" customWidth="1"/>
     <col min="11" max="11" width="9.5" style="72" customWidth="1"/>
@@ -1700,14 +1774,14 @@
   <sheetData>
     <row r="1" spans="1:67" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="60" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-      <c r="E1" s="2"/>
-      <c r="F1" s="67"/>
-      <c r="G1" s="2"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="2"/>
+      <c r="G1" s="67"/>
       <c r="H1" s="2"/>
       <c r="I1" s="9"/>
       <c r="J1" s="2"/>
@@ -1720,60 +1794,63 @@
     </row>
     <row r="2" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
       <c r="M2" s="69"/>
     </row>
     <row r="3" spans="1:67" s="72" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="71" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" s="71"/>
-      <c r="C3" s="14"/>
+      <c r="C3" s="71"/>
       <c r="D3" s="14"/>
-      <c r="F3" s="73"/>
+      <c r="E3" s="14"/>
+      <c r="G3" s="73"/>
       <c r="I3" s="73"/>
       <c r="M3" s="69"/>
     </row>
     <row r="4" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" s="71"/>
-      <c r="E4" s="35" t="s">
+      <c r="C4" s="71"/>
+      <c r="F4" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="F4" s="76">
+      <c r="G4" s="76">
         <v>43851</v>
       </c>
-      <c r="G4" s="77"/>
+      <c r="H4" s="77"/>
     </row>
     <row r="5" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="35"/>
-      <c r="E5" s="35" t="s">
-        <v>32</v>
-      </c>
-      <c r="F5" s="61" t="s">
-        <v>51</v>
+      <c r="F5" s="35" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="61" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:67" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="35"/>
-      <c r="E6" s="35" t="s">
-        <v>33</v>
-      </c>
-      <c r="F6" s="36">
+      <c r="F6" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="36">
         <v>1</v>
       </c>
       <c r="M6" s="37">
-        <f>IF(F5="Weekly",F4+7*(F6-1),IF(F5="Daily",F4+(F6-1),IF(F5="Monthly",EDATE($F$4,($F$6-1)),EDATE($F$4,3*($F$6-1)))))</f>
+        <f>IF(G5="Weekly",G4+7*(G6-1),IF(G5="Daily",G4+(G6-1),IF(G5="Monthly",EDATE($G$4,($G$6-1)),EDATE($G$4,3*($G$6-1)))))</f>
         <v>43851</v>
       </c>
       <c r="N6" s="37">
-        <f t="shared" ref="N6:BO6" si="0">IF($F$5="Daily",M6+1,IF($F$5="Weekly",M6+7,IF($F$5="Monthly",EDATE($F$4,N8-1),EDATE($F$4,3*(N8-1)))))</f>
+        <f t="shared" ref="N6:BO6" si="0">IF($G$5="Daily",M6+1,IF($G$5="Weekly",M6+7,IF($G$5="Monthly",EDATE($G$4,N8-1),EDATE($G$4,3*(N8-1)))))</f>
         <v>43852</v>
       </c>
       <c r="O6" s="37">
@@ -1991,7 +2068,7 @@
     </row>
     <row r="7" spans="1:67" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="74" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="M7" s="38" t="str">
         <f>DAY(M6)&amp;CHAR(10)&amp;LEFT(TEXT(M6,"mmm"),3)&amp;CHAR(10)&amp;"'"&amp;RIGHT(YEAR(M6),2)</f>
@@ -2331,23 +2408,23 @@
       <c r="B8" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="13" t="s">
-        <v>34</v>
+      <c r="C8" s="12" t="s">
+        <v>81</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>66</v>
+        <v>33</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="F8" s="70" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G8" s="70" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="70" t="s">
+      <c r="H8" s="70" t="s">
         <v>9</v>
-      </c>
-      <c r="H8" s="70" t="s">
-        <v>30</v>
       </c>
       <c r="I8" s="13" t="s">
         <v>29</v>
@@ -2356,13 +2433,13 @@
         <v>28</v>
       </c>
       <c r="K8" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L8" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="L8" s="13" t="s">
-        <v>55</v>
-      </c>
       <c r="M8" s="39">
-        <f>F6</f>
+        <f>G6</f>
         <v>1</v>
       </c>
       <c r="N8" s="39">
@@ -2581,15 +2658,12 @@
     <row r="9" spans="1:67" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="44"/>
-      <c r="C9" s="41"/>
+      <c r="C9" s="44"/>
       <c r="D9" s="41"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="54"/>
-      <c r="G9" s="55"/>
-      <c r="H9" s="62" t="str">
-        <f>IF(OR(ISBLANK(F9),ISBLANK(G9)),"",G9-F9+1)</f>
-        <v/>
-      </c>
+      <c r="E9" s="41"/>
+      <c r="F9" s="51"/>
+      <c r="G9" s="54"/>
+      <c r="H9" s="55"/>
       <c r="I9" s="54"/>
       <c r="J9" s="55"/>
       <c r="K9" s="55"/>
@@ -2655,20 +2729,17 @@
     <row r="10" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
       <c r="B10" s="45" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" s="42"/>
+        <v>49</v>
+      </c>
+      <c r="C10" s="45"/>
       <c r="D10" s="42"/>
-      <c r="E10" s="52"/>
-      <c r="F10" s="56">
+      <c r="E10" s="42"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="56">
         <v>43851</v>
       </c>
-      <c r="G10" s="57">
+      <c r="H10" s="57">
         <v>43854</v>
-      </c>
-      <c r="H10" s="63">
-        <f>IF(OR(ISBLANK(F10),ISBLANK(G10)),"",G10-F10+1)</f>
-        <v>4</v>
       </c>
       <c r="I10" s="56">
         <v>43851</v>
@@ -2737,14 +2808,14 @@
     <row r="11" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="48"/>
       <c r="B11" s="45" t="s">
-        <v>78</v>
-      </c>
-      <c r="C11" s="42"/>
+        <v>77</v>
+      </c>
+      <c r="C11" s="45"/>
       <c r="D11" s="42"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="56"/>
-      <c r="G11" s="57"/>
-      <c r="H11" s="63"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="56"/>
+      <c r="H11" s="57"/>
       <c r="I11" s="56"/>
       <c r="J11" s="57"/>
       <c r="K11" s="57"/>
@@ -2807,26 +2878,23 @@
     <row r="12" spans="1:67" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="C12" s="75" t="s">
-        <v>60</v>
-      </c>
+        <v>56</v>
+      </c>
+      <c r="C12" s="15"/>
       <c r="D12" s="75" t="s">
-        <v>67</v>
-      </c>
-      <c r="E12" s="51">
+        <v>59</v>
+      </c>
+      <c r="E12" s="75" t="s">
+        <v>66</v>
+      </c>
+      <c r="F12" s="51">
         <v>1</v>
       </c>
-      <c r="F12" s="54">
+      <c r="G12" s="54">
         <v>43852</v>
       </c>
-      <c r="G12" s="55">
+      <c r="H12" s="55">
         <v>43853</v>
-      </c>
-      <c r="H12" s="62">
-        <f t="shared" ref="H12:H25" si="3">IF(OR(ISBLANK(F12),ISBLANK(G12)),"",G12-F12+1)</f>
-        <v>2</v>
       </c>
       <c r="I12" s="54">
         <v>43852</v>
@@ -2894,26 +2962,23 @@
     <row r="13" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="15" t="s">
-        <v>58</v>
-      </c>
-      <c r="C13" s="41" t="s">
-        <v>61</v>
-      </c>
+        <v>57</v>
+      </c>
+      <c r="C13" s="15"/>
       <c r="D13" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E13" s="51">
+        <v>60</v>
+      </c>
+      <c r="E13" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F13" s="51">
         <v>1</v>
       </c>
-      <c r="F13" s="54">
+      <c r="G13" s="54">
         <v>43854</v>
       </c>
-      <c r="G13" s="55">
+      <c r="H13" s="55">
         <v>43854</v>
-      </c>
-      <c r="H13" s="62">
-        <f t="shared" si="3"/>
-        <v>1</v>
       </c>
       <c r="I13" s="54">
         <v>43854</v>
@@ -2981,26 +3046,23 @@
     <row r="14" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C14" s="41" t="s">
-        <v>68</v>
-      </c>
+        <v>58</v>
+      </c>
+      <c r="C14" s="15"/>
       <c r="D14" s="41" t="s">
         <v>67</v>
       </c>
-      <c r="E14" s="51">
+      <c r="E14" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F14" s="51">
         <v>1</v>
       </c>
-      <c r="F14" s="54">
+      <c r="G14" s="54">
         <v>43854</v>
       </c>
-      <c r="G14" s="55">
+      <c r="H14" s="55">
         <v>43854</v>
-      </c>
-      <c r="H14" s="62">
-        <f t="shared" si="3"/>
-        <v>1</v>
       </c>
       <c r="I14" s="54">
         <v>43854</v>
@@ -3068,26 +3130,23 @@
     <row r="15" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
       <c r="B15" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C15" s="41" t="s">
-        <v>65</v>
-      </c>
+        <v>61</v>
+      </c>
+      <c r="C15" s="15"/>
       <c r="D15" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E15" s="51">
+        <v>64</v>
+      </c>
+      <c r="E15" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F15" s="51">
         <v>1</v>
       </c>
-      <c r="F15" s="54">
+      <c r="G15" s="54">
         <v>43853</v>
       </c>
-      <c r="G15" s="55">
+      <c r="H15" s="55">
         <v>43853</v>
-      </c>
-      <c r="H15" s="62">
-        <f t="shared" si="3"/>
-        <v>1</v>
       </c>
       <c r="I15" s="54">
         <v>43852</v>
@@ -3155,26 +3214,23 @@
     <row r="16" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="15" t="s">
+        <v>62</v>
+      </c>
+      <c r="C16" s="15"/>
+      <c r="D16" s="41" t="s">
         <v>63</v>
       </c>
-      <c r="C16" s="41" t="s">
-        <v>64</v>
-      </c>
-      <c r="D16" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E16" s="51">
+      <c r="E16" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F16" s="51">
         <v>1</v>
       </c>
-      <c r="F16" s="54">
+      <c r="G16" s="54">
         <v>43867</v>
       </c>
-      <c r="G16" s="55">
+      <c r="H16" s="55">
         <v>43868</v>
-      </c>
-      <c r="H16" s="62">
-        <f t="shared" si="3"/>
-        <v>2</v>
       </c>
       <c r="I16" s="54">
         <v>43867</v>
@@ -3239,107 +3295,275 @@
       <c r="BM16" s="16"/>
       <c r="BN16" s="16"/>
     </row>
-    <row r="17" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="48"/>
-      <c r="B17" s="45" t="s">
-        <v>79</v>
-      </c>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="52"/>
-      <c r="F17" s="56"/>
-      <c r="G17" s="57"/>
-      <c r="H17" s="63"/>
-      <c r="I17" s="56"/>
-      <c r="J17" s="57"/>
-      <c r="K17" s="57"/>
-      <c r="L17" s="63"/>
-      <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
-      <c r="P17" s="16"/>
-      <c r="Q17" s="16"/>
-      <c r="R17" s="16"/>
-      <c r="S17" s="16"/>
-      <c r="T17" s="16"/>
-      <c r="U17" s="16"/>
-      <c r="V17" s="16"/>
-      <c r="W17" s="16"/>
-      <c r="X17" s="16"/>
-      <c r="Y17" s="16"/>
-      <c r="Z17" s="16"/>
-      <c r="AA17" s="16"/>
-      <c r="AB17" s="16"/>
-      <c r="AC17" s="16"/>
-      <c r="AD17" s="16"/>
-      <c r="AE17" s="16"/>
-      <c r="AF17" s="16"/>
-      <c r="AG17" s="16"/>
-      <c r="AH17" s="16"/>
-      <c r="AI17" s="16"/>
-      <c r="AJ17" s="16"/>
-      <c r="AK17" s="16"/>
-      <c r="AL17" s="16"/>
-      <c r="AM17" s="16"/>
-      <c r="AN17" s="16"/>
-      <c r="AO17" s="16"/>
-      <c r="AP17" s="16"/>
-      <c r="AQ17" s="16"/>
-      <c r="AR17" s="16"/>
-      <c r="AS17" s="16"/>
-      <c r="AT17" s="16"/>
-      <c r="AU17" s="16"/>
-      <c r="AV17" s="16"/>
-      <c r="AW17" s="16"/>
-      <c r="AX17" s="16"/>
-      <c r="AY17" s="16"/>
-      <c r="AZ17" s="16"/>
-      <c r="BA17" s="16"/>
-      <c r="BB17" s="16"/>
-      <c r="BC17" s="16"/>
-      <c r="BD17" s="16"/>
-      <c r="BE17" s="16"/>
-      <c r="BF17" s="16"/>
-      <c r="BG17" s="16"/>
-      <c r="BH17" s="16"/>
-      <c r="BI17" s="16"/>
-      <c r="BJ17" s="16"/>
-      <c r="BK17" s="16"/>
-      <c r="BL17" s="16"/>
-      <c r="BM17" s="16"/>
-      <c r="BN17" s="16"/>
+    <row r="17" spans="1:66" s="72" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B17" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F17" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G17" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="H17" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="I17" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J17" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L17" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="M17" s="39">
+        <f>G15</f>
+        <v>43853</v>
+      </c>
+      <c r="N17" s="39">
+        <f>M17+1</f>
+        <v>43854</v>
+      </c>
+      <c r="O17" s="39">
+        <f t="shared" ref="O17" si="3">N17+1</f>
+        <v>43855</v>
+      </c>
+      <c r="P17" s="39">
+        <f t="shared" ref="P17" si="4">O17+1</f>
+        <v>43856</v>
+      </c>
+      <c r="Q17" s="39">
+        <f t="shared" ref="Q17" si="5">P17+1</f>
+        <v>43857</v>
+      </c>
+      <c r="R17" s="39">
+        <f t="shared" ref="R17" si="6">Q17+1</f>
+        <v>43858</v>
+      </c>
+      <c r="S17" s="39">
+        <f t="shared" ref="S17" si="7">R17+1</f>
+        <v>43859</v>
+      </c>
+      <c r="T17" s="39">
+        <f t="shared" ref="T17" si="8">S17+1</f>
+        <v>43860</v>
+      </c>
+      <c r="U17" s="39">
+        <f t="shared" ref="U17" si="9">T17+1</f>
+        <v>43861</v>
+      </c>
+      <c r="V17" s="39">
+        <f t="shared" ref="V17" si="10">U17+1</f>
+        <v>43862</v>
+      </c>
+      <c r="W17" s="39">
+        <f t="shared" ref="W17" si="11">V17+1</f>
+        <v>43863</v>
+      </c>
+      <c r="X17" s="39">
+        <f t="shared" ref="X17" si="12">W17+1</f>
+        <v>43864</v>
+      </c>
+      <c r="Y17" s="39">
+        <f t="shared" ref="Y17" si="13">X17+1</f>
+        <v>43865</v>
+      </c>
+      <c r="Z17" s="39">
+        <f t="shared" ref="Z17" si="14">Y17+1</f>
+        <v>43866</v>
+      </c>
+      <c r="AA17" s="39">
+        <f t="shared" ref="AA17" si="15">Z17+1</f>
+        <v>43867</v>
+      </c>
+      <c r="AB17" s="39">
+        <f t="shared" ref="AB17" si="16">AA17+1</f>
+        <v>43868</v>
+      </c>
+      <c r="AC17" s="39">
+        <f t="shared" ref="AC17" si="17">AB17+1</f>
+        <v>43869</v>
+      </c>
+      <c r="AD17" s="39">
+        <f t="shared" ref="AD17" si="18">AC17+1</f>
+        <v>43870</v>
+      </c>
+      <c r="AE17" s="39">
+        <f t="shared" ref="AE17" si="19">AD17+1</f>
+        <v>43871</v>
+      </c>
+      <c r="AF17" s="39">
+        <f t="shared" ref="AF17" si="20">AE17+1</f>
+        <v>43872</v>
+      </c>
+      <c r="AG17" s="39">
+        <f t="shared" ref="AG17" si="21">AF17+1</f>
+        <v>43873</v>
+      </c>
+      <c r="AH17" s="39">
+        <f t="shared" ref="AH17" si="22">AG17+1</f>
+        <v>43874</v>
+      </c>
+      <c r="AI17" s="39">
+        <f t="shared" ref="AI17" si="23">AH17+1</f>
+        <v>43875</v>
+      </c>
+      <c r="AJ17" s="39">
+        <f t="shared" ref="AJ17" si="24">AI17+1</f>
+        <v>43876</v>
+      </c>
+      <c r="AK17" s="39">
+        <f t="shared" ref="AK17" si="25">AJ17+1</f>
+        <v>43877</v>
+      </c>
+      <c r="AL17" s="39">
+        <f t="shared" ref="AL17" si="26">AK17+1</f>
+        <v>43878</v>
+      </c>
+      <c r="AM17" s="39">
+        <f t="shared" ref="AM17" si="27">AL17+1</f>
+        <v>43879</v>
+      </c>
+      <c r="AN17" s="39">
+        <f t="shared" ref="AN17" si="28">AM17+1</f>
+        <v>43880</v>
+      </c>
+      <c r="AO17" s="39">
+        <f t="shared" ref="AO17" si="29">AN17+1</f>
+        <v>43881</v>
+      </c>
+      <c r="AP17" s="39">
+        <f t="shared" ref="AP17" si="30">AO17+1</f>
+        <v>43882</v>
+      </c>
+      <c r="AQ17" s="39">
+        <f t="shared" ref="AQ17" si="31">AP17+1</f>
+        <v>43883</v>
+      </c>
+      <c r="AR17" s="39">
+        <f t="shared" ref="AR17" si="32">AQ17+1</f>
+        <v>43884</v>
+      </c>
+      <c r="AS17" s="39">
+        <f t="shared" ref="AS17" si="33">AR17+1</f>
+        <v>43885</v>
+      </c>
+      <c r="AT17" s="39">
+        <f t="shared" ref="AT17" si="34">AS17+1</f>
+        <v>43886</v>
+      </c>
+      <c r="AU17" s="39">
+        <f t="shared" ref="AU17" si="35">AT17+1</f>
+        <v>43887</v>
+      </c>
+      <c r="AV17" s="39">
+        <f t="shared" ref="AV17" si="36">AU17+1</f>
+        <v>43888</v>
+      </c>
+      <c r="AW17" s="39">
+        <f t="shared" ref="AW17" si="37">AV17+1</f>
+        <v>43889</v>
+      </c>
+      <c r="AX17" s="39">
+        <f t="shared" ref="AX17" si="38">AW17+1</f>
+        <v>43890</v>
+      </c>
+      <c r="AY17" s="39">
+        <f t="shared" ref="AY17" si="39">AX17+1</f>
+        <v>43891</v>
+      </c>
+      <c r="AZ17" s="39">
+        <f t="shared" ref="AZ17" si="40">AY17+1</f>
+        <v>43892</v>
+      </c>
+      <c r="BA17" s="39">
+        <f t="shared" ref="BA17" si="41">AZ17+1</f>
+        <v>43893</v>
+      </c>
+      <c r="BB17" s="39">
+        <f t="shared" ref="BB17" si="42">BA17+1</f>
+        <v>43894</v>
+      </c>
+      <c r="BC17" s="39">
+        <f t="shared" ref="BC17" si="43">BB17+1</f>
+        <v>43895</v>
+      </c>
+      <c r="BD17" s="39">
+        <f t="shared" ref="BD17" si="44">BC17+1</f>
+        <v>43896</v>
+      </c>
+      <c r="BE17" s="39">
+        <f t="shared" ref="BE17" si="45">BD17+1</f>
+        <v>43897</v>
+      </c>
+      <c r="BF17" s="39">
+        <f t="shared" ref="BF17" si="46">BE17+1</f>
+        <v>43898</v>
+      </c>
+      <c r="BG17" s="39">
+        <f t="shared" ref="BG17" si="47">BF17+1</f>
+        <v>43899</v>
+      </c>
+      <c r="BH17" s="39">
+        <f t="shared" ref="BH17" si="48">BG17+1</f>
+        <v>43900</v>
+      </c>
+      <c r="BI17" s="39">
+        <f t="shared" ref="BI17" si="49">BH17+1</f>
+        <v>43901</v>
+      </c>
+      <c r="BJ17" s="39">
+        <f t="shared" ref="BJ17" si="50">BI17+1</f>
+        <v>43902</v>
+      </c>
+      <c r="BK17" s="39">
+        <f t="shared" ref="BK17" si="51">BJ17+1</f>
+        <v>43903</v>
+      </c>
+      <c r="BL17" s="39">
+        <f t="shared" ref="BL17" si="52">BK17+1</f>
+        <v>43904</v>
+      </c>
+      <c r="BM17" s="39">
+        <f t="shared" ref="BM17" si="53">BL17+1</f>
+        <v>43905</v>
+      </c>
+      <c r="BN17" s="39">
+        <f t="shared" ref="BN17" si="54">BM17+1</f>
+        <v>43906</v>
+      </c>
     </row>
     <row r="18" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="47"/>
-      <c r="B18" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C18" s="41" t="s">
-        <v>70</v>
-      </c>
-      <c r="D18" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E18" s="51">
-        <v>1</v>
-      </c>
-      <c r="F18" s="54">
-        <v>43862</v>
-      </c>
-      <c r="G18" s="55">
-        <v>43863</v>
-      </c>
-      <c r="H18" s="62">
-        <v>4</v>
-      </c>
-      <c r="I18" s="54">
-        <v>43862</v>
-      </c>
-      <c r="J18" s="55">
-        <v>43867</v>
-      </c>
-      <c r="K18" s="55"/>
-      <c r="L18" s="62"/>
+      <c r="A18" s="48"/>
+      <c r="B18" s="45" t="s">
+        <v>78</v>
+      </c>
+      <c r="C18" s="45"/>
+      <c r="D18" s="42"/>
+      <c r="E18" s="42"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="56"/>
+      <c r="H18" s="57"/>
+      <c r="I18" s="56"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="63"/>
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
@@ -3398,29 +3622,26 @@
     <row r="19" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C19" s="41" t="s">
-        <v>61</v>
-      </c>
+        <v>68</v>
+      </c>
+      <c r="C19" s="15"/>
       <c r="D19" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" s="51">
+        <v>69</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F19" s="51">
         <v>1</v>
       </c>
-      <c r="F19" s="54">
-        <v>43865</v>
-      </c>
-      <c r="G19" s="55">
-        <v>43866</v>
-      </c>
-      <c r="H19" s="62">
-        <f t="shared" ref="H19:H24" si="4">IF(OR(ISBLANK(F19),ISBLANK(G19)),"",G19-F19+1)</f>
-        <v>2</v>
+      <c r="G19" s="54">
+        <v>43862</v>
+      </c>
+      <c r="H19" s="55">
+        <v>43863</v>
       </c>
       <c r="I19" s="54">
-        <v>43865</v>
+        <v>43862</v>
       </c>
       <c r="J19" s="55">
         <v>43867</v>
@@ -3485,29 +3706,26 @@
     <row r="20" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="15" t="s">
-        <v>72</v>
-      </c>
-      <c r="C20" s="41" t="s">
-        <v>80</v>
-      </c>
+        <v>70</v>
+      </c>
+      <c r="C20" s="15"/>
       <c r="D20" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E20" s="51">
+        <v>60</v>
+      </c>
+      <c r="E20" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F20" s="51">
         <v>1</v>
       </c>
-      <c r="F20" s="54">
-        <v>43862</v>
-      </c>
-      <c r="G20" s="55">
-        <v>43864</v>
-      </c>
-      <c r="H20" s="62">
-        <f t="shared" si="4"/>
-        <v>3</v>
+      <c r="G20" s="54">
+        <v>43865</v>
+      </c>
+      <c r="H20" s="55">
+        <v>43866</v>
       </c>
       <c r="I20" s="54">
-        <v>43862</v>
+        <v>43865</v>
       </c>
       <c r="J20" s="55">
         <v>43867</v>
@@ -3572,32 +3790,29 @@
     <row r="21" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="C21" s="41" t="s">
-        <v>65</v>
-      </c>
+        <v>71</v>
+      </c>
+      <c r="C21" s="15"/>
       <c r="D21" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E21" s="51">
+        <v>79</v>
+      </c>
+      <c r="E21" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="51">
         <v>1</v>
       </c>
-      <c r="F21" s="54">
+      <c r="G21" s="54">
+        <v>43862</v>
+      </c>
+      <c r="H21" s="55">
         <v>43864</v>
       </c>
-      <c r="G21" s="55">
-        <v>43865</v>
-      </c>
-      <c r="H21" s="62">
-        <f t="shared" si="4"/>
-        <v>2</v>
-      </c>
       <c r="I21" s="54">
-        <v>43865</v>
+        <v>43862</v>
       </c>
       <c r="J21" s="55">
-        <v>43865</v>
+        <v>43867</v>
       </c>
       <c r="K21" s="55"/>
       <c r="L21" s="62"/>
@@ -3659,32 +3874,29 @@
     <row r="22" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
       <c r="B22" s="15" t="s">
-        <v>74</v>
-      </c>
-      <c r="C22" s="41" t="s">
-        <v>70</v>
-      </c>
+        <v>72</v>
+      </c>
+      <c r="C22" s="15"/>
       <c r="D22" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E22" s="51">
+        <v>64</v>
+      </c>
+      <c r="E22" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F22" s="51">
         <v>1</v>
       </c>
-      <c r="F22" s="54">
-        <v>43866</v>
-      </c>
-      <c r="G22" s="55">
-        <v>43866</v>
-      </c>
-      <c r="H22" s="62">
-        <f t="shared" si="4"/>
-        <v>1</v>
+      <c r="G22" s="54">
+        <v>43864</v>
+      </c>
+      <c r="H22" s="55">
+        <v>43865</v>
       </c>
       <c r="I22" s="54">
-        <v>43862</v>
+        <v>43865</v>
       </c>
       <c r="J22" s="55">
-        <v>43867</v>
+        <v>43865</v>
       </c>
       <c r="K22" s="55"/>
       <c r="L22" s="62"/>
@@ -3746,32 +3958,29 @@
     <row r="23" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
       <c r="B23" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="C23" s="41" t="s">
-        <v>76</v>
-      </c>
+        <v>73</v>
+      </c>
+      <c r="C23" s="15"/>
       <c r="D23" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E23" s="51">
+        <v>69</v>
+      </c>
+      <c r="E23" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F23" s="51">
         <v>1</v>
       </c>
-      <c r="F23" s="54">
-        <v>43864</v>
-      </c>
-      <c r="G23" s="55">
-        <v>43865</v>
-      </c>
-      <c r="H23" s="62">
-        <f t="shared" si="4"/>
-        <v>2</v>
+      <c r="G23" s="54">
+        <v>43866</v>
+      </c>
+      <c r="H23" s="55">
+        <v>43866</v>
       </c>
       <c r="I23" s="54">
-        <v>43868</v>
+        <v>43862</v>
       </c>
       <c r="J23" s="55">
-        <v>43868</v>
+        <v>43867</v>
       </c>
       <c r="K23" s="55"/>
       <c r="L23" s="62"/>
@@ -3833,26 +4042,23 @@
     <row r="24" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47"/>
       <c r="B24" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="C24" s="41" t="s">
-        <v>64</v>
-      </c>
+        <v>74</v>
+      </c>
+      <c r="C24" s="15"/>
       <c r="D24" s="41" t="s">
-        <v>67</v>
-      </c>
-      <c r="E24" s="51">
+        <v>75</v>
+      </c>
+      <c r="E24" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F24" s="51">
         <v>1</v>
       </c>
-      <c r="F24" s="54">
-        <v>43867</v>
-      </c>
-      <c r="G24" s="55">
-        <v>43868</v>
-      </c>
-      <c r="H24" s="62">
-        <f t="shared" si="4"/>
-        <v>2</v>
+      <c r="G24" s="54">
+        <v>43864</v>
+      </c>
+      <c r="H24" s="55">
+        <v>43865</v>
       </c>
       <c r="I24" s="54">
         <v>43868</v>
@@ -3920,24 +4126,32 @@
     <row r="25" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
       <c r="B25" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="54"/>
-      <c r="G25" s="55"/>
-      <c r="H25" s="62" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-      <c r="I25" s="54"/>
-      <c r="J25" s="55"/>
+        <v>76</v>
+      </c>
+      <c r="C25" s="15"/>
+      <c r="D25" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F25" s="51">
+        <v>1</v>
+      </c>
+      <c r="G25" s="54">
+        <v>43867</v>
+      </c>
+      <c r="H25" s="55">
+        <v>43868</v>
+      </c>
+      <c r="I25" s="54">
+        <v>43868</v>
+      </c>
+      <c r="J25" s="55">
+        <v>43868</v>
+      </c>
       <c r="K25" s="55"/>
-      <c r="L25" s="62" t="str">
-        <f>IF(OR(ISBLANK(I25),ISBLANK(J25)),"",J25-I25+1)</f>
-        <v/>
-      </c>
+      <c r="L25" s="62"/>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
@@ -3950,10 +4164,10 @@
       <c r="V25" s="16"/>
       <c r="W25" s="16"/>
       <c r="X25" s="16"/>
-      <c r="Y25" s="17"/>
+      <c r="Y25" s="16"/>
       <c r="Z25" s="16"/>
       <c r="AA25" s="16"/>
-      <c r="AB25" s="17"/>
+      <c r="AB25" s="16"/>
       <c r="AC25" s="16"/>
       <c r="AD25" s="16"/>
       <c r="AE25" s="16"/>
@@ -3993,97 +4207,275 @@
       <c r="BM25" s="16"/>
       <c r="BN25" s="16"/>
     </row>
-    <row r="26" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="48"/>
-      <c r="B26" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="52"/>
-      <c r="F26" s="56"/>
-      <c r="G26" s="57"/>
-      <c r="H26" s="63" t="str">
-        <f t="shared" ref="H26:H42" si="5">IF(OR(ISBLANK(F26),ISBLANK(G26)),"",G26-F26+1)</f>
-        <v/>
-      </c>
-      <c r="I26" s="56"/>
-      <c r="J26" s="57"/>
-      <c r="K26" s="57"/>
-      <c r="L26" s="63" t="str">
-        <f>IF(OR(ISBLANK(I26),ISBLANK(J26)),"",J26-I26+1)</f>
-        <v/>
-      </c>
-      <c r="M26" s="16"/>
-      <c r="N26" s="16"/>
-      <c r="O26" s="16"/>
-      <c r="P26" s="16"/>
-      <c r="Q26" s="16"/>
-      <c r="R26" s="16"/>
-      <c r="S26" s="16"/>
-      <c r="T26" s="16"/>
-      <c r="U26" s="16"/>
-      <c r="V26" s="16"/>
-      <c r="W26" s="16"/>
-      <c r="X26" s="16"/>
-      <c r="Y26" s="16"/>
-      <c r="Z26" s="16"/>
-      <c r="AA26" s="16"/>
-      <c r="AB26" s="16"/>
-      <c r="AC26" s="16"/>
-      <c r="AD26" s="16"/>
-      <c r="AE26" s="16"/>
-      <c r="AF26" s="16"/>
-      <c r="AG26" s="16"/>
-      <c r="AH26" s="16"/>
-      <c r="AI26" s="16"/>
-      <c r="AJ26" s="16"/>
-      <c r="AK26" s="16"/>
-      <c r="AL26" s="16"/>
-      <c r="AM26" s="16"/>
-      <c r="AN26" s="16"/>
-      <c r="AO26" s="16"/>
-      <c r="AP26" s="16"/>
-      <c r="AQ26" s="16"/>
-      <c r="AR26" s="16"/>
-      <c r="AS26" s="16"/>
-      <c r="AT26" s="16"/>
-      <c r="AU26" s="16"/>
-      <c r="AV26" s="16"/>
-      <c r="AW26" s="16"/>
-      <c r="AX26" s="16"/>
-      <c r="AY26" s="16"/>
-      <c r="AZ26" s="16"/>
-      <c r="BA26" s="16"/>
-      <c r="BB26" s="16"/>
-      <c r="BC26" s="16"/>
-      <c r="BD26" s="16"/>
-      <c r="BE26" s="16"/>
-      <c r="BF26" s="16"/>
-      <c r="BG26" s="16"/>
-      <c r="BH26" s="16"/>
-      <c r="BI26" s="16"/>
-      <c r="BJ26" s="16"/>
-      <c r="BK26" s="16"/>
-      <c r="BL26" s="16"/>
-      <c r="BM26" s="16"/>
-      <c r="BN26" s="16"/>
+    <row r="26" spans="1:66" s="72" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>10</v>
+      </c>
+      <c r="C26" s="12" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>65</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>30</v>
+      </c>
+      <c r="G26" s="70" t="s">
+        <v>8</v>
+      </c>
+      <c r="H26" s="70" t="s">
+        <v>9</v>
+      </c>
+      <c r="I26" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>54</v>
+      </c>
+      <c r="M26" s="39">
+        <f>G24</f>
+        <v>43864</v>
+      </c>
+      <c r="N26" s="39">
+        <f>M26+1</f>
+        <v>43865</v>
+      </c>
+      <c r="O26" s="39">
+        <f t="shared" ref="O26" si="55">N26+1</f>
+        <v>43866</v>
+      </c>
+      <c r="P26" s="39">
+        <f t="shared" ref="P26" si="56">O26+1</f>
+        <v>43867</v>
+      </c>
+      <c r="Q26" s="39">
+        <f t="shared" ref="Q26" si="57">P26+1</f>
+        <v>43868</v>
+      </c>
+      <c r="R26" s="39">
+        <f t="shared" ref="R26" si="58">Q26+1</f>
+        <v>43869</v>
+      </c>
+      <c r="S26" s="39">
+        <f t="shared" ref="S26" si="59">R26+1</f>
+        <v>43870</v>
+      </c>
+      <c r="T26" s="39">
+        <f t="shared" ref="T26" si="60">S26+1</f>
+        <v>43871</v>
+      </c>
+      <c r="U26" s="39">
+        <f t="shared" ref="U26" si="61">T26+1</f>
+        <v>43872</v>
+      </c>
+      <c r="V26" s="39">
+        <f t="shared" ref="V26" si="62">U26+1</f>
+        <v>43873</v>
+      </c>
+      <c r="W26" s="39">
+        <f t="shared" ref="W26" si="63">V26+1</f>
+        <v>43874</v>
+      </c>
+      <c r="X26" s="39">
+        <f t="shared" ref="X26" si="64">W26+1</f>
+        <v>43875</v>
+      </c>
+      <c r="Y26" s="39">
+        <f t="shared" ref="Y26" si="65">X26+1</f>
+        <v>43876</v>
+      </c>
+      <c r="Z26" s="39">
+        <f t="shared" ref="Z26" si="66">Y26+1</f>
+        <v>43877</v>
+      </c>
+      <c r="AA26" s="39">
+        <f t="shared" ref="AA26" si="67">Z26+1</f>
+        <v>43878</v>
+      </c>
+      <c r="AB26" s="39">
+        <f t="shared" ref="AB26" si="68">AA26+1</f>
+        <v>43879</v>
+      </c>
+      <c r="AC26" s="39">
+        <f t="shared" ref="AC26" si="69">AB26+1</f>
+        <v>43880</v>
+      </c>
+      <c r="AD26" s="39">
+        <f t="shared" ref="AD26" si="70">AC26+1</f>
+        <v>43881</v>
+      </c>
+      <c r="AE26" s="39">
+        <f t="shared" ref="AE26" si="71">AD26+1</f>
+        <v>43882</v>
+      </c>
+      <c r="AF26" s="39">
+        <f t="shared" ref="AF26" si="72">AE26+1</f>
+        <v>43883</v>
+      </c>
+      <c r="AG26" s="39">
+        <f t="shared" ref="AG26" si="73">AF26+1</f>
+        <v>43884</v>
+      </c>
+      <c r="AH26" s="39">
+        <f t="shared" ref="AH26" si="74">AG26+1</f>
+        <v>43885</v>
+      </c>
+      <c r="AI26" s="39">
+        <f t="shared" ref="AI26" si="75">AH26+1</f>
+        <v>43886</v>
+      </c>
+      <c r="AJ26" s="39">
+        <f t="shared" ref="AJ26" si="76">AI26+1</f>
+        <v>43887</v>
+      </c>
+      <c r="AK26" s="39">
+        <f t="shared" ref="AK26" si="77">AJ26+1</f>
+        <v>43888</v>
+      </c>
+      <c r="AL26" s="39">
+        <f t="shared" ref="AL26" si="78">AK26+1</f>
+        <v>43889</v>
+      </c>
+      <c r="AM26" s="39">
+        <f t="shared" ref="AM26" si="79">AL26+1</f>
+        <v>43890</v>
+      </c>
+      <c r="AN26" s="39">
+        <f t="shared" ref="AN26" si="80">AM26+1</f>
+        <v>43891</v>
+      </c>
+      <c r="AO26" s="39">
+        <f t="shared" ref="AO26" si="81">AN26+1</f>
+        <v>43892</v>
+      </c>
+      <c r="AP26" s="39">
+        <f t="shared" ref="AP26" si="82">AO26+1</f>
+        <v>43893</v>
+      </c>
+      <c r="AQ26" s="39">
+        <f t="shared" ref="AQ26" si="83">AP26+1</f>
+        <v>43894</v>
+      </c>
+      <c r="AR26" s="39">
+        <f t="shared" ref="AR26" si="84">AQ26+1</f>
+        <v>43895</v>
+      </c>
+      <c r="AS26" s="39">
+        <f t="shared" ref="AS26" si="85">AR26+1</f>
+        <v>43896</v>
+      </c>
+      <c r="AT26" s="39">
+        <f t="shared" ref="AT26" si="86">AS26+1</f>
+        <v>43897</v>
+      </c>
+      <c r="AU26" s="39">
+        <f t="shared" ref="AU26" si="87">AT26+1</f>
+        <v>43898</v>
+      </c>
+      <c r="AV26" s="39">
+        <f t="shared" ref="AV26" si="88">AU26+1</f>
+        <v>43899</v>
+      </c>
+      <c r="AW26" s="39">
+        <f t="shared" ref="AW26" si="89">AV26+1</f>
+        <v>43900</v>
+      </c>
+      <c r="AX26" s="39">
+        <f t="shared" ref="AX26" si="90">AW26+1</f>
+        <v>43901</v>
+      </c>
+      <c r="AY26" s="39">
+        <f t="shared" ref="AY26" si="91">AX26+1</f>
+        <v>43902</v>
+      </c>
+      <c r="AZ26" s="39">
+        <f t="shared" ref="AZ26" si="92">AY26+1</f>
+        <v>43903</v>
+      </c>
+      <c r="BA26" s="39">
+        <f t="shared" ref="BA26" si="93">AZ26+1</f>
+        <v>43904</v>
+      </c>
+      <c r="BB26" s="39">
+        <f t="shared" ref="BB26" si="94">BA26+1</f>
+        <v>43905</v>
+      </c>
+      <c r="BC26" s="39">
+        <f t="shared" ref="BC26" si="95">BB26+1</f>
+        <v>43906</v>
+      </c>
+      <c r="BD26" s="39">
+        <f t="shared" ref="BD26" si="96">BC26+1</f>
+        <v>43907</v>
+      </c>
+      <c r="BE26" s="39">
+        <f t="shared" ref="BE26" si="97">BD26+1</f>
+        <v>43908</v>
+      </c>
+      <c r="BF26" s="39">
+        <f t="shared" ref="BF26" si="98">BE26+1</f>
+        <v>43909</v>
+      </c>
+      <c r="BG26" s="39">
+        <f t="shared" ref="BG26" si="99">BF26+1</f>
+        <v>43910</v>
+      </c>
+      <c r="BH26" s="39">
+        <f t="shared" ref="BH26" si="100">BG26+1</f>
+        <v>43911</v>
+      </c>
+      <c r="BI26" s="39">
+        <f t="shared" ref="BI26" si="101">BH26+1</f>
+        <v>43912</v>
+      </c>
+      <c r="BJ26" s="39">
+        <f t="shared" ref="BJ26" si="102">BI26+1</f>
+        <v>43913</v>
+      </c>
+      <c r="BK26" s="39">
+        <f t="shared" ref="BK26" si="103">BJ26+1</f>
+        <v>43914</v>
+      </c>
+      <c r="BL26" s="39">
+        <f t="shared" ref="BL26" si="104">BK26+1</f>
+        <v>43915</v>
+      </c>
+      <c r="BM26" s="39">
+        <f t="shared" ref="BM26" si="105">BL26+1</f>
+        <v>43916</v>
+      </c>
+      <c r="BN26" s="39">
+        <f t="shared" ref="BN26" si="106">BM26+1</f>
+        <v>43917</v>
+      </c>
     </row>
     <row r="27" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="47"/>
-      <c r="B27" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="54"/>
-      <c r="G27" s="55"/>
-      <c r="H27" s="62"/>
-      <c r="I27" s="54"/>
-      <c r="J27" s="55"/>
-      <c r="K27" s="55"/>
-      <c r="L27" s="62"/>
+      <c r="A27" s="48"/>
+      <c r="B27" s="45" t="s">
+        <v>80</v>
+      </c>
+      <c r="C27" s="45"/>
+      <c r="D27" s="42"/>
+      <c r="E27" s="42"/>
+      <c r="F27" s="52"/>
+      <c r="G27" s="56"/>
+      <c r="H27" s="57"/>
+      <c r="I27" s="56"/>
+      <c r="J27" s="57"/>
+      <c r="K27" s="57"/>
+      <c r="L27" s="63"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
@@ -4096,10 +4488,10 @@
       <c r="V27" s="16"/>
       <c r="W27" s="16"/>
       <c r="X27" s="16"/>
-      <c r="Y27" s="16"/>
+      <c r="Y27" s="17"/>
       <c r="Z27" s="16"/>
       <c r="AA27" s="16"/>
-      <c r="AB27" s="16"/>
+      <c r="AB27" s="17"/>
       <c r="AC27" s="16"/>
       <c r="AD27" s="16"/>
       <c r="AE27" s="16"/>
@@ -4139,17 +4531,29 @@
       <c r="BM27" s="16"/>
       <c r="BN27" s="16"/>
     </row>
-    <row r="28" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:66" s="8" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
       <c r="B28" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="54"/>
-      <c r="G28" s="55"/>
-      <c r="H28" s="62"/>
+        <v>68</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D28" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E28" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" s="51">
+        <v>0</v>
+      </c>
+      <c r="G28" s="54">
+        <v>43869</v>
+      </c>
+      <c r="H28" s="55">
+        <v>43869</v>
+      </c>
       <c r="I28" s="54"/>
       <c r="J28" s="55"/>
       <c r="K28" s="55"/>
@@ -4212,14 +4616,26 @@
     <row r="29" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
       <c r="B29" s="15" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="54"/>
-      <c r="G29" s="55"/>
-      <c r="H29" s="62"/>
+        <v>70</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>83</v>
+      </c>
+      <c r="D29" s="41" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F29" s="51">
+        <v>0</v>
+      </c>
+      <c r="G29" s="54">
+        <v>43869</v>
+      </c>
+      <c r="H29" s="55">
+        <v>43872</v>
+      </c>
       <c r="I29" s="54"/>
       <c r="J29" s="55"/>
       <c r="K29" s="55"/>
@@ -4282,14 +4698,26 @@
     <row r="30" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="47"/>
       <c r="B30" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="54"/>
-      <c r="G30" s="55"/>
-      <c r="H30" s="62"/>
+        <v>71</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="D30" s="41" t="s">
+        <v>79</v>
+      </c>
+      <c r="E30" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F30" s="51">
+        <v>0</v>
+      </c>
+      <c r="G30" s="54">
+        <v>43869</v>
+      </c>
+      <c r="H30" s="55">
+        <v>43869</v>
+      </c>
       <c r="I30" s="54"/>
       <c r="J30" s="55"/>
       <c r="K30" s="55"/>
@@ -4352,14 +4780,26 @@
     <row r="31" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="47"/>
       <c r="B31" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="54"/>
-      <c r="G31" s="55"/>
-      <c r="H31" s="62"/>
+        <v>72</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D31" s="41" t="s">
+        <v>64</v>
+      </c>
+      <c r="E31" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F31" s="51">
+        <v>0</v>
+      </c>
+      <c r="G31" s="54">
+        <v>43869</v>
+      </c>
+      <c r="H31" s="55">
+        <v>43869</v>
+      </c>
       <c r="I31" s="54"/>
       <c r="J31" s="55"/>
       <c r="K31" s="55"/>
@@ -4422,14 +4862,26 @@
     <row r="32" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="47"/>
       <c r="B32" s="15" t="s">
-        <v>17</v>
-      </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="54"/>
-      <c r="G32" s="55"/>
-      <c r="H32" s="62"/>
+        <v>73</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="D32" s="41" t="s">
+        <v>75</v>
+      </c>
+      <c r="E32" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F32" s="51">
+        <v>0</v>
+      </c>
+      <c r="G32" s="54">
+        <v>43872</v>
+      </c>
+      <c r="H32" s="55">
+        <v>43872</v>
+      </c>
       <c r="I32" s="54"/>
       <c r="J32" s="55"/>
       <c r="K32" s="55"/>
@@ -4491,23 +4943,31 @@
     </row>
     <row r="33" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="47"/>
-      <c r="B33" s="44"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="54"/>
-      <c r="G33" s="55"/>
-      <c r="H33" s="62" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+      <c r="B33" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="D33" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="E33" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F33" s="51">
+        <v>0</v>
+      </c>
+      <c r="G33" s="54">
+        <v>43869</v>
+      </c>
+      <c r="H33" s="55">
+        <v>43869</v>
       </c>
       <c r="I33" s="54"/>
       <c r="J33" s="55"/>
       <c r="K33" s="55"/>
-      <c r="L33" s="62" t="str">
-        <f>IF(OR(ISBLANK(I33),ISBLANK(J33)),"",J33-I33+1)</f>
-        <v/>
-      </c>
+      <c r="L33" s="62"/>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
       <c r="O33" s="16"/>
@@ -4565,23 +5025,31 @@
     </row>
     <row r="34" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="47"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="41"/>
-      <c r="D34" s="41"/>
-      <c r="E34" s="51"/>
-      <c r="F34" s="54"/>
-      <c r="G34" s="55"/>
-      <c r="H34" s="62" t="str">
-        <f t="shared" si="5"/>
-        <v/>
+      <c r="B34" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="C34" s="79" t="s">
+        <v>88</v>
+      </c>
+      <c r="D34" s="41" t="s">
+        <v>63</v>
+      </c>
+      <c r="E34" s="41" t="s">
+        <v>66</v>
+      </c>
+      <c r="F34" s="51">
+        <v>0</v>
+      </c>
+      <c r="G34" s="54">
+        <v>43873</v>
+      </c>
+      <c r="H34" s="55">
+        <v>43873</v>
       </c>
       <c r="I34" s="54"/>
       <c r="J34" s="55"/>
       <c r="K34" s="55"/>
-      <c r="L34" s="62" t="str">
-        <f>IF(OR(ISBLANK(I34),ISBLANK(J34)),"",J34-I34+1)</f>
-        <v/>
-      </c>
+      <c r="L34" s="62"/>
       <c r="M34" s="16"/>
       <c r="N34" s="16"/>
       <c r="O34" s="16"/>
@@ -4639,16 +5107,15 @@
     </row>
     <row r="35" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="47"/>
-      <c r="B35" s="44"/>
-      <c r="C35" s="41"/>
+      <c r="B35" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="C35" s="15"/>
       <c r="D35" s="41"/>
-      <c r="E35" s="51"/>
-      <c r="F35" s="54"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="62" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="E35" s="41"/>
+      <c r="F35" s="51"/>
+      <c r="G35" s="54"/>
+      <c r="H35" s="55"/>
       <c r="I35" s="54"/>
       <c r="J35" s="55"/>
       <c r="K35" s="55"/>
@@ -4712,18 +5179,23 @@
       <c r="BN35" s="16"/>
     </row>
     <row r="36" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="47"/>
-      <c r="B36" s="44"/>
-      <c r="C36" s="41"/>
-      <c r="D36" s="41"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="54"/>
-      <c r="G36" s="55"/>
-      <c r="H36" s="62"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="55"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="62"/>
+      <c r="A36" s="48"/>
+      <c r="B36" s="45" t="s">
+        <v>14</v>
+      </c>
+      <c r="C36" s="45"/>
+      <c r="D36" s="42"/>
+      <c r="E36" s="42"/>
+      <c r="F36" s="52"/>
+      <c r="G36" s="56"/>
+      <c r="H36" s="57"/>
+      <c r="I36" s="56"/>
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="63" t="str">
+        <f>IF(OR(ISBLANK(I36),ISBLANK(J36)),"",J36-I36+1)</f>
+        <v/>
+      </c>
       <c r="M36" s="16"/>
       <c r="N36" s="16"/>
       <c r="O36" s="16"/>
@@ -4781,13 +5253,15 @@
     </row>
     <row r="37" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="47"/>
-      <c r="B37" s="44"/>
-      <c r="C37" s="41"/>
+      <c r="B37" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="C37" s="15"/>
       <c r="D37" s="41"/>
-      <c r="E37" s="51"/>
-      <c r="F37" s="54"/>
-      <c r="G37" s="55"/>
-      <c r="H37" s="62"/>
+      <c r="E37" s="41"/>
+      <c r="F37" s="51"/>
+      <c r="G37" s="54"/>
+      <c r="H37" s="55"/>
       <c r="I37" s="54"/>
       <c r="J37" s="55"/>
       <c r="K37" s="55"/>
@@ -4849,13 +5323,15 @@
     </row>
     <row r="38" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="47"/>
-      <c r="B38" s="44"/>
-      <c r="C38" s="41"/>
+      <c r="B38" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="C38" s="15"/>
       <c r="D38" s="41"/>
-      <c r="E38" s="51"/>
-      <c r="F38" s="54"/>
-      <c r="G38" s="55"/>
-      <c r="H38" s="62"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="54"/>
+      <c r="H38" s="55"/>
       <c r="I38" s="54"/>
       <c r="J38" s="55"/>
       <c r="K38" s="55"/>
@@ -4917,13 +5393,15 @@
     </row>
     <row r="39" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="47"/>
-      <c r="B39" s="44"/>
-      <c r="C39" s="41"/>
+      <c r="B39" s="15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="15"/>
       <c r="D39" s="41"/>
-      <c r="E39" s="51"/>
-      <c r="F39" s="54"/>
-      <c r="G39" s="55"/>
-      <c r="H39" s="62"/>
+      <c r="E39" s="41"/>
+      <c r="F39" s="51"/>
+      <c r="G39" s="54"/>
+      <c r="H39" s="55"/>
       <c r="I39" s="54"/>
       <c r="J39" s="55"/>
       <c r="K39" s="55"/>
@@ -4985,13 +5463,15 @@
     </row>
     <row r="40" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="47"/>
-      <c r="B40" s="44"/>
-      <c r="C40" s="41"/>
+      <c r="B40" s="15" t="s">
+        <v>12</v>
+      </c>
+      <c r="C40" s="15"/>
       <c r="D40" s="41"/>
-      <c r="E40" s="51"/>
-      <c r="F40" s="54"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="62"/>
+      <c r="E40" s="41"/>
+      <c r="F40" s="51"/>
+      <c r="G40" s="54"/>
+      <c r="H40" s="55"/>
       <c r="I40" s="54"/>
       <c r="J40" s="55"/>
       <c r="K40" s="55"/>
@@ -5053,23 +5533,19 @@
     </row>
     <row r="41" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="47"/>
-      <c r="B41" s="44"/>
-      <c r="C41" s="41"/>
+      <c r="B41" s="15" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" s="15"/>
       <c r="D41" s="41"/>
-      <c r="E41" s="51"/>
-      <c r="F41" s="54"/>
-      <c r="G41" s="55"/>
-      <c r="H41" s="62" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
+      <c r="E41" s="41"/>
+      <c r="F41" s="51"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="55"/>
       <c r="I41" s="54"/>
       <c r="J41" s="55"/>
       <c r="K41" s="55"/>
-      <c r="L41" s="62" t="str">
-        <f>IF(OR(ISBLANK(I41),ISBLANK(J41)),"",J41-I41+1)</f>
-        <v/>
-      </c>
+      <c r="L41" s="62"/>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
@@ -5126,93 +5602,352 @@
       <c r="BN41" s="16"/>
     </row>
     <row r="42" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="49"/>
-      <c r="B42" s="46" t="s">
+      <c r="A42" s="47"/>
+      <c r="B42" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C42" s="15"/>
+      <c r="D42" s="41"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="51"/>
+      <c r="G42" s="54"/>
+      <c r="H42" s="55"/>
+      <c r="I42" s="54"/>
+      <c r="J42" s="55"/>
+      <c r="K42" s="55"/>
+      <c r="L42" s="62"/>
+      <c r="M42" s="16"/>
+      <c r="N42" s="16"/>
+      <c r="O42" s="16"/>
+      <c r="P42" s="16"/>
+      <c r="Q42" s="16"/>
+      <c r="R42" s="16"/>
+      <c r="S42" s="16"/>
+      <c r="T42" s="16"/>
+      <c r="U42" s="16"/>
+      <c r="V42" s="16"/>
+      <c r="W42" s="16"/>
+      <c r="X42" s="16"/>
+      <c r="Y42" s="16"/>
+      <c r="Z42" s="16"/>
+      <c r="AA42" s="16"/>
+      <c r="AB42" s="16"/>
+      <c r="AC42" s="16"/>
+      <c r="AD42" s="16"/>
+      <c r="AE42" s="16"/>
+      <c r="AF42" s="16"/>
+      <c r="AG42" s="16"/>
+      <c r="AH42" s="16"/>
+      <c r="AI42" s="16"/>
+      <c r="AJ42" s="16"/>
+      <c r="AK42" s="16"/>
+      <c r="AL42" s="16"/>
+      <c r="AM42" s="16"/>
+      <c r="AN42" s="16"/>
+      <c r="AO42" s="16"/>
+      <c r="AP42" s="16"/>
+      <c r="AQ42" s="16"/>
+      <c r="AR42" s="16"/>
+      <c r="AS42" s="16"/>
+      <c r="AT42" s="16"/>
+      <c r="AU42" s="16"/>
+      <c r="AV42" s="16"/>
+      <c r="AW42" s="16"/>
+      <c r="AX42" s="16"/>
+      <c r="AY42" s="16"/>
+      <c r="AZ42" s="16"/>
+      <c r="BA42" s="16"/>
+      <c r="BB42" s="16"/>
+      <c r="BC42" s="16"/>
+      <c r="BD42" s="16"/>
+      <c r="BE42" s="16"/>
+      <c r="BF42" s="16"/>
+      <c r="BG42" s="16"/>
+      <c r="BH42" s="16"/>
+      <c r="BI42" s="16"/>
+      <c r="BJ42" s="16"/>
+      <c r="BK42" s="16"/>
+      <c r="BL42" s="16"/>
+      <c r="BM42" s="16"/>
+      <c r="BN42" s="16"/>
+    </row>
+    <row r="43" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="47"/>
+      <c r="B43" s="44"/>
+      <c r="C43" s="44"/>
+      <c r="D43" s="41"/>
+      <c r="E43" s="41"/>
+      <c r="F43" s="51"/>
+      <c r="G43" s="54"/>
+      <c r="H43" s="55"/>
+      <c r="I43" s="54"/>
+      <c r="J43" s="55"/>
+      <c r="K43" s="55"/>
+      <c r="L43" s="62" t="str">
+        <f>IF(OR(ISBLANK(I43),ISBLANK(J43)),"",J43-I43+1)</f>
+        <v/>
+      </c>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="16"/>
+      <c r="X43" s="16"/>
+      <c r="Y43" s="16"/>
+      <c r="Z43" s="16"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="16"/>
+      <c r="AC43" s="16"/>
+      <c r="AD43" s="16"/>
+      <c r="AE43" s="16"/>
+      <c r="AF43" s="16"/>
+      <c r="AG43" s="16"/>
+      <c r="AH43" s="16"/>
+      <c r="AI43" s="16"/>
+      <c r="AJ43" s="16"/>
+      <c r="AK43" s="16"/>
+      <c r="AL43" s="16"/>
+      <c r="AM43" s="16"/>
+      <c r="AN43" s="16"/>
+      <c r="AO43" s="16"/>
+      <c r="AP43" s="16"/>
+      <c r="AQ43" s="16"/>
+      <c r="AR43" s="16"/>
+      <c r="AS43" s="16"/>
+      <c r="AT43" s="16"/>
+      <c r="AU43" s="16"/>
+      <c r="AV43" s="16"/>
+      <c r="AW43" s="16"/>
+      <c r="AX43" s="16"/>
+      <c r="AY43" s="16"/>
+      <c r="AZ43" s="16"/>
+      <c r="BA43" s="16"/>
+      <c r="BB43" s="16"/>
+      <c r="BC43" s="16"/>
+      <c r="BD43" s="16"/>
+      <c r="BE43" s="16"/>
+      <c r="BF43" s="16"/>
+      <c r="BG43" s="16"/>
+      <c r="BH43" s="16"/>
+      <c r="BI43" s="16"/>
+      <c r="BJ43" s="16"/>
+      <c r="BK43" s="16"/>
+      <c r="BL43" s="16"/>
+      <c r="BM43" s="16"/>
+      <c r="BN43" s="16"/>
+    </row>
+    <row r="44" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="47"/>
+      <c r="B44" s="44"/>
+      <c r="C44" s="44"/>
+      <c r="D44" s="41"/>
+      <c r="E44" s="41"/>
+      <c r="F44" s="51"/>
+      <c r="G44" s="54"/>
+      <c r="H44" s="55"/>
+      <c r="I44" s="54"/>
+      <c r="J44" s="55"/>
+      <c r="K44" s="55"/>
+      <c r="L44" s="62" t="str">
+        <f>IF(OR(ISBLANK(I44),ISBLANK(J44)),"",J44-I44+1)</f>
+        <v/>
+      </c>
+      <c r="M44" s="18"/>
+      <c r="N44" s="18"/>
+      <c r="O44" s="18"/>
+      <c r="P44" s="18"/>
+      <c r="Q44" s="18"/>
+      <c r="R44" s="18"/>
+      <c r="S44" s="18"/>
+      <c r="T44" s="18"/>
+      <c r="U44" s="18"/>
+      <c r="V44" s="18"/>
+      <c r="W44" s="18"/>
+      <c r="X44" s="18"/>
+      <c r="Y44" s="18"/>
+      <c r="Z44" s="18"/>
+      <c r="AA44" s="18"/>
+      <c r="AB44" s="18"/>
+      <c r="AC44" s="18"/>
+      <c r="AD44" s="18"/>
+      <c r="AE44" s="18"/>
+      <c r="AF44" s="18"/>
+      <c r="AG44" s="18"/>
+      <c r="AH44" s="18"/>
+      <c r="AI44" s="18"/>
+      <c r="AJ44" s="18"/>
+      <c r="AK44" s="18"/>
+      <c r="AL44" s="18"/>
+      <c r="AM44" s="18"/>
+      <c r="AN44" s="18"/>
+      <c r="AO44" s="18"/>
+      <c r="AP44" s="18"/>
+      <c r="AQ44" s="18"/>
+      <c r="AR44" s="18"/>
+      <c r="AS44" s="18"/>
+      <c r="AT44" s="18"/>
+      <c r="AU44" s="18"/>
+      <c r="AV44" s="18"/>
+      <c r="AW44" s="18"/>
+      <c r="AX44" s="18"/>
+      <c r="AY44" s="18"/>
+      <c r="AZ44" s="18"/>
+      <c r="BA44" s="18"/>
+      <c r="BB44" s="18"/>
+      <c r="BC44" s="18"/>
+      <c r="BD44" s="18"/>
+      <c r="BE44" s="18"/>
+      <c r="BF44" s="18"/>
+      <c r="BG44" s="18"/>
+      <c r="BH44" s="18"/>
+      <c r="BI44" s="18"/>
+      <c r="BJ44" s="18"/>
+      <c r="BK44" s="18"/>
+      <c r="BL44" s="18"/>
+      <c r="BM44" s="18"/>
+      <c r="BN44" s="18"/>
+    </row>
+    <row r="45" spans="1:66" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="47"/>
+      <c r="B45" s="44"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="41"/>
+      <c r="E45" s="41"/>
+      <c r="F45" s="51"/>
+      <c r="G45" s="54"/>
+      <c r="H45" s="55"/>
+      <c r="I45" s="54"/>
+      <c r="J45" s="55"/>
+      <c r="K45" s="55"/>
+      <c r="L45" s="62" t="str">
+        <f>IF(OR(ISBLANK(I45),ISBLANK(J45)),"",J45-I45+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="46" spans="1:66" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="47"/>
+      <c r="B46" s="44"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="41"/>
+      <c r="E46" s="41"/>
+      <c r="F46" s="51"/>
+      <c r="G46" s="54"/>
+      <c r="H46" s="55"/>
+      <c r="I46" s="54"/>
+      <c r="J46" s="55"/>
+      <c r="K46" s="55"/>
+      <c r="L46" s="62"/>
+    </row>
+    <row r="47" spans="1:66" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="47"/>
+      <c r="B47" s="44"/>
+      <c r="C47" s="44"/>
+      <c r="D47" s="41"/>
+      <c r="E47" s="41"/>
+      <c r="F47" s="51"/>
+      <c r="G47" s="54"/>
+      <c r="H47" s="55"/>
+      <c r="I47" s="54"/>
+      <c r="J47" s="55"/>
+      <c r="K47" s="55"/>
+      <c r="L47" s="62"/>
+    </row>
+    <row r="48" spans="1:66" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="47"/>
+      <c r="B48" s="44"/>
+      <c r="C48" s="44"/>
+      <c r="D48" s="41"/>
+      <c r="E48" s="41"/>
+      <c r="F48" s="51"/>
+      <c r="G48" s="54"/>
+      <c r="H48" s="55"/>
+      <c r="I48" s="54"/>
+      <c r="J48" s="55"/>
+      <c r="K48" s="55"/>
+      <c r="L48" s="62"/>
+    </row>
+    <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="47"/>
+      <c r="B49" s="44"/>
+      <c r="C49" s="44"/>
+      <c r="D49" s="41"/>
+      <c r="E49" s="41"/>
+      <c r="F49" s="51"/>
+      <c r="G49" s="54"/>
+      <c r="H49" s="55"/>
+      <c r="I49" s="54"/>
+      <c r="J49" s="55"/>
+      <c r="K49" s="55"/>
+      <c r="L49" s="62"/>
+    </row>
+    <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="47"/>
+      <c r="B50" s="44"/>
+      <c r="C50" s="44"/>
+      <c r="D50" s="41"/>
+      <c r="E50" s="41"/>
+      <c r="F50" s="51"/>
+      <c r="G50" s="54"/>
+      <c r="H50" s="55"/>
+      <c r="I50" s="54"/>
+      <c r="J50" s="55"/>
+      <c r="K50" s="55"/>
+      <c r="L50" s="62"/>
+    </row>
+    <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="47"/>
+      <c r="B51" s="44"/>
+      <c r="C51" s="44"/>
+      <c r="D51" s="41"/>
+      <c r="E51" s="41"/>
+      <c r="F51" s="51"/>
+      <c r="G51" s="54"/>
+      <c r="H51" s="55"/>
+      <c r="I51" s="54"/>
+      <c r="J51" s="55"/>
+      <c r="K51" s="55"/>
+      <c r="L51" s="62" t="str">
+        <f>IF(OR(ISBLANK(I51),ISBLANK(J51)),"",J51-I51+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="52" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="49"/>
+      <c r="B52" s="46" t="s">
         <v>19</v>
       </c>
-      <c r="C42" s="43"/>
-      <c r="D42" s="43"/>
-      <c r="E42" s="53"/>
-      <c r="F42" s="58"/>
-      <c r="G42" s="59"/>
-      <c r="H42" s="64" t="str">
-        <f t="shared" si="5"/>
+      <c r="C52" s="46"/>
+      <c r="D52" s="43"/>
+      <c r="E52" s="43"/>
+      <c r="F52" s="53"/>
+      <c r="G52" s="58"/>
+      <c r="H52" s="59"/>
+      <c r="I52" s="58"/>
+      <c r="J52" s="59"/>
+      <c r="K52" s="59"/>
+      <c r="L52" s="64" t="str">
+        <f>IF(OR(ISBLANK(I52),ISBLANK(J52)),"",J52-I52+1)</f>
         <v/>
       </c>
-      <c r="I42" s="58"/>
-      <c r="J42" s="59"/>
-      <c r="K42" s="59"/>
-      <c r="L42" s="64" t="str">
-        <f>IF(OR(ISBLANK(I42),ISBLANK(J42)),"",J42-I42+1)</f>
-        <v/>
-      </c>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
-      <c r="U42" s="18"/>
-      <c r="V42" s="18"/>
-      <c r="W42" s="18"/>
-      <c r="X42" s="18"/>
-      <c r="Y42" s="18"/>
-      <c r="Z42" s="18"/>
-      <c r="AA42" s="18"/>
-      <c r="AB42" s="18"/>
-      <c r="AC42" s="18"/>
-      <c r="AD42" s="18"/>
-      <c r="AE42" s="18"/>
-      <c r="AF42" s="18"/>
-      <c r="AG42" s="18"/>
-      <c r="AH42" s="18"/>
-      <c r="AI42" s="18"/>
-      <c r="AJ42" s="18"/>
-      <c r="AK42" s="18"/>
-      <c r="AL42" s="18"/>
-      <c r="AM42" s="18"/>
-      <c r="AN42" s="18"/>
-      <c r="AO42" s="18"/>
-      <c r="AP42" s="18"/>
-      <c r="AQ42" s="18"/>
-      <c r="AR42" s="18"/>
-      <c r="AS42" s="18"/>
-      <c r="AT42" s="18"/>
-      <c r="AU42" s="18"/>
-      <c r="AV42" s="18"/>
-      <c r="AW42" s="18"/>
-      <c r="AX42" s="18"/>
-      <c r="AY42" s="18"/>
-      <c r="AZ42" s="18"/>
-      <c r="BA42" s="18"/>
-      <c r="BB42" s="18"/>
-      <c r="BC42" s="18"/>
-      <c r="BD42" s="18"/>
-      <c r="BE42" s="18"/>
-      <c r="BF42" s="18"/>
-      <c r="BG42" s="18"/>
-      <c r="BH42" s="18"/>
-      <c r="BI42" s="18"/>
-      <c r="BJ42" s="18"/>
-      <c r="BK42" s="18"/>
-      <c r="BL42" s="18"/>
-      <c r="BM42" s="18"/>
-      <c r="BN42" s="18"/>
-    </row>
-    <row r="44" spans="1:66" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="19"/>
-    </row>
-    <row r="45" spans="1:66" x14ac:dyDescent="0.2">
-      <c r="A45" s="65"/>
+    </row>
+    <row r="54" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A54" s="19"/>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A55" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="G4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="E9:E16 E18:E42">
-    <cfRule type="dataBar" priority="9">
+  <conditionalFormatting sqref="F9:F16 F19:F25 F35:F52">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5225,24 +5960,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M9:BN16 M18:BN42">
-    <cfRule type="expression" dxfId="7" priority="10" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J9,$G9)&gt;=M$6,MIN($I9,$F9)&lt;N$6))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="11">
-      <formula>AND($G9&gt;=M$6,$F9&lt;N$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="13" stopIfTrue="1">
-      <formula>AND($J9&gt;=M$6,$I9&lt;N$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M7:BN16 M18:BN42">
-    <cfRule type="expression" dxfId="4" priority="6">
+  <conditionalFormatting sqref="M7:BN16 M19:BN25 M27:BN44">
+    <cfRule type="expression" dxfId="9" priority="10">
       <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="E17">
-    <cfRule type="dataBar" priority="2">
+  <conditionalFormatting sqref="F18">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5255,24 +5979,73 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M17:BN17">
-    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J17,$G17)&gt;=M$6,MIN($I17,$F17)&lt;N$6))</formula>
+  <conditionalFormatting sqref="M18:BN18">
+    <cfRule type="expression" dxfId="8" priority="5">
+      <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="4">
-      <formula>AND($G17&gt;=M$6,$F17&lt;N$6)</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F28:F34">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="7" tint="0.59999389629810485"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BBCB907A-6A62-4D17-AA3D-3F138FBA1094}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
-      <formula>AND($J17&gt;=M$6,$I17&lt;N$6)</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F27">
+    <cfRule type="dataBar" priority="3">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="7" tint="0.59999389629810485"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{58C1B727-9B84-4E8B-BD44-F81E58086481}</x14:id>
+        </ext>
+      </extLst>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M17:BN17">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="7" priority="2">
       <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
     </cfRule>
   </conditionalFormatting>
+  <conditionalFormatting sqref="M26:BN26">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M9:BN16 M18:BN25">
+    <cfRule type="expression" dxfId="5" priority="26" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J9,$H9)&gt;=M$6,MIN($I9,$G9)&lt;N$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="27">
+      <formula>AND($H9&gt;=M$6,$G9&lt;N$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="28" stopIfTrue="1">
+      <formula>AND($J9&gt;=M$6,$I9&lt;N$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M27:BN44">
+    <cfRule type="expression" dxfId="2" priority="35" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J35,$H35)&gt;=M$6,MIN($I35,$G35)&lt;N$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="36">
+      <formula>AND($H35&gt;=M$6,$G35&lt;N$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="37" stopIfTrue="1">
+      <formula>AND($J35&gt;=M$6,$I35&lt;N$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F5">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G5">
       <formula1>"Daily,Weekly,Monthly,Quarterly"</formula1>
     </dataValidation>
   </dataValidations>
@@ -5327,7 +6100,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E9:E16 E18:E42</xm:sqref>
+          <xm:sqref>F9:F16 F19:F25 F35:F52</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{35B0E45D-0F80-4816-B43B-129D908BE9C3}">
@@ -5342,7 +6115,37 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>E17</xm:sqref>
+          <xm:sqref>F18</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BBCB907A-6A62-4D17-AA3D-3F138FBA1094}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F28:F34</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{58C1B727-9B84-4E8B-BD44-F81E58086481}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F27</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
@@ -5374,7 +6177,7 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B2" s="78" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C2" s="78"/>
     </row>
@@ -5392,7 +6195,7 @@
     </row>
     <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -5412,7 +6215,7 @@
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="22" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D9" s="5"/>
     </row>
@@ -5443,14 +6246,14 @@
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="7"/>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D16" s="5"/>
     </row>
@@ -5467,7 +6270,7 @@
     </row>
     <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D19" s="5"/>
     </row>
@@ -5484,7 +6287,7 @@
     </row>
     <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -5497,18 +6300,18 @@
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="68" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -5540,7 +6343,7 @@
     <row r="1" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24"/>
       <c r="B1" s="25" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C1" s="26"/>
     </row>
@@ -5559,7 +6362,7 @@
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="24"/>
       <c r="B4" s="33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C4" s="26"/>
     </row>
@@ -5631,7 +6434,7 @@
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="66" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C16" s="26"/>
     </row>

</xml_diff>

<commit_message>
Updating the project plan to solve the issues 9,10,12 in the CYRS and issues 8,9,10,11 in HSI Signed-off-by: May Alaa <mayelfkiy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="86">
   <si>
     <t>HELP</t>
   </si>
@@ -73,27 +73,6 @@
     <t>TASK DESCRIPTION</t>
   </si>
   <si>
-    <t>Task 3</t>
-  </si>
-  <si>
-    <t>Task 4</t>
-  </si>
-  <si>
-    <t>Task 5</t>
-  </si>
-  <si>
-    <t>Phase 2 Title</t>
-  </si>
-  <si>
-    <t>Task 1</t>
-  </si>
-  <si>
-    <t>Task 2</t>
-  </si>
-  <si>
-    <t>Task 6</t>
-  </si>
-  <si>
     <t>When you insert new rows, you should insert a blank row between rows that have the formatting you want. If you do that, the formatting will be copied automatically.</t>
   </si>
   <si>
@@ -202,9 +181,6 @@
     <t>Project Leader: May Alaa El-din</t>
   </si>
   <si>
-    <t>ACTUAL DAYS</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -308,6 +284,21 @@
   </si>
   <si>
     <t>Updating RTM to reflect modified requirements</t>
+  </si>
+  <si>
+    <t>Week 3 Update</t>
+  </si>
+  <si>
+    <t>Solve issues described in point 9,10 and 12 in the review sheet</t>
+  </si>
+  <si>
+    <t>2/8//20</t>
+  </si>
+  <si>
+    <t>_</t>
+  </si>
+  <si>
+    <t>Solve issues described in point 8,9,10,11 in the review sheet</t>
   </si>
 </sst>
 </file>
@@ -979,6 +970,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -988,16 +982,13 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="28">
     <dxf>
       <fill>
         <patternFill>
@@ -1045,24 +1036,69 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
         <right style="thin">
-          <color rgb="FFC00000"/>
+          <color theme="0" tint="-0.14996795556505021"/>
         </right>
         <vertical/>
         <horizontal/>
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
         <right style="thin">
-          <color rgb="FFC00000"/>
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
         </right>
         <vertical/>
         <horizontal/>
@@ -1212,15 +1248,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="totalRow" dxfId="18"/>
-      <tableStyleElement type="firstColumn" dxfId="17"/>
-      <tableStyleElement type="lastColumn" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="secondRowStripe" dxfId="14"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="13"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="27"/>
+      <tableStyleElement type="headerRow" dxfId="26"/>
+      <tableStyleElement type="totalRow" dxfId="25"/>
+      <tableStyleElement type="firstColumn" dxfId="24"/>
+      <tableStyleElement type="lastColumn" dxfId="23"/>
+      <tableStyleElement type="firstRowStripe" dxfId="22"/>
+      <tableStyleElement type="secondRowStripe" dxfId="21"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="20"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="19"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1323,13 +1359,13 @@
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
       <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
-          <xdr:col>11</xdr:col>
+          <xdr:col>10</xdr:col>
           <xdr:colOff>552450</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>171450</xdr:rowOff>
         </xdr:from>
         <xdr:to>
-          <xdr:col>28</xdr:col>
+          <xdr:col>27</xdr:col>
           <xdr:colOff>76200</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>180975</xdr:rowOff>
@@ -1748,10 +1784,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BO55"/>
+  <dimension ref="A1:BN53"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A25" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="D32" sqref="D32"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A32" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="C37" sqref="C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -1766,15 +1802,14 @@
     <col min="8" max="8" width="9.5" customWidth="1"/>
     <col min="9" max="9" width="9.5" style="10" customWidth="1"/>
     <col min="10" max="10" width="9.625" customWidth="1"/>
-    <col min="11" max="11" width="9.5" style="72" customWidth="1"/>
-    <col min="12" max="12" width="13.75" customWidth="1"/>
-    <col min="13" max="66" width="3.125" customWidth="1"/>
-    <col min="67" max="67" width="3.75" customWidth="1"/>
+    <col min="11" max="11" width="13.75" customWidth="1"/>
+    <col min="12" max="65" width="3.125" customWidth="1"/>
+    <col min="66" max="66" width="3.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:67" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:66" ht="26.25" x14ac:dyDescent="0.4">
       <c r="A1" s="60" t="s">
-        <v>47</v>
+        <v>40</v>
       </c>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1786,25 +1821,24 @@
       <c r="I1" s="9"/>
       <c r="J1" s="2"/>
       <c r="K1" s="2"/>
-      <c r="L1" s="2"/>
-      <c r="M1" s="40"/>
-      <c r="BI1" s="11" t="s">
+      <c r="L1" s="40"/>
+      <c r="BH1" s="11" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:66" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="14" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
       <c r="D2" s="14"/>
       <c r="E2" s="14"/>
-      <c r="M2" s="69"/>
-    </row>
-    <row r="3" spans="1:67" s="72" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="L2" s="69"/>
+    </row>
+    <row r="3" spans="1:66" s="72" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="71" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="B3" s="71"/>
       <c r="C3" s="71"/>
@@ -1812,613 +1846,613 @@
       <c r="E3" s="14"/>
       <c r="G3" s="73"/>
       <c r="I3" s="73"/>
-      <c r="M3" s="69"/>
-    </row>
-    <row r="4" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="L3" s="69"/>
+    </row>
+    <row r="4" spans="1:66" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B4" s="71"/>
       <c r="C4" s="71"/>
       <c r="F4" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="76">
+        <v>19</v>
+      </c>
+      <c r="G4" s="77">
         <v>43851</v>
       </c>
-      <c r="H4" s="77"/>
-    </row>
-    <row r="5" spans="1:67" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H4" s="78"/>
+    </row>
+    <row r="5" spans="1:66" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="35"/>
       <c r="F5" s="35" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
       <c r="G5" s="61" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:67" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="6" spans="1:66" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="35"/>
       <c r="F6" s="35" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
       <c r="G6" s="36">
         <v>1</v>
       </c>
-      <c r="M6" s="37">
+      <c r="L6" s="37">
         <f>IF(G5="Weekly",G4+7*(G6-1),IF(G5="Daily",G4+(G6-1),IF(G5="Monthly",EDATE($G$4,($G$6-1)),EDATE($G$4,3*($G$6-1)))))</f>
         <v>43851</v>
       </c>
+      <c r="M6" s="37">
+        <f t="shared" ref="M6:BN6" si="0">IF($G$5="Daily",L6+1,IF($G$5="Weekly",L6+7,IF($G$5="Monthly",EDATE($G$4,M8-1),EDATE($G$4,3*(M8-1)))))</f>
+        <v>43852</v>
+      </c>
       <c r="N6" s="37">
-        <f t="shared" ref="N6:BO6" si="0">IF($G$5="Daily",M6+1,IF($G$5="Weekly",M6+7,IF($G$5="Monthly",EDATE($G$4,N8-1),EDATE($G$4,3*(N8-1)))))</f>
-        <v>43852</v>
+        <f t="shared" si="0"/>
+        <v>43853</v>
       </c>
       <c r="O6" s="37">
         <f t="shared" si="0"/>
-        <v>43853</v>
+        <v>43854</v>
       </c>
       <c r="P6" s="37">
         <f t="shared" si="0"/>
-        <v>43854</v>
+        <v>43855</v>
       </c>
       <c r="Q6" s="37">
         <f t="shared" si="0"/>
-        <v>43855</v>
+        <v>43856</v>
       </c>
       <c r="R6" s="37">
         <f t="shared" si="0"/>
-        <v>43856</v>
+        <v>43857</v>
       </c>
       <c r="S6" s="37">
         <f t="shared" si="0"/>
-        <v>43857</v>
+        <v>43858</v>
       </c>
       <c r="T6" s="37">
         <f t="shared" si="0"/>
-        <v>43858</v>
+        <v>43859</v>
       </c>
       <c r="U6" s="37">
         <f t="shared" si="0"/>
-        <v>43859</v>
+        <v>43860</v>
       </c>
       <c r="V6" s="37">
         <f t="shared" si="0"/>
-        <v>43860</v>
+        <v>43861</v>
       </c>
       <c r="W6" s="37">
         <f t="shared" si="0"/>
-        <v>43861</v>
+        <v>43862</v>
       </c>
       <c r="X6" s="37">
         <f t="shared" si="0"/>
-        <v>43862</v>
+        <v>43863</v>
       </c>
       <c r="Y6" s="37">
         <f t="shared" si="0"/>
-        <v>43863</v>
+        <v>43864</v>
       </c>
       <c r="Z6" s="37">
         <f t="shared" si="0"/>
-        <v>43864</v>
+        <v>43865</v>
       </c>
       <c r="AA6" s="37">
         <f t="shared" si="0"/>
-        <v>43865</v>
+        <v>43866</v>
       </c>
       <c r="AB6" s="37">
         <f t="shared" si="0"/>
-        <v>43866</v>
+        <v>43867</v>
       </c>
       <c r="AC6" s="37">
         <f t="shared" si="0"/>
-        <v>43867</v>
+        <v>43868</v>
       </c>
       <c r="AD6" s="37">
         <f t="shared" si="0"/>
-        <v>43868</v>
+        <v>43869</v>
       </c>
       <c r="AE6" s="37">
         <f t="shared" si="0"/>
-        <v>43869</v>
+        <v>43870</v>
       </c>
       <c r="AF6" s="37">
         <f t="shared" si="0"/>
-        <v>43870</v>
+        <v>43871</v>
       </c>
       <c r="AG6" s="37">
         <f t="shared" si="0"/>
-        <v>43871</v>
+        <v>43872</v>
       </c>
       <c r="AH6" s="37">
         <f t="shared" si="0"/>
-        <v>43872</v>
+        <v>43873</v>
       </c>
       <c r="AI6" s="37">
         <f t="shared" si="0"/>
-        <v>43873</v>
+        <v>43874</v>
       </c>
       <c r="AJ6" s="37">
         <f t="shared" si="0"/>
-        <v>43874</v>
+        <v>43875</v>
       </c>
       <c r="AK6" s="37">
         <f t="shared" si="0"/>
-        <v>43875</v>
+        <v>43876</v>
       </c>
       <c r="AL6" s="37">
         <f t="shared" si="0"/>
-        <v>43876</v>
+        <v>43877</v>
       </c>
       <c r="AM6" s="37">
         <f t="shared" si="0"/>
-        <v>43877</v>
+        <v>43878</v>
       </c>
       <c r="AN6" s="37">
         <f t="shared" si="0"/>
-        <v>43878</v>
+        <v>43879</v>
       </c>
       <c r="AO6" s="37">
         <f t="shared" si="0"/>
-        <v>43879</v>
+        <v>43880</v>
       </c>
       <c r="AP6" s="37">
         <f t="shared" si="0"/>
-        <v>43880</v>
+        <v>43881</v>
       </c>
       <c r="AQ6" s="37">
         <f t="shared" si="0"/>
-        <v>43881</v>
+        <v>43882</v>
       </c>
       <c r="AR6" s="37">
         <f t="shared" si="0"/>
-        <v>43882</v>
+        <v>43883</v>
       </c>
       <c r="AS6" s="37">
         <f t="shared" si="0"/>
-        <v>43883</v>
+        <v>43884</v>
       </c>
       <c r="AT6" s="37">
         <f t="shared" si="0"/>
-        <v>43884</v>
+        <v>43885</v>
       </c>
       <c r="AU6" s="37">
         <f t="shared" si="0"/>
-        <v>43885</v>
+        <v>43886</v>
       </c>
       <c r="AV6" s="37">
         <f t="shared" si="0"/>
-        <v>43886</v>
+        <v>43887</v>
       </c>
       <c r="AW6" s="37">
         <f t="shared" si="0"/>
-        <v>43887</v>
+        <v>43888</v>
       </c>
       <c r="AX6" s="37">
         <f t="shared" si="0"/>
-        <v>43888</v>
+        <v>43889</v>
       </c>
       <c r="AY6" s="37">
         <f t="shared" si="0"/>
-        <v>43889</v>
+        <v>43890</v>
       </c>
       <c r="AZ6" s="37">
         <f t="shared" si="0"/>
-        <v>43890</v>
+        <v>43891</v>
       </c>
       <c r="BA6" s="37">
         <f t="shared" si="0"/>
-        <v>43891</v>
+        <v>43892</v>
       </c>
       <c r="BB6" s="37">
         <f t="shared" si="0"/>
-        <v>43892</v>
+        <v>43893</v>
       </c>
       <c r="BC6" s="37">
         <f t="shared" si="0"/>
-        <v>43893</v>
+        <v>43894</v>
       </c>
       <c r="BD6" s="37">
         <f t="shared" si="0"/>
-        <v>43894</v>
+        <v>43895</v>
       </c>
       <c r="BE6" s="37">
         <f t="shared" si="0"/>
-        <v>43895</v>
+        <v>43896</v>
       </c>
       <c r="BF6" s="37">
         <f t="shared" si="0"/>
-        <v>43896</v>
+        <v>43897</v>
       </c>
       <c r="BG6" s="37">
         <f t="shared" si="0"/>
-        <v>43897</v>
+        <v>43898</v>
       </c>
       <c r="BH6" s="37">
         <f t="shared" si="0"/>
-        <v>43898</v>
+        <v>43899</v>
       </c>
       <c r="BI6" s="37">
         <f t="shared" si="0"/>
-        <v>43899</v>
+        <v>43900</v>
       </c>
       <c r="BJ6" s="37">
         <f t="shared" si="0"/>
-        <v>43900</v>
+        <v>43901</v>
       </c>
       <c r="BK6" s="37">
         <f t="shared" si="0"/>
-        <v>43901</v>
+        <v>43902</v>
       </c>
       <c r="BL6" s="37">
         <f t="shared" si="0"/>
-        <v>43902</v>
+        <v>43903</v>
       </c>
       <c r="BM6" s="37">
         <f t="shared" si="0"/>
-        <v>43903</v>
+        <v>43904</v>
       </c>
       <c r="BN6" s="37">
         <f t="shared" si="0"/>
-        <v>43904</v>
-      </c>
-      <c r="BO6" s="37">
-        <f t="shared" si="0"/>
         <v>43905</v>
       </c>
     </row>
-    <row r="7" spans="1:67" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:66" ht="47.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="74" t="s">
-        <v>55</v>
-      </c>
-      <c r="M7" s="38" t="str">
-        <f>DAY(M6)&amp;CHAR(10)&amp;LEFT(TEXT(M6,"mmm"),3)&amp;CHAR(10)&amp;"'"&amp;RIGHT(YEAR(M6),2)</f>
+        <v>47</v>
+      </c>
+      <c r="L7" s="38" t="str">
+        <f>DAY(L6)&amp;CHAR(10)&amp;LEFT(TEXT(L6,"mmm"),3)&amp;CHAR(10)&amp;"'"&amp;RIGHT(YEAR(L6),2)</f>
         <v>21
 Jan
 '20</v>
       </c>
-      <c r="N7" s="38" t="str">
-        <f t="shared" ref="N7:BO7" si="1">DAY(N6)&amp;CHAR(10)&amp;LEFT(TEXT(N6,"mmm"),3)&amp;CHAR(10)&amp;"'"&amp;RIGHT(YEAR(N6),2)</f>
+      <c r="M7" s="38" t="str">
+        <f t="shared" ref="M7:BN7" si="1">DAY(M6)&amp;CHAR(10)&amp;LEFT(TEXT(M6,"mmm"),3)&amp;CHAR(10)&amp;"'"&amp;RIGHT(YEAR(M6),2)</f>
         <v>22
 Jan
 '20</v>
       </c>
-      <c r="O7" s="38" t="str">
+      <c r="N7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>23
 Jan
 '20</v>
       </c>
-      <c r="P7" s="38" t="str">
+      <c r="O7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>24
 Jan
 '20</v>
       </c>
-      <c r="Q7" s="38" t="str">
+      <c r="P7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>25
 Jan
 '20</v>
       </c>
-      <c r="R7" s="38" t="str">
+      <c r="Q7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>26
 Jan
 '20</v>
       </c>
-      <c r="S7" s="38" t="str">
+      <c r="R7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>27
 Jan
 '20</v>
       </c>
-      <c r="T7" s="38" t="str">
+      <c r="S7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>28
 Jan
 '20</v>
       </c>
-      <c r="U7" s="38" t="str">
+      <c r="T7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>29
 Jan
 '20</v>
       </c>
-      <c r="V7" s="38" t="str">
+      <c r="U7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>30
 Jan
 '20</v>
       </c>
-      <c r="W7" s="38" t="str">
+      <c r="V7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>31
 Jan
 '20</v>
       </c>
-      <c r="X7" s="38" t="str">
+      <c r="W7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>1
 Feb
 '20</v>
       </c>
-      <c r="Y7" s="38" t="str">
+      <c r="X7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>2
 Feb
 '20</v>
       </c>
-      <c r="Z7" s="38" t="str">
+      <c r="Y7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>3
 Feb
 '20</v>
       </c>
-      <c r="AA7" s="38" t="str">
+      <c r="Z7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>4
 Feb
 '20</v>
       </c>
-      <c r="AB7" s="38" t="str">
+      <c r="AA7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>5
 Feb
 '20</v>
       </c>
-      <c r="AC7" s="38" t="str">
+      <c r="AB7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>6
 Feb
 '20</v>
       </c>
-      <c r="AD7" s="38" t="str">
+      <c r="AC7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>7
 Feb
 '20</v>
       </c>
-      <c r="AE7" s="38" t="str">
+      <c r="AD7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>8
 Feb
 '20</v>
       </c>
-      <c r="AF7" s="38" t="str">
+      <c r="AE7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>9
 Feb
 '20</v>
       </c>
-      <c r="AG7" s="38" t="str">
+      <c r="AF7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>10
 Feb
 '20</v>
       </c>
-      <c r="AH7" s="38" t="str">
+      <c r="AG7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>11
 Feb
 '20</v>
       </c>
-      <c r="AI7" s="38" t="str">
+      <c r="AH7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>12
 Feb
 '20</v>
       </c>
-      <c r="AJ7" s="38" t="str">
+      <c r="AI7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>13
 Feb
 '20</v>
       </c>
-      <c r="AK7" s="38" t="str">
+      <c r="AJ7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>14
 Feb
 '20</v>
       </c>
-      <c r="AL7" s="38" t="str">
+      <c r="AK7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>15
 Feb
 '20</v>
       </c>
-      <c r="AM7" s="38" t="str">
+      <c r="AL7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>16
 Feb
 '20</v>
       </c>
-      <c r="AN7" s="38" t="str">
+      <c r="AM7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>17
 Feb
 '20</v>
       </c>
-      <c r="AO7" s="38" t="str">
+      <c r="AN7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>18
 Feb
 '20</v>
       </c>
-      <c r="AP7" s="38" t="str">
+      <c r="AO7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>19
 Feb
 '20</v>
       </c>
-      <c r="AQ7" s="38" t="str">
+      <c r="AP7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>20
 Feb
 '20</v>
       </c>
-      <c r="AR7" s="38" t="str">
+      <c r="AQ7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>21
 Feb
 '20</v>
       </c>
-      <c r="AS7" s="38" t="str">
+      <c r="AR7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>22
 Feb
 '20</v>
       </c>
-      <c r="AT7" s="38" t="str">
+      <c r="AS7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>23
 Feb
 '20</v>
       </c>
-      <c r="AU7" s="38" t="str">
+      <c r="AT7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>24
 Feb
 '20</v>
       </c>
-      <c r="AV7" s="38" t="str">
+      <c r="AU7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>25
 Feb
 '20</v>
       </c>
-      <c r="AW7" s="38" t="str">
+      <c r="AV7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>26
 Feb
 '20</v>
       </c>
-      <c r="AX7" s="38" t="str">
+      <c r="AW7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>27
 Feb
 '20</v>
       </c>
-      <c r="AY7" s="38" t="str">
+      <c r="AX7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>28
 Feb
 '20</v>
       </c>
-      <c r="AZ7" s="38" t="str">
+      <c r="AY7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>29
 Feb
 '20</v>
       </c>
-      <c r="BA7" s="38" t="str">
+      <c r="AZ7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>1
 Mar
 '20</v>
       </c>
-      <c r="BB7" s="38" t="str">
+      <c r="BA7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>2
 Mar
 '20</v>
       </c>
-      <c r="BC7" s="38" t="str">
+      <c r="BB7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>3
 Mar
 '20</v>
       </c>
-      <c r="BD7" s="38" t="str">
+      <c r="BC7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>4
 Mar
 '20</v>
       </c>
-      <c r="BE7" s="38" t="str">
+      <c r="BD7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>5
 Mar
 '20</v>
       </c>
-      <c r="BF7" s="38" t="str">
+      <c r="BE7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>6
 Mar
 '20</v>
       </c>
-      <c r="BG7" s="38" t="str">
+      <c r="BF7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>7
 Mar
 '20</v>
       </c>
-      <c r="BH7" s="38" t="str">
+      <c r="BG7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>8
 Mar
 '20</v>
       </c>
-      <c r="BI7" s="38" t="str">
+      <c r="BH7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>9
 Mar
 '20</v>
       </c>
-      <c r="BJ7" s="38" t="str">
+      <c r="BI7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>10
 Mar
 '20</v>
       </c>
-      <c r="BK7" s="38" t="str">
+      <c r="BJ7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>11
 Mar
 '20</v>
       </c>
-      <c r="BL7" s="38" t="str">
+      <c r="BK7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>12
 Mar
 '20</v>
       </c>
-      <c r="BM7" s="38" t="str">
+      <c r="BL7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>13
 Mar
 '20</v>
       </c>
-      <c r="BN7" s="38" t="str">
+      <c r="BM7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>14
 Mar
 '20</v>
       </c>
-      <c r="BO7" s="38" t="str">
+      <c r="BN7" s="38" t="str">
         <f t="shared" si="1"/>
         <v>15
 Mar
 '20</v>
       </c>
     </row>
-    <row r="8" spans="1:67" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:66" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="50" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="12" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D8" s="13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E8" s="13" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G8" s="70" t="s">
         <v>8</v>
@@ -2427,235 +2461,232 @@
         <v>9</v>
       </c>
       <c r="I8" s="13" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="K8" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L8" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="M8" s="39">
+        <v>46</v>
+      </c>
+      <c r="L8" s="39">
         <f>G6</f>
         <v>1</v>
       </c>
+      <c r="M8" s="39">
+        <f>L8+1</f>
+        <v>2</v>
+      </c>
       <c r="N8" s="39">
-        <f>M8+1</f>
-        <v>2</v>
+        <f t="shared" ref="N8:BM8" si="2">M8+1</f>
+        <v>3</v>
       </c>
       <c r="O8" s="39">
-        <f t="shared" ref="O8:BN8" si="2">N8+1</f>
-        <v>3</v>
+        <f t="shared" si="2"/>
+        <v>4</v>
       </c>
       <c r="P8" s="39">
         <f t="shared" si="2"/>
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="Q8" s="39">
         <f t="shared" si="2"/>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="R8" s="39">
         <f t="shared" si="2"/>
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="S8" s="39">
         <f t="shared" si="2"/>
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="T8" s="39">
         <f t="shared" si="2"/>
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="U8" s="39">
         <f t="shared" si="2"/>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="V8" s="39">
         <f t="shared" si="2"/>
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="W8" s="39">
         <f t="shared" si="2"/>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="X8" s="39">
         <f t="shared" si="2"/>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="Y8" s="39">
         <f t="shared" si="2"/>
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="Z8" s="39">
         <f t="shared" si="2"/>
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="AA8" s="39">
         <f t="shared" si="2"/>
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="AB8" s="39">
         <f t="shared" si="2"/>
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="AC8" s="39">
         <f t="shared" si="2"/>
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="AD8" s="39">
         <f t="shared" si="2"/>
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="AE8" s="39">
         <f t="shared" si="2"/>
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="AF8" s="39">
         <f t="shared" si="2"/>
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="AG8" s="39">
         <f t="shared" si="2"/>
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="AH8" s="39">
         <f t="shared" si="2"/>
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="AI8" s="39">
         <f t="shared" si="2"/>
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="AJ8" s="39">
         <f t="shared" si="2"/>
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AK8" s="39">
         <f t="shared" si="2"/>
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AL8" s="39">
         <f t="shared" si="2"/>
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="AM8" s="39">
         <f t="shared" si="2"/>
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="AN8" s="39">
         <f t="shared" si="2"/>
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="AO8" s="39">
         <f t="shared" si="2"/>
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="AP8" s="39">
         <f t="shared" si="2"/>
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="AQ8" s="39">
         <f t="shared" si="2"/>
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="AR8" s="39">
         <f t="shared" si="2"/>
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="AS8" s="39">
         <f t="shared" si="2"/>
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="AT8" s="39">
         <f t="shared" si="2"/>
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="AU8" s="39">
         <f t="shared" si="2"/>
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="AV8" s="39">
         <f t="shared" si="2"/>
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="AW8" s="39">
         <f t="shared" si="2"/>
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="AX8" s="39">
         <f t="shared" si="2"/>
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="AY8" s="39">
         <f t="shared" si="2"/>
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="AZ8" s="39">
         <f t="shared" si="2"/>
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="BA8" s="39">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="BB8" s="39">
         <f t="shared" si="2"/>
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="BC8" s="39">
         <f t="shared" si="2"/>
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="BD8" s="39">
         <f t="shared" si="2"/>
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="BE8" s="39">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="BF8" s="39">
         <f t="shared" si="2"/>
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="BG8" s="39">
         <f t="shared" si="2"/>
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="BH8" s="39">
         <f t="shared" si="2"/>
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="BI8" s="39">
         <f t="shared" si="2"/>
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="BJ8" s="39">
         <f t="shared" si="2"/>
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="BK8" s="39">
         <f t="shared" si="2"/>
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="BL8" s="39">
         <f t="shared" si="2"/>
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="BM8" s="39">
         <f t="shared" si="2"/>
-        <v>53</v>
-      </c>
-      <c r="BN8" s="39">
-        <f t="shared" si="2"/>
         <v>54</v>
       </c>
     </row>
-    <row r="9" spans="1:67" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:66" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="47"/>
       <c r="B9" s="44"/>
       <c r="C9" s="44"/>
@@ -2666,11 +2697,11 @@
       <c r="H9" s="55"/>
       <c r="I9" s="54"/>
       <c r="J9" s="55"/>
-      <c r="K9" s="55"/>
-      <c r="L9" s="62" t="str">
+      <c r="K9" s="62" t="str">
         <f>IF(OR(ISBLANK(I9),ISBLANK(J9)),"",J9-I9+1)</f>
         <v/>
       </c>
+      <c r="L9" s="16"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
       <c r="O9" s="16"/>
@@ -2724,12 +2755,11 @@
       <c r="BK9" s="16"/>
       <c r="BL9" s="16"/>
       <c r="BM9" s="16"/>
-      <c r="BN9" s="16"/>
-    </row>
-    <row r="10" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="48"/>
       <c r="B10" s="45" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="C10" s="45"/>
       <c r="D10" s="42"/>
@@ -2745,11 +2775,11 @@
         <v>43851</v>
       </c>
       <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="63" t="str">
+      <c r="K10" s="63" t="str">
         <f>IF(OR(ISBLANK(I10),ISBLANK(J10)),"",J10-I10+1)</f>
         <v/>
       </c>
+      <c r="L10" s="16"/>
       <c r="M10" s="16"/>
       <c r="N10" s="16"/>
       <c r="O10" s="16"/>
@@ -2803,12 +2833,11 @@
       <c r="BK10" s="16"/>
       <c r="BL10" s="16"/>
       <c r="BM10" s="16"/>
-      <c r="BN10" s="16"/>
-    </row>
-    <row r="11" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="48"/>
       <c r="B11" s="45" t="s">
-        <v>77</v>
+        <v>69</v>
       </c>
       <c r="C11" s="45"/>
       <c r="D11" s="42"/>
@@ -2818,8 +2847,8 @@
       <c r="H11" s="57"/>
       <c r="I11" s="56"/>
       <c r="J11" s="57"/>
-      <c r="K11" s="57"/>
-      <c r="L11" s="63"/>
+      <c r="K11" s="63"/>
+      <c r="L11" s="16"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
       <c r="O11" s="16"/>
@@ -2873,19 +2902,18 @@
       <c r="BK11" s="16"/>
       <c r="BL11" s="16"/>
       <c r="BM11" s="16"/>
-      <c r="BN11" s="16"/>
-    </row>
-    <row r="12" spans="1:67" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:66" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="47"/>
       <c r="B12" s="15" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
       <c r="C12" s="15"/>
       <c r="D12" s="75" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E12" s="75" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F12" s="51">
         <v>1</v>
@@ -2902,8 +2930,8 @@
       <c r="J12" s="55">
         <v>43853</v>
       </c>
-      <c r="K12" s="55"/>
-      <c r="L12" s="62"/>
+      <c r="K12" s="62"/>
+      <c r="L12" s="16"/>
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
       <c r="O12" s="16"/>
@@ -2957,19 +2985,18 @@
       <c r="BK12" s="16"/>
       <c r="BL12" s="16"/>
       <c r="BM12" s="16"/>
-      <c r="BN12" s="16"/>
-    </row>
-    <row r="13" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="47"/>
       <c r="B13" s="15" t="s">
-        <v>57</v>
+        <v>49</v>
       </c>
       <c r="C13" s="15"/>
       <c r="D13" s="41" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E13" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F13" s="51">
         <v>1</v>
@@ -2986,8 +3013,8 @@
       <c r="J13" s="55">
         <v>43854</v>
       </c>
-      <c r="K13" s="55"/>
-      <c r="L13" s="62"/>
+      <c r="K13" s="62"/>
+      <c r="L13" s="16"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
       <c r="O13" s="16"/>
@@ -2999,9 +3026,9 @@
       <c r="U13" s="16"/>
       <c r="V13" s="16"/>
       <c r="W13" s="16"/>
-      <c r="X13" s="16"/>
+      <c r="X13" s="17"/>
       <c r="Y13" s="17"/>
-      <c r="Z13" s="17"/>
+      <c r="Z13" s="16"/>
       <c r="AA13" s="16"/>
       <c r="AB13" s="16"/>
       <c r="AC13" s="16"/>
@@ -3041,19 +3068,18 @@
       <c r="BK13" s="16"/>
       <c r="BL13" s="16"/>
       <c r="BM13" s="16"/>
-      <c r="BN13" s="16"/>
-    </row>
-    <row r="14" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="47"/>
       <c r="B14" s="15" t="s">
-        <v>58</v>
+        <v>50</v>
       </c>
       <c r="C14" s="15"/>
       <c r="D14" s="41" t="s">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="E14" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F14" s="51">
         <v>1</v>
@@ -3070,8 +3096,8 @@
       <c r="J14" s="55">
         <v>43854</v>
       </c>
-      <c r="K14" s="55"/>
-      <c r="L14" s="62"/>
+      <c r="K14" s="62"/>
+      <c r="L14" s="16"/>
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
       <c r="O14" s="16"/>
@@ -3125,19 +3151,18 @@
       <c r="BK14" s="16"/>
       <c r="BL14" s="16"/>
       <c r="BM14" s="16"/>
-      <c r="BN14" s="16"/>
-    </row>
-    <row r="15" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="47"/>
       <c r="B15" s="15" t="s">
-        <v>61</v>
+        <v>53</v>
       </c>
       <c r="C15" s="15"/>
       <c r="D15" s="41" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F15" s="51">
         <v>1</v>
@@ -3154,8 +3179,8 @@
       <c r="J15" s="55">
         <v>43853</v>
       </c>
-      <c r="K15" s="55"/>
-      <c r="L15" s="62"/>
+      <c r="K15" s="62"/>
+      <c r="L15" s="16"/>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
       <c r="O15" s="16"/>
@@ -3171,8 +3196,8 @@
       <c r="Y15" s="16"/>
       <c r="Z15" s="16"/>
       <c r="AA15" s="16"/>
-      <c r="AB15" s="16"/>
-      <c r="AC15" s="17"/>
+      <c r="AB15" s="17"/>
+      <c r="AC15" s="16"/>
       <c r="AD15" s="16"/>
       <c r="AE15" s="16"/>
       <c r="AF15" s="16"/>
@@ -3209,19 +3234,18 @@
       <c r="BK15" s="16"/>
       <c r="BL15" s="16"/>
       <c r="BM15" s="16"/>
-      <c r="BN15" s="16"/>
-    </row>
-    <row r="16" spans="1:67" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="47"/>
       <c r="B16" s="15" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
       <c r="C16" s="15"/>
       <c r="D16" s="41" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E16" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F16" s="51">
         <v>1</v>
@@ -3238,8 +3262,8 @@
       <c r="J16" s="55">
         <v>43868</v>
       </c>
-      <c r="K16" s="55"/>
-      <c r="L16" s="62"/>
+      <c r="K16" s="62"/>
+      <c r="L16" s="16"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
       <c r="O16" s="16"/>
@@ -3293,26 +3317,25 @@
       <c r="BK16" s="16"/>
       <c r="BL16" s="16"/>
       <c r="BM16" s="16"/>
-      <c r="BN16" s="16"/>
-    </row>
-    <row r="17" spans="1:66" s="72" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:65" s="72" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="50" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B17" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D17" s="13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E17" s="13" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G17" s="70" t="s">
         <v>8</v>
@@ -3321,238 +3344,235 @@
         <v>9</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="K17" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L17" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="M17" s="39">
+        <v>46</v>
+      </c>
+      <c r="L17" s="39">
         <f>G15</f>
         <v>43853</v>
       </c>
+      <c r="M17" s="39">
+        <f>L17+1</f>
+        <v>43854</v>
+      </c>
       <c r="N17" s="39">
-        <f>M17+1</f>
-        <v>43854</v>
+        <f t="shared" ref="N17" si="3">M17+1</f>
+        <v>43855</v>
       </c>
       <c r="O17" s="39">
-        <f t="shared" ref="O17" si="3">N17+1</f>
-        <v>43855</v>
+        <f t="shared" ref="O17" si="4">N17+1</f>
+        <v>43856</v>
       </c>
       <c r="P17" s="39">
-        <f t="shared" ref="P17" si="4">O17+1</f>
-        <v>43856</v>
+        <f t="shared" ref="P17" si="5">O17+1</f>
+        <v>43857</v>
       </c>
       <c r="Q17" s="39">
-        <f t="shared" ref="Q17" si="5">P17+1</f>
-        <v>43857</v>
+        <f t="shared" ref="Q17" si="6">P17+1</f>
+        <v>43858</v>
       </c>
       <c r="R17" s="39">
-        <f t="shared" ref="R17" si="6">Q17+1</f>
-        <v>43858</v>
+        <f t="shared" ref="R17" si="7">Q17+1</f>
+        <v>43859</v>
       </c>
       <c r="S17" s="39">
-        <f t="shared" ref="S17" si="7">R17+1</f>
-        <v>43859</v>
+        <f t="shared" ref="S17" si="8">R17+1</f>
+        <v>43860</v>
       </c>
       <c r="T17" s="39">
-        <f t="shared" ref="T17" si="8">S17+1</f>
-        <v>43860</v>
+        <f t="shared" ref="T17" si="9">S17+1</f>
+        <v>43861</v>
       </c>
       <c r="U17" s="39">
-        <f t="shared" ref="U17" si="9">T17+1</f>
-        <v>43861</v>
+        <f t="shared" ref="U17" si="10">T17+1</f>
+        <v>43862</v>
       </c>
       <c r="V17" s="39">
-        <f t="shared" ref="V17" si="10">U17+1</f>
-        <v>43862</v>
+        <f t="shared" ref="V17" si="11">U17+1</f>
+        <v>43863</v>
       </c>
       <c r="W17" s="39">
-        <f t="shared" ref="W17" si="11">V17+1</f>
-        <v>43863</v>
+        <f t="shared" ref="W17" si="12">V17+1</f>
+        <v>43864</v>
       </c>
       <c r="X17" s="39">
-        <f t="shared" ref="X17" si="12">W17+1</f>
-        <v>43864</v>
+        <f t="shared" ref="X17" si="13">W17+1</f>
+        <v>43865</v>
       </c>
       <c r="Y17" s="39">
-        <f t="shared" ref="Y17" si="13">X17+1</f>
-        <v>43865</v>
+        <f t="shared" ref="Y17" si="14">X17+1</f>
+        <v>43866</v>
       </c>
       <c r="Z17" s="39">
-        <f t="shared" ref="Z17" si="14">Y17+1</f>
-        <v>43866</v>
+        <f t="shared" ref="Z17" si="15">Y17+1</f>
+        <v>43867</v>
       </c>
       <c r="AA17" s="39">
-        <f t="shared" ref="AA17" si="15">Z17+1</f>
-        <v>43867</v>
+        <f t="shared" ref="AA17" si="16">Z17+1</f>
+        <v>43868</v>
       </c>
       <c r="AB17" s="39">
-        <f t="shared" ref="AB17" si="16">AA17+1</f>
-        <v>43868</v>
+        <f t="shared" ref="AB17" si="17">AA17+1</f>
+        <v>43869</v>
       </c>
       <c r="AC17" s="39">
-        <f t="shared" ref="AC17" si="17">AB17+1</f>
-        <v>43869</v>
+        <f t="shared" ref="AC17" si="18">AB17+1</f>
+        <v>43870</v>
       </c>
       <c r="AD17" s="39">
-        <f t="shared" ref="AD17" si="18">AC17+1</f>
-        <v>43870</v>
+        <f t="shared" ref="AD17" si="19">AC17+1</f>
+        <v>43871</v>
       </c>
       <c r="AE17" s="39">
-        <f t="shared" ref="AE17" si="19">AD17+1</f>
-        <v>43871</v>
+        <f t="shared" ref="AE17" si="20">AD17+1</f>
+        <v>43872</v>
       </c>
       <c r="AF17" s="39">
-        <f t="shared" ref="AF17" si="20">AE17+1</f>
-        <v>43872</v>
+        <f t="shared" ref="AF17" si="21">AE17+1</f>
+        <v>43873</v>
       </c>
       <c r="AG17" s="39">
-        <f t="shared" ref="AG17" si="21">AF17+1</f>
-        <v>43873</v>
+        <f t="shared" ref="AG17" si="22">AF17+1</f>
+        <v>43874</v>
       </c>
       <c r="AH17" s="39">
-        <f t="shared" ref="AH17" si="22">AG17+1</f>
-        <v>43874</v>
+        <f t="shared" ref="AH17" si="23">AG17+1</f>
+        <v>43875</v>
       </c>
       <c r="AI17" s="39">
-        <f t="shared" ref="AI17" si="23">AH17+1</f>
-        <v>43875</v>
+        <f t="shared" ref="AI17" si="24">AH17+1</f>
+        <v>43876</v>
       </c>
       <c r="AJ17" s="39">
-        <f t="shared" ref="AJ17" si="24">AI17+1</f>
-        <v>43876</v>
+        <f t="shared" ref="AJ17" si="25">AI17+1</f>
+        <v>43877</v>
       </c>
       <c r="AK17" s="39">
-        <f t="shared" ref="AK17" si="25">AJ17+1</f>
-        <v>43877</v>
+        <f t="shared" ref="AK17" si="26">AJ17+1</f>
+        <v>43878</v>
       </c>
       <c r="AL17" s="39">
-        <f t="shared" ref="AL17" si="26">AK17+1</f>
-        <v>43878</v>
+        <f t="shared" ref="AL17" si="27">AK17+1</f>
+        <v>43879</v>
       </c>
       <c r="AM17" s="39">
-        <f t="shared" ref="AM17" si="27">AL17+1</f>
-        <v>43879</v>
+        <f t="shared" ref="AM17" si="28">AL17+1</f>
+        <v>43880</v>
       </c>
       <c r="AN17" s="39">
-        <f t="shared" ref="AN17" si="28">AM17+1</f>
-        <v>43880</v>
+        <f t="shared" ref="AN17" si="29">AM17+1</f>
+        <v>43881</v>
       </c>
       <c r="AO17" s="39">
-        <f t="shared" ref="AO17" si="29">AN17+1</f>
-        <v>43881</v>
+        <f t="shared" ref="AO17" si="30">AN17+1</f>
+        <v>43882</v>
       </c>
       <c r="AP17" s="39">
-        <f t="shared" ref="AP17" si="30">AO17+1</f>
-        <v>43882</v>
+        <f t="shared" ref="AP17" si="31">AO17+1</f>
+        <v>43883</v>
       </c>
       <c r="AQ17" s="39">
-        <f t="shared" ref="AQ17" si="31">AP17+1</f>
-        <v>43883</v>
+        <f t="shared" ref="AQ17" si="32">AP17+1</f>
+        <v>43884</v>
       </c>
       <c r="AR17" s="39">
-        <f t="shared" ref="AR17" si="32">AQ17+1</f>
-        <v>43884</v>
+        <f t="shared" ref="AR17" si="33">AQ17+1</f>
+        <v>43885</v>
       </c>
       <c r="AS17" s="39">
-        <f t="shared" ref="AS17" si="33">AR17+1</f>
-        <v>43885</v>
+        <f t="shared" ref="AS17" si="34">AR17+1</f>
+        <v>43886</v>
       </c>
       <c r="AT17" s="39">
-        <f t="shared" ref="AT17" si="34">AS17+1</f>
-        <v>43886</v>
+        <f t="shared" ref="AT17" si="35">AS17+1</f>
+        <v>43887</v>
       </c>
       <c r="AU17" s="39">
-        <f t="shared" ref="AU17" si="35">AT17+1</f>
-        <v>43887</v>
+        <f t="shared" ref="AU17" si="36">AT17+1</f>
+        <v>43888</v>
       </c>
       <c r="AV17" s="39">
-        <f t="shared" ref="AV17" si="36">AU17+1</f>
-        <v>43888</v>
+        <f t="shared" ref="AV17" si="37">AU17+1</f>
+        <v>43889</v>
       </c>
       <c r="AW17" s="39">
-        <f t="shared" ref="AW17" si="37">AV17+1</f>
-        <v>43889</v>
+        <f t="shared" ref="AW17" si="38">AV17+1</f>
+        <v>43890</v>
       </c>
       <c r="AX17" s="39">
-        <f t="shared" ref="AX17" si="38">AW17+1</f>
-        <v>43890</v>
+        <f t="shared" ref="AX17" si="39">AW17+1</f>
+        <v>43891</v>
       </c>
       <c r="AY17" s="39">
-        <f t="shared" ref="AY17" si="39">AX17+1</f>
-        <v>43891</v>
+        <f t="shared" ref="AY17" si="40">AX17+1</f>
+        <v>43892</v>
       </c>
       <c r="AZ17" s="39">
-        <f t="shared" ref="AZ17" si="40">AY17+1</f>
-        <v>43892</v>
+        <f t="shared" ref="AZ17" si="41">AY17+1</f>
+        <v>43893</v>
       </c>
       <c r="BA17" s="39">
-        <f t="shared" ref="BA17" si="41">AZ17+1</f>
-        <v>43893</v>
+        <f t="shared" ref="BA17" si="42">AZ17+1</f>
+        <v>43894</v>
       </c>
       <c r="BB17" s="39">
-        <f t="shared" ref="BB17" si="42">BA17+1</f>
-        <v>43894</v>
+        <f t="shared" ref="BB17" si="43">BA17+1</f>
+        <v>43895</v>
       </c>
       <c r="BC17" s="39">
-        <f t="shared" ref="BC17" si="43">BB17+1</f>
-        <v>43895</v>
+        <f t="shared" ref="BC17" si="44">BB17+1</f>
+        <v>43896</v>
       </c>
       <c r="BD17" s="39">
-        <f t="shared" ref="BD17" si="44">BC17+1</f>
-        <v>43896</v>
+        <f t="shared" ref="BD17" si="45">BC17+1</f>
+        <v>43897</v>
       </c>
       <c r="BE17" s="39">
-        <f t="shared" ref="BE17" si="45">BD17+1</f>
-        <v>43897</v>
+        <f t="shared" ref="BE17" si="46">BD17+1</f>
+        <v>43898</v>
       </c>
       <c r="BF17" s="39">
-        <f t="shared" ref="BF17" si="46">BE17+1</f>
-        <v>43898</v>
+        <f t="shared" ref="BF17" si="47">BE17+1</f>
+        <v>43899</v>
       </c>
       <c r="BG17" s="39">
-        <f t="shared" ref="BG17" si="47">BF17+1</f>
-        <v>43899</v>
+        <f t="shared" ref="BG17" si="48">BF17+1</f>
+        <v>43900</v>
       </c>
       <c r="BH17" s="39">
-        <f t="shared" ref="BH17" si="48">BG17+1</f>
-        <v>43900</v>
+        <f t="shared" ref="BH17" si="49">BG17+1</f>
+        <v>43901</v>
       </c>
       <c r="BI17" s="39">
-        <f t="shared" ref="BI17" si="49">BH17+1</f>
-        <v>43901</v>
+        <f t="shared" ref="BI17" si="50">BH17+1</f>
+        <v>43902</v>
       </c>
       <c r="BJ17" s="39">
-        <f t="shared" ref="BJ17" si="50">BI17+1</f>
-        <v>43902</v>
+        <f t="shared" ref="BJ17" si="51">BI17+1</f>
+        <v>43903</v>
       </c>
       <c r="BK17" s="39">
-        <f t="shared" ref="BK17" si="51">BJ17+1</f>
-        <v>43903</v>
+        <f t="shared" ref="BK17" si="52">BJ17+1</f>
+        <v>43904</v>
       </c>
       <c r="BL17" s="39">
-        <f t="shared" ref="BL17" si="52">BK17+1</f>
-        <v>43904</v>
+        <f t="shared" ref="BL17" si="53">BK17+1</f>
+        <v>43905</v>
       </c>
       <c r="BM17" s="39">
-        <f t="shared" ref="BM17" si="53">BL17+1</f>
-        <v>43905</v>
-      </c>
-      <c r="BN17" s="39">
-        <f t="shared" ref="BN17" si="54">BM17+1</f>
+        <f t="shared" ref="BM17" si="54">BL17+1</f>
         <v>43906</v>
       </c>
     </row>
-    <row r="18" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="48"/>
       <c r="B18" s="45" t="s">
-        <v>78</v>
+        <v>70</v>
       </c>
       <c r="C18" s="45"/>
       <c r="D18" s="42"/>
@@ -3562,8 +3582,8 @@
       <c r="H18" s="57"/>
       <c r="I18" s="56"/>
       <c r="J18" s="57"/>
-      <c r="K18" s="57"/>
-      <c r="L18" s="63"/>
+      <c r="K18" s="63"/>
+      <c r="L18" s="16"/>
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
       <c r="O18" s="16"/>
@@ -3617,19 +3637,18 @@
       <c r="BK18" s="16"/>
       <c r="BL18" s="16"/>
       <c r="BM18" s="16"/>
-      <c r="BN18" s="16"/>
-    </row>
-    <row r="19" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="19" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="47"/>
       <c r="B19" s="15" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C19" s="15"/>
       <c r="D19" s="41" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E19" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F19" s="51">
         <v>1</v>
@@ -3646,8 +3665,8 @@
       <c r="J19" s="55">
         <v>43867</v>
       </c>
-      <c r="K19" s="55"/>
-      <c r="L19" s="62"/>
+      <c r="K19" s="62"/>
+      <c r="L19" s="16"/>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
       <c r="O19" s="16"/>
@@ -3701,19 +3720,18 @@
       <c r="BK19" s="16"/>
       <c r="BL19" s="16"/>
       <c r="BM19" s="16"/>
-      <c r="BN19" s="16"/>
-    </row>
-    <row r="20" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="20" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="47"/>
       <c r="B20" s="15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C20" s="15"/>
       <c r="D20" s="41" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E20" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F20" s="51">
         <v>1</v>
@@ -3730,8 +3748,8 @@
       <c r="J20" s="55">
         <v>43867</v>
       </c>
-      <c r="K20" s="55"/>
-      <c r="L20" s="62"/>
+      <c r="K20" s="62"/>
+      <c r="L20" s="16"/>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
       <c r="O20" s="16"/>
@@ -3785,19 +3803,18 @@
       <c r="BK20" s="16"/>
       <c r="BL20" s="16"/>
       <c r="BM20" s="16"/>
-      <c r="BN20" s="16"/>
-    </row>
-    <row r="21" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="15" t="s">
-        <v>71</v>
+        <v>63</v>
       </c>
       <c r="C21" s="15"/>
       <c r="D21" s="41" t="s">
-        <v>79</v>
+        <v>71</v>
       </c>
       <c r="E21" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F21" s="51">
         <v>1</v>
@@ -3814,8 +3831,8 @@
       <c r="J21" s="55">
         <v>43867</v>
       </c>
-      <c r="K21" s="55"/>
-      <c r="L21" s="62"/>
+      <c r="K21" s="62"/>
+      <c r="L21" s="16"/>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
       <c r="O21" s="16"/>
@@ -3869,19 +3886,18 @@
       <c r="BK21" s="16"/>
       <c r="BL21" s="16"/>
       <c r="BM21" s="16"/>
-      <c r="BN21" s="16"/>
-    </row>
-    <row r="22" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="47"/>
       <c r="B22" s="15" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C22" s="15"/>
       <c r="D22" s="41" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E22" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F22" s="51">
         <v>1</v>
@@ -3898,8 +3914,8 @@
       <c r="J22" s="55">
         <v>43865</v>
       </c>
-      <c r="K22" s="55"/>
-      <c r="L22" s="62"/>
+      <c r="K22" s="62"/>
+      <c r="L22" s="16"/>
       <c r="M22" s="16"/>
       <c r="N22" s="16"/>
       <c r="O22" s="16"/>
@@ -3953,19 +3969,18 @@
       <c r="BK22" s="16"/>
       <c r="BL22" s="16"/>
       <c r="BM22" s="16"/>
-      <c r="BN22" s="16"/>
-    </row>
-    <row r="23" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="47"/>
       <c r="B23" s="15" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C23" s="15"/>
       <c r="D23" s="41" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E23" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F23" s="51">
         <v>1</v>
@@ -3982,8 +3997,8 @@
       <c r="J23" s="55">
         <v>43867</v>
       </c>
-      <c r="K23" s="55"/>
-      <c r="L23" s="62"/>
+      <c r="K23" s="62"/>
+      <c r="L23" s="16"/>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
       <c r="O23" s="16"/>
@@ -4037,19 +4052,18 @@
       <c r="BK23" s="16"/>
       <c r="BL23" s="16"/>
       <c r="BM23" s="16"/>
-      <c r="BN23" s="16"/>
-    </row>
-    <row r="24" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="47"/>
       <c r="B24" s="15" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C24" s="15"/>
       <c r="D24" s="41" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E24" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F24" s="51">
         <v>1</v>
@@ -4066,8 +4080,8 @@
       <c r="J24" s="55">
         <v>43868</v>
       </c>
-      <c r="K24" s="55"/>
-      <c r="L24" s="62"/>
+      <c r="K24" s="62"/>
+      <c r="L24" s="16"/>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
       <c r="O24" s="16"/>
@@ -4121,19 +4135,18 @@
       <c r="BK24" s="16"/>
       <c r="BL24" s="16"/>
       <c r="BM24" s="16"/>
-      <c r="BN24" s="16"/>
-    </row>
-    <row r="25" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="25" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="47"/>
       <c r="B25" s="15" t="s">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="C25" s="15"/>
       <c r="D25" s="41" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E25" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F25" s="51">
         <v>1</v>
@@ -4150,8 +4163,8 @@
       <c r="J25" s="55">
         <v>43868</v>
       </c>
-      <c r="K25" s="55"/>
-      <c r="L25" s="62"/>
+      <c r="K25" s="62"/>
+      <c r="L25" s="16"/>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
       <c r="O25" s="16"/>
@@ -4205,26 +4218,25 @@
       <c r="BK25" s="16"/>
       <c r="BL25" s="16"/>
       <c r="BM25" s="16"/>
-      <c r="BN25" s="16"/>
-    </row>
-    <row r="26" spans="1:66" s="72" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:65" s="72" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="50" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
       <c r="B26" s="12" t="s">
         <v>10</v>
       </c>
       <c r="C26" s="12" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="D26" s="13" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="E26" s="13" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="G26" s="70" t="s">
         <v>8</v>
@@ -4233,238 +4245,235 @@
         <v>9</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
       <c r="J26" s="13" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
       <c r="K26" s="13" t="s">
-        <v>53</v>
-      </c>
-      <c r="L26" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="M26" s="39">
+        <v>46</v>
+      </c>
+      <c r="L26" s="39">
         <f>G24</f>
         <v>43864</v>
       </c>
+      <c r="M26" s="39">
+        <f>L26+1</f>
+        <v>43865</v>
+      </c>
       <c r="N26" s="39">
-        <f>M26+1</f>
-        <v>43865</v>
+        <f t="shared" ref="N26" si="55">M26+1</f>
+        <v>43866</v>
       </c>
       <c r="O26" s="39">
-        <f t="shared" ref="O26" si="55">N26+1</f>
-        <v>43866</v>
+        <f t="shared" ref="O26" si="56">N26+1</f>
+        <v>43867</v>
       </c>
       <c r="P26" s="39">
-        <f t="shared" ref="P26" si="56">O26+1</f>
-        <v>43867</v>
+        <f t="shared" ref="P26" si="57">O26+1</f>
+        <v>43868</v>
       </c>
       <c r="Q26" s="39">
-        <f t="shared" ref="Q26" si="57">P26+1</f>
-        <v>43868</v>
+        <f t="shared" ref="Q26" si="58">P26+1</f>
+        <v>43869</v>
       </c>
       <c r="R26" s="39">
-        <f t="shared" ref="R26" si="58">Q26+1</f>
-        <v>43869</v>
+        <f t="shared" ref="R26" si="59">Q26+1</f>
+        <v>43870</v>
       </c>
       <c r="S26" s="39">
-        <f t="shared" ref="S26" si="59">R26+1</f>
-        <v>43870</v>
+        <f t="shared" ref="S26" si="60">R26+1</f>
+        <v>43871</v>
       </c>
       <c r="T26" s="39">
-        <f t="shared" ref="T26" si="60">S26+1</f>
-        <v>43871</v>
+        <f t="shared" ref="T26" si="61">S26+1</f>
+        <v>43872</v>
       </c>
       <c r="U26" s="39">
-        <f t="shared" ref="U26" si="61">T26+1</f>
-        <v>43872</v>
+        <f t="shared" ref="U26" si="62">T26+1</f>
+        <v>43873</v>
       </c>
       <c r="V26" s="39">
-        <f t="shared" ref="V26" si="62">U26+1</f>
-        <v>43873</v>
+        <f t="shared" ref="V26" si="63">U26+1</f>
+        <v>43874</v>
       </c>
       <c r="W26" s="39">
-        <f t="shared" ref="W26" si="63">V26+1</f>
-        <v>43874</v>
+        <f t="shared" ref="W26" si="64">V26+1</f>
+        <v>43875</v>
       </c>
       <c r="X26" s="39">
-        <f t="shared" ref="X26" si="64">W26+1</f>
-        <v>43875</v>
+        <f t="shared" ref="X26" si="65">W26+1</f>
+        <v>43876</v>
       </c>
       <c r="Y26" s="39">
-        <f t="shared" ref="Y26" si="65">X26+1</f>
-        <v>43876</v>
+        <f t="shared" ref="Y26" si="66">X26+1</f>
+        <v>43877</v>
       </c>
       <c r="Z26" s="39">
-        <f t="shared" ref="Z26" si="66">Y26+1</f>
-        <v>43877</v>
+        <f t="shared" ref="Z26" si="67">Y26+1</f>
+        <v>43878</v>
       </c>
       <c r="AA26" s="39">
-        <f t="shared" ref="AA26" si="67">Z26+1</f>
-        <v>43878</v>
+        <f t="shared" ref="AA26" si="68">Z26+1</f>
+        <v>43879</v>
       </c>
       <c r="AB26" s="39">
-        <f t="shared" ref="AB26" si="68">AA26+1</f>
-        <v>43879</v>
+        <f t="shared" ref="AB26" si="69">AA26+1</f>
+        <v>43880</v>
       </c>
       <c r="AC26" s="39">
-        <f t="shared" ref="AC26" si="69">AB26+1</f>
-        <v>43880</v>
+        <f t="shared" ref="AC26" si="70">AB26+1</f>
+        <v>43881</v>
       </c>
       <c r="AD26" s="39">
-        <f t="shared" ref="AD26" si="70">AC26+1</f>
-        <v>43881</v>
+        <f t="shared" ref="AD26" si="71">AC26+1</f>
+        <v>43882</v>
       </c>
       <c r="AE26" s="39">
-        <f t="shared" ref="AE26" si="71">AD26+1</f>
-        <v>43882</v>
+        <f t="shared" ref="AE26" si="72">AD26+1</f>
+        <v>43883</v>
       </c>
       <c r="AF26" s="39">
-        <f t="shared" ref="AF26" si="72">AE26+1</f>
-        <v>43883</v>
+        <f t="shared" ref="AF26" si="73">AE26+1</f>
+        <v>43884</v>
       </c>
       <c r="AG26" s="39">
-        <f t="shared" ref="AG26" si="73">AF26+1</f>
-        <v>43884</v>
+        <f t="shared" ref="AG26" si="74">AF26+1</f>
+        <v>43885</v>
       </c>
       <c r="AH26" s="39">
-        <f t="shared" ref="AH26" si="74">AG26+1</f>
-        <v>43885</v>
+        <f t="shared" ref="AH26" si="75">AG26+1</f>
+        <v>43886</v>
       </c>
       <c r="AI26" s="39">
-        <f t="shared" ref="AI26" si="75">AH26+1</f>
-        <v>43886</v>
+        <f t="shared" ref="AI26" si="76">AH26+1</f>
+        <v>43887</v>
       </c>
       <c r="AJ26" s="39">
-        <f t="shared" ref="AJ26" si="76">AI26+1</f>
-        <v>43887</v>
+        <f t="shared" ref="AJ26" si="77">AI26+1</f>
+        <v>43888</v>
       </c>
       <c r="AK26" s="39">
-        <f t="shared" ref="AK26" si="77">AJ26+1</f>
-        <v>43888</v>
+        <f t="shared" ref="AK26" si="78">AJ26+1</f>
+        <v>43889</v>
       </c>
       <c r="AL26" s="39">
-        <f t="shared" ref="AL26" si="78">AK26+1</f>
-        <v>43889</v>
+        <f t="shared" ref="AL26" si="79">AK26+1</f>
+        <v>43890</v>
       </c>
       <c r="AM26" s="39">
-        <f t="shared" ref="AM26" si="79">AL26+1</f>
-        <v>43890</v>
+        <f t="shared" ref="AM26" si="80">AL26+1</f>
+        <v>43891</v>
       </c>
       <c r="AN26" s="39">
-        <f t="shared" ref="AN26" si="80">AM26+1</f>
-        <v>43891</v>
+        <f t="shared" ref="AN26" si="81">AM26+1</f>
+        <v>43892</v>
       </c>
       <c r="AO26" s="39">
-        <f t="shared" ref="AO26" si="81">AN26+1</f>
-        <v>43892</v>
+        <f t="shared" ref="AO26" si="82">AN26+1</f>
+        <v>43893</v>
       </c>
       <c r="AP26" s="39">
-        <f t="shared" ref="AP26" si="82">AO26+1</f>
-        <v>43893</v>
+        <f t="shared" ref="AP26" si="83">AO26+1</f>
+        <v>43894</v>
       </c>
       <c r="AQ26" s="39">
-        <f t="shared" ref="AQ26" si="83">AP26+1</f>
-        <v>43894</v>
+        <f t="shared" ref="AQ26" si="84">AP26+1</f>
+        <v>43895</v>
       </c>
       <c r="AR26" s="39">
-        <f t="shared" ref="AR26" si="84">AQ26+1</f>
-        <v>43895</v>
+        <f t="shared" ref="AR26" si="85">AQ26+1</f>
+        <v>43896</v>
       </c>
       <c r="AS26" s="39">
-        <f t="shared" ref="AS26" si="85">AR26+1</f>
-        <v>43896</v>
+        <f t="shared" ref="AS26" si="86">AR26+1</f>
+        <v>43897</v>
       </c>
       <c r="AT26" s="39">
-        <f t="shared" ref="AT26" si="86">AS26+1</f>
-        <v>43897</v>
+        <f t="shared" ref="AT26" si="87">AS26+1</f>
+        <v>43898</v>
       </c>
       <c r="AU26" s="39">
-        <f t="shared" ref="AU26" si="87">AT26+1</f>
-        <v>43898</v>
+        <f t="shared" ref="AU26" si="88">AT26+1</f>
+        <v>43899</v>
       </c>
       <c r="AV26" s="39">
-        <f t="shared" ref="AV26" si="88">AU26+1</f>
-        <v>43899</v>
+        <f t="shared" ref="AV26" si="89">AU26+1</f>
+        <v>43900</v>
       </c>
       <c r="AW26" s="39">
-        <f t="shared" ref="AW26" si="89">AV26+1</f>
-        <v>43900</v>
+        <f t="shared" ref="AW26" si="90">AV26+1</f>
+        <v>43901</v>
       </c>
       <c r="AX26" s="39">
-        <f t="shared" ref="AX26" si="90">AW26+1</f>
-        <v>43901</v>
+        <f t="shared" ref="AX26" si="91">AW26+1</f>
+        <v>43902</v>
       </c>
       <c r="AY26" s="39">
-        <f t="shared" ref="AY26" si="91">AX26+1</f>
-        <v>43902</v>
+        <f t="shared" ref="AY26" si="92">AX26+1</f>
+        <v>43903</v>
       </c>
       <c r="AZ26" s="39">
-        <f t="shared" ref="AZ26" si="92">AY26+1</f>
-        <v>43903</v>
+        <f t="shared" ref="AZ26" si="93">AY26+1</f>
+        <v>43904</v>
       </c>
       <c r="BA26" s="39">
-        <f t="shared" ref="BA26" si="93">AZ26+1</f>
-        <v>43904</v>
+        <f t="shared" ref="BA26" si="94">AZ26+1</f>
+        <v>43905</v>
       </c>
       <c r="BB26" s="39">
-        <f t="shared" ref="BB26" si="94">BA26+1</f>
-        <v>43905</v>
+        <f t="shared" ref="BB26" si="95">BA26+1</f>
+        <v>43906</v>
       </c>
       <c r="BC26" s="39">
-        <f t="shared" ref="BC26" si="95">BB26+1</f>
-        <v>43906</v>
+        <f t="shared" ref="BC26" si="96">BB26+1</f>
+        <v>43907</v>
       </c>
       <c r="BD26" s="39">
-        <f t="shared" ref="BD26" si="96">BC26+1</f>
-        <v>43907</v>
+        <f t="shared" ref="BD26" si="97">BC26+1</f>
+        <v>43908</v>
       </c>
       <c r="BE26" s="39">
-        <f t="shared" ref="BE26" si="97">BD26+1</f>
-        <v>43908</v>
+        <f t="shared" ref="BE26" si="98">BD26+1</f>
+        <v>43909</v>
       </c>
       <c r="BF26" s="39">
-        <f t="shared" ref="BF26" si="98">BE26+1</f>
-        <v>43909</v>
+        <f t="shared" ref="BF26" si="99">BE26+1</f>
+        <v>43910</v>
       </c>
       <c r="BG26" s="39">
-        <f t="shared" ref="BG26" si="99">BF26+1</f>
-        <v>43910</v>
+        <f t="shared" ref="BG26" si="100">BF26+1</f>
+        <v>43911</v>
       </c>
       <c r="BH26" s="39">
-        <f t="shared" ref="BH26" si="100">BG26+1</f>
-        <v>43911</v>
+        <f t="shared" ref="BH26" si="101">BG26+1</f>
+        <v>43912</v>
       </c>
       <c r="BI26" s="39">
-        <f t="shared" ref="BI26" si="101">BH26+1</f>
-        <v>43912</v>
+        <f t="shared" ref="BI26" si="102">BH26+1</f>
+        <v>43913</v>
       </c>
       <c r="BJ26" s="39">
-        <f t="shared" ref="BJ26" si="102">BI26+1</f>
-        <v>43913</v>
+        <f t="shared" ref="BJ26" si="103">BI26+1</f>
+        <v>43914</v>
       </c>
       <c r="BK26" s="39">
-        <f t="shared" ref="BK26" si="103">BJ26+1</f>
-        <v>43914</v>
+        <f t="shared" ref="BK26" si="104">BJ26+1</f>
+        <v>43915</v>
       </c>
       <c r="BL26" s="39">
-        <f t="shared" ref="BL26" si="104">BK26+1</f>
-        <v>43915</v>
+        <f t="shared" ref="BL26" si="105">BK26+1</f>
+        <v>43916</v>
       </c>
       <c r="BM26" s="39">
-        <f t="shared" ref="BM26" si="105">BL26+1</f>
-        <v>43916</v>
-      </c>
-      <c r="BN26" s="39">
-        <f t="shared" ref="BN26" si="106">BM26+1</f>
+        <f t="shared" ref="BM26" si="106">BL26+1</f>
         <v>43917</v>
       </c>
     </row>
-    <row r="27" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="48"/>
       <c r="B27" s="45" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="C27" s="45"/>
       <c r="D27" s="42"/>
@@ -4474,8 +4483,8 @@
       <c r="H27" s="57"/>
       <c r="I27" s="56"/>
       <c r="J27" s="57"/>
-      <c r="K27" s="57"/>
-      <c r="L27" s="63"/>
+      <c r="K27" s="63"/>
+      <c r="L27" s="16"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
       <c r="O27" s="16"/>
@@ -4487,11 +4496,11 @@
       <c r="U27" s="16"/>
       <c r="V27" s="16"/>
       <c r="W27" s="16"/>
-      <c r="X27" s="16"/>
-      <c r="Y27" s="17"/>
+      <c r="X27" s="17"/>
+      <c r="Y27" s="16"/>
       <c r="Z27" s="16"/>
-      <c r="AA27" s="16"/>
-      <c r="AB27" s="17"/>
+      <c r="AA27" s="17"/>
+      <c r="AB27" s="16"/>
       <c r="AC27" s="16"/>
       <c r="AD27" s="16"/>
       <c r="AE27" s="16"/>
@@ -4529,21 +4538,20 @@
       <c r="BK27" s="16"/>
       <c r="BL27" s="16"/>
       <c r="BM27" s="16"/>
-      <c r="BN27" s="16"/>
-    </row>
-    <row r="28" spans="1:66" s="8" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="28" spans="1:65" s="8" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="47"/>
       <c r="B28" s="15" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="D28" s="41" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E28" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F28" s="51">
         <v>0</v>
@@ -4554,10 +4562,14 @@
       <c r="H28" s="55">
         <v>43869</v>
       </c>
-      <c r="I28" s="54"/>
-      <c r="J28" s="55"/>
-      <c r="K28" s="55"/>
-      <c r="L28" s="62"/>
+      <c r="I28" s="54" t="s">
+        <v>83</v>
+      </c>
+      <c r="J28" s="55" t="s">
+        <v>83</v>
+      </c>
+      <c r="K28" s="62"/>
+      <c r="L28" s="16"/>
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
       <c r="O28" s="16"/>
@@ -4611,21 +4623,20 @@
       <c r="BK28" s="16"/>
       <c r="BL28" s="16"/>
       <c r="BM28" s="16"/>
-      <c r="BN28" s="16"/>
-    </row>
-    <row r="29" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="47"/>
       <c r="B29" s="15" t="s">
-        <v>70</v>
+        <v>62</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>83</v>
+        <v>75</v>
       </c>
       <c r="D29" s="41" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="E29" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F29" s="51">
         <v>0</v>
@@ -4636,10 +4647,14 @@
       <c r="H29" s="55">
         <v>43872</v>
       </c>
-      <c r="I29" s="54"/>
-      <c r="J29" s="55"/>
-      <c r="K29" s="55"/>
-      <c r="L29" s="62"/>
+      <c r="I29" s="54">
+        <v>43869</v>
+      </c>
+      <c r="J29" s="55">
+        <v>43872</v>
+      </c>
+      <c r="K29" s="62"/>
+      <c r="L29" s="16"/>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
       <c r="O29" s="16"/>
@@ -4693,21 +4708,20 @@
       <c r="BK29" s="16"/>
       <c r="BL29" s="16"/>
       <c r="BM29" s="16"/>
-      <c r="BN29" s="16"/>
-    </row>
-    <row r="30" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="30" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="47"/>
       <c r="B30" s="15" t="s">
+        <v>63</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D30" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="C30" s="15" t="s">
-        <v>84</v>
-      </c>
-      <c r="D30" s="41" t="s">
-        <v>79</v>
-      </c>
       <c r="E30" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F30" s="51">
         <v>0</v>
@@ -4718,10 +4732,14 @@
       <c r="H30" s="55">
         <v>43869</v>
       </c>
-      <c r="I30" s="54"/>
-      <c r="J30" s="55"/>
-      <c r="K30" s="55"/>
-      <c r="L30" s="62"/>
+      <c r="I30" s="54">
+        <v>43869</v>
+      </c>
+      <c r="J30" s="55">
+        <v>43869</v>
+      </c>
+      <c r="K30" s="62"/>
+      <c r="L30" s="16"/>
       <c r="M30" s="16"/>
       <c r="N30" s="16"/>
       <c r="O30" s="16"/>
@@ -4775,21 +4793,20 @@
       <c r="BK30" s="16"/>
       <c r="BL30" s="16"/>
       <c r="BM30" s="16"/>
-      <c r="BN30" s="16"/>
-    </row>
-    <row r="31" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="47"/>
       <c r="B31" s="15" t="s">
-        <v>72</v>
+        <v>64</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
       <c r="D31" s="41" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="E31" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F31" s="51">
         <v>0</v>
@@ -4800,10 +4817,14 @@
       <c r="H31" s="55">
         <v>43869</v>
       </c>
-      <c r="I31" s="54"/>
-      <c r="J31" s="55"/>
-      <c r="K31" s="55"/>
-      <c r="L31" s="62"/>
+      <c r="I31" s="54">
+        <v>43869</v>
+      </c>
+      <c r="J31" s="55">
+        <v>43869</v>
+      </c>
+      <c r="K31" s="62"/>
+      <c r="L31" s="16"/>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
       <c r="O31" s="16"/>
@@ -4857,21 +4878,20 @@
       <c r="BK31" s="16"/>
       <c r="BL31" s="16"/>
       <c r="BM31" s="16"/>
-      <c r="BN31" s="16"/>
-    </row>
-    <row r="32" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="32" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="47"/>
       <c r="B32" s="15" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
       <c r="D32" s="41" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="E32" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F32" s="51">
         <v>0</v>
@@ -4884,8 +4904,8 @@
       </c>
       <c r="I32" s="54"/>
       <c r="J32" s="55"/>
-      <c r="K32" s="55"/>
-      <c r="L32" s="62"/>
+      <c r="K32" s="62"/>
+      <c r="L32" s="16"/>
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
       <c r="O32" s="16"/>
@@ -4939,21 +4959,20 @@
       <c r="BK32" s="16"/>
       <c r="BL32" s="16"/>
       <c r="BM32" s="16"/>
-      <c r="BN32" s="16"/>
-    </row>
-    <row r="33" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="33" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="47"/>
       <c r="B33" s="15" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="D33" s="41" t="s">
-        <v>69</v>
+        <v>61</v>
       </c>
       <c r="E33" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F33" s="51">
         <v>0</v>
@@ -4964,10 +4983,14 @@
       <c r="H33" s="55">
         <v>43869</v>
       </c>
-      <c r="I33" s="54"/>
-      <c r="J33" s="55"/>
-      <c r="K33" s="55"/>
-      <c r="L33" s="62"/>
+      <c r="I33" s="54">
+        <v>43869</v>
+      </c>
+      <c r="J33" s="55">
+        <v>43869</v>
+      </c>
+      <c r="K33" s="62"/>
+      <c r="L33" s="16"/>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
       <c r="O33" s="16"/>
@@ -5021,21 +5044,20 @@
       <c r="BK33" s="16"/>
       <c r="BL33" s="16"/>
       <c r="BM33" s="16"/>
-      <c r="BN33" s="16"/>
-    </row>
-    <row r="34" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="34" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="47"/>
       <c r="B34" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="C34" s="79" t="s">
-        <v>88</v>
+        <v>68</v>
+      </c>
+      <c r="C34" s="76" t="s">
+        <v>80</v>
       </c>
       <c r="D34" s="41" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="E34" s="41" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="F34" s="51">
         <v>0</v>
@@ -5046,10 +5068,14 @@
       <c r="H34" s="55">
         <v>43873</v>
       </c>
-      <c r="I34" s="54"/>
-      <c r="J34" s="55"/>
-      <c r="K34" s="55"/>
-      <c r="L34" s="62"/>
+      <c r="I34" s="54" t="s">
+        <v>84</v>
+      </c>
+      <c r="J34" s="55" t="s">
+        <v>84</v>
+      </c>
+      <c r="K34" s="62"/>
+      <c r="L34" s="16"/>
       <c r="M34" s="16"/>
       <c r="N34" s="16"/>
       <c r="O34" s="16"/>
@@ -5103,26 +5129,22 @@
       <c r="BK34" s="16"/>
       <c r="BL34" s="16"/>
       <c r="BM34" s="16"/>
-      <c r="BN34" s="16"/>
-    </row>
-    <row r="35" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
-      <c r="B35" s="15" t="s">
-        <v>43</v>
-      </c>
-      <c r="C35" s="15"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="54"/>
-      <c r="H35" s="55"/>
-      <c r="I35" s="54"/>
-      <c r="J35" s="55"/>
-      <c r="K35" s="55"/>
-      <c r="L35" s="62" t="str">
-        <f>IF(OR(ISBLANK(I35),ISBLANK(J35)),"",J35-I35+1)</f>
-        <v/>
-      </c>
+    </row>
+    <row r="35" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="48"/>
+      <c r="B35" s="45" t="s">
+        <v>81</v>
+      </c>
+      <c r="C35" s="45"/>
+      <c r="D35" s="42"/>
+      <c r="E35" s="42"/>
+      <c r="F35" s="52"/>
+      <c r="G35" s="56"/>
+      <c r="H35" s="57"/>
+      <c r="I35" s="56"/>
+      <c r="J35" s="57"/>
+      <c r="K35" s="63"/>
+      <c r="L35" s="16"/>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
       <c r="O35" s="16"/>
@@ -5176,26 +5198,34 @@
       <c r="BK35" s="16"/>
       <c r="BL35" s="16"/>
       <c r="BM35" s="16"/>
-      <c r="BN35" s="16"/>
-    </row>
-    <row r="36" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="48"/>
-      <c r="B36" s="45" t="s">
-        <v>14</v>
-      </c>
-      <c r="C36" s="45"/>
-      <c r="D36" s="42"/>
-      <c r="E36" s="42"/>
-      <c r="F36" s="52"/>
-      <c r="G36" s="56"/>
-      <c r="H36" s="57"/>
-      <c r="I36" s="56"/>
-      <c r="J36" s="57"/>
-      <c r="K36" s="57"/>
-      <c r="L36" s="63" t="str">
-        <f>IF(OR(ISBLANK(I36),ISBLANK(J36)),"",J36-I36+1)</f>
-        <v/>
-      </c>
+    </row>
+    <row r="36" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="47"/>
+      <c r="B36" s="15" t="s">
+        <v>60</v>
+      </c>
+      <c r="C36" s="15" t="s">
+        <v>82</v>
+      </c>
+      <c r="D36" s="41" t="s">
+        <v>61</v>
+      </c>
+      <c r="E36" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="F36" s="51">
+        <v>0</v>
+      </c>
+      <c r="G36" s="54">
+        <v>43872</v>
+      </c>
+      <c r="H36" s="55">
+        <v>43872</v>
+      </c>
+      <c r="I36" s="54"/>
+      <c r="J36" s="55"/>
+      <c r="K36" s="62"/>
+      <c r="L36" s="16"/>
       <c r="M36" s="16"/>
       <c r="N36" s="16"/>
       <c r="O36" s="16"/>
@@ -5249,23 +5279,34 @@
       <c r="BK36" s="16"/>
       <c r="BL36" s="16"/>
       <c r="BM36" s="16"/>
-      <c r="BN36" s="16"/>
-    </row>
-    <row r="37" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="37" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="47"/>
       <c r="B37" s="15" t="s">
-        <v>15</v>
-      </c>
-      <c r="C37" s="15"/>
-      <c r="D37" s="41"/>
-      <c r="E37" s="41"/>
-      <c r="F37" s="51"/>
-      <c r="G37" s="54"/>
-      <c r="H37" s="55"/>
+        <v>63</v>
+      </c>
+      <c r="C37" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="D37" s="41" t="s">
+        <v>71</v>
+      </c>
+      <c r="E37" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="F37" s="51">
+        <v>0</v>
+      </c>
+      <c r="G37" s="54">
+        <v>43873</v>
+      </c>
+      <c r="H37" s="55">
+        <v>43874</v>
+      </c>
       <c r="I37" s="54"/>
       <c r="J37" s="55"/>
-      <c r="K37" s="55"/>
-      <c r="L37" s="62"/>
+      <c r="K37" s="62"/>
+      <c r="L37" s="16"/>
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
       <c r="O37" s="16"/>
@@ -5319,23 +5360,34 @@
       <c r="BK37" s="16"/>
       <c r="BL37" s="16"/>
       <c r="BM37" s="16"/>
-      <c r="BN37" s="16"/>
-    </row>
-    <row r="38" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="38" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="47"/>
       <c r="B38" s="15" t="s">
-        <v>16</v>
-      </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="41"/>
-      <c r="E38" s="41"/>
-      <c r="F38" s="51"/>
-      <c r="G38" s="54"/>
-      <c r="H38" s="55"/>
+        <v>68</v>
+      </c>
+      <c r="C38" s="76" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="E38" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="51">
+        <v>0</v>
+      </c>
+      <c r="G38" s="54">
+        <v>43875</v>
+      </c>
+      <c r="H38" s="55">
+        <v>43875</v>
+      </c>
       <c r="I38" s="54"/>
       <c r="J38" s="55"/>
-      <c r="K38" s="55"/>
-      <c r="L38" s="62"/>
+      <c r="K38" s="62"/>
+      <c r="L38" s="16"/>
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
       <c r="O38" s="16"/>
@@ -5389,13 +5441,10 @@
       <c r="BK38" s="16"/>
       <c r="BL38" s="16"/>
       <c r="BM38" s="16"/>
-      <c r="BN38" s="16"/>
-    </row>
-    <row r="39" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="39" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="47"/>
-      <c r="B39" s="15" t="s">
-        <v>11</v>
-      </c>
+      <c r="B39" s="15"/>
       <c r="C39" s="15"/>
       <c r="D39" s="41"/>
       <c r="E39" s="41"/>
@@ -5404,8 +5453,8 @@
       <c r="H39" s="55"/>
       <c r="I39" s="54"/>
       <c r="J39" s="55"/>
-      <c r="K39" s="55"/>
-      <c r="L39" s="62"/>
+      <c r="K39" s="62"/>
+      <c r="L39" s="16"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
       <c r="O39" s="16"/>
@@ -5459,13 +5508,10 @@
       <c r="BK39" s="16"/>
       <c r="BL39" s="16"/>
       <c r="BM39" s="16"/>
-      <c r="BN39" s="16"/>
-    </row>
-    <row r="40" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="47"/>
-      <c r="B40" s="15" t="s">
-        <v>12</v>
-      </c>
+      <c r="B40" s="15"/>
       <c r="C40" s="15"/>
       <c r="D40" s="41"/>
       <c r="E40" s="41"/>
@@ -5474,8 +5520,8 @@
       <c r="H40" s="55"/>
       <c r="I40" s="54"/>
       <c r="J40" s="55"/>
-      <c r="K40" s="55"/>
-      <c r="L40" s="62"/>
+      <c r="K40" s="62"/>
+      <c r="L40" s="16"/>
       <c r="M40" s="16"/>
       <c r="N40" s="16"/>
       <c r="O40" s="16"/>
@@ -5529,14 +5575,11 @@
       <c r="BK40" s="16"/>
       <c r="BL40" s="16"/>
       <c r="BM40" s="16"/>
-      <c r="BN40" s="16"/>
-    </row>
-    <row r="41" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="41" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="47"/>
-      <c r="B41" s="15" t="s">
-        <v>13</v>
-      </c>
-      <c r="C41" s="15"/>
+      <c r="B41" s="15"/>
+      <c r="C41" s="76"/>
       <c r="D41" s="41"/>
       <c r="E41" s="41"/>
       <c r="F41" s="51"/>
@@ -5544,8 +5587,8 @@
       <c r="H41" s="55"/>
       <c r="I41" s="54"/>
       <c r="J41" s="55"/>
-      <c r="K41" s="55"/>
-      <c r="L41" s="62"/>
+      <c r="K41" s="62"/>
+      <c r="L41" s="16"/>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
       <c r="O41" s="16"/>
@@ -5599,12 +5642,11 @@
       <c r="BK41" s="16"/>
       <c r="BL41" s="16"/>
       <c r="BM41" s="16"/>
-      <c r="BN41" s="16"/>
-    </row>
-    <row r="42" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="47"/>
       <c r="B42" s="15" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C42" s="15"/>
       <c r="D42" s="41"/>
@@ -5614,64 +5656,66 @@
       <c r="H42" s="55"/>
       <c r="I42" s="54"/>
       <c r="J42" s="55"/>
-      <c r="K42" s="55"/>
-      <c r="L42" s="62"/>
-      <c r="M42" s="16"/>
-      <c r="N42" s="16"/>
-      <c r="O42" s="16"/>
-      <c r="P42" s="16"/>
-      <c r="Q42" s="16"/>
-      <c r="R42" s="16"/>
-      <c r="S42" s="16"/>
-      <c r="T42" s="16"/>
-      <c r="U42" s="16"/>
-      <c r="V42" s="16"/>
-      <c r="W42" s="16"/>
-      <c r="X42" s="16"/>
-      <c r="Y42" s="16"/>
-      <c r="Z42" s="16"/>
-      <c r="AA42" s="16"/>
-      <c r="AB42" s="16"/>
-      <c r="AC42" s="16"/>
-      <c r="AD42" s="16"/>
-      <c r="AE42" s="16"/>
-      <c r="AF42" s="16"/>
-      <c r="AG42" s="16"/>
-      <c r="AH42" s="16"/>
-      <c r="AI42" s="16"/>
-      <c r="AJ42" s="16"/>
-      <c r="AK42" s="16"/>
-      <c r="AL42" s="16"/>
-      <c r="AM42" s="16"/>
-      <c r="AN42" s="16"/>
-      <c r="AO42" s="16"/>
-      <c r="AP42" s="16"/>
-      <c r="AQ42" s="16"/>
-      <c r="AR42" s="16"/>
-      <c r="AS42" s="16"/>
-      <c r="AT42" s="16"/>
-      <c r="AU42" s="16"/>
-      <c r="AV42" s="16"/>
-      <c r="AW42" s="16"/>
-      <c r="AX42" s="16"/>
-      <c r="AY42" s="16"/>
-      <c r="AZ42" s="16"/>
-      <c r="BA42" s="16"/>
-      <c r="BB42" s="16"/>
-      <c r="BC42" s="16"/>
-      <c r="BD42" s="16"/>
-      <c r="BE42" s="16"/>
-      <c r="BF42" s="16"/>
-      <c r="BG42" s="16"/>
-      <c r="BH42" s="16"/>
-      <c r="BI42" s="16"/>
-      <c r="BJ42" s="16"/>
-      <c r="BK42" s="16"/>
-      <c r="BL42" s="16"/>
-      <c r="BM42" s="16"/>
-      <c r="BN42" s="16"/>
-    </row>
-    <row r="43" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K42" s="62" t="str">
+        <f>IF(OR(ISBLANK(I42),ISBLANK(J42)),"",J42-I42+1)</f>
+        <v/>
+      </c>
+      <c r="L42" s="18"/>
+      <c r="M42" s="18"/>
+      <c r="N42" s="18"/>
+      <c r="O42" s="18"/>
+      <c r="P42" s="18"/>
+      <c r="Q42" s="18"/>
+      <c r="R42" s="18"/>
+      <c r="S42" s="18"/>
+      <c r="T42" s="18"/>
+      <c r="U42" s="18"/>
+      <c r="V42" s="18"/>
+      <c r="W42" s="18"/>
+      <c r="X42" s="18"/>
+      <c r="Y42" s="18"/>
+      <c r="Z42" s="18"/>
+      <c r="AA42" s="18"/>
+      <c r="AB42" s="18"/>
+      <c r="AC42" s="18"/>
+      <c r="AD42" s="18"/>
+      <c r="AE42" s="18"/>
+      <c r="AF42" s="18"/>
+      <c r="AG42" s="18"/>
+      <c r="AH42" s="18"/>
+      <c r="AI42" s="18"/>
+      <c r="AJ42" s="18"/>
+      <c r="AK42" s="18"/>
+      <c r="AL42" s="18"/>
+      <c r="AM42" s="18"/>
+      <c r="AN42" s="18"/>
+      <c r="AO42" s="18"/>
+      <c r="AP42" s="18"/>
+      <c r="AQ42" s="18"/>
+      <c r="AR42" s="18"/>
+      <c r="AS42" s="18"/>
+      <c r="AT42" s="18"/>
+      <c r="AU42" s="18"/>
+      <c r="AV42" s="18"/>
+      <c r="AW42" s="18"/>
+      <c r="AX42" s="18"/>
+      <c r="AY42" s="18"/>
+      <c r="AZ42" s="18"/>
+      <c r="BA42" s="18"/>
+      <c r="BB42" s="18"/>
+      <c r="BC42" s="18"/>
+      <c r="BD42" s="18"/>
+      <c r="BE42" s="18"/>
+      <c r="BF42" s="18"/>
+      <c r="BG42" s="18"/>
+      <c r="BH42" s="18"/>
+      <c r="BI42" s="18"/>
+      <c r="BJ42" s="18"/>
+      <c r="BK42" s="18"/>
+      <c r="BL42" s="18"/>
+      <c r="BM42" s="18"/>
+    </row>
+    <row r="43" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="47"/>
       <c r="B43" s="44"/>
       <c r="C43" s="44"/>
@@ -5682,67 +5726,12 @@
       <c r="H43" s="55"/>
       <c r="I43" s="54"/>
       <c r="J43" s="55"/>
-      <c r="K43" s="55"/>
-      <c r="L43" s="62" t="str">
+      <c r="K43" s="62" t="str">
         <f>IF(OR(ISBLANK(I43),ISBLANK(J43)),"",J43-I43+1)</f>
         <v/>
       </c>
-      <c r="M43" s="16"/>
-      <c r="N43" s="16"/>
-      <c r="O43" s="16"/>
-      <c r="P43" s="16"/>
-      <c r="Q43" s="16"/>
-      <c r="R43" s="16"/>
-      <c r="S43" s="16"/>
-      <c r="T43" s="16"/>
-      <c r="U43" s="16"/>
-      <c r="V43" s="16"/>
-      <c r="W43" s="16"/>
-      <c r="X43" s="16"/>
-      <c r="Y43" s="16"/>
-      <c r="Z43" s="16"/>
-      <c r="AA43" s="16"/>
-      <c r="AB43" s="16"/>
-      <c r="AC43" s="16"/>
-      <c r="AD43" s="16"/>
-      <c r="AE43" s="16"/>
-      <c r="AF43" s="16"/>
-      <c r="AG43" s="16"/>
-      <c r="AH43" s="16"/>
-      <c r="AI43" s="16"/>
-      <c r="AJ43" s="16"/>
-      <c r="AK43" s="16"/>
-      <c r="AL43" s="16"/>
-      <c r="AM43" s="16"/>
-      <c r="AN43" s="16"/>
-      <c r="AO43" s="16"/>
-      <c r="AP43" s="16"/>
-      <c r="AQ43" s="16"/>
-      <c r="AR43" s="16"/>
-      <c r="AS43" s="16"/>
-      <c r="AT43" s="16"/>
-      <c r="AU43" s="16"/>
-      <c r="AV43" s="16"/>
-      <c r="AW43" s="16"/>
-      <c r="AX43" s="16"/>
-      <c r="AY43" s="16"/>
-      <c r="AZ43" s="16"/>
-      <c r="BA43" s="16"/>
-      <c r="BB43" s="16"/>
-      <c r="BC43" s="16"/>
-      <c r="BD43" s="16"/>
-      <c r="BE43" s="16"/>
-      <c r="BF43" s="16"/>
-      <c r="BG43" s="16"/>
-      <c r="BH43" s="16"/>
-      <c r="BI43" s="16"/>
-      <c r="BJ43" s="16"/>
-      <c r="BK43" s="16"/>
-      <c r="BL43" s="16"/>
-      <c r="BM43" s="16"/>
-      <c r="BN43" s="16"/>
-    </row>
-    <row r="44" spans="1:66" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="47"/>
       <c r="B44" s="44"/>
       <c r="C44" s="44"/>
@@ -5753,67 +5742,9 @@
       <c r="H44" s="55"/>
       <c r="I44" s="54"/>
       <c r="J44" s="55"/>
-      <c r="K44" s="55"/>
-      <c r="L44" s="62" t="str">
-        <f>IF(OR(ISBLANK(I44),ISBLANK(J44)),"",J44-I44+1)</f>
-        <v/>
-      </c>
-      <c r="M44" s="18"/>
-      <c r="N44" s="18"/>
-      <c r="O44" s="18"/>
-      <c r="P44" s="18"/>
-      <c r="Q44" s="18"/>
-      <c r="R44" s="18"/>
-      <c r="S44" s="18"/>
-      <c r="T44" s="18"/>
-      <c r="U44" s="18"/>
-      <c r="V44" s="18"/>
-      <c r="W44" s="18"/>
-      <c r="X44" s="18"/>
-      <c r="Y44" s="18"/>
-      <c r="Z44" s="18"/>
-      <c r="AA44" s="18"/>
-      <c r="AB44" s="18"/>
-      <c r="AC44" s="18"/>
-      <c r="AD44" s="18"/>
-      <c r="AE44" s="18"/>
-      <c r="AF44" s="18"/>
-      <c r="AG44" s="18"/>
-      <c r="AH44" s="18"/>
-      <c r="AI44" s="18"/>
-      <c r="AJ44" s="18"/>
-      <c r="AK44" s="18"/>
-      <c r="AL44" s="18"/>
-      <c r="AM44" s="18"/>
-      <c r="AN44" s="18"/>
-      <c r="AO44" s="18"/>
-      <c r="AP44" s="18"/>
-      <c r="AQ44" s="18"/>
-      <c r="AR44" s="18"/>
-      <c r="AS44" s="18"/>
-      <c r="AT44" s="18"/>
-      <c r="AU44" s="18"/>
-      <c r="AV44" s="18"/>
-      <c r="AW44" s="18"/>
-      <c r="AX44" s="18"/>
-      <c r="AY44" s="18"/>
-      <c r="AZ44" s="18"/>
-      <c r="BA44" s="18"/>
-      <c r="BB44" s="18"/>
-      <c r="BC44" s="18"/>
-      <c r="BD44" s="18"/>
-      <c r="BE44" s="18"/>
-      <c r="BF44" s="18"/>
-      <c r="BG44" s="18"/>
-      <c r="BH44" s="18"/>
-      <c r="BI44" s="18"/>
-      <c r="BJ44" s="18"/>
-      <c r="BK44" s="18"/>
-      <c r="BL44" s="18"/>
-      <c r="BM44" s="18"/>
-      <c r="BN44" s="18"/>
-    </row>
-    <row r="45" spans="1:66" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K44" s="62"/>
+    </row>
+    <row r="45" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="47"/>
       <c r="B45" s="44"/>
       <c r="C45" s="44"/>
@@ -5824,13 +5755,9 @@
       <c r="H45" s="55"/>
       <c r="I45" s="54"/>
       <c r="J45" s="55"/>
-      <c r="K45" s="55"/>
-      <c r="L45" s="62" t="str">
-        <f>IF(OR(ISBLANK(I45),ISBLANK(J45)),"",J45-I45+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="46" spans="1:66" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K45" s="62"/>
+    </row>
+    <row r="46" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="47"/>
       <c r="B46" s="44"/>
       <c r="C46" s="44"/>
@@ -5841,10 +5768,9 @@
       <c r="H46" s="55"/>
       <c r="I46" s="54"/>
       <c r="J46" s="55"/>
-      <c r="K46" s="55"/>
-      <c r="L46" s="62"/>
-    </row>
-    <row r="47" spans="1:66" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K46" s="62"/>
+    </row>
+    <row r="47" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="47"/>
       <c r="B47" s="44"/>
       <c r="C47" s="44"/>
@@ -5855,10 +5781,9 @@
       <c r="H47" s="55"/>
       <c r="I47" s="54"/>
       <c r="J47" s="55"/>
-      <c r="K47" s="55"/>
-      <c r="L47" s="62"/>
-    </row>
-    <row r="48" spans="1:66" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K47" s="62"/>
+    </row>
+    <row r="48" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="47"/>
       <c r="B48" s="44"/>
       <c r="C48" s="44"/>
@@ -5869,10 +5794,9 @@
       <c r="H48" s="55"/>
       <c r="I48" s="54"/>
       <c r="J48" s="55"/>
-      <c r="K48" s="55"/>
-      <c r="L48" s="62"/>
-    </row>
-    <row r="49" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K48" s="62"/>
+    </row>
+    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="47"/>
       <c r="B49" s="44"/>
       <c r="C49" s="44"/>
@@ -5883,71 +5807,41 @@
       <c r="H49" s="55"/>
       <c r="I49" s="54"/>
       <c r="J49" s="55"/>
-      <c r="K49" s="55"/>
-      <c r="L49" s="62"/>
-    </row>
-    <row r="50" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="47"/>
-      <c r="B50" s="44"/>
-      <c r="C50" s="44"/>
-      <c r="D50" s="41"/>
-      <c r="E50" s="41"/>
-      <c r="F50" s="51"/>
-      <c r="G50" s="54"/>
-      <c r="H50" s="55"/>
-      <c r="I50" s="54"/>
-      <c r="J50" s="55"/>
-      <c r="K50" s="55"/>
-      <c r="L50" s="62"/>
-    </row>
-    <row r="51" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="47"/>
-      <c r="B51" s="44"/>
-      <c r="C51" s="44"/>
-      <c r="D51" s="41"/>
-      <c r="E51" s="41"/>
-      <c r="F51" s="51"/>
-      <c r="G51" s="54"/>
-      <c r="H51" s="55"/>
-      <c r="I51" s="54"/>
-      <c r="J51" s="55"/>
-      <c r="K51" s="55"/>
-      <c r="L51" s="62" t="str">
-        <f>IF(OR(ISBLANK(I51),ISBLANK(J51)),"",J51-I51+1)</f>
+      <c r="K49" s="62" t="str">
+        <f>IF(OR(ISBLANK(I49),ISBLANK(J49)),"",J49-I49+1)</f>
         <v/>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="49"/>
-      <c r="B52" s="46" t="s">
-        <v>19</v>
-      </c>
-      <c r="C52" s="46"/>
-      <c r="D52" s="43"/>
-      <c r="E52" s="43"/>
-      <c r="F52" s="53"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="59"/>
-      <c r="I52" s="58"/>
-      <c r="J52" s="59"/>
-      <c r="K52" s="59"/>
-      <c r="L52" s="64" t="str">
-        <f>IF(OR(ISBLANK(I52),ISBLANK(J52)),"",J52-I52+1)</f>
+    <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="49"/>
+      <c r="B50" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C50" s="46"/>
+      <c r="D50" s="43"/>
+      <c r="E50" s="43"/>
+      <c r="F50" s="53"/>
+      <c r="G50" s="58"/>
+      <c r="H50" s="59"/>
+      <c r="I50" s="58"/>
+      <c r="J50" s="59"/>
+      <c r="K50" s="64" t="str">
+        <f>IF(OR(ISBLANK(I50),ISBLANK(J50)),"",J50-I50+1)</f>
         <v/>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A54" s="19"/>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="A55" s="65"/>
+    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A52" s="19"/>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="F9:F16 F19:F25 F35:F52">
-    <cfRule type="dataBar" priority="13">
+  <conditionalFormatting sqref="F9:F16 F19:F25 F43:F50 F36:F37 F39:F41">
+    <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5960,13 +5854,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M7:BN16 M19:BN25 M27:BN44">
-    <cfRule type="expression" dxfId="9" priority="10">
-      <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
+  <conditionalFormatting sqref="L7:BM16 L19:BM25 L27:BM42">
+    <cfRule type="expression" dxfId="18" priority="14">
+      <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="dataBar" priority="6">
+    <cfRule type="dataBar" priority="10">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5979,13 +5873,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M18:BN18">
-    <cfRule type="expression" dxfId="8" priority="5">
-      <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
+  <conditionalFormatting sqref="L18:BM18">
+    <cfRule type="expression" dxfId="17" priority="9">
+      <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F34">
-    <cfRule type="dataBar" priority="4">
+    <cfRule type="dataBar" priority="8">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5999,7 +5893,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="dataBar" priority="3">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6012,36 +5906,111 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M17:BN17">
-    <cfRule type="expression" dxfId="7" priority="2">
-      <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
+  <conditionalFormatting sqref="L17:BM17">
+    <cfRule type="expression" dxfId="16" priority="6">
+      <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M26:BN26">
-    <cfRule type="expression" dxfId="6" priority="1">
-      <formula>AND(TODAY()&gt;=M$6,TODAY()&lt;N$6)</formula>
+  <conditionalFormatting sqref="L26:BM26">
+    <cfRule type="expression" dxfId="15" priority="5">
+      <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M9:BN16 M18:BN25">
-    <cfRule type="expression" dxfId="5" priority="26" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J9,$H9)&gt;=M$6,MIN($I9,$G9)&lt;N$6))</formula>
+  <conditionalFormatting sqref="L9:BM16 L18:BM25">
+    <cfRule type="expression" dxfId="14" priority="30" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J9,$H9)&gt;=L$6,MIN($I9,$G9)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="27">
-      <formula>AND($H9&gt;=M$6,$G9&lt;N$6)</formula>
+    <cfRule type="expression" dxfId="13" priority="31">
+      <formula>AND($H9&gt;=L$6,$G9&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="28" stopIfTrue="1">
-      <formula>AND($J9&gt;=M$6,$I9&lt;N$6)</formula>
+    <cfRule type="expression" dxfId="12" priority="32" stopIfTrue="1">
+      <formula>AND($J9&gt;=L$6,$I9&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="M27:BN44">
-    <cfRule type="expression" dxfId="2" priority="35" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J35,$H35)&gt;=M$6,MIN($I35,$G35)&lt;N$6))</formula>
+  <conditionalFormatting sqref="L37:BM42">
+    <cfRule type="expression" dxfId="11" priority="39" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J45,$H45)&gt;=L$6,MIN($I45,$G45)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="36">
-      <formula>AND($H35&gt;=M$6,$G35&lt;N$6)</formula>
+    <cfRule type="expression" dxfId="10" priority="40">
+      <formula>AND($H45&gt;=L$6,$G45&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="37" stopIfTrue="1">
-      <formula>AND($J35&gt;=M$6,$I35&lt;N$6)</formula>
+    <cfRule type="expression" dxfId="9" priority="41" stopIfTrue="1">
+      <formula>AND($J45&gt;=L$6,$I45&lt;M$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F42">
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="7" tint="0.59999389629810485"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{17210854-4160-4B93-8A92-DED649320E0C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F35">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="7" tint="0.59999389629810485"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{2670910B-E0F6-4EF0-A1D0-239C69147E1F}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L28:BM29 L35:BM36">
+    <cfRule type="expression" dxfId="8" priority="50" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J35,$H35)&gt;=L$6,MIN($I35,$G35)&lt;M$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="51">
+      <formula>AND($H35&gt;=L$6,$G35&lt;M$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="6" priority="52" stopIfTrue="1">
+      <formula>AND($J35&gt;=L$6,$I35&lt;M$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L30:BM30 L27:BM27">
+    <cfRule type="expression" dxfId="5" priority="53" stopIfTrue="1">
+      <formula>NOT(AND(MAX(#REF!,#REF!)&gt;=L$6,MIN(#REF!,#REF!)&lt;M$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="54">
+      <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="55" stopIfTrue="1">
+      <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F38">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="7" tint="0.59999389629810485"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{0DE15629-E527-4F3E-8102-95C9E03B8401}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L31:BM34">
+    <cfRule type="expression" dxfId="2" priority="67" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J37,$H37)&gt;=L$6,MIN($I37,$G37)&lt;M$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="68">
+      <formula>AND($H37&gt;=L$6,$G37&lt;M$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="69" stopIfTrue="1">
+      <formula>AND($J37&gt;=L$6,$I37&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
@@ -6065,13 +6034,13 @@
               <controlPr defaultSize="0" print="0" autoPict="0">
                 <anchor moveWithCells="1">
                   <from>
-                    <xdr:col>11</xdr:col>
+                    <xdr:col>10</xdr:col>
                     <xdr:colOff>552450</xdr:colOff>
                     <xdr:row>3</xdr:row>
                     <xdr:rowOff>171450</xdr:rowOff>
                   </from>
                   <to>
-                    <xdr:col>28</xdr:col>
+                    <xdr:col>27</xdr:col>
                     <xdr:colOff>76200</xdr:colOff>
                     <xdr:row>4</xdr:row>
                     <xdr:rowOff>180975</xdr:rowOff>
@@ -6100,7 +6069,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F9:F16 F19:F25 F35:F52</xm:sqref>
+          <xm:sqref>F9:F16 F19:F25 F43:F50 F36:F37 F39:F41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{35B0E45D-0F80-4816-B43B-129D908BE9C3}">
@@ -6147,6 +6116,51 @@
           </x14:cfRule>
           <xm:sqref>F27</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{17210854-4160-4B93-8A92-DED649320E0C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F42</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{2670910B-E0F6-4EF0-A1D0-239C69147E1F}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F35</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{0DE15629-E527-4F3E-8102-95C9E03B8401}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F38</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -6176,14 +6190,14 @@
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="78" t="s">
-        <v>34</v>
-      </c>
-      <c r="C2" s="78"/>
+      <c r="B2" s="79" t="s">
+        <v>27</v>
+      </c>
+      <c r="C2" s="79"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3" s="23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -6195,7 +6209,7 @@
     </row>
     <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -6209,13 +6223,13 @@
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="21" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="22" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D9" s="5"/>
     </row>
@@ -6236,7 +6250,7 @@
     </row>
     <row r="13" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B13" s="7" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="D13" s="5"/>
     </row>
@@ -6246,14 +6260,14 @@
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="B15" s="7"/>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="D16" s="5"/>
     </row>
@@ -6263,14 +6277,14 @@
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B18" s="7"/>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>37</v>
+        <v>30</v>
       </c>
       <c r="D19" s="5"/>
     </row>
@@ -6287,7 +6301,7 @@
     </row>
     <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -6300,18 +6314,18 @@
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B28" s="68" t="s">
-        <v>45</v>
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -6343,7 +6357,7 @@
     <row r="1" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="24"/>
       <c r="B1" s="25" t="s">
-        <v>41</v>
+        <v>34</v>
       </c>
       <c r="C1" s="26"/>
     </row>
@@ -6355,14 +6369,14 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="24"/>
       <c r="B3" s="28" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="C3" s="26"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="24"/>
       <c r="B4" s="33" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="C4" s="26"/>
     </row>
@@ -6374,7 +6388,7 @@
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="24"/>
       <c r="B6" s="30" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="C6" s="26"/>
     </row>
@@ -6398,7 +6412,7 @@
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="24"/>
       <c r="B10" s="29" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
       <c r="C10" s="26"/>
     </row>
@@ -6410,7 +6424,7 @@
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="24"/>
       <c r="B12" s="29" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C12" s="26"/>
     </row>
@@ -6434,7 +6448,7 @@
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="24"/>
       <c r="B16" s="66" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C16" s="26"/>
     </row>

</xml_diff>

<commit_message>
Updating the CYRS status to released and updating the project plan with start and end dates Signed-off-by: May Alaa <mayelfkiy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="86">
   <si>
     <t>HELP</t>
   </si>
@@ -988,7 +988,65 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="28">
+  <dxfs count="39">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1153,6 +1211,41 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <border>
         <left style="thin">
           <color theme="0" tint="-0.24994659260841701"/>
@@ -1248,15 +1341,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9">
-      <tableStyleElement type="wholeTable" dxfId="27"/>
-      <tableStyleElement type="headerRow" dxfId="26"/>
-      <tableStyleElement type="totalRow" dxfId="25"/>
-      <tableStyleElement type="firstColumn" dxfId="24"/>
-      <tableStyleElement type="lastColumn" dxfId="23"/>
-      <tableStyleElement type="firstRowStripe" dxfId="22"/>
-      <tableStyleElement type="secondRowStripe" dxfId="21"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="20"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="19"/>
+      <tableStyleElement type="wholeTable" dxfId="38"/>
+      <tableStyleElement type="headerRow" dxfId="37"/>
+      <tableStyleElement type="totalRow" dxfId="36"/>
+      <tableStyleElement type="firstColumn" dxfId="35"/>
+      <tableStyleElement type="lastColumn" dxfId="34"/>
+      <tableStyleElement type="firstRowStripe" dxfId="33"/>
+      <tableStyleElement type="secondRowStripe" dxfId="32"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="31"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="30"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1378,7 +1471,7 @@
                   <a14:compatExt spid="_x0000_s6145"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1428,7 +1521,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1483,7 +1576,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1784,10 +1877,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN53"/>
+  <dimension ref="A1:BN52"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A32" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+      <selection activeCell="I38" sqref="I38:J38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -5222,8 +5315,12 @@
       <c r="H36" s="55">
         <v>43872</v>
       </c>
-      <c r="I36" s="54"/>
-      <c r="J36" s="55"/>
+      <c r="I36" s="54">
+        <v>43872</v>
+      </c>
+      <c r="J36" s="55">
+        <v>43872</v>
+      </c>
       <c r="K36" s="62"/>
       <c r="L36" s="16"/>
       <c r="M36" s="16"/>
@@ -5364,11 +5461,9 @@
     <row r="38" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="47"/>
       <c r="B38" s="15" t="s">
-        <v>68</v>
-      </c>
-      <c r="C38" s="76" t="s">
-        <v>80</v>
-      </c>
+        <v>64</v>
+      </c>
+      <c r="C38" s="15"/>
       <c r="D38" s="41" t="s">
         <v>55</v>
       </c>
@@ -5379,13 +5474,17 @@
         <v>0</v>
       </c>
       <c r="G38" s="54">
-        <v>43875</v>
+        <v>43872</v>
       </c>
       <c r="H38" s="55">
-        <v>43875</v>
-      </c>
-      <c r="I38" s="54"/>
-      <c r="J38" s="55"/>
+        <v>43872</v>
+      </c>
+      <c r="I38" s="54">
+        <v>43872</v>
+      </c>
+      <c r="J38" s="55">
+        <v>43872</v>
+      </c>
       <c r="K38" s="62"/>
       <c r="L38" s="16"/>
       <c r="M38" s="16"/>
@@ -5444,13 +5543,27 @@
     </row>
     <row r="39" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="47"/>
-      <c r="B39" s="15"/>
-      <c r="C39" s="15"/>
-      <c r="D39" s="41"/>
-      <c r="E39" s="41"/>
-      <c r="F39" s="51"/>
-      <c r="G39" s="54"/>
-      <c r="H39" s="55"/>
+      <c r="B39" s="15" t="s">
+        <v>68</v>
+      </c>
+      <c r="C39" s="76" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="E39" s="41" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="51">
+        <v>0</v>
+      </c>
+      <c r="G39" s="54">
+        <v>43875</v>
+      </c>
+      <c r="H39" s="55">
+        <v>43875</v>
+      </c>
       <c r="I39" s="54"/>
       <c r="J39" s="55"/>
       <c r="K39" s="62"/>
@@ -5512,7 +5625,7 @@
     <row r="40" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="47"/>
       <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
+      <c r="C40" s="76"/>
       <c r="D40" s="41"/>
       <c r="E40" s="41"/>
       <c r="F40" s="51"/>
@@ -5578,8 +5691,10 @@
     </row>
     <row r="41" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="47"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="76"/>
+      <c r="B41" s="15" t="s">
+        <v>36</v>
+      </c>
+      <c r="C41" s="15"/>
       <c r="D41" s="41"/>
       <c r="E41" s="41"/>
       <c r="F41" s="51"/>
@@ -5587,68 +5702,69 @@
       <c r="H41" s="55"/>
       <c r="I41" s="54"/>
       <c r="J41" s="55"/>
-      <c r="K41" s="62"/>
-      <c r="L41" s="16"/>
-      <c r="M41" s="16"/>
-      <c r="N41" s="16"/>
-      <c r="O41" s="16"/>
-      <c r="P41" s="16"/>
-      <c r="Q41" s="16"/>
-      <c r="R41" s="16"/>
-      <c r="S41" s="16"/>
-      <c r="T41" s="16"/>
-      <c r="U41" s="16"/>
-      <c r="V41" s="16"/>
-      <c r="W41" s="16"/>
-      <c r="X41" s="16"/>
-      <c r="Y41" s="16"/>
-      <c r="Z41" s="16"/>
-      <c r="AA41" s="16"/>
-      <c r="AB41" s="16"/>
-      <c r="AC41" s="16"/>
-      <c r="AD41" s="16"/>
-      <c r="AE41" s="16"/>
-      <c r="AF41" s="16"/>
-      <c r="AG41" s="16"/>
-      <c r="AH41" s="16"/>
-      <c r="AI41" s="16"/>
-      <c r="AJ41" s="16"/>
-      <c r="AK41" s="16"/>
-      <c r="AL41" s="16"/>
-      <c r="AM41" s="16"/>
-      <c r="AN41" s="16"/>
-      <c r="AO41" s="16"/>
-      <c r="AP41" s="16"/>
-      <c r="AQ41" s="16"/>
-      <c r="AR41" s="16"/>
-      <c r="AS41" s="16"/>
-      <c r="AT41" s="16"/>
-      <c r="AU41" s="16"/>
-      <c r="AV41" s="16"/>
-      <c r="AW41" s="16"/>
-      <c r="AX41" s="16"/>
-      <c r="AY41" s="16"/>
-      <c r="AZ41" s="16"/>
-      <c r="BA41" s="16"/>
-      <c r="BB41" s="16"/>
-      <c r="BC41" s="16"/>
-      <c r="BD41" s="16"/>
-      <c r="BE41" s="16"/>
-      <c r="BF41" s="16"/>
-      <c r="BG41" s="16"/>
-      <c r="BH41" s="16"/>
-      <c r="BI41" s="16"/>
-      <c r="BJ41" s="16"/>
-      <c r="BK41" s="16"/>
-      <c r="BL41" s="16"/>
-      <c r="BM41" s="16"/>
-    </row>
-    <row r="42" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="K41" s="62" t="str">
+        <f>IF(OR(ISBLANK(I41),ISBLANK(J41)),"",J41-I41+1)</f>
+        <v/>
+      </c>
+      <c r="L41" s="18"/>
+      <c r="M41" s="18"/>
+      <c r="N41" s="18"/>
+      <c r="O41" s="18"/>
+      <c r="P41" s="18"/>
+      <c r="Q41" s="18"/>
+      <c r="R41" s="18"/>
+      <c r="S41" s="18"/>
+      <c r="T41" s="18"/>
+      <c r="U41" s="18"/>
+      <c r="V41" s="18"/>
+      <c r="W41" s="18"/>
+      <c r="X41" s="18"/>
+      <c r="Y41" s="18"/>
+      <c r="Z41" s="18"/>
+      <c r="AA41" s="18"/>
+      <c r="AB41" s="18"/>
+      <c r="AC41" s="18"/>
+      <c r="AD41" s="18"/>
+      <c r="AE41" s="18"/>
+      <c r="AF41" s="18"/>
+      <c r="AG41" s="18"/>
+      <c r="AH41" s="18"/>
+      <c r="AI41" s="18"/>
+      <c r="AJ41" s="18"/>
+      <c r="AK41" s="18"/>
+      <c r="AL41" s="18"/>
+      <c r="AM41" s="18"/>
+      <c r="AN41" s="18"/>
+      <c r="AO41" s="18"/>
+      <c r="AP41" s="18"/>
+      <c r="AQ41" s="18"/>
+      <c r="AR41" s="18"/>
+      <c r="AS41" s="18"/>
+      <c r="AT41" s="18"/>
+      <c r="AU41" s="18"/>
+      <c r="AV41" s="18"/>
+      <c r="AW41" s="18"/>
+      <c r="AX41" s="18"/>
+      <c r="AY41" s="18"/>
+      <c r="AZ41" s="18"/>
+      <c r="BA41" s="18"/>
+      <c r="BB41" s="18"/>
+      <c r="BC41" s="18"/>
+      <c r="BD41" s="18"/>
+      <c r="BE41" s="18"/>
+      <c r="BF41" s="18"/>
+      <c r="BG41" s="18"/>
+      <c r="BH41" s="18"/>
+      <c r="BI41" s="18"/>
+      <c r="BJ41" s="18"/>
+      <c r="BK41" s="18"/>
+      <c r="BL41" s="18"/>
+      <c r="BM41" s="18"/>
+    </row>
+    <row r="42" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="47"/>
-      <c r="B42" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="C42" s="15"/>
+      <c r="B42" s="44"/>
+      <c r="C42" s="44"/>
       <c r="D42" s="41"/>
       <c r="E42" s="41"/>
       <c r="F42" s="51"/>
@@ -5660,60 +5776,6 @@
         <f>IF(OR(ISBLANK(I42),ISBLANK(J42)),"",J42-I42+1)</f>
         <v/>
       </c>
-      <c r="L42" s="18"/>
-      <c r="M42" s="18"/>
-      <c r="N42" s="18"/>
-      <c r="O42" s="18"/>
-      <c r="P42" s="18"/>
-      <c r="Q42" s="18"/>
-      <c r="R42" s="18"/>
-      <c r="S42" s="18"/>
-      <c r="T42" s="18"/>
-      <c r="U42" s="18"/>
-      <c r="V42" s="18"/>
-      <c r="W42" s="18"/>
-      <c r="X42" s="18"/>
-      <c r="Y42" s="18"/>
-      <c r="Z42" s="18"/>
-      <c r="AA42" s="18"/>
-      <c r="AB42" s="18"/>
-      <c r="AC42" s="18"/>
-      <c r="AD42" s="18"/>
-      <c r="AE42" s="18"/>
-      <c r="AF42" s="18"/>
-      <c r="AG42" s="18"/>
-      <c r="AH42" s="18"/>
-      <c r="AI42" s="18"/>
-      <c r="AJ42" s="18"/>
-      <c r="AK42" s="18"/>
-      <c r="AL42" s="18"/>
-      <c r="AM42" s="18"/>
-      <c r="AN42" s="18"/>
-      <c r="AO42" s="18"/>
-      <c r="AP42" s="18"/>
-      <c r="AQ42" s="18"/>
-      <c r="AR42" s="18"/>
-      <c r="AS42" s="18"/>
-      <c r="AT42" s="18"/>
-      <c r="AU42" s="18"/>
-      <c r="AV42" s="18"/>
-      <c r="AW42" s="18"/>
-      <c r="AX42" s="18"/>
-      <c r="AY42" s="18"/>
-      <c r="AZ42" s="18"/>
-      <c r="BA42" s="18"/>
-      <c r="BB42" s="18"/>
-      <c r="BC42" s="18"/>
-      <c r="BD42" s="18"/>
-      <c r="BE42" s="18"/>
-      <c r="BF42" s="18"/>
-      <c r="BG42" s="18"/>
-      <c r="BH42" s="18"/>
-      <c r="BI42" s="18"/>
-      <c r="BJ42" s="18"/>
-      <c r="BK42" s="18"/>
-      <c r="BL42" s="18"/>
-      <c r="BM42" s="18"/>
     </row>
     <row r="43" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="47"/>
@@ -5726,10 +5788,7 @@
       <c r="H43" s="55"/>
       <c r="I43" s="54"/>
       <c r="J43" s="55"/>
-      <c r="K43" s="62" t="str">
-        <f>IF(OR(ISBLANK(I43),ISBLANK(J43)),"",J43-I43+1)</f>
-        <v/>
-      </c>
+      <c r="K43" s="62"/>
     </row>
     <row r="44" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="47"/>
@@ -5794,54 +5853,41 @@
       <c r="H48" s="55"/>
       <c r="I48" s="54"/>
       <c r="J48" s="55"/>
-      <c r="K48" s="62"/>
+      <c r="K48" s="62" t="str">
+        <f>IF(OR(ISBLANK(I48),ISBLANK(J48)),"",J48-I48+1)</f>
+        <v/>
+      </c>
     </row>
     <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="47"/>
-      <c r="B49" s="44"/>
-      <c r="C49" s="44"/>
-      <c r="D49" s="41"/>
-      <c r="E49" s="41"/>
-      <c r="F49" s="51"/>
-      <c r="G49" s="54"/>
-      <c r="H49" s="55"/>
-      <c r="I49" s="54"/>
-      <c r="J49" s="55"/>
-      <c r="K49" s="62" t="str">
+      <c r="A49" s="49"/>
+      <c r="B49" s="46" t="s">
+        <v>12</v>
+      </c>
+      <c r="C49" s="46"/>
+      <c r="D49" s="43"/>
+      <c r="E49" s="43"/>
+      <c r="F49" s="53"/>
+      <c r="G49" s="58"/>
+      <c r="H49" s="59"/>
+      <c r="I49" s="58"/>
+      <c r="J49" s="59"/>
+      <c r="K49" s="64" t="str">
         <f>IF(OR(ISBLANK(I49),ISBLANK(J49)),"",J49-I49+1)</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="49"/>
-      <c r="B50" s="46" t="s">
-        <v>12</v>
-      </c>
-      <c r="C50" s="46"/>
-      <c r="D50" s="43"/>
-      <c r="E50" s="43"/>
-      <c r="F50" s="53"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="59"/>
-      <c r="I50" s="58"/>
-      <c r="J50" s="59"/>
-      <c r="K50" s="64" t="str">
-        <f>IF(OR(ISBLANK(I50),ISBLANK(J50)),"",J50-I50+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="52" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A52" s="19"/>
-    </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A53" s="65"/>
+    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="19"/>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="F9:F16 F19:F25 F43:F50 F36:F37 F39:F41">
-    <cfRule type="dataBar" priority="17">
+  <conditionalFormatting sqref="F9:F16 F19:F25 F42:F49 F36:F37 F40">
+    <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5854,13 +5900,13 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7:BM16 L19:BM25 L27:BM42">
-    <cfRule type="expression" dxfId="18" priority="14">
+  <conditionalFormatting sqref="L7:BM16 L19:BM25 L27:BM37 L39:BM41">
+    <cfRule type="expression" dxfId="25" priority="19">
       <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F18">
-    <cfRule type="dataBar" priority="10">
+    <cfRule type="dataBar" priority="15">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5874,12 +5920,12 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:BM18">
-    <cfRule type="expression" dxfId="17" priority="9">
+    <cfRule type="expression" dxfId="24" priority="14">
       <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F28:F34">
-    <cfRule type="dataBar" priority="8">
+    <cfRule type="dataBar" priority="13">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5893,7 +5939,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F27">
-    <cfRule type="dataBar" priority="7">
+    <cfRule type="dataBar" priority="12">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5907,39 +5953,39 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:BM17">
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="23" priority="11">
       <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26:BM26">
-    <cfRule type="expression" dxfId="15" priority="5">
+    <cfRule type="expression" dxfId="22" priority="10">
       <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:BM16 L18:BM25">
-    <cfRule type="expression" dxfId="14" priority="30" stopIfTrue="1">
+    <cfRule type="expression" dxfId="21" priority="35" stopIfTrue="1">
       <formula>NOT(AND(MAX($J9,$H9)&gt;=L$6,MIN($I9,$G9)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="31">
+    <cfRule type="expression" dxfId="20" priority="36">
       <formula>AND($H9&gt;=L$6,$G9&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="12" priority="32" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="37" stopIfTrue="1">
       <formula>AND($J9&gt;=L$6,$I9&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L37:BM42">
-    <cfRule type="expression" dxfId="11" priority="39" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J45,$H45)&gt;=L$6,MIN($I45,$G45)&lt;M$6))</formula>
+  <conditionalFormatting sqref="L40:BM41 L38:BM38">
+    <cfRule type="expression" dxfId="18" priority="44" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J46,$H46)&gt;=L$6,MIN($I46,$G46)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="40">
-      <formula>AND($H45&gt;=L$6,$G45&lt;M$6)</formula>
+    <cfRule type="expression" dxfId="17" priority="45">
+      <formula>AND($H46&gt;=L$6,$G46&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="9" priority="41" stopIfTrue="1">
-      <formula>AND($J45&gt;=L$6,$I45&lt;M$6)</formula>
+    <cfRule type="expression" dxfId="16" priority="46" stopIfTrue="1">
+      <formula>AND($J46&gt;=L$6,$I46&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F42">
-    <cfRule type="dataBar" priority="4">
+  <conditionalFormatting sqref="F41">
+    <cfRule type="dataBar" priority="9">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5953,7 +5999,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F35">
-    <cfRule type="dataBar" priority="2">
+    <cfRule type="dataBar" priority="7">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -5966,30 +6012,30 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L28:BM29 L35:BM36">
-    <cfRule type="expression" dxfId="8" priority="50" stopIfTrue="1">
+  <conditionalFormatting sqref="L28:BM29 L37:BM37 L32:BM32">
+    <cfRule type="expression" dxfId="15" priority="55" stopIfTrue="1">
       <formula>NOT(AND(MAX($J35,$H35)&gt;=L$6,MIN($I35,$G35)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="51">
+    <cfRule type="expression" dxfId="14" priority="56">
       <formula>AND($H35&gt;=L$6,$G35&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="13" priority="57" stopIfTrue="1">
       <formula>AND($J35&gt;=L$6,$I35&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30:BM30 L27:BM27">
-    <cfRule type="expression" dxfId="5" priority="53" stopIfTrue="1">
+    <cfRule type="expression" dxfId="12" priority="58" stopIfTrue="1">
       <formula>NOT(AND(MAX(#REF!,#REF!)&gt;=L$6,MIN(#REF!,#REF!)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="54">
+    <cfRule type="expression" dxfId="11" priority="59">
       <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="60" stopIfTrue="1">
       <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F38">
-    <cfRule type="dataBar" priority="1">
+  <conditionalFormatting sqref="F39">
+    <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
         <cfvo type="num" val="1"/>
@@ -6002,15 +6048,56 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L31:BM34">
-    <cfRule type="expression" dxfId="2" priority="67" stopIfTrue="1">
+  <conditionalFormatting sqref="L31:BM31 L35:BM36 L39:BM39">
+    <cfRule type="expression" dxfId="9" priority="72" stopIfTrue="1">
       <formula>NOT(AND(MAX($J37,$H37)&gt;=L$6,MIN($I37,$G37)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="68">
+    <cfRule type="expression" dxfId="8" priority="73">
       <formula>AND($H37&gt;=L$6,$G37&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="69" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="74" stopIfTrue="1">
       <formula>AND($J37&gt;=L$6,$I37&lt;M$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F38">
+    <cfRule type="dataBar" priority="2">
+      <dataBar>
+        <cfvo type="num" val="0"/>
+        <cfvo type="num" val="1"/>
+        <color theme="7" tint="0.59999389629810485"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{413F1A60-1EE0-4F7F-888D-36D618AEFC7A}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L38:BM38">
+    <cfRule type="expression" dxfId="6" priority="1">
+      <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L34:BM34">
+    <cfRule type="expression" dxfId="5" priority="95" stopIfTrue="1">
+      <formula>NOT(AND(MAX(#REF!,#REF!)&gt;=L$6,MIN(#REF!,#REF!)&lt;M$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="96">
+      <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="97" stopIfTrue="1">
+      <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L33:BM33">
+    <cfRule type="expression" dxfId="2" priority="116" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J38,$H38)&gt;=L$6,MIN($I38,$G38)&lt;M$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="117">
+      <formula>AND($H38&gt;=L$6,$G38&lt;M$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="118" stopIfTrue="1">
+      <formula>AND($J38&gt;=L$6,$I38&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
@@ -6069,7 +6156,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F9:F16 F19:F25 F43:F50 F36:F37 F39:F41</xm:sqref>
+          <xm:sqref>F9:F16 F19:F25 F42:F49 F36:F37 F40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{35B0E45D-0F80-4816-B43B-129D908BE9C3}">
@@ -6129,7 +6216,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F42</xm:sqref>
+          <xm:sqref>F41</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{2670910B-E0F6-4EF0-A1D0-239C69147E1F}">
@@ -6148,6 +6235,21 @@
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{0DE15629-E527-4F3E-8102-95C9E03B8401}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="num">
+                <xm:f>0</xm:f>
+              </x14:cfvo>
+              <x14:cfvo type="num">
+                <xm:f>1</xm:f>
+              </x14:cfvo>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>F39</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{413F1A60-1EE0-4F7F-888D-36D618AEFC7A}">
             <x14:dataBar minLength="0" maxLength="100" gradient="0">
               <x14:cfvo type="num">
                 <xm:f>0</xm:f>

</xml_diff>

<commit_message>
Updating actual start and end dates in project plan for week 3 update 2 Signed-off-by: May Alaa <mayelfkiy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="86">
   <si>
     <t>HELP</t>
   </si>
@@ -280,9 +280,6 @@
     <t>Cross review on the HSI</t>
   </si>
   <si>
-    <t>Updating RTM to reflect modified requirements</t>
-  </si>
-  <si>
     <t>Week 3 Update</t>
   </si>
   <si>
@@ -290,9 +287,6 @@
   </si>
   <si>
     <t>2/8//20</t>
-  </si>
-  <si>
-    <t>_</t>
   </si>
   <si>
     <t>Solve issues described in point 8,9,10,11 in the review sheet</t>
@@ -991,123 +985,7 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
-  <dxfs count="79">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="40">
     <dxf>
       <fill>
         <patternFill>
@@ -1173,215 +1051,6 @@
         </left>
         <right style="thin">
           <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
         </right>
         <vertical/>
         <horizontal/>
@@ -1681,15 +1350,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9">
-      <tableStyleElement type="wholeTable" dxfId="78"/>
-      <tableStyleElement type="headerRow" dxfId="77"/>
-      <tableStyleElement type="totalRow" dxfId="76"/>
-      <tableStyleElement type="firstColumn" dxfId="75"/>
-      <tableStyleElement type="lastColumn" dxfId="74"/>
-      <tableStyleElement type="firstRowStripe" dxfId="73"/>
-      <tableStyleElement type="secondRowStripe" dxfId="72"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="71"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="70"/>
+      <tableStyleElement type="wholeTable" dxfId="39"/>
+      <tableStyleElement type="headerRow" dxfId="38"/>
+      <tableStyleElement type="totalRow" dxfId="37"/>
+      <tableStyleElement type="firstColumn" dxfId="36"/>
+      <tableStyleElement type="lastColumn" dxfId="35"/>
+      <tableStyleElement type="firstRowStripe" dxfId="34"/>
+      <tableStyleElement type="secondRowStripe" dxfId="33"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="32"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="31"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -2217,10 +1886,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BN52"/>
+  <dimension ref="A1:BN50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A34" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A37" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A42" sqref="A42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -4996,10 +4665,10 @@
         <v>43869</v>
       </c>
       <c r="I28" s="53" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J28" s="54" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="K28" s="61"/>
       <c r="L28" s="16"/>
@@ -5479,35 +5148,19 @@
       <c r="BM33" s="16"/>
     </row>
     <row r="34" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="46"/>
-      <c r="B34" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C34" s="75" t="s">
+      <c r="A34" s="47"/>
+      <c r="B34" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="E34" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="F34" s="50">
-        <v>0</v>
-      </c>
-      <c r="G34" s="53">
-        <v>43873</v>
-      </c>
-      <c r="H34" s="54">
-        <v>43873</v>
-      </c>
-      <c r="I34" s="53" t="s">
-        <v>83</v>
-      </c>
-      <c r="J34" s="54" t="s">
-        <v>83</v>
-      </c>
-      <c r="K34" s="61"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="41"/>
+      <c r="E34" s="41"/>
+      <c r="F34" s="51"/>
+      <c r="G34" s="55"/>
+      <c r="H34" s="56"/>
+      <c r="I34" s="55"/>
+      <c r="J34" s="56"/>
+      <c r="K34" s="62"/>
       <c r="L34" s="16"/>
       <c r="M34" s="16"/>
       <c r="N34" s="16"/>
@@ -5564,19 +5217,35 @@
       <c r="BM34" s="16"/>
     </row>
     <row r="35" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="47"/>
-      <c r="B35" s="44" t="s">
+      <c r="A35" s="46"/>
+      <c r="B35" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C35" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C35" s="44"/>
-      <c r="D35" s="41"/>
-      <c r="E35" s="41"/>
-      <c r="F35" s="51"/>
-      <c r="G35" s="55"/>
-      <c r="H35" s="56"/>
-      <c r="I35" s="55"/>
-      <c r="J35" s="56"/>
-      <c r="K35" s="62"/>
+      <c r="D35" s="40" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="50">
+        <v>0</v>
+      </c>
+      <c r="G35" s="53">
+        <v>43872</v>
+      </c>
+      <c r="H35" s="54">
+        <v>43872</v>
+      </c>
+      <c r="I35" s="53">
+        <v>43872</v>
+      </c>
+      <c r="J35" s="54">
+        <v>43872</v>
+      </c>
+      <c r="K35" s="61"/>
       <c r="L35" s="16"/>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
@@ -5635,13 +5304,13 @@
     <row r="36" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="46"/>
       <c r="B36" s="15" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="C36" s="15" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D36" s="40" t="s">
-        <v>60</v>
+        <v>70</v>
       </c>
       <c r="E36" s="40" t="s">
         <v>57</v>
@@ -5650,17 +5319,13 @@
         <v>0</v>
       </c>
       <c r="G36" s="53">
-        <v>43872</v>
+        <v>43873</v>
       </c>
       <c r="H36" s="54">
-        <v>43872</v>
-      </c>
-      <c r="I36" s="53">
-        <v>43872</v>
-      </c>
-      <c r="J36" s="54">
-        <v>43872</v>
-      </c>
+        <v>43874</v>
+      </c>
+      <c r="I36" s="53"/>
+      <c r="J36" s="54"/>
       <c r="K36" s="61"/>
       <c r="L36" s="16"/>
       <c r="M36" s="16"/>
@@ -5720,13 +5385,11 @@
     <row r="37" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="46"/>
       <c r="B37" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="C37" s="15" t="s">
-        <v>84</v>
-      </c>
+        <v>63</v>
+      </c>
+      <c r="C37" s="15"/>
       <c r="D37" s="40" t="s">
-        <v>70</v>
+        <v>54</v>
       </c>
       <c r="E37" s="40" t="s">
         <v>57</v>
@@ -5735,13 +5398,17 @@
         <v>0</v>
       </c>
       <c r="G37" s="53">
-        <v>43873</v>
+        <v>43872</v>
       </c>
       <c r="H37" s="54">
-        <v>43874</v>
-      </c>
-      <c r="I37" s="53"/>
-      <c r="J37" s="54"/>
+        <v>43872</v>
+      </c>
+      <c r="I37" s="53">
+        <v>43872</v>
+      </c>
+      <c r="J37" s="54">
+        <v>43872</v>
+      </c>
       <c r="K37" s="61"/>
       <c r="L37" s="16"/>
       <c r="M37" s="16"/>
@@ -5799,33 +5466,19 @@
       <c r="BM37" s="16"/>
     </row>
     <row r="38" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="46"/>
-      <c r="B38" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="C38" s="15"/>
-      <c r="D38" s="40" t="s">
-        <v>54</v>
-      </c>
-      <c r="E38" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="F38" s="50">
-        <v>0</v>
-      </c>
-      <c r="G38" s="53">
-        <v>43872</v>
-      </c>
-      <c r="H38" s="54">
-        <v>43872</v>
-      </c>
-      <c r="I38" s="53">
-        <v>43872</v>
-      </c>
-      <c r="J38" s="54">
-        <v>43872</v>
-      </c>
-      <c r="K38" s="61"/>
+      <c r="A38" s="47"/>
+      <c r="B38" s="44" t="s">
+        <v>83</v>
+      </c>
+      <c r="C38" s="44"/>
+      <c r="D38" s="41"/>
+      <c r="E38" s="41"/>
+      <c r="F38" s="51"/>
+      <c r="G38" s="55"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="55"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="62"/>
       <c r="L38" s="16"/>
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
@@ -5884,13 +5537,13 @@
     <row r="39" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="46"/>
       <c r="B39" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C39" s="75" t="s">
-        <v>79</v>
+        <v>59</v>
+      </c>
+      <c r="C39" s="15" t="s">
+        <v>84</v>
       </c>
       <c r="D39" s="40" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
       <c r="E39" s="40" t="s">
         <v>57</v>
@@ -5899,13 +5552,17 @@
         <v>0</v>
       </c>
       <c r="G39" s="53">
-        <v>43875</v>
+        <v>43880</v>
       </c>
       <c r="H39" s="54">
-        <v>43875</v>
-      </c>
-      <c r="I39" s="53"/>
-      <c r="J39" s="54"/>
+        <v>43881</v>
+      </c>
+      <c r="I39" s="53">
+        <v>43880</v>
+      </c>
+      <c r="J39" s="54">
+        <v>43881</v>
+      </c>
       <c r="K39" s="61"/>
       <c r="L39" s="16"/>
       <c r="M39" s="16"/>
@@ -5963,19 +5620,35 @@
       <c r="BM39" s="16"/>
     </row>
     <row r="40" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="47"/>
-      <c r="B40" s="44" t="s">
+      <c r="A40" s="46"/>
+      <c r="B40" s="15" t="s">
+        <v>61</v>
+      </c>
+      <c r="C40" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="C40" s="44"/>
-      <c r="D40" s="41"/>
-      <c r="E40" s="41"/>
-      <c r="F40" s="51"/>
-      <c r="G40" s="55"/>
-      <c r="H40" s="56"/>
-      <c r="I40" s="55"/>
-      <c r="J40" s="56"/>
-      <c r="K40" s="62"/>
+      <c r="D40" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="E40" s="40" t="s">
+        <v>57</v>
+      </c>
+      <c r="F40" s="50">
+        <v>0</v>
+      </c>
+      <c r="G40" s="53">
+        <v>43880</v>
+      </c>
+      <c r="H40" s="54">
+        <v>43881</v>
+      </c>
+      <c r="I40" s="53">
+        <v>43880</v>
+      </c>
+      <c r="J40" s="54">
+        <v>43881</v>
+      </c>
+      <c r="K40" s="61"/>
       <c r="L40" s="16"/>
       <c r="M40" s="16"/>
       <c r="N40" s="16"/>
@@ -6033,27 +5706,13 @@
     </row>
     <row r="41" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="46"/>
-      <c r="B41" s="15" t="s">
-        <v>59</v>
-      </c>
-      <c r="C41" s="15" t="s">
-        <v>86</v>
-      </c>
-      <c r="D41" s="40" t="s">
-        <v>60</v>
-      </c>
-      <c r="E41" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="F41" s="50">
-        <v>0</v>
-      </c>
-      <c r="G41" s="53">
-        <v>43880</v>
-      </c>
-      <c r="H41" s="54">
-        <v>43881</v>
-      </c>
+      <c r="B41" s="15"/>
+      <c r="C41" s="15"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="50"/>
+      <c r="G41" s="53"/>
+      <c r="H41" s="54"/>
       <c r="I41" s="53"/>
       <c r="J41" s="54"/>
       <c r="K41" s="61"/>
@@ -6114,27 +5773,13 @@
     </row>
     <row r="42" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="46"/>
-      <c r="B42" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="C42" s="15" t="s">
-        <v>87</v>
-      </c>
-      <c r="D42" s="40" t="s">
-        <v>51</v>
-      </c>
-      <c r="E42" s="40" t="s">
-        <v>57</v>
-      </c>
-      <c r="F42" s="50">
-        <v>0</v>
-      </c>
-      <c r="G42" s="53">
-        <v>43880</v>
-      </c>
-      <c r="H42" s="54">
-        <v>43881</v>
-      </c>
+      <c r="B42" s="15"/>
+      <c r="C42" s="75"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="50"/>
+      <c r="G42" s="53"/>
+      <c r="H42" s="54"/>
       <c r="I42" s="53"/>
       <c r="J42" s="54"/>
       <c r="K42" s="61"/>
@@ -6193,10 +5838,10 @@
       <c r="BL42" s="16"/>
       <c r="BM42" s="16"/>
     </row>
-    <row r="43" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="46"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
+      <c r="B43" s="43"/>
+      <c r="C43" s="43"/>
       <c r="D43" s="40"/>
       <c r="E43" s="40"/>
       <c r="F43" s="50"/>
@@ -6205,65 +5850,11 @@
       <c r="I43" s="53"/>
       <c r="J43" s="54"/>
       <c r="K43" s="61"/>
-      <c r="L43" s="16"/>
-      <c r="M43" s="16"/>
-      <c r="N43" s="16"/>
-      <c r="O43" s="16"/>
-      <c r="P43" s="16"/>
-      <c r="Q43" s="16"/>
-      <c r="R43" s="16"/>
-      <c r="S43" s="16"/>
-      <c r="T43" s="16"/>
-      <c r="U43" s="16"/>
-      <c r="V43" s="16"/>
-      <c r="W43" s="16"/>
-      <c r="X43" s="16"/>
-      <c r="Y43" s="16"/>
-      <c r="Z43" s="16"/>
-      <c r="AA43" s="16"/>
-      <c r="AB43" s="16"/>
-      <c r="AC43" s="16"/>
-      <c r="AD43" s="16"/>
-      <c r="AE43" s="16"/>
-      <c r="AF43" s="16"/>
-      <c r="AG43" s="16"/>
-      <c r="AH43" s="16"/>
-      <c r="AI43" s="16"/>
-      <c r="AJ43" s="16"/>
-      <c r="AK43" s="16"/>
-      <c r="AL43" s="16"/>
-      <c r="AM43" s="16"/>
-      <c r="AN43" s="16"/>
-      <c r="AO43" s="16"/>
-      <c r="AP43" s="16"/>
-      <c r="AQ43" s="16"/>
-      <c r="AR43" s="16"/>
-      <c r="AS43" s="16"/>
-      <c r="AT43" s="16"/>
-      <c r="AU43" s="16"/>
-      <c r="AV43" s="16"/>
-      <c r="AW43" s="16"/>
-      <c r="AX43" s="16"/>
-      <c r="AY43" s="16"/>
-      <c r="AZ43" s="16"/>
-      <c r="BA43" s="16"/>
-      <c r="BB43" s="16"/>
-      <c r="BC43" s="16"/>
-      <c r="BD43" s="16"/>
-      <c r="BE43" s="16"/>
-      <c r="BF43" s="16"/>
-      <c r="BG43" s="16"/>
-      <c r="BH43" s="16"/>
-      <c r="BI43" s="16"/>
-      <c r="BJ43" s="16"/>
-      <c r="BK43" s="16"/>
-      <c r="BL43" s="16"/>
-      <c r="BM43" s="16"/>
-    </row>
-    <row r="44" spans="1:65" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="46"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="75"/>
+      <c r="B44" s="43"/>
+      <c r="C44" s="43"/>
       <c r="D44" s="40"/>
       <c r="E44" s="40"/>
       <c r="F44" s="50"/>
@@ -6272,60 +5863,6 @@
       <c r="I44" s="53"/>
       <c r="J44" s="54"/>
       <c r="K44" s="61"/>
-      <c r="L44" s="16"/>
-      <c r="M44" s="16"/>
-      <c r="N44" s="16"/>
-      <c r="O44" s="16"/>
-      <c r="P44" s="16"/>
-      <c r="Q44" s="16"/>
-      <c r="R44" s="16"/>
-      <c r="S44" s="16"/>
-      <c r="T44" s="16"/>
-      <c r="U44" s="16"/>
-      <c r="V44" s="16"/>
-      <c r="W44" s="16"/>
-      <c r="X44" s="16"/>
-      <c r="Y44" s="16"/>
-      <c r="Z44" s="16"/>
-      <c r="AA44" s="16"/>
-      <c r="AB44" s="16"/>
-      <c r="AC44" s="16"/>
-      <c r="AD44" s="16"/>
-      <c r="AE44" s="16"/>
-      <c r="AF44" s="16"/>
-      <c r="AG44" s="16"/>
-      <c r="AH44" s="16"/>
-      <c r="AI44" s="16"/>
-      <c r="AJ44" s="16"/>
-      <c r="AK44" s="16"/>
-      <c r="AL44" s="16"/>
-      <c r="AM44" s="16"/>
-      <c r="AN44" s="16"/>
-      <c r="AO44" s="16"/>
-      <c r="AP44" s="16"/>
-      <c r="AQ44" s="16"/>
-      <c r="AR44" s="16"/>
-      <c r="AS44" s="16"/>
-      <c r="AT44" s="16"/>
-      <c r="AU44" s="16"/>
-      <c r="AV44" s="16"/>
-      <c r="AW44" s="16"/>
-      <c r="AX44" s="16"/>
-      <c r="AY44" s="16"/>
-      <c r="AZ44" s="16"/>
-      <c r="BA44" s="16"/>
-      <c r="BB44" s="16"/>
-      <c r="BC44" s="16"/>
-      <c r="BD44" s="16"/>
-      <c r="BE44" s="16"/>
-      <c r="BF44" s="16"/>
-      <c r="BG44" s="16"/>
-      <c r="BH44" s="16"/>
-      <c r="BI44" s="16"/>
-      <c r="BJ44" s="16"/>
-      <c r="BK44" s="16"/>
-      <c r="BL44" s="16"/>
-      <c r="BM44" s="16"/>
     </row>
     <row r="45" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="46"/>
@@ -6351,66 +5888,40 @@
       <c r="H46" s="54"/>
       <c r="I46" s="53"/>
       <c r="J46" s="54"/>
-      <c r="K46" s="61"/>
+      <c r="K46" s="61" t="str">
+        <f>IF(OR(ISBLANK(I46),ISBLANK(J46)),"",J46-I46+1)</f>
+        <v/>
+      </c>
     </row>
     <row r="47" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="46"/>
-      <c r="B47" s="43"/>
-      <c r="C47" s="43"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="40"/>
-      <c r="F47" s="50"/>
-      <c r="G47" s="53"/>
-      <c r="H47" s="54"/>
-      <c r="I47" s="53"/>
-      <c r="J47" s="54"/>
-      <c r="K47" s="61"/>
-    </row>
-    <row r="48" spans="1:65" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="46"/>
-      <c r="B48" s="43"/>
-      <c r="C48" s="43"/>
-      <c r="D48" s="40"/>
-      <c r="E48" s="40"/>
-      <c r="F48" s="50"/>
-      <c r="G48" s="53"/>
-      <c r="H48" s="54"/>
-      <c r="I48" s="53"/>
-      <c r="J48" s="54"/>
-      <c r="K48" s="61" t="str">
-        <f>IF(OR(ISBLANK(I48),ISBLANK(J48)),"",J48-I48+1)</f>
+      <c r="A47" s="48"/>
+      <c r="B47" s="45" t="s">
+        <v>12</v>
+      </c>
+      <c r="C47" s="45"/>
+      <c r="D47" s="42"/>
+      <c r="E47" s="42"/>
+      <c r="F47" s="52"/>
+      <c r="G47" s="57"/>
+      <c r="H47" s="58"/>
+      <c r="I47" s="57"/>
+      <c r="J47" s="58"/>
+      <c r="K47" s="63" t="str">
+        <f>IF(OR(ISBLANK(I47),ISBLANK(J47)),"",J47-I47+1)</f>
         <v/>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="48"/>
-      <c r="B49" s="45" t="s">
-        <v>12</v>
-      </c>
-      <c r="C49" s="45"/>
-      <c r="D49" s="42"/>
-      <c r="E49" s="42"/>
-      <c r="F49" s="52"/>
-      <c r="G49" s="57"/>
-      <c r="H49" s="58"/>
-      <c r="I49" s="57"/>
-      <c r="J49" s="58"/>
-      <c r="K49" s="63" t="str">
-        <f>IF(OR(ISBLANK(I49),ISBLANK(J49)),"",J49-I49+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.25">
-      <c r="A51" s="18"/>
-    </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A52" s="64"/>
+    <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A49" s="18"/>
+    </row>
+    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A50" s="64"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="G4:H4"/>
   </mergeCells>
-  <conditionalFormatting sqref="F9:F16 F19:F25 F45:F49 F36:F37">
+  <conditionalFormatting sqref="F9:F16 F19:F25 F43:F47 F35:F36">
     <cfRule type="dataBar" priority="37">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6424,8 +5935,8 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L7:BM16 L19:BM25 L27:BM37 L39:BM39">
-    <cfRule type="expression" dxfId="69" priority="34">
+  <conditionalFormatting sqref="L7:BM16 L19:BM25 L27:BM36">
+    <cfRule type="expression" dxfId="30" priority="34">
       <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -6444,11 +5955,11 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L18:BM18">
-    <cfRule type="expression" dxfId="68" priority="29">
+    <cfRule type="expression" dxfId="29" priority="29">
       <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F28:F34">
+  <conditionalFormatting sqref="F28:F33">
     <cfRule type="dataBar" priority="28">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6477,38 +5988,38 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L17:BM17">
-    <cfRule type="expression" dxfId="67" priority="26">
+    <cfRule type="expression" dxfId="28" priority="26">
       <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L26:BM26">
-    <cfRule type="expression" dxfId="66" priority="25">
+    <cfRule type="expression" dxfId="27" priority="25">
       <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L9:BM16 L18:BM25">
-    <cfRule type="expression" dxfId="65" priority="50" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="50" stopIfTrue="1">
       <formula>NOT(AND(MAX($J9,$H9)&gt;=L$6,MIN($I9,$G9)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="64" priority="51">
+    <cfRule type="expression" dxfId="25" priority="51">
       <formula>AND($H9&gt;=L$6,$G9&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="63" priority="52" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="52" stopIfTrue="1">
       <formula>AND($J9&gt;=L$6,$I9&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L38:BM38">
-    <cfRule type="expression" dxfId="62" priority="59" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J46,$H46)&gt;=L$6,MIN($I46,$G46)&lt;M$6))</formula>
+  <conditionalFormatting sqref="L41:BM41">
+    <cfRule type="expression" dxfId="23" priority="59" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J49,$H49)&gt;=L$6,MIN($I49,$G49)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="61" priority="60">
-      <formula>AND($H46&gt;=L$6,$G46&lt;M$6)</formula>
+    <cfRule type="expression" dxfId="22" priority="60">
+      <formula>AND($H49&gt;=L$6,$G49&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="60" priority="61" stopIfTrue="1">
-      <formula>AND($J46&gt;=L$6,$I46&lt;M$6)</formula>
+    <cfRule type="expression" dxfId="21" priority="61" stopIfTrue="1">
+      <formula>AND($J49&gt;=L$6,$I49&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F35">
+  <conditionalFormatting sqref="F34">
     <cfRule type="dataBar" priority="22">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6522,54 +6033,40 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L28:BM29 L37:BM37 L32:BM32">
-    <cfRule type="expression" dxfId="59" priority="70" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J35,$H35)&gt;=L$6,MIN($I35,$G35)&lt;M$6))</formula>
+  <conditionalFormatting sqref="L37:BM37 L40:BM40">
+    <cfRule type="expression" dxfId="20" priority="70" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J44,$H44)&gt;=L$6,MIN($I44,$G44)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="58" priority="71">
-      <formula>AND($H35&gt;=L$6,$G35&lt;M$6)</formula>
+    <cfRule type="expression" dxfId="19" priority="71">
+      <formula>AND($H44&gt;=L$6,$G44&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="57" priority="72" stopIfTrue="1">
-      <formula>AND($J35&gt;=L$6,$I35&lt;M$6)</formula>
+    <cfRule type="expression" dxfId="18" priority="72" stopIfTrue="1">
+      <formula>AND($J44&gt;=L$6,$I44&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="L30:BM30 L27:BM27">
-    <cfRule type="expression" dxfId="56" priority="73" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="73" stopIfTrue="1">
       <formula>NOT(AND(MAX(#REF!,#REF!)&gt;=L$6,MIN(#REF!,#REF!)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="55" priority="74">
+    <cfRule type="expression" dxfId="16" priority="74">
       <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="54" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="15" priority="75" stopIfTrue="1">
       <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="F39">
-    <cfRule type="dataBar" priority="21">
-      <dataBar>
-        <cfvo type="num" val="0"/>
-        <cfvo type="num" val="1"/>
-        <color theme="7" tint="0.59999389629810485"/>
-      </dataBar>
-      <extLst>
-        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
-          <x14:id>{0DE15629-E527-4F3E-8102-95C9E03B8401}</x14:id>
-        </ext>
-      </extLst>
+  <conditionalFormatting sqref="L28:BM29 L36:BM36 L38:BM39 L42:BM42">
+    <cfRule type="expression" dxfId="14" priority="87" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J34,$H34)&gt;=L$6,MIN($I34,$G34)&lt;M$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="13" priority="88">
+      <formula>AND($H34&gt;=L$6,$G34&lt;M$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="89" stopIfTrue="1">
+      <formula>AND($J34&gt;=L$6,$I34&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L31:BM31 L35:BM36 L39:BM39">
-    <cfRule type="expression" dxfId="53" priority="87" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J37,$H37)&gt;=L$6,MIN($I37,$G37)&lt;M$6))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="52" priority="88">
-      <formula>AND($H37&gt;=L$6,$G37&lt;M$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="51" priority="89" stopIfTrue="1">
-      <formula>AND($J37&gt;=L$6,$I37&lt;M$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F38">
+  <conditionalFormatting sqref="F37">
     <cfRule type="dataBar" priority="17">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6583,34 +6080,23 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L38:BM38">
-    <cfRule type="expression" dxfId="50" priority="16">
+  <conditionalFormatting sqref="L37:BM37">
+    <cfRule type="expression" dxfId="11" priority="16">
       <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L34:BM34">
-    <cfRule type="expression" dxfId="49" priority="110" stopIfTrue="1">
-      <formula>NOT(AND(MAX(#REF!,#REF!)&gt;=L$6,MIN(#REF!,#REF!)&lt;M$6))</formula>
+  <conditionalFormatting sqref="L31:BM31 L34:BM35">
+    <cfRule type="expression" dxfId="10" priority="131" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J36,$H36)&gt;=L$6,MIN($I36,$G36)&lt;M$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="48" priority="111">
-      <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
+    <cfRule type="expression" dxfId="9" priority="132">
+      <formula>AND($H36&gt;=L$6,$G36&lt;M$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="47" priority="112" stopIfTrue="1">
-      <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
+    <cfRule type="expression" dxfId="8" priority="133" stopIfTrue="1">
+      <formula>AND($J36&gt;=L$6,$I36&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L33:BM33">
-    <cfRule type="expression" dxfId="46" priority="131" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J38,$H38)&gt;=L$6,MIN($I38,$G38)&lt;M$6))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="45" priority="132">
-      <formula>AND($H38&gt;=L$6,$G38&lt;M$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="44" priority="133" stopIfTrue="1">
-      <formula>AND($J38&gt;=L$6,$I38&lt;M$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F41:F42">
+  <conditionalFormatting sqref="F39:F40">
     <cfRule type="dataBar" priority="6">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6624,23 +6110,12 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L40:BM42 L44:BM44">
-    <cfRule type="expression" dxfId="21" priority="5">
+  <conditionalFormatting sqref="L38:BM40 L42:BM42">
+    <cfRule type="expression" dxfId="7" priority="5">
       <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L43:BM43">
-    <cfRule type="expression" dxfId="19" priority="7" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J51,$H51)&gt;=L$6,MIN($I51,$G51)&lt;M$6))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="18" priority="8">
-      <formula>AND($H51&gt;=L$6,$G51&lt;M$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="17" priority="9" stopIfTrue="1">
-      <formula>AND($J51&gt;=L$6,$I51&lt;M$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F40">
+  <conditionalFormatting sqref="F38">
     <cfRule type="dataBar" priority="4">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6654,18 +6129,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L42:BM42">
-    <cfRule type="expression" dxfId="13" priority="10" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J49,$H49)&gt;=L$6,MIN($I49,$G49)&lt;M$6))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="12" priority="11">
-      <formula>AND($H49&gt;=L$6,$G49&lt;M$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="11" priority="12" stopIfTrue="1">
-      <formula>AND($J49&gt;=L$6,$I49&lt;M$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F44">
+  <conditionalFormatting sqref="F42">
     <cfRule type="dataBar" priority="3">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6679,18 +6143,7 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L40:BM41 L44:BM44">
-    <cfRule type="expression" dxfId="7" priority="13" stopIfTrue="1">
-      <formula>NOT(AND(MAX($J46,$H46)&gt;=L$6,MIN($I46,$G46)&lt;M$6))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="6" priority="14">
-      <formula>AND($H46&gt;=L$6,$G46&lt;M$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="15" stopIfTrue="1">
-      <formula>AND($J46&gt;=L$6,$I46&lt;M$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="F43">
+  <conditionalFormatting sqref="F41">
     <cfRule type="dataBar" priority="2">
       <dataBar>
         <cfvo type="num" val="0"/>
@@ -6704,9 +6157,31 @@
       </extLst>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="L43:BM43">
-    <cfRule type="expression" dxfId="1" priority="1">
+  <conditionalFormatting sqref="L41:BM41">
+    <cfRule type="expression" dxfId="6" priority="1">
       <formula>AND(TODAY()&gt;=L$6,TODAY()&lt;M$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L32:BM32">
+    <cfRule type="expression" dxfId="5" priority="140" stopIfTrue="1">
+      <formula>NOT(AND(MAX(#REF!,#REF!)&gt;=L$6,MIN(#REF!,#REF!)&lt;M$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="4" priority="141">
+      <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="3" priority="142" stopIfTrue="1">
+      <formula>AND(#REF!&gt;=L$6,#REF!&lt;M$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="L33:BM33">
+    <cfRule type="expression" dxfId="2" priority="169" stopIfTrue="1">
+      <formula>NOT(AND(MAX($J37,$H37)&gt;=L$6,MIN($I37,$G37)&lt;M$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="170">
+      <formula>AND($H37&gt;=L$6,$G37&lt;M$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="171" stopIfTrue="1">
+      <formula>AND($J37&gt;=L$6,$I37&lt;M$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
@@ -6765,7 +6240,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F9:F16 F19:F25 F45:F49 F36:F37</xm:sqref>
+          <xm:sqref>F9:F16 F19:F25 F43:F47 F35:F36</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{35B0E45D-0F80-4816-B43B-129D908BE9C3}">
@@ -6795,7 +6270,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F28:F34</xm:sqref>
+          <xm:sqref>F28:F33</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{58C1B727-9B84-4E8B-BD44-F81E58086481}">
@@ -6825,22 +6300,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F35</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="dataBar" id="{0DE15629-E527-4F3E-8102-95C9E03B8401}">
-            <x14:dataBar minLength="0" maxLength="100" gradient="0">
-              <x14:cfvo type="num">
-                <xm:f>0</xm:f>
-              </x14:cfvo>
-              <x14:cfvo type="num">
-                <xm:f>1</xm:f>
-              </x14:cfvo>
-              <x14:negativeFillColor rgb="FFFF0000"/>
-              <x14:axisColor rgb="FF000000"/>
-            </x14:dataBar>
-          </x14:cfRule>
-          <xm:sqref>F39</xm:sqref>
+          <xm:sqref>F34</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{413F1A60-1EE0-4F7F-888D-36D618AEFC7A}">
@@ -6855,7 +6315,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F38</xm:sqref>
+          <xm:sqref>F37</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{8D2C64B7-A22D-4862-8F8D-9C270D57F227}">
@@ -6870,7 +6330,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F41:F42</xm:sqref>
+          <xm:sqref>F39:F40</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{46FE4CD9-66BA-403E-AD18-5FE4EA8CFC9E}">
@@ -6885,7 +6345,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F40</xm:sqref>
+          <xm:sqref>F38</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{426987FE-C82C-4CCE-8C87-6246EF4E50B5}">
@@ -6900,7 +6360,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F44</xm:sqref>
+          <xm:sqref>F42</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
           <x14:cfRule type="dataBar" id="{1A686C7A-121A-49C0-B1BE-B8569A441288}">
@@ -6915,7 +6375,7 @@
               <x14:axisColor rgb="FF000000"/>
             </x14:dataBar>
           </x14:cfRule>
-          <xm:sqref>F43</xm:sqref>
+          <xm:sqref>F41</xm:sqref>
         </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>

</xml_diff>

<commit_message>
Updating work progress in project plan Signed-off-by: May Alaa <mayelfkiy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -1480,7 +1480,7 @@
                   <a14:compatExt spid="_x0000_s6145"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1530,7 +1530,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1585,7 +1585,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1888,14 +1888,14 @@
   </sheetPr>
   <dimension ref="A1:BN50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A37" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A42" sqref="A42"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A5" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="H32" sqref="H32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.375" customWidth="1"/>
-    <col min="2" max="2" width="19.75" customWidth="1"/>
+    <col min="2" max="2" width="20.5" customWidth="1"/>
     <col min="3" max="3" width="34.875" style="71" customWidth="1"/>
     <col min="4" max="4" width="13.25" customWidth="1"/>
     <col min="5" max="5" width="13.25" style="71" customWidth="1"/>
@@ -4656,7 +4656,7 @@
         <v>57</v>
       </c>
       <c r="F28" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28" s="53">
         <v>43869</v>
@@ -4741,7 +4741,7 @@
         <v>57</v>
       </c>
       <c r="F29" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29" s="53">
         <v>43869</v>
@@ -4826,7 +4826,7 @@
         <v>57</v>
       </c>
       <c r="F30" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G30" s="53">
         <v>43869</v>
@@ -4911,7 +4911,7 @@
         <v>57</v>
       </c>
       <c r="F31" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G31" s="53">
         <v>43869</v>
@@ -5077,7 +5077,7 @@
         <v>57</v>
       </c>
       <c r="F33" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33" s="53">
         <v>43869</v>
@@ -5231,7 +5231,7 @@
         <v>57</v>
       </c>
       <c r="F35" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G35" s="53">
         <v>43872</v>
@@ -5316,7 +5316,7 @@
         <v>57</v>
       </c>
       <c r="F36" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G36" s="53">
         <v>43873</v>
@@ -5324,8 +5324,12 @@
       <c r="H36" s="54">
         <v>43874</v>
       </c>
-      <c r="I36" s="53"/>
-      <c r="J36" s="54"/>
+      <c r="I36" s="53">
+        <v>43873</v>
+      </c>
+      <c r="J36" s="54">
+        <v>43874</v>
+      </c>
       <c r="K36" s="61"/>
       <c r="L36" s="16"/>
       <c r="M36" s="16"/>
@@ -5395,7 +5399,7 @@
         <v>57</v>
       </c>
       <c r="F37" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G37" s="53">
         <v>43872</v>
@@ -5549,7 +5553,7 @@
         <v>57</v>
       </c>
       <c r="F39" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G39" s="53">
         <v>43880</v>
@@ -5634,7 +5638,7 @@
         <v>57</v>
       </c>
       <c r="F40" s="50">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G40" s="53">
         <v>43880</v>

</xml_diff>

<commit_message>
Updating project plan for week 5 Updating tasks for GDD Adding tasks for the CDD
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="95">
   <si>
     <t>HELP</t>
   </si>
@@ -73,9 +73,6 @@
     <t>When you insert new rows, you should insert a blank row between rows that have the formatting you want. If you do that, the formatting will be copied automatically.</t>
   </si>
   <si>
-    <t>Insert new rows ABOVE this one</t>
-  </si>
-  <si>
     <t>Adding More Columns to the Gantt Chart</t>
   </si>
   <si>
@@ -296,6 +293,39 @@
   </si>
   <si>
     <t xml:space="preserve">   Updating HSI requirements to reflect the system  constraints defined in CYRS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   GDD Document</t>
+  </si>
+  <si>
+    <t>Updating layered Architecture (Update) , Input and ouptut signals</t>
+  </si>
+  <si>
+    <t>Software Context, Software Features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">May </t>
+  </si>
+  <si>
+    <t>GDD Document</t>
+  </si>
+  <si>
+    <t>Adding requirements table and APIs</t>
+  </si>
+  <si>
+    <t>Switch CDD</t>
+  </si>
+  <si>
+    <t>May, Ibrahim</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   GDD Cross-Review</t>
+  </si>
+  <si>
+    <t>Switch CDD Cross Review</t>
+  </si>
+  <si>
+    <t>Week 5</t>
   </si>
 </sst>
 </file>
@@ -306,7 +336,7 @@
     <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
     <numFmt numFmtId="165" formatCode="ddd\,\ m/d/yyyy"/>
   </numFmts>
-  <fonts count="28" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -409,14 +439,6 @@
     </font>
     <font>
       <sz val="16"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="9"/>
       <color theme="1"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -724,7 +746,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="68">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -775,48 +797,48 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="16" fillId="5" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="24" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="23" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="23" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="22" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -825,18 +847,12 @@
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -867,20 +883,20 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -888,6 +904,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -896,12 +957,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -909,6 +964,41 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="51">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -1230,41 +1320,6 @@
         </left>
         <right style="thin">
           <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color rgb="FFC00000"/>
-        </left>
-        <right style="thin">
-          <color rgb="FFC00000"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
         </right>
         <vertical/>
         <horizontal/>
@@ -1902,16 +1957,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BK51"/>
+  <dimension ref="A1:BK75"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A36" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A48" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="20.5" customWidth="1"/>
-    <col min="2" max="2" width="49.375" style="60" customWidth="1"/>
+    <col min="2" max="2" width="49.375" style="58" customWidth="1"/>
     <col min="3" max="3" width="13.25" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="10" customWidth="1"/>
     <col min="5" max="5" width="9.5" customWidth="1"/>
@@ -1926,7 +1981,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-      <c r="D1" s="55"/>
+      <c r="D1" s="53"/>
       <c r="E1" s="2"/>
       <c r="F1" s="9"/>
       <c r="G1" s="2"/>
@@ -1938,27 +1993,27 @@
       <c r="A2" s="14"/>
       <c r="B2" s="14"/>
       <c r="C2" s="14"/>
-      <c r="I2" s="57"/>
-    </row>
-    <row r="3" spans="1:63" s="60" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="59"/>
-      <c r="B3" s="59"/>
+      <c r="I2" s="55"/>
+    </row>
+    <row r="3" spans="1:63" s="58" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="57"/>
+      <c r="B3" s="57"/>
       <c r="C3" s="14"/>
-      <c r="D3" s="61"/>
-      <c r="F3" s="61"/>
-      <c r="I3" s="57"/>
+      <c r="D3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="I3" s="55"/>
     </row>
     <row r="4" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="59"/>
-      <c r="B4" s="59"/>
-      <c r="D4" s="63">
+      <c r="A4" s="57"/>
+      <c r="B4" s="57"/>
+      <c r="D4" s="76">
         <v>43851</v>
       </c>
-      <c r="E4" s="64"/>
+      <c r="E4" s="77"/>
     </row>
     <row r="5" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="D5" s="50" t="s">
-        <v>34</v>
+      <c r="D5" s="48" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:63" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
@@ -2091,25 +2146,25 @@
         <v>9</v>
       </c>
       <c r="B8" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C8" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D8" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="E8" s="58" t="s">
+      <c r="E8" s="56" t="s">
         <v>8</v>
       </c>
       <c r="F8" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G8" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H8" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I8" s="36"/>
       <c r="J8" s="36"/>
@@ -2167,14 +2222,14 @@
       <c r="BJ8" s="36"/>
     </row>
     <row r="9" spans="1:63" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="41"/>
-      <c r="B9" s="41"/>
+      <c r="A9" s="40"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="38"/>
-      <c r="D9" s="44"/>
-      <c r="E9" s="45"/>
-      <c r="F9" s="44"/>
-      <c r="G9" s="45"/>
-      <c r="H9" s="51" t="str">
+      <c r="D9" s="42"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="42"/>
+      <c r="G9" s="43"/>
+      <c r="H9" s="49" t="str">
         <f>IF(OR(ISBLANK(F9),ISBLANK(G9)),"",G9-F9+1)</f>
         <v/>
       </c>
@@ -2234,22 +2289,22 @@
       <c r="BJ9" s="16"/>
     </row>
     <row r="10" spans="1:63" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" s="42"/>
+      <c r="A10" s="41" t="s">
+        <v>32</v>
+      </c>
+      <c r="B10" s="41"/>
       <c r="C10" s="39"/>
-      <c r="D10" s="46">
+      <c r="D10" s="44">
         <v>43851</v>
       </c>
-      <c r="E10" s="47">
+      <c r="E10" s="45">
         <v>43854</v>
       </c>
-      <c r="F10" s="46">
+      <c r="F10" s="44">
         <v>43851</v>
       </c>
-      <c r="G10" s="47"/>
-      <c r="H10" s="52" t="str">
+      <c r="G10" s="45"/>
+      <c r="H10" s="50" t="str">
         <f>IF(OR(ISBLANK(F10),ISBLANK(G10)),"",G10-F10+1)</f>
         <v/>
       </c>
@@ -2309,16 +2364,16 @@
       <c r="BJ10" s="16"/>
     </row>
     <row r="11" spans="1:63" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="42" t="s">
-        <v>55</v>
-      </c>
-      <c r="B11" s="42"/>
+      <c r="A11" s="41" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="41"/>
       <c r="C11" s="39"/>
-      <c r="D11" s="46"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="46"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="52"/>
+      <c r="D11" s="44"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="44"/>
+      <c r="G11" s="45"/>
+      <c r="H11" s="50"/>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
@@ -2376,25 +2431,25 @@
     </row>
     <row r="12" spans="1:63" s="8" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="15" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B12" s="15"/>
-      <c r="C12" s="62" t="s">
-        <v>39</v>
-      </c>
-      <c r="D12" s="44">
+      <c r="C12" s="60" t="s">
+        <v>38</v>
+      </c>
+      <c r="D12" s="42">
         <v>43852</v>
       </c>
-      <c r="E12" s="45">
+      <c r="E12" s="43">
         <v>43853</v>
       </c>
-      <c r="F12" s="44">
+      <c r="F12" s="42">
         <v>43852</v>
       </c>
-      <c r="G12" s="45">
+      <c r="G12" s="43">
         <v>43853</v>
       </c>
-      <c r="H12" s="51"/>
+      <c r="H12" s="49"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
@@ -2452,25 +2507,25 @@
     </row>
     <row r="13" spans="1:63" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B13" s="15"/>
       <c r="C13" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D13" s="44">
+        <v>39</v>
+      </c>
+      <c r="D13" s="42">
         <v>43854</v>
       </c>
-      <c r="E13" s="45">
+      <c r="E13" s="43">
         <v>43854</v>
       </c>
-      <c r="F13" s="44">
+      <c r="F13" s="42">
         <v>43854</v>
       </c>
-      <c r="G13" s="45">
+      <c r="G13" s="43">
         <v>43854</v>
       </c>
-      <c r="H13" s="51"/>
+      <c r="H13" s="49"/>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
@@ -2528,25 +2583,25 @@
     </row>
     <row r="14" spans="1:63" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B14" s="15"/>
       <c r="C14" s="38" t="s">
-        <v>45</v>
-      </c>
-      <c r="D14" s="44">
+        <v>44</v>
+      </c>
+      <c r="D14" s="42">
         <v>43854</v>
       </c>
-      <c r="E14" s="45">
+      <c r="E14" s="43">
         <v>43854</v>
       </c>
-      <c r="F14" s="44">
+      <c r="F14" s="42">
         <v>43854</v>
       </c>
-      <c r="G14" s="45">
+      <c r="G14" s="43">
         <v>43854</v>
       </c>
-      <c r="H14" s="51"/>
+      <c r="H14" s="49"/>
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
@@ -2604,25 +2659,25 @@
     </row>
     <row r="15" spans="1:63" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B15" s="15"/>
       <c r="C15" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="44">
+        <v>43</v>
+      </c>
+      <c r="D15" s="42">
         <v>43853</v>
       </c>
-      <c r="E15" s="45">
+      <c r="E15" s="43">
         <v>43853</v>
       </c>
-      <c r="F15" s="44">
+      <c r="F15" s="42">
         <v>43852</v>
       </c>
-      <c r="G15" s="45">
+      <c r="G15" s="43">
         <v>43853</v>
       </c>
-      <c r="H15" s="51"/>
+      <c r="H15" s="49"/>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
@@ -2680,25 +2735,25 @@
     </row>
     <row r="16" spans="1:63" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" s="15"/>
       <c r="C16" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D16" s="44">
+        <v>42</v>
+      </c>
+      <c r="D16" s="42">
         <v>43867</v>
       </c>
-      <c r="E16" s="45">
+      <c r="E16" s="43">
         <v>43868</v>
       </c>
-      <c r="F16" s="44">
+      <c r="F16" s="42">
         <v>43867</v>
       </c>
-      <c r="G16" s="45">
+      <c r="G16" s="43">
         <v>43868</v>
       </c>
-      <c r="H16" s="51"/>
+      <c r="H16" s="49"/>
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
@@ -2754,30 +2809,30 @@
       <c r="BI16" s="16"/>
       <c r="BJ16" s="16"/>
     </row>
-    <row r="17" spans="1:62" s="60" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:62" s="58" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B17" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C17" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D17" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="E17" s="58" t="s">
+      <c r="E17" s="56" t="s">
         <v>8</v>
       </c>
       <c r="F17" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G17" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H17" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I17" s="36"/>
       <c r="J17" s="36"/>
@@ -2835,16 +2890,16 @@
       <c r="BJ17" s="36"/>
     </row>
     <row r="18" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="B18" s="42"/>
+      <c r="A18" s="41" t="s">
+        <v>55</v>
+      </c>
+      <c r="B18" s="41"/>
       <c r="C18" s="39"/>
-      <c r="D18" s="46"/>
-      <c r="E18" s="47"/>
-      <c r="F18" s="46"/>
-      <c r="G18" s="47"/>
-      <c r="H18" s="52"/>
+      <c r="D18" s="44"/>
+      <c r="E18" s="45"/>
+      <c r="F18" s="44"/>
+      <c r="G18" s="45"/>
+      <c r="H18" s="50"/>
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
@@ -2902,25 +2957,25 @@
     </row>
     <row r="19" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="15" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B19" s="15"/>
       <c r="C19" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="44">
+        <v>46</v>
+      </c>
+      <c r="D19" s="42">
         <v>43862</v>
       </c>
-      <c r="E19" s="45">
+      <c r="E19" s="43">
         <v>43863</v>
       </c>
-      <c r="F19" s="44">
+      <c r="F19" s="42">
         <v>43862</v>
       </c>
-      <c r="G19" s="45">
+      <c r="G19" s="43">
         <v>43867</v>
       </c>
-      <c r="H19" s="51"/>
+      <c r="H19" s="49"/>
       <c r="I19" s="16"/>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
@@ -2978,25 +3033,25 @@
     </row>
     <row r="20" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B20" s="15"/>
       <c r="C20" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D20" s="44">
+        <v>39</v>
+      </c>
+      <c r="D20" s="42">
         <v>43865</v>
       </c>
-      <c r="E20" s="45">
+      <c r="E20" s="43">
         <v>43866</v>
       </c>
-      <c r="F20" s="44">
+      <c r="F20" s="42">
         <v>43865</v>
       </c>
-      <c r="G20" s="45">
+      <c r="G20" s="43">
         <v>43867</v>
       </c>
-      <c r="H20" s="51"/>
+      <c r="H20" s="49"/>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
@@ -3054,25 +3109,25 @@
     </row>
     <row r="21" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B21" s="15"/>
       <c r="C21" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D21" s="44">
+        <v>56</v>
+      </c>
+      <c r="D21" s="42">
         <v>43862</v>
       </c>
-      <c r="E21" s="45">
+      <c r="E21" s="43">
         <v>43864</v>
       </c>
-      <c r="F21" s="44">
+      <c r="F21" s="42">
         <v>43862</v>
       </c>
-      <c r="G21" s="45">
+      <c r="G21" s="43">
         <v>43867</v>
       </c>
-      <c r="H21" s="51"/>
+      <c r="H21" s="49"/>
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
@@ -3130,25 +3185,25 @@
     </row>
     <row r="22" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B22" s="15"/>
       <c r="C22" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="44">
+        <v>43</v>
+      </c>
+      <c r="D22" s="42">
         <v>43864</v>
       </c>
-      <c r="E22" s="45">
+      <c r="E22" s="43">
         <v>43865</v>
       </c>
-      <c r="F22" s="44">
+      <c r="F22" s="42">
         <v>43865</v>
       </c>
-      <c r="G22" s="45">
+      <c r="G22" s="43">
         <v>43865</v>
       </c>
-      <c r="H22" s="51"/>
+      <c r="H22" s="49"/>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
@@ -3206,25 +3261,25 @@
     </row>
     <row r="23" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B23" s="15"/>
       <c r="C23" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="44">
+        <v>46</v>
+      </c>
+      <c r="D23" s="42">
         <v>43866</v>
       </c>
-      <c r="E23" s="45">
+      <c r="E23" s="43">
         <v>43866</v>
       </c>
-      <c r="F23" s="44">
+      <c r="F23" s="42">
         <v>43862</v>
       </c>
-      <c r="G23" s="45">
+      <c r="G23" s="43">
         <v>43867</v>
       </c>
-      <c r="H23" s="51"/>
+      <c r="H23" s="49"/>
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
@@ -3282,25 +3337,25 @@
     </row>
     <row r="24" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B24" s="15"/>
       <c r="C24" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="D24" s="44">
+        <v>52</v>
+      </c>
+      <c r="D24" s="42">
         <v>43864</v>
       </c>
-      <c r="E24" s="45">
+      <c r="E24" s="43">
         <v>43865</v>
       </c>
-      <c r="F24" s="44">
+      <c r="F24" s="42">
         <v>43868</v>
       </c>
-      <c r="G24" s="45">
+      <c r="G24" s="43">
         <v>43868</v>
       </c>
-      <c r="H24" s="51"/>
+      <c r="H24" s="49"/>
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
@@ -3358,25 +3413,25 @@
     </row>
     <row r="25" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="15" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B25" s="15"/>
       <c r="C25" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D25" s="44">
+        <v>42</v>
+      </c>
+      <c r="D25" s="42">
         <v>43867</v>
       </c>
-      <c r="E25" s="45">
+      <c r="E25" s="43">
         <v>43868</v>
       </c>
-      <c r="F25" s="44">
+      <c r="F25" s="42">
         <v>43868</v>
       </c>
-      <c r="G25" s="45">
+      <c r="G25" s="43">
         <v>43868</v>
       </c>
-      <c r="H25" s="51"/>
+      <c r="H25" s="49"/>
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
@@ -3432,30 +3487,30 @@
       <c r="BI25" s="16"/>
       <c r="BJ25" s="16"/>
     </row>
-    <row r="26" spans="1:62" s="60" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:62" s="58" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="12" t="s">
         <v>9</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="D26" s="58" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26" s="56" t="s">
         <v>7</v>
       </c>
-      <c r="E26" s="58" t="s">
+      <c r="E26" s="56" t="s">
         <v>8</v>
       </c>
       <c r="F26" s="13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G26" s="13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I26" s="36"/>
       <c r="J26" s="36"/>
@@ -3513,16 +3568,16 @@
       <c r="BJ26" s="36"/>
     </row>
     <row r="27" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="42" t="s">
-        <v>58</v>
-      </c>
-      <c r="B27" s="42"/>
+      <c r="A27" s="41" t="s">
+        <v>57</v>
+      </c>
+      <c r="B27" s="41"/>
       <c r="C27" s="39"/>
-      <c r="D27" s="46"/>
-      <c r="E27" s="47"/>
-      <c r="F27" s="46"/>
-      <c r="G27" s="47"/>
-      <c r="H27" s="52"/>
+      <c r="D27" s="44"/>
+      <c r="E27" s="45"/>
+      <c r="F27" s="44"/>
+      <c r="G27" s="45"/>
+      <c r="H27" s="50"/>
       <c r="I27" s="16"/>
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
@@ -3580,27 +3635,27 @@
     </row>
     <row r="28" spans="1:62" s="8" customFormat="1" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B28" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B28" s="15" t="s">
-        <v>60</v>
-      </c>
-      <c r="C28" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D28" s="44">
+      <c r="D28" s="42">
         <v>43869</v>
       </c>
-      <c r="E28" s="45">
+      <c r="E28" s="43">
         <v>43869</v>
       </c>
-      <c r="F28" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="G28" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="H28" s="51"/>
+      <c r="F28" s="42" t="s">
+        <v>67</v>
+      </c>
+      <c r="G28" s="43" t="s">
+        <v>67</v>
+      </c>
+      <c r="H28" s="49"/>
       <c r="I28" s="16"/>
       <c r="J28" s="16"/>
       <c r="K28" s="16"/>
@@ -3658,27 +3713,27 @@
     </row>
     <row r="29" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B29" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D29" s="44">
+        <v>39</v>
+      </c>
+      <c r="D29" s="42">
         <v>43869</v>
       </c>
-      <c r="E29" s="45">
+      <c r="E29" s="43">
         <v>43872</v>
       </c>
-      <c r="F29" s="44">
+      <c r="F29" s="42">
         <v>43869</v>
       </c>
-      <c r="G29" s="45">
+      <c r="G29" s="43">
         <v>43872</v>
       </c>
-      <c r="H29" s="51"/>
+      <c r="H29" s="49"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
       <c r="K29" s="16"/>
@@ -3736,27 +3791,27 @@
     </row>
     <row r="30" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C30" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D30" s="44">
+        <v>56</v>
+      </c>
+      <c r="D30" s="42">
         <v>43869</v>
       </c>
-      <c r="E30" s="45">
+      <c r="E30" s="43">
         <v>43869</v>
       </c>
-      <c r="F30" s="44">
+      <c r="F30" s="42">
         <v>43869</v>
       </c>
-      <c r="G30" s="45">
+      <c r="G30" s="43">
         <v>43869</v>
       </c>
-      <c r="H30" s="51"/>
+      <c r="H30" s="49"/>
       <c r="I30" s="16"/>
       <c r="J30" s="16"/>
       <c r="K30" s="16"/>
@@ -3814,27 +3869,27 @@
     </row>
     <row r="31" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="38" t="s">
-        <v>44</v>
-      </c>
-      <c r="D31" s="44">
+        <v>43</v>
+      </c>
+      <c r="D31" s="42">
         <v>43869</v>
       </c>
-      <c r="E31" s="45">
+      <c r="E31" s="43">
         <v>43869</v>
       </c>
-      <c r="F31" s="44">
+      <c r="F31" s="42">
         <v>43869</v>
       </c>
-      <c r="G31" s="45">
+      <c r="G31" s="43">
         <v>43869</v>
       </c>
-      <c r="H31" s="51"/>
+      <c r="H31" s="49"/>
       <c r="I31" s="16"/>
       <c r="J31" s="16"/>
       <c r="K31" s="16"/>
@@ -3892,23 +3947,23 @@
     </row>
     <row r="32" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B32" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C32" s="38" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="44">
+        <v>52</v>
+      </c>
+      <c r="D32" s="42">
         <v>43872</v>
       </c>
-      <c r="E32" s="45">
+      <c r="E32" s="43">
         <v>43872</v>
       </c>
-      <c r="F32" s="44"/>
-      <c r="G32" s="45"/>
-      <c r="H32" s="51"/>
+      <c r="F32" s="42"/>
+      <c r="G32" s="43"/>
+      <c r="H32" s="49"/>
       <c r="I32" s="16"/>
       <c r="J32" s="16"/>
       <c r="K32" s="16"/>
@@ -3966,27 +4021,27 @@
     </row>
     <row r="33" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B33" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C33" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D33" s="44">
+        <v>46</v>
+      </c>
+      <c r="D33" s="42">
         <v>43869</v>
       </c>
-      <c r="E33" s="45">
+      <c r="E33" s="43">
         <v>43869</v>
       </c>
-      <c r="F33" s="44">
+      <c r="F33" s="42">
         <v>43869</v>
       </c>
-      <c r="G33" s="45">
+      <c r="G33" s="43">
         <v>43869</v>
       </c>
-      <c r="H33" s="51"/>
+      <c r="H33" s="49"/>
       <c r="I33" s="16"/>
       <c r="J33" s="16"/>
       <c r="K33" s="16"/>
@@ -4043,16 +4098,16 @@
       <c r="BJ33" s="16"/>
     </row>
     <row r="34" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="42" t="s">
-        <v>66</v>
-      </c>
-      <c r="B34" s="42"/>
+      <c r="A34" s="41" t="s">
+        <v>65</v>
+      </c>
+      <c r="B34" s="41"/>
       <c r="C34" s="39"/>
-      <c r="D34" s="46"/>
-      <c r="E34" s="47"/>
-      <c r="F34" s="46"/>
-      <c r="G34" s="47"/>
-      <c r="H34" s="52"/>
+      <c r="D34" s="44"/>
+      <c r="E34" s="45"/>
+      <c r="F34" s="44"/>
+      <c r="G34" s="45"/>
+      <c r="H34" s="50"/>
       <c r="I34" s="16"/>
       <c r="J34" s="16"/>
       <c r="K34" s="16"/>
@@ -4110,27 +4165,27 @@
     </row>
     <row r="35" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B35" s="15" t="s">
+        <v>66</v>
+      </c>
+      <c r="C35" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B35" s="15" t="s">
-        <v>67</v>
-      </c>
-      <c r="C35" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D35" s="44">
+      <c r="D35" s="42">
         <v>43872</v>
       </c>
-      <c r="E35" s="45">
+      <c r="E35" s="43">
         <v>43872</v>
       </c>
-      <c r="F35" s="44">
+      <c r="F35" s="42">
         <v>43872</v>
       </c>
-      <c r="G35" s="45">
+      <c r="G35" s="43">
         <v>43872</v>
       </c>
-      <c r="H35" s="51"/>
+      <c r="H35" s="49"/>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
       <c r="K35" s="16"/>
@@ -4188,27 +4243,27 @@
     </row>
     <row r="36" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B36" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C36" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D36" s="44">
+        <v>56</v>
+      </c>
+      <c r="D36" s="42">
         <v>43873</v>
       </c>
-      <c r="E36" s="45">
+      <c r="E36" s="43">
         <v>43874</v>
       </c>
-      <c r="F36" s="44">
+      <c r="F36" s="42">
         <v>43873</v>
       </c>
-      <c r="G36" s="45">
+      <c r="G36" s="43">
         <v>43874</v>
       </c>
-      <c r="H36" s="51"/>
+      <c r="H36" s="49"/>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
@@ -4266,25 +4321,25 @@
     </row>
     <row r="37" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="15" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B37" s="15"/>
       <c r="C37" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D37" s="44">
+        <v>42</v>
+      </c>
+      <c r="D37" s="42">
         <v>43872</v>
       </c>
-      <c r="E37" s="45">
+      <c r="E37" s="43">
         <v>43872</v>
       </c>
-      <c r="F37" s="44">
+      <c r="F37" s="42">
         <v>43872</v>
       </c>
-      <c r="G37" s="45">
+      <c r="G37" s="43">
         <v>43872</v>
       </c>
-      <c r="H37" s="51"/>
+      <c r="H37" s="49"/>
       <c r="I37" s="16"/>
       <c r="J37" s="16"/>
       <c r="K37" s="16"/>
@@ -4341,16 +4396,16 @@
       <c r="BJ37" s="16"/>
     </row>
     <row r="38" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="42" t="s">
-        <v>70</v>
-      </c>
-      <c r="B38" s="42"/>
+      <c r="A38" s="41" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="41"/>
       <c r="C38" s="39"/>
-      <c r="D38" s="46"/>
-      <c r="E38" s="47"/>
-      <c r="F38" s="46"/>
-      <c r="G38" s="47"/>
-      <c r="H38" s="52"/>
+      <c r="D38" s="44"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="44"/>
+      <c r="G38" s="45"/>
+      <c r="H38" s="50"/>
       <c r="I38" s="16"/>
       <c r="J38" s="16"/>
       <c r="K38" s="16"/>
@@ -4408,27 +4463,27 @@
     </row>
     <row r="39" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="15" t="s">
+        <v>70</v>
+      </c>
+      <c r="C39" s="38" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="C39" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D39" s="44">
+      <c r="D39" s="42">
         <v>43880</v>
       </c>
-      <c r="E39" s="45">
+      <c r="E39" s="43">
         <v>43881</v>
       </c>
-      <c r="F39" s="44">
+      <c r="F39" s="42">
         <v>43880</v>
       </c>
-      <c r="G39" s="45">
+      <c r="G39" s="43">
         <v>43881</v>
       </c>
-      <c r="H39" s="51"/>
+      <c r="H39" s="49"/>
       <c r="I39" s="16"/>
       <c r="J39" s="16"/>
       <c r="K39" s="16"/>
@@ -4486,27 +4541,27 @@
     </row>
     <row r="40" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B40" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C40" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D40" s="44">
+        <v>39</v>
+      </c>
+      <c r="D40" s="42">
         <v>43880</v>
       </c>
-      <c r="E40" s="45">
+      <c r="E40" s="43">
         <v>43881</v>
       </c>
-      <c r="F40" s="44">
+      <c r="F40" s="42">
         <v>43880</v>
       </c>
-      <c r="G40" s="45">
+      <c r="G40" s="43">
         <v>43881</v>
       </c>
-      <c r="H40" s="51"/>
+      <c r="H40" s="49"/>
       <c r="I40" s="16"/>
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
@@ -4566,11 +4621,11 @@
       <c r="A41" s="15"/>
       <c r="B41" s="15"/>
       <c r="C41" s="38"/>
-      <c r="D41" s="44"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="44"/>
-      <c r="G41" s="45"/>
-      <c r="H41" s="51"/>
+      <c r="D41" s="42"/>
+      <c r="E41" s="43"/>
+      <c r="F41" s="42"/>
+      <c r="G41" s="43"/>
+      <c r="H41" s="49"/>
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
@@ -4627,16 +4682,16 @@
       <c r="BJ41" s="16"/>
     </row>
     <row r="42" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="42" t="s">
-        <v>73</v>
-      </c>
-      <c r="B42" s="42"/>
-      <c r="C42" s="39"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="47"/>
-      <c r="F42" s="46"/>
-      <c r="G42" s="47"/>
-      <c r="H42" s="52"/>
+      <c r="A42" s="66" t="s">
+        <v>72</v>
+      </c>
+      <c r="B42" s="66"/>
+      <c r="C42" s="67"/>
+      <c r="D42" s="68"/>
+      <c r="E42" s="69"/>
+      <c r="F42" s="44"/>
+      <c r="G42" s="45"/>
+      <c r="H42" s="50"/>
       <c r="I42" s="16"/>
       <c r="J42" s="16"/>
       <c r="K42" s="16"/>
@@ -4693,316 +4748,708 @@
       <c r="BJ42" s="16"/>
     </row>
     <row r="43" spans="1:62" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="15" t="s">
+      <c r="A43" s="70" t="s">
+        <v>73</v>
+      </c>
+      <c r="B43" s="70" t="s">
+        <v>76</v>
+      </c>
+      <c r="C43" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="D43" s="72">
+        <v>43882</v>
+      </c>
+      <c r="E43" s="73">
+        <v>43883</v>
+      </c>
+      <c r="F43" s="72">
+        <v>43882</v>
+      </c>
+      <c r="G43" s="73">
+        <v>43883</v>
+      </c>
+      <c r="H43" s="49"/>
+    </row>
+    <row r="44" spans="1:62" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="70" t="s">
+        <v>75</v>
+      </c>
+      <c r="B44" s="70" t="s">
+        <v>77</v>
+      </c>
+      <c r="C44" s="71" t="s">
+        <v>39</v>
+      </c>
+      <c r="D44" s="72">
+        <v>43883</v>
+      </c>
+      <c r="E44" s="73">
+        <v>43884</v>
+      </c>
+      <c r="F44" s="72">
+        <v>43883</v>
+      </c>
+      <c r="G44" s="73">
+        <v>43884</v>
+      </c>
+      <c r="H44" s="49"/>
+    </row>
+    <row r="45" spans="1:62" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="70" t="s">
         <v>74</v>
       </c>
-      <c r="B43" s="66" t="s">
-        <v>77</v>
-      </c>
-      <c r="C43" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D43" s="44">
-        <v>43882</v>
-      </c>
-      <c r="E43" s="45">
+      <c r="B45" s="70" t="s">
+        <v>83</v>
+      </c>
+      <c r="C45" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="D45" s="72">
         <v>43883</v>
       </c>
-      <c r="F43" s="44"/>
-      <c r="G43" s="45"/>
-      <c r="H43" s="51"/>
-    </row>
-    <row r="44" spans="1:62" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="15" t="s">
-        <v>76</v>
-      </c>
-      <c r="B44" s="66" t="s">
+      <c r="E45" s="73">
+        <v>43884</v>
+      </c>
+      <c r="F45" s="72">
+        <v>43888</v>
+      </c>
+      <c r="G45" s="73">
+        <v>43889</v>
+      </c>
+      <c r="H45" s="49"/>
+    </row>
+    <row r="46" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="74" t="s">
         <v>78</v>
       </c>
-      <c r="C44" s="38" t="s">
-        <v>40</v>
-      </c>
-      <c r="D44" s="44">
+      <c r="B46" s="70" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="71" t="s">
+        <v>80</v>
+      </c>
+      <c r="D46" s="72">
+        <v>43884</v>
+      </c>
+      <c r="E46" s="73">
+        <v>43887</v>
+      </c>
+      <c r="F46" s="59"/>
+    </row>
+    <row r="47" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="74" t="s">
+        <v>79</v>
+      </c>
+      <c r="B47" s="70"/>
+      <c r="C47" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="D47" s="72">
+        <v>43887</v>
+      </c>
+      <c r="E47" s="73">
+        <v>43888</v>
+      </c>
+    </row>
+    <row r="48" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="70" t="s">
+        <v>49</v>
+      </c>
+      <c r="B48" s="70"/>
+      <c r="C48" s="71" t="s">
+        <v>42</v>
+      </c>
+      <c r="D48" s="72">
         <v>43883</v>
       </c>
-      <c r="E44" s="45">
+      <c r="E48" s="73">
+        <v>43883</v>
+      </c>
+      <c r="F48" s="72">
+        <v>43883</v>
+      </c>
+      <c r="G48" s="73">
+        <v>43883</v>
+      </c>
+      <c r="H48" s="49"/>
+    </row>
+    <row r="49" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="70" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="70"/>
+      <c r="C49" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="D49" s="72">
         <v>43884</v>
       </c>
-      <c r="F44" s="44"/>
-      <c r="G44" s="45"/>
-      <c r="H44" s="51"/>
-    </row>
-    <row r="45" spans="1:62" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="41" t="s">
-        <v>75</v>
-      </c>
-      <c r="B45" s="67" t="s">
-        <v>84</v>
-      </c>
-      <c r="C45" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D45" s="44">
-        <v>43883</v>
-      </c>
-      <c r="E45" s="45">
+      <c r="E49" s="73">
         <v>43884</v>
       </c>
-      <c r="F45" s="44"/>
-      <c r="G45" s="45"/>
-      <c r="H45" s="51"/>
-    </row>
-    <row r="46" spans="1:62" s="60" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="41" t="s">
-        <v>79</v>
-      </c>
-      <c r="B46" s="41" t="s">
-        <v>83</v>
-      </c>
-      <c r="C46" s="38" t="s">
-        <v>81</v>
-      </c>
-      <c r="D46" s="44">
-        <v>43884</v>
-      </c>
-      <c r="E46" s="45">
-        <v>43887</v>
-      </c>
-      <c r="F46" s="61"/>
-    </row>
-    <row r="47" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="41" t="s">
-        <v>80</v>
-      </c>
-      <c r="B47" s="41"/>
-      <c r="C47" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D47" s="44">
-        <v>43887</v>
-      </c>
-      <c r="E47" s="45">
-        <v>43888</v>
-      </c>
-    </row>
-    <row r="48" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="15"/>
-      <c r="C48" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="D48" s="44">
-        <v>43883</v>
-      </c>
-      <c r="E48" s="45">
-        <v>43883</v>
-      </c>
-      <c r="F48" s="44"/>
-      <c r="G48" s="45"/>
-      <c r="H48" s="51" t="str">
-        <f>IF(OR(ISBLANK(F48),ISBLANK(G48)),"",G48-F48+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="15" t="s">
-        <v>51</v>
-      </c>
-      <c r="B49" s="15"/>
-      <c r="C49" s="38" t="s">
-        <v>57</v>
-      </c>
-      <c r="D49" s="44">
-        <v>43884</v>
-      </c>
-      <c r="E49" s="45">
-        <v>43884</v>
-      </c>
-      <c r="F49" s="48"/>
-      <c r="G49" s="49"/>
-      <c r="H49" s="53" t="str">
+      <c r="F49" s="46"/>
+      <c r="G49" s="47"/>
+      <c r="H49" s="51" t="str">
         <f>IF(OR(ISBLANK(F49),ISBLANK(G49)),"",G49-F49+1)</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="41" t="s">
-        <v>82</v>
-      </c>
-      <c r="B50" s="41"/>
-      <c r="C50" s="38" t="s">
-        <v>47</v>
-      </c>
-      <c r="D50" s="44">
+    <row r="50" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="70" t="s">
+        <v>81</v>
+      </c>
+      <c r="B50" s="70"/>
+      <c r="C50" s="71" t="s">
+        <v>46</v>
+      </c>
+      <c r="D50" s="72">
         <v>43884</v>
       </c>
-      <c r="E50" s="45">
+      <c r="E50" s="73">
         <v>43884</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="43" t="s">
-        <v>11</v>
-      </c>
-      <c r="B51" s="43"/>
-      <c r="C51" s="40"/>
-      <c r="D51" s="48"/>
-      <c r="E51" s="49"/>
+    <row r="51" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="66" t="s">
+        <v>94</v>
+      </c>
+      <c r="B51" s="66"/>
+      <c r="C51" s="67"/>
+      <c r="D51" s="68"/>
+      <c r="E51" s="69"/>
+      <c r="F51" s="44"/>
+      <c r="G51" s="45"/>
+      <c r="H51" s="50"/>
+      <c r="I51" s="16"/>
+      <c r="J51" s="16"/>
+      <c r="K51" s="16"/>
+      <c r="L51" s="16"/>
+      <c r="M51" s="16"/>
+      <c r="N51" s="16"/>
+      <c r="O51" s="16"/>
+      <c r="P51" s="16"/>
+      <c r="Q51" s="16"/>
+      <c r="R51" s="16"/>
+      <c r="S51" s="16"/>
+      <c r="T51" s="16"/>
+      <c r="U51" s="16"/>
+      <c r="V51" s="16"/>
+      <c r="W51" s="16"/>
+      <c r="X51" s="16"/>
+      <c r="Y51" s="16"/>
+      <c r="Z51" s="16"/>
+      <c r="AA51" s="16"/>
+      <c r="AB51" s="16"/>
+      <c r="AC51" s="16"/>
+      <c r="AD51" s="16"/>
+      <c r="AE51" s="16"/>
+      <c r="AF51" s="16"/>
+      <c r="AG51" s="16"/>
+      <c r="AH51" s="16"/>
+      <c r="AI51" s="16"/>
+      <c r="AJ51" s="16"/>
+      <c r="AK51" s="16"/>
+      <c r="AL51" s="16"/>
+      <c r="AM51" s="16"/>
+      <c r="AN51" s="16"/>
+      <c r="AO51" s="16"/>
+      <c r="AP51" s="16"/>
+      <c r="AQ51" s="16"/>
+      <c r="AR51" s="16"/>
+      <c r="AS51" s="16"/>
+      <c r="AT51" s="16"/>
+      <c r="AU51" s="16"/>
+      <c r="AV51" s="16"/>
+      <c r="AW51" s="16"/>
+      <c r="AX51" s="16"/>
+      <c r="AY51" s="16"/>
+      <c r="AZ51" s="16"/>
+      <c r="BA51" s="16"/>
+      <c r="BB51" s="16"/>
+      <c r="BC51" s="16"/>
+      <c r="BD51" s="16"/>
+      <c r="BE51" s="16"/>
+      <c r="BF51" s="16"/>
+      <c r="BG51" s="16"/>
+      <c r="BH51" s="16"/>
+      <c r="BI51" s="16"/>
+      <c r="BJ51" s="16"/>
+    </row>
+    <row r="52" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="B52" s="70" t="s">
+        <v>86</v>
+      </c>
+      <c r="C52" s="71" t="s">
+        <v>43</v>
+      </c>
+      <c r="D52" s="72">
+        <v>43890</v>
+      </c>
+      <c r="E52" s="72">
+        <v>43891</v>
+      </c>
+      <c r="F52" s="42"/>
+      <c r="G52" s="43"/>
+      <c r="H52" s="49"/>
+    </row>
+    <row r="53" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="75" t="s">
+        <v>88</v>
+      </c>
+      <c r="B53" s="70" t="s">
+        <v>89</v>
+      </c>
+      <c r="C53" s="71" t="s">
+        <v>87</v>
+      </c>
+      <c r="D53" s="72">
+        <v>43889</v>
+      </c>
+      <c r="E53" s="73">
+        <v>43890</v>
+      </c>
+      <c r="F53" s="72">
+        <v>43889</v>
+      </c>
+      <c r="G53" s="73">
+        <v>43890</v>
+      </c>
+      <c r="H53" s="49"/>
+    </row>
+    <row r="54" spans="1:62" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="75" t="s">
+        <v>84</v>
+      </c>
+      <c r="B54" s="70" t="s">
+        <v>85</v>
+      </c>
+      <c r="C54" s="71" t="s">
+        <v>52</v>
+      </c>
+      <c r="D54" s="72">
+        <v>43891</v>
+      </c>
+      <c r="E54" s="73">
+        <v>43892</v>
+      </c>
+      <c r="F54" s="42"/>
+      <c r="G54" s="43"/>
+      <c r="H54" s="49"/>
+    </row>
+    <row r="55" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="75" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="70"/>
+      <c r="C55" s="71" t="s">
+        <v>56</v>
+      </c>
+      <c r="D55" s="72">
+        <v>43892</v>
+      </c>
+      <c r="E55" s="73">
+        <v>43892</v>
+      </c>
+      <c r="F55" s="42"/>
+      <c r="G55" s="43"/>
+      <c r="H55" s="49"/>
+    </row>
+    <row r="56" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B56" s="40"/>
+      <c r="C56" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D56" s="42">
+        <v>43893</v>
+      </c>
+      <c r="E56" s="43">
+        <v>43895</v>
+      </c>
+      <c r="F56" s="42"/>
+      <c r="G56" s="43"/>
+      <c r="H56" s="49"/>
+    </row>
+    <row r="57" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B57" s="40"/>
+      <c r="C57" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D57" s="42">
+        <v>43893</v>
+      </c>
+      <c r="E57" s="43">
+        <v>43895</v>
+      </c>
+      <c r="F57" s="42"/>
+      <c r="G57" s="43"/>
+      <c r="H57" s="49"/>
+    </row>
+    <row r="58" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="15"/>
+      <c r="B58" s="15"/>
+      <c r="C58" s="38"/>
+      <c r="D58" s="42"/>
+      <c r="E58" s="43"/>
+      <c r="F58" s="42"/>
+      <c r="G58" s="43"/>
+      <c r="H58" s="49" t="str">
+        <f>IF(OR(ISBLANK(F58),ISBLANK(G58)),"",G58-F58+1)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="59" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="15"/>
+      <c r="B59" s="61"/>
+      <c r="C59" s="38"/>
+      <c r="D59" s="42"/>
+      <c r="E59" s="43"/>
+      <c r="F59" s="42"/>
+      <c r="G59" s="43"/>
+      <c r="H59" s="49"/>
+      <c r="I59" s="58"/>
+    </row>
+    <row r="60" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="15"/>
+      <c r="B60" s="61"/>
+      <c r="C60" s="38"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="43"/>
+      <c r="F60" s="42"/>
+      <c r="G60" s="43"/>
+      <c r="H60" s="49"/>
+      <c r="I60" s="58"/>
+    </row>
+    <row r="61" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="40"/>
+      <c r="B61" s="62"/>
+      <c r="C61" s="38"/>
+      <c r="D61" s="42"/>
+      <c r="E61" s="43"/>
+      <c r="F61" s="42"/>
+      <c r="G61" s="43"/>
+      <c r="H61" s="49"/>
+      <c r="I61" s="58"/>
+    </row>
+    <row r="62" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="40"/>
+      <c r="B62" s="40"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="43"/>
+      <c r="F62" s="42"/>
+      <c r="G62" s="43"/>
+      <c r="H62" s="49"/>
+      <c r="I62" s="58"/>
+    </row>
+    <row r="63" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="40"/>
+      <c r="B63" s="40"/>
+      <c r="C63" s="38"/>
+      <c r="D63" s="42"/>
+      <c r="E63" s="43"/>
+      <c r="F63" s="42"/>
+      <c r="G63" s="43"/>
+      <c r="H63" s="49"/>
+      <c r="I63" s="58"/>
+    </row>
+    <row r="64" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="15"/>
+      <c r="B64" s="15"/>
+      <c r="C64" s="38"/>
+      <c r="D64" s="42"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="42"/>
+      <c r="G64" s="43"/>
+      <c r="H64" s="49"/>
+      <c r="I64" s="58"/>
+    </row>
+    <row r="65" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="15"/>
+      <c r="B65" s="15"/>
+      <c r="C65" s="38"/>
+      <c r="D65" s="42"/>
+      <c r="E65" s="43"/>
+      <c r="F65" s="46"/>
+      <c r="G65" s="47"/>
+      <c r="H65" s="51"/>
+      <c r="I65" s="58"/>
+    </row>
+    <row r="66" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="15"/>
+      <c r="B66" s="15"/>
+      <c r="C66" s="38"/>
+      <c r="D66" s="42"/>
+      <c r="E66" s="43"/>
+      <c r="F66" s="63"/>
+      <c r="G66" s="64"/>
+      <c r="H66" s="65"/>
+    </row>
+    <row r="67" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="15"/>
+      <c r="B67" s="15"/>
+      <c r="C67" s="38"/>
+      <c r="D67" s="42"/>
+      <c r="E67" s="43"/>
+      <c r="F67" s="63"/>
+      <c r="G67" s="64"/>
+      <c r="H67" s="65"/>
+    </row>
+    <row r="68" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="15"/>
+      <c r="B68" s="61"/>
+      <c r="C68" s="38"/>
+      <c r="D68" s="42"/>
+      <c r="E68" s="43"/>
+      <c r="F68" s="42"/>
+      <c r="G68" s="43"/>
+      <c r="H68" s="49"/>
+    </row>
+    <row r="69" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="15"/>
+      <c r="B69" s="61"/>
+      <c r="C69" s="38"/>
+      <c r="D69" s="42"/>
+      <c r="E69" s="43"/>
+      <c r="F69" s="42"/>
+      <c r="G69" s="43"/>
+      <c r="H69" s="49"/>
+    </row>
+    <row r="70" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="40"/>
+      <c r="B70" s="62"/>
+      <c r="C70" s="38"/>
+      <c r="D70" s="42"/>
+      <c r="E70" s="43"/>
+      <c r="F70" s="42"/>
+      <c r="G70" s="43"/>
+      <c r="H70" s="49"/>
+    </row>
+    <row r="71" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="40"/>
+      <c r="B71" s="40"/>
+      <c r="C71" s="38"/>
+      <c r="D71" s="42"/>
+      <c r="E71" s="43"/>
+      <c r="F71" s="42"/>
+      <c r="G71" s="43"/>
+      <c r="H71" s="49"/>
+    </row>
+    <row r="72" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="40"/>
+      <c r="B72" s="40"/>
+      <c r="C72" s="38"/>
+      <c r="D72" s="42"/>
+      <c r="E72" s="43"/>
+      <c r="F72" s="42"/>
+      <c r="G72" s="43"/>
+      <c r="H72" s="49"/>
+    </row>
+    <row r="73" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A73" s="15"/>
+      <c r="B73" s="15"/>
+      <c r="C73" s="38"/>
+      <c r="D73" s="42"/>
+      <c r="E73" s="43"/>
+      <c r="F73" s="42"/>
+      <c r="G73" s="43"/>
+      <c r="H73" s="49"/>
+    </row>
+    <row r="74" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="15"/>
+      <c r="B74" s="15"/>
+      <c r="C74" s="38"/>
+      <c r="D74" s="42"/>
+      <c r="E74" s="43"/>
+      <c r="F74" s="46"/>
+      <c r="G74" s="47"/>
+      <c r="H74" s="51"/>
+    </row>
+    <row r="75" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A75" s="40"/>
+      <c r="B75" s="40"/>
+      <c r="C75" s="38"/>
+      <c r="D75" s="42"/>
+      <c r="E75" s="43"/>
+      <c r="F75" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BJ16 I19:BJ25 I27:BJ36">
-    <cfRule type="expression" dxfId="37" priority="39">
+    <cfRule type="expression" dxfId="41" priority="43">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:BJ18">
-    <cfRule type="expression" dxfId="36" priority="34">
+    <cfRule type="expression" dxfId="40" priority="38">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:BJ17">
-    <cfRule type="expression" dxfId="35" priority="31">
+    <cfRule type="expression" dxfId="39" priority="35">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:BJ26">
-    <cfRule type="expression" dxfId="34" priority="30">
+    <cfRule type="expression" dxfId="38" priority="34">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:BJ16 I18:BJ25">
-    <cfRule type="expression" dxfId="33" priority="55" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="59" stopIfTrue="1">
       <formula>NOT(AND(MAX($G9,$E9)&gt;=I$6,MIN($F9,$D9)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="56">
+    <cfRule type="expression" dxfId="36" priority="60">
       <formula>AND($E9&gt;=I$6,$D9&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="31" priority="57" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="61" stopIfTrue="1">
       <formula>AND($G9&gt;=I$6,$F9&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37:BJ37">
-    <cfRule type="expression" dxfId="30" priority="75" stopIfTrue="1">
+    <cfRule type="expression" dxfId="34" priority="79" stopIfTrue="1">
       <formula>NOT(AND(MAX($G44,$E44)&gt;=I$6,MIN($F44,$D44)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="76">
+    <cfRule type="expression" dxfId="33" priority="80">
       <formula>AND($E44&gt;=I$6,$D44&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="77" stopIfTrue="1">
+    <cfRule type="expression" dxfId="32" priority="81" stopIfTrue="1">
       <formula>AND($G44&gt;=I$6,$F44&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:BJ30 I27:BJ27">
-    <cfRule type="expression" dxfId="27" priority="78" stopIfTrue="1">
+    <cfRule type="expression" dxfId="31" priority="82" stopIfTrue="1">
       <formula>NOT(AND(MAX(#REF!,#REF!)&gt;=I$6,MIN(#REF!,#REF!)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="79">
+    <cfRule type="expression" dxfId="30" priority="83">
       <formula>AND(#REF!&gt;=I$6,#REF!&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="25" priority="80" stopIfTrue="1">
+    <cfRule type="expression" dxfId="29" priority="84" stopIfTrue="1">
       <formula>AND(#REF!&gt;=I$6,#REF!&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I28:BJ29 I36:BJ36 I38:BJ39">
-    <cfRule type="expression" dxfId="24" priority="92" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="96" stopIfTrue="1">
       <formula>NOT(AND(MAX($G34,$E34)&gt;=I$6,MIN($F34,$D34)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="93">
+    <cfRule type="expression" dxfId="27" priority="97">
       <formula>AND($E34&gt;=I$6,$D34&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="94" stopIfTrue="1">
+    <cfRule type="expression" dxfId="26" priority="98" stopIfTrue="1">
       <formula>AND($G34&gt;=I$6,$F34&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37:BJ37">
-    <cfRule type="expression" dxfId="21" priority="21">
+    <cfRule type="expression" dxfId="25" priority="25">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:BJ31 I34:BJ35">
-    <cfRule type="expression" dxfId="20" priority="136" stopIfTrue="1">
+    <cfRule type="expression" dxfId="24" priority="140" stopIfTrue="1">
       <formula>NOT(AND(MAX($G36,$E36)&gt;=I$6,MIN($F36,$D36)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="19" priority="137">
+    <cfRule type="expression" dxfId="23" priority="141">
       <formula>AND($E36&gt;=I$6,$D36&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="138" stopIfTrue="1">
+    <cfRule type="expression" dxfId="22" priority="142" stopIfTrue="1">
       <formula>AND($G36&gt;=I$6,$F36&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:BJ40">
-    <cfRule type="expression" dxfId="17" priority="10">
+    <cfRule type="expression" dxfId="21" priority="14">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:BJ41">
-    <cfRule type="expression" dxfId="16" priority="6">
+    <cfRule type="expression" dxfId="20" priority="10">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:BJ32">
-    <cfRule type="expression" dxfId="15" priority="145" stopIfTrue="1">
+    <cfRule type="expression" dxfId="19" priority="149" stopIfTrue="1">
       <formula>NOT(AND(MAX(#REF!,#REF!)&gt;=I$6,MIN(#REF!,#REF!)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="146">
+    <cfRule type="expression" dxfId="18" priority="150">
       <formula>AND(#REF!&gt;=I$6,#REF!&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="13" priority="147" stopIfTrue="1">
+    <cfRule type="expression" dxfId="17" priority="151" stopIfTrue="1">
       <formula>AND(#REF!&gt;=I$6,#REF!&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:BJ33">
-    <cfRule type="expression" dxfId="12" priority="174" stopIfTrue="1">
+    <cfRule type="expression" dxfId="16" priority="178" stopIfTrue="1">
       <formula>NOT(AND(MAX($G37,$E37)&gt;=I$6,MIN($F37,$D37)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="175">
+    <cfRule type="expression" dxfId="15" priority="179">
       <formula>AND($E37&gt;=I$6,$D37&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="176" stopIfTrue="1">
+    <cfRule type="expression" dxfId="14" priority="180" stopIfTrue="1">
       <formula>AND($G37&gt;=I$6,$F37&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42:BJ42">
-    <cfRule type="expression" dxfId="9" priority="2">
+    <cfRule type="expression" dxfId="13" priority="6">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:BJ41">
-    <cfRule type="expression" dxfId="8" priority="195" stopIfTrue="1">
-      <formula>NOT(AND(MAX($G47,$E53)&gt;=I$6,MIN($F47,$D53)&lt;J$6))</formula>
+    <cfRule type="expression" dxfId="12" priority="199" stopIfTrue="1">
+      <formula>NOT(AND(MAX($G47,$E56)&gt;=I$6,MIN($F47,$D56)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="196">
-      <formula>AND($E53&gt;=I$6,$D53&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="11" priority="200">
+      <formula>AND($E56&gt;=I$6,$D56&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="6" priority="197" stopIfTrue="1">
+    <cfRule type="expression" dxfId="10" priority="201" stopIfTrue="1">
       <formula>AND($G47&gt;=I$6,$F47&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:BJ40">
-    <cfRule type="expression" dxfId="5" priority="198" stopIfTrue="1">
-      <formula>NOT(AND(MAX($G49,$E51)&gt;=I$6,MIN($F49,$D51)&lt;J$6))</formula>
+    <cfRule type="expression" dxfId="9" priority="202" stopIfTrue="1">
+      <formula>NOT(AND(MAX($G49,$E54)&gt;=I$6,MIN($F49,$D54)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="4" priority="199">
-      <formula>AND($E51&gt;=I$6,$D51&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="8" priority="203">
+      <formula>AND($E54&gt;=I$6,$D54&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="3" priority="200" stopIfTrue="1">
+    <cfRule type="expression" dxfId="7" priority="204" stopIfTrue="1">
       <formula>AND($G49&gt;=I$6,$F49&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42:BJ42">
-    <cfRule type="expression" dxfId="2" priority="201" stopIfTrue="1">
-      <formula>NOT(AND(MAX($G50,$E52)&gt;=I$6,MIN($F50,$D52)&lt;J$6))</formula>
+    <cfRule type="expression" dxfId="6" priority="214" stopIfTrue="1">
+      <formula>NOT(AND(MAX($G50,$E55)&gt;=I$6,MIN($F50,$D55)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="202">
-      <formula>AND($E52&gt;=I$6,$D52&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="5" priority="215">
+      <formula>AND($E55&gt;=I$6,$D55&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="203" stopIfTrue="1">
+    <cfRule type="expression" dxfId="4" priority="216" stopIfTrue="1">
       <formula>AND($G50&gt;=I$6,$F50&lt;J$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I51:BJ51">
+    <cfRule type="expression" dxfId="3" priority="1">
+      <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I51:BJ51">
+    <cfRule type="expression" dxfId="2" priority="217" stopIfTrue="1">
+      <formula>NOT(AND(MAX($G60,$E64)&gt;=I$6,MIN($F60,$D64)&lt;J$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="218">
+      <formula>AND($E64&gt;=I$6,$D64&lt;J$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="0" priority="219" stopIfTrue="1">
+      <formula>AND($G60&gt;=I$6,$F60&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
@@ -5071,14 +5518,14 @@
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="65" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" s="65"/>
+      <c r="B2" s="78" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="78"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3" s="21" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15" x14ac:dyDescent="0.25">
@@ -5090,7 +5537,7 @@
     </row>
     <row r="5" spans="1:4" ht="57" x14ac:dyDescent="0.2">
       <c r="B5" s="7" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D5" s="5"/>
     </row>
@@ -5104,13 +5551,13 @@
     </row>
     <row r="8" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="B8" s="19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D8" s="5"/>
     </row>
     <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.2">
       <c r="B9" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D9" s="5"/>
     </row>
@@ -5141,14 +5588,14 @@
     </row>
     <row r="15" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A15" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="7"/>
       <c r="D15" s="5"/>
     </row>
     <row r="16" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B16" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D16" s="5"/>
     </row>
@@ -5158,14 +5605,14 @@
     </row>
     <row r="18" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B18" s="7"/>
       <c r="D18" s="5"/>
     </row>
     <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.2">
       <c r="B19" s="7" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D19" s="5"/>
     </row>
@@ -5182,7 +5629,7 @@
     </row>
     <row r="22" spans="1:4" ht="42.75" x14ac:dyDescent="0.2">
       <c r="B22" s="7" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -5195,18 +5642,18 @@
     </row>
     <row r="26" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="7"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
       <c r="B27" s="7" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B28" s="56" t="s">
-        <v>31</v>
+      <c r="B28" s="54" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -5238,7 +5685,7 @@
     <row r="1" spans="1:3" ht="35.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="22"/>
       <c r="B1" s="23" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C1" s="24"/>
     </row>
@@ -5250,14 +5697,14 @@
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="22"/>
       <c r="B3" s="26" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C3" s="24"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="31" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C4" s="24"/>
     </row>
@@ -5269,7 +5716,7 @@
     <row r="6" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="28" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C6" s="24"/>
     </row>
@@ -5293,7 +5740,7 @@
     <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="22"/>
       <c r="B10" s="27" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C10" s="24"/>
     </row>
@@ -5305,7 +5752,7 @@
     <row r="12" spans="1:3" ht="30" x14ac:dyDescent="0.2">
       <c r="A12" s="22"/>
       <c r="B12" s="27" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" s="24"/>
     </row>
@@ -5328,8 +5775,8 @@
     </row>
     <row r="16" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
-      <c r="B16" s="54" t="s">
-        <v>29</v>
+      <c r="B16" s="52" t="s">
+        <v>28</v>
       </c>
       <c r="C16" s="24"/>
     </row>

</xml_diff>

<commit_message>
Updating the software context diagram  for GDD Updating input/output signals  for GDD Updating requirement coverage for GDD Adding the equivalent numerical values for API inputs and returns for CDD and GDD Updating Project Plan
Signed-off-by: May Alaa <mayelfkiy@gmail.com>
</commit_message>
<xml_diff>
--- a/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
+++ b/SW deliveries log/Project_Plan/PO2EBL_Project_Plan.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="107">
   <si>
     <t>HELP</t>
   </si>
@@ -326,6 +326,42 @@
   </si>
   <si>
     <t>Week 5</t>
+  </si>
+  <si>
+    <t>Week 6</t>
+  </si>
+  <si>
+    <t>GDD Document Update</t>
+  </si>
+  <si>
+    <t>Updating GDD document considering the review points</t>
+  </si>
+  <si>
+    <t>CDD Document Update</t>
+  </si>
+  <si>
+    <t>Updating CDD document considering the review points</t>
+  </si>
+  <si>
+    <t>May, Ibrahem</t>
+  </si>
+  <si>
+    <t>CDD Cross Review</t>
+  </si>
+  <si>
+    <t>Phase 2: Implementation</t>
+  </si>
+  <si>
+    <t>Desigining the Blender Body on solid works</t>
+  </si>
+  <si>
+    <t>Outer body design</t>
+  </si>
+  <si>
+    <t>Dimension Calculations</t>
+  </si>
+  <si>
+    <t>RTM Update</t>
   </si>
 </sst>
 </file>
@@ -746,7 +782,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="78">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -910,15 +946,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -958,35 +985,16 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="51">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
+  <dxfs count="70">
     <dxf>
       <border>
         <left style="thin">
@@ -1023,52 +1031,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -1081,52 +1043,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF3969AD"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="darkUp">
-          <fgColor theme="1" tint="0.499984740745262"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <border>
-        <right style="thin">
-          <color theme="0" tint="-0.14996795556505021"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
       <border>
         <left style="thin">
           <color rgb="FFC00000"/>
@@ -1209,6 +1125,18 @@
       </border>
     </dxf>
     <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FF3969AD"/>
@@ -1249,6 +1177,298 @@
       <border>
         <right style="thin">
           <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF3969AD"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="darkUp">
+          <fgColor theme="1" tint="0.499984740745262"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border>
+        <right style="thin">
+          <color theme="0" tint="-0.14996795556505021"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
+        </right>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <left style="thin">
+          <color rgb="FFC00000"/>
+        </left>
+        <right style="thin">
+          <color rgb="FFC00000"/>
         </right>
         <vertical/>
         <horizontal/>
@@ -1421,15 +1641,15 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="ToDoList" pivot="0" count="9">
-      <tableStyleElement type="wholeTable" dxfId="50"/>
-      <tableStyleElement type="headerRow" dxfId="49"/>
-      <tableStyleElement type="totalRow" dxfId="48"/>
-      <tableStyleElement type="firstColumn" dxfId="47"/>
-      <tableStyleElement type="lastColumn" dxfId="46"/>
-      <tableStyleElement type="firstRowStripe" dxfId="45"/>
-      <tableStyleElement type="secondRowStripe" dxfId="44"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="43"/>
-      <tableStyleElement type="secondColumnStripe" dxfId="42"/>
+      <tableStyleElement type="wholeTable" dxfId="69"/>
+      <tableStyleElement type="headerRow" dxfId="68"/>
+      <tableStyleElement type="totalRow" dxfId="67"/>
+      <tableStyleElement type="firstColumn" dxfId="66"/>
+      <tableStyleElement type="lastColumn" dxfId="65"/>
+      <tableStyleElement type="firstRowStripe" dxfId="64"/>
+      <tableStyleElement type="secondRowStripe" dxfId="63"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="62"/>
+      <tableStyleElement type="secondColumnStripe" dxfId="61"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1551,7 +1771,7 @@
                   <a14:compatExt spid="_x0000_s6145"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000001180000}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000001180000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -1601,7 +1821,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1656,7 +1876,7 @@
         <xdr:cNvPr id="2" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1957,15 +2177,15 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BK75"/>
+  <dimension ref="A1:BK79"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A48" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
-      <selection activeCell="A51" sqref="A51"/>
+    <sheetView showGridLines="0" tabSelected="1" showRuler="0" topLeftCell="A57" zoomScaleNormal="100" zoomScalePageLayoutView="70" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="20.5" customWidth="1"/>
+    <col min="1" max="1" width="23.25" customWidth="1"/>
     <col min="2" max="2" width="49.375" style="58" customWidth="1"/>
     <col min="3" max="3" width="13.25" customWidth="1"/>
     <col min="4" max="4" width="9.5" style="10" customWidth="1"/>
@@ -2006,10 +2226,10 @@
     <row r="4" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="57"/>
       <c r="B4" s="57"/>
-      <c r="D4" s="76">
+      <c r="D4" s="73">
         <v>43851</v>
       </c>
-      <c r="E4" s="77"/>
+      <c r="E4" s="74"/>
     </row>
     <row r="5" spans="1:63" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="D5" s="48" t="s">
@@ -4681,582 +4901,986 @@
       <c r="BI41" s="16"/>
       <c r="BJ41" s="16"/>
     </row>
-    <row r="42" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="66" t="s">
+    <row r="42" spans="1:62" s="58" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B42" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C42" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D42" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E42" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F42" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G42" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H42" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I42" s="36"/>
+      <c r="J42" s="36"/>
+      <c r="K42" s="36"/>
+      <c r="L42" s="36"/>
+      <c r="M42" s="36"/>
+      <c r="N42" s="36"/>
+      <c r="O42" s="36"/>
+      <c r="P42" s="36"/>
+      <c r="Q42" s="36"/>
+      <c r="R42" s="36"/>
+      <c r="S42" s="36"/>
+      <c r="T42" s="36"/>
+      <c r="U42" s="36"/>
+      <c r="V42" s="36"/>
+      <c r="W42" s="36"/>
+      <c r="X42" s="36"/>
+      <c r="Y42" s="36"/>
+      <c r="Z42" s="36"/>
+      <c r="AA42" s="36"/>
+      <c r="AB42" s="36"/>
+      <c r="AC42" s="36"/>
+      <c r="AD42" s="36"/>
+      <c r="AE42" s="36"/>
+      <c r="AF42" s="36"/>
+      <c r="AG42" s="36"/>
+      <c r="AH42" s="36"/>
+      <c r="AI42" s="36"/>
+      <c r="AJ42" s="36"/>
+      <c r="AK42" s="36"/>
+      <c r="AL42" s="36"/>
+      <c r="AM42" s="36"/>
+      <c r="AN42" s="36"/>
+      <c r="AO42" s="36"/>
+      <c r="AP42" s="36"/>
+      <c r="AQ42" s="36"/>
+      <c r="AR42" s="36"/>
+      <c r="AS42" s="36"/>
+      <c r="AT42" s="36"/>
+      <c r="AU42" s="36"/>
+      <c r="AV42" s="36"/>
+      <c r="AW42" s="36"/>
+      <c r="AX42" s="36"/>
+      <c r="AY42" s="36"/>
+      <c r="AZ42" s="36"/>
+      <c r="BA42" s="36"/>
+      <c r="BB42" s="36"/>
+      <c r="BC42" s="36"/>
+      <c r="BD42" s="36"/>
+      <c r="BE42" s="36"/>
+      <c r="BF42" s="36"/>
+      <c r="BG42" s="36"/>
+      <c r="BH42" s="36"/>
+      <c r="BI42" s="36"/>
+      <c r="BJ42" s="36"/>
+    </row>
+    <row r="43" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="B42" s="66"/>
-      <c r="C42" s="67"/>
-      <c r="D42" s="68"/>
-      <c r="E42" s="69"/>
-      <c r="F42" s="44"/>
-      <c r="G42" s="45"/>
-      <c r="H42" s="50"/>
-      <c r="I42" s="16"/>
-      <c r="J42" s="16"/>
-      <c r="K42" s="16"/>
-      <c r="L42" s="16"/>
-      <c r="M42" s="16"/>
-      <c r="N42" s="16"/>
-      <c r="O42" s="16"/>
-      <c r="P42" s="16"/>
-      <c r="Q42" s="16"/>
-      <c r="R42" s="16"/>
-      <c r="S42" s="16"/>
-      <c r="T42" s="16"/>
-      <c r="U42" s="16"/>
-      <c r="V42" s="16"/>
-      <c r="W42" s="16"/>
-      <c r="X42" s="16"/>
-      <c r="Y42" s="16"/>
-      <c r="Z42" s="16"/>
-      <c r="AA42" s="16"/>
-      <c r="AB42" s="16"/>
-      <c r="AC42" s="16"/>
-      <c r="AD42" s="16"/>
-      <c r="AE42" s="16"/>
-      <c r="AF42" s="16"/>
-      <c r="AG42" s="16"/>
-      <c r="AH42" s="16"/>
-      <c r="AI42" s="16"/>
-      <c r="AJ42" s="16"/>
-      <c r="AK42" s="16"/>
-      <c r="AL42" s="16"/>
-      <c r="AM42" s="16"/>
-      <c r="AN42" s="16"/>
-      <c r="AO42" s="16"/>
-      <c r="AP42" s="16"/>
-      <c r="AQ42" s="16"/>
-      <c r="AR42" s="16"/>
-      <c r="AS42" s="16"/>
-      <c r="AT42" s="16"/>
-      <c r="AU42" s="16"/>
-      <c r="AV42" s="16"/>
-      <c r="AW42" s="16"/>
-      <c r="AX42" s="16"/>
-      <c r="AY42" s="16"/>
-      <c r="AZ42" s="16"/>
-      <c r="BA42" s="16"/>
-      <c r="BB42" s="16"/>
-      <c r="BC42" s="16"/>
-      <c r="BD42" s="16"/>
-      <c r="BE42" s="16"/>
-      <c r="BF42" s="16"/>
-      <c r="BG42" s="16"/>
-      <c r="BH42" s="16"/>
-      <c r="BI42" s="16"/>
-      <c r="BJ42" s="16"/>
-    </row>
-    <row r="43" spans="1:62" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="70" t="s">
+      <c r="B43" s="63"/>
+      <c r="C43" s="64"/>
+      <c r="D43" s="65"/>
+      <c r="E43" s="66"/>
+      <c r="F43" s="44"/>
+      <c r="G43" s="45"/>
+      <c r="H43" s="50"/>
+      <c r="I43" s="16"/>
+      <c r="J43" s="16"/>
+      <c r="K43" s="16"/>
+      <c r="L43" s="16"/>
+      <c r="M43" s="16"/>
+      <c r="N43" s="16"/>
+      <c r="O43" s="16"/>
+      <c r="P43" s="16"/>
+      <c r="Q43" s="16"/>
+      <c r="R43" s="16"/>
+      <c r="S43" s="16"/>
+      <c r="T43" s="16"/>
+      <c r="U43" s="16"/>
+      <c r="V43" s="16"/>
+      <c r="W43" s="16"/>
+      <c r="X43" s="16"/>
+      <c r="Y43" s="16"/>
+      <c r="Z43" s="16"/>
+      <c r="AA43" s="16"/>
+      <c r="AB43" s="16"/>
+      <c r="AC43" s="16"/>
+      <c r="AD43" s="16"/>
+      <c r="AE43" s="16"/>
+      <c r="AF43" s="16"/>
+      <c r="AG43" s="16"/>
+      <c r="AH43" s="16"/>
+      <c r="AI43" s="16"/>
+      <c r="AJ43" s="16"/>
+      <c r="AK43" s="16"/>
+      <c r="AL43" s="16"/>
+      <c r="AM43" s="16"/>
+      <c r="AN43" s="16"/>
+      <c r="AO43" s="16"/>
+      <c r="AP43" s="16"/>
+      <c r="AQ43" s="16"/>
+      <c r="AR43" s="16"/>
+      <c r="AS43" s="16"/>
+      <c r="AT43" s="16"/>
+      <c r="AU43" s="16"/>
+      <c r="AV43" s="16"/>
+      <c r="AW43" s="16"/>
+      <c r="AX43" s="16"/>
+      <c r="AY43" s="16"/>
+      <c r="AZ43" s="16"/>
+      <c r="BA43" s="16"/>
+      <c r="BB43" s="16"/>
+      <c r="BC43" s="16"/>
+      <c r="BD43" s="16"/>
+      <c r="BE43" s="16"/>
+      <c r="BF43" s="16"/>
+      <c r="BG43" s="16"/>
+      <c r="BH43" s="16"/>
+      <c r="BI43" s="16"/>
+      <c r="BJ43" s="16"/>
+    </row>
+    <row r="44" spans="1:62" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="67" t="s">
         <v>73</v>
       </c>
-      <c r="B43" s="70" t="s">
+      <c r="B44" s="67" t="s">
         <v>76</v>
       </c>
-      <c r="C43" s="71" t="s">
+      <c r="C44" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="72">
+      <c r="D44" s="69">
         <v>43882</v>
       </c>
-      <c r="E43" s="73">
+      <c r="E44" s="70">
         <v>43883</v>
       </c>
-      <c r="F43" s="72">
+      <c r="F44" s="69">
         <v>43882</v>
       </c>
-      <c r="G43" s="73">
+      <c r="G44" s="70">
         <v>43883</v>
       </c>
-      <c r="H43" s="49"/>
-    </row>
-    <row r="44" spans="1:62" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="70" t="s">
+      <c r="H44" s="49"/>
+    </row>
+    <row r="45" spans="1:62" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="67" t="s">
         <v>75</v>
       </c>
-      <c r="B44" s="70" t="s">
+      <c r="B45" s="67" t="s">
         <v>77</v>
       </c>
-      <c r="C44" s="71" t="s">
+      <c r="C45" s="68" t="s">
         <v>39</v>
       </c>
-      <c r="D44" s="72">
+      <c r="D45" s="69">
         <v>43883</v>
       </c>
-      <c r="E44" s="73">
+      <c r="E45" s="70">
         <v>43884</v>
       </c>
-      <c r="F44" s="72">
+      <c r="F45" s="69">
         <v>43883</v>
       </c>
-      <c r="G44" s="73">
+      <c r="G45" s="70">
         <v>43884</v>
       </c>
-      <c r="H44" s="49"/>
-    </row>
-    <row r="45" spans="1:62" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="70" t="s">
+      <c r="H45" s="49"/>
+    </row>
+    <row r="46" spans="1:62" ht="29.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="67" t="s">
         <v>74</v>
       </c>
-      <c r="B45" s="70" t="s">
+      <c r="B46" s="67" t="s">
         <v>83</v>
       </c>
-      <c r="C45" s="71" t="s">
+      <c r="C46" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="D45" s="72">
+      <c r="D46" s="69">
         <v>43883</v>
       </c>
-      <c r="E45" s="73">
+      <c r="E46" s="70">
         <v>43884</v>
       </c>
-      <c r="F45" s="72">
+      <c r="F46" s="69">
         <v>43888</v>
       </c>
-      <c r="G45" s="73">
+      <c r="G46" s="70">
         <v>43889</v>
       </c>
-      <c r="H45" s="49"/>
-    </row>
-    <row r="46" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="74" t="s">
+      <c r="H46" s="49"/>
+    </row>
+    <row r="47" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="71" t="s">
         <v>78</v>
       </c>
-      <c r="B46" s="70" t="s">
+      <c r="B47" s="67" t="s">
         <v>82</v>
       </c>
-      <c r="C46" s="71" t="s">
+      <c r="C47" s="68" t="s">
         <v>80</v>
       </c>
-      <c r="D46" s="72">
+      <c r="D47" s="69">
         <v>43884</v>
       </c>
-      <c r="E46" s="73">
+      <c r="E47" s="70">
         <v>43887</v>
       </c>
-      <c r="F46" s="59"/>
-    </row>
-    <row r="47" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="74" t="s">
+      <c r="F47" s="59"/>
+    </row>
+    <row r="48" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="71" t="s">
         <v>79</v>
       </c>
-      <c r="B47" s="70"/>
-      <c r="C47" s="71" t="s">
+      <c r="B48" s="67"/>
+      <c r="C48" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D47" s="72">
+      <c r="D48" s="69">
         <v>43887</v>
       </c>
-      <c r="E47" s="73">
+      <c r="E48" s="70">
         <v>43888</v>
       </c>
     </row>
-    <row r="48" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="70" t="s">
+    <row r="49" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="67" t="s">
         <v>49</v>
       </c>
-      <c r="B48" s="70"/>
-      <c r="C48" s="71" t="s">
+      <c r="B49" s="67"/>
+      <c r="C49" s="68" t="s">
         <v>42</v>
       </c>
-      <c r="D48" s="72">
+      <c r="D49" s="69">
         <v>43883</v>
       </c>
-      <c r="E48" s="73">
+      <c r="E49" s="70">
         <v>43883</v>
       </c>
-      <c r="F48" s="72">
+      <c r="F49" s="69">
         <v>43883</v>
       </c>
-      <c r="G48" s="73">
+      <c r="G49" s="70">
         <v>43883</v>
       </c>
-      <c r="H48" s="49"/>
-    </row>
-    <row r="49" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="70" t="s">
+      <c r="H49" s="49"/>
+    </row>
+    <row r="50" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="67" t="s">
         <v>50</v>
       </c>
-      <c r="B49" s="70"/>
-      <c r="C49" s="71" t="s">
+      <c r="B50" s="67"/>
+      <c r="C50" s="68" t="s">
         <v>56</v>
       </c>
-      <c r="D49" s="72">
+      <c r="D50" s="69">
         <v>43884</v>
       </c>
-      <c r="E49" s="73">
+      <c r="E50" s="70">
         <v>43884</v>
       </c>
-      <c r="F49" s="46"/>
-      <c r="G49" s="47"/>
-      <c r="H49" s="51" t="str">
-        <f>IF(OR(ISBLANK(F49),ISBLANK(G49)),"",G49-F49+1)</f>
+      <c r="F50" s="46"/>
+      <c r="G50" s="47"/>
+      <c r="H50" s="51" t="str">
+        <f>IF(OR(ISBLANK(F50),ISBLANK(G50)),"",G50-F50+1)</f>
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="70" t="s">
+    <row r="51" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="67" t="s">
         <v>81</v>
       </c>
-      <c r="B50" s="70"/>
-      <c r="C50" s="71" t="s">
+      <c r="B51" s="67"/>
+      <c r="C51" s="68" t="s">
         <v>46</v>
       </c>
-      <c r="D50" s="72">
+      <c r="D51" s="69">
         <v>43884</v>
       </c>
-      <c r="E50" s="73">
+      <c r="E51" s="70">
         <v>43884</v>
       </c>
     </row>
-    <row r="51" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="66" t="s">
+    <row r="52" spans="1:62" s="58" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B52" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C52" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D52" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E52" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G52" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H52" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I52" s="36"/>
+      <c r="J52" s="36"/>
+      <c r="K52" s="36"/>
+      <c r="L52" s="36"/>
+      <c r="M52" s="36"/>
+      <c r="N52" s="36"/>
+      <c r="O52" s="36"/>
+      <c r="P52" s="36"/>
+      <c r="Q52" s="36"/>
+      <c r="R52" s="36"/>
+      <c r="S52" s="36"/>
+      <c r="T52" s="36"/>
+      <c r="U52" s="36"/>
+      <c r="V52" s="36"/>
+      <c r="W52" s="36"/>
+      <c r="X52" s="36"/>
+      <c r="Y52" s="36"/>
+      <c r="Z52" s="36"/>
+      <c r="AA52" s="36"/>
+      <c r="AB52" s="36"/>
+      <c r="AC52" s="36"/>
+      <c r="AD52" s="36"/>
+      <c r="AE52" s="36"/>
+      <c r="AF52" s="36"/>
+      <c r="AG52" s="36"/>
+      <c r="AH52" s="36"/>
+      <c r="AI52" s="36"/>
+      <c r="AJ52" s="36"/>
+      <c r="AK52" s="36"/>
+      <c r="AL52" s="36"/>
+      <c r="AM52" s="36"/>
+      <c r="AN52" s="36"/>
+      <c r="AO52" s="36"/>
+      <c r="AP52" s="36"/>
+      <c r="AQ52" s="36"/>
+      <c r="AR52" s="36"/>
+      <c r="AS52" s="36"/>
+      <c r="AT52" s="36"/>
+      <c r="AU52" s="36"/>
+      <c r="AV52" s="36"/>
+      <c r="AW52" s="36"/>
+      <c r="AX52" s="36"/>
+      <c r="AY52" s="36"/>
+      <c r="AZ52" s="36"/>
+      <c r="BA52" s="36"/>
+      <c r="BB52" s="36"/>
+      <c r="BC52" s="36"/>
+      <c r="BD52" s="36"/>
+      <c r="BE52" s="36"/>
+      <c r="BF52" s="36"/>
+      <c r="BG52" s="36"/>
+      <c r="BH52" s="36"/>
+      <c r="BI52" s="36"/>
+      <c r="BJ52" s="36"/>
+    </row>
+    <row r="53" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="66"/>
-      <c r="C51" s="67"/>
-      <c r="D51" s="68"/>
-      <c r="E51" s="69"/>
-      <c r="F51" s="44"/>
-      <c r="G51" s="45"/>
-      <c r="H51" s="50"/>
-      <c r="I51" s="16"/>
-      <c r="J51" s="16"/>
-      <c r="K51" s="16"/>
-      <c r="L51" s="16"/>
-      <c r="M51" s="16"/>
-      <c r="N51" s="16"/>
-      <c r="O51" s="16"/>
-      <c r="P51" s="16"/>
-      <c r="Q51" s="16"/>
-      <c r="R51" s="16"/>
-      <c r="S51" s="16"/>
-      <c r="T51" s="16"/>
-      <c r="U51" s="16"/>
-      <c r="V51" s="16"/>
-      <c r="W51" s="16"/>
-      <c r="X51" s="16"/>
-      <c r="Y51" s="16"/>
-      <c r="Z51" s="16"/>
-      <c r="AA51" s="16"/>
-      <c r="AB51" s="16"/>
-      <c r="AC51" s="16"/>
-      <c r="AD51" s="16"/>
-      <c r="AE51" s="16"/>
-      <c r="AF51" s="16"/>
-      <c r="AG51" s="16"/>
-      <c r="AH51" s="16"/>
-      <c r="AI51" s="16"/>
-      <c r="AJ51" s="16"/>
-      <c r="AK51" s="16"/>
-      <c r="AL51" s="16"/>
-      <c r="AM51" s="16"/>
-      <c r="AN51" s="16"/>
-      <c r="AO51" s="16"/>
-      <c r="AP51" s="16"/>
-      <c r="AQ51" s="16"/>
-      <c r="AR51" s="16"/>
-      <c r="AS51" s="16"/>
-      <c r="AT51" s="16"/>
-      <c r="AU51" s="16"/>
-      <c r="AV51" s="16"/>
-      <c r="AW51" s="16"/>
-      <c r="AX51" s="16"/>
-      <c r="AY51" s="16"/>
-      <c r="AZ51" s="16"/>
-      <c r="BA51" s="16"/>
-      <c r="BB51" s="16"/>
-      <c r="BC51" s="16"/>
-      <c r="BD51" s="16"/>
-      <c r="BE51" s="16"/>
-      <c r="BF51" s="16"/>
-      <c r="BG51" s="16"/>
-      <c r="BH51" s="16"/>
-      <c r="BI51" s="16"/>
-      <c r="BJ51" s="16"/>
-    </row>
-    <row r="52" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="75" t="s">
+      <c r="B53" s="63"/>
+      <c r="C53" s="64"/>
+      <c r="D53" s="65"/>
+      <c r="E53" s="66"/>
+      <c r="F53" s="44"/>
+      <c r="G53" s="45"/>
+      <c r="H53" s="50"/>
+      <c r="I53" s="16"/>
+      <c r="J53" s="16"/>
+      <c r="K53" s="16"/>
+      <c r="L53" s="16"/>
+      <c r="M53" s="16"/>
+      <c r="N53" s="16"/>
+      <c r="O53" s="16"/>
+      <c r="P53" s="16"/>
+      <c r="Q53" s="16"/>
+      <c r="R53" s="16"/>
+      <c r="S53" s="16"/>
+      <c r="T53" s="16"/>
+      <c r="U53" s="16"/>
+      <c r="V53" s="16"/>
+      <c r="W53" s="16"/>
+      <c r="X53" s="16"/>
+      <c r="Y53" s="16"/>
+      <c r="Z53" s="16"/>
+      <c r="AA53" s="16"/>
+      <c r="AB53" s="16"/>
+      <c r="AC53" s="16"/>
+      <c r="AD53" s="16"/>
+      <c r="AE53" s="16"/>
+      <c r="AF53" s="16"/>
+      <c r="AG53" s="16"/>
+      <c r="AH53" s="16"/>
+      <c r="AI53" s="16"/>
+      <c r="AJ53" s="16"/>
+      <c r="AK53" s="16"/>
+      <c r="AL53" s="16"/>
+      <c r="AM53" s="16"/>
+      <c r="AN53" s="16"/>
+      <c r="AO53" s="16"/>
+      <c r="AP53" s="16"/>
+      <c r="AQ53" s="16"/>
+      <c r="AR53" s="16"/>
+      <c r="AS53" s="16"/>
+      <c r="AT53" s="16"/>
+      <c r="AU53" s="16"/>
+      <c r="AV53" s="16"/>
+      <c r="AW53" s="16"/>
+      <c r="AX53" s="16"/>
+      <c r="AY53" s="16"/>
+      <c r="AZ53" s="16"/>
+      <c r="BA53" s="16"/>
+      <c r="BB53" s="16"/>
+      <c r="BC53" s="16"/>
+      <c r="BD53" s="16"/>
+      <c r="BE53" s="16"/>
+      <c r="BF53" s="16"/>
+      <c r="BG53" s="16"/>
+      <c r="BH53" s="16"/>
+      <c r="BI53" s="16"/>
+      <c r="BJ53" s="16"/>
+    </row>
+    <row r="54" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="72" t="s">
         <v>84</v>
       </c>
-      <c r="B52" s="70" t="s">
+      <c r="B54" s="67" t="s">
         <v>86</v>
       </c>
-      <c r="C52" s="71" t="s">
+      <c r="C54" s="68" t="s">
         <v>43</v>
       </c>
-      <c r="D52" s="72">
+      <c r="D54" s="69">
         <v>43890</v>
       </c>
-      <c r="E52" s="72">
+      <c r="E54" s="69">
         <v>43891</v>
-      </c>
-      <c r="F52" s="42"/>
-      <c r="G52" s="43"/>
-      <c r="H52" s="49"/>
-    </row>
-    <row r="53" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A53" s="75" t="s">
-        <v>88</v>
-      </c>
-      <c r="B53" s="70" t="s">
-        <v>89</v>
-      </c>
-      <c r="C53" s="71" t="s">
-        <v>87</v>
-      </c>
-      <c r="D53" s="72">
-        <v>43889</v>
-      </c>
-      <c r="E53" s="73">
-        <v>43890</v>
-      </c>
-      <c r="F53" s="72">
-        <v>43889</v>
-      </c>
-      <c r="G53" s="73">
-        <v>43890</v>
-      </c>
-      <c r="H53" s="49"/>
-    </row>
-    <row r="54" spans="1:62" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="75" t="s">
-        <v>84</v>
-      </c>
-      <c r="B54" s="70" t="s">
-        <v>85</v>
-      </c>
-      <c r="C54" s="71" t="s">
-        <v>52</v>
-      </c>
-      <c r="D54" s="72">
-        <v>43891</v>
-      </c>
-      <c r="E54" s="73">
-        <v>43892</v>
       </c>
       <c r="F54" s="42"/>
       <c r="G54" s="43"/>
       <c r="H54" s="49"/>
     </row>
-    <row r="55" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="75" t="s">
-        <v>92</v>
-      </c>
-      <c r="B55" s="70"/>
-      <c r="C55" s="71" t="s">
-        <v>56</v>
-      </c>
-      <c r="D55" s="72">
+    <row r="55" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="72" t="s">
+        <v>88</v>
+      </c>
+      <c r="B55" s="67" t="s">
+        <v>89</v>
+      </c>
+      <c r="C55" s="68" t="s">
+        <v>87</v>
+      </c>
+      <c r="D55" s="69">
+        <v>43889</v>
+      </c>
+      <c r="E55" s="70">
+        <v>43890</v>
+      </c>
+      <c r="F55" s="69">
+        <v>43889</v>
+      </c>
+      <c r="G55" s="70">
+        <v>43890</v>
+      </c>
+      <c r="H55" s="49"/>
+    </row>
+    <row r="56" spans="1:62" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="72" t="s">
+        <v>84</v>
+      </c>
+      <c r="B56" s="67" t="s">
+        <v>85</v>
+      </c>
+      <c r="C56" s="68" t="s">
+        <v>52</v>
+      </c>
+      <c r="D56" s="69">
+        <v>43891</v>
+      </c>
+      <c r="E56" s="70">
         <v>43892</v>
-      </c>
-      <c r="E55" s="73">
-        <v>43892</v>
-      </c>
-      <c r="F55" s="42"/>
-      <c r="G55" s="43"/>
-      <c r="H55" s="49"/>
-    </row>
-    <row r="56" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="38" t="s">
-        <v>90</v>
-      </c>
-      <c r="B56" s="40"/>
-      <c r="C56" s="38" t="s">
-        <v>91</v>
-      </c>
-      <c r="D56" s="42">
-        <v>43893</v>
-      </c>
-      <c r="E56" s="43">
-        <v>43895</v>
       </c>
       <c r="F56" s="42"/>
       <c r="G56" s="43"/>
       <c r="H56" s="49"/>
     </row>
-    <row r="57" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="38" t="s">
-        <v>93</v>
-      </c>
-      <c r="B57" s="40"/>
-      <c r="C57" s="38" t="s">
-        <v>39</v>
-      </c>
-      <c r="D57" s="42">
-        <v>43893</v>
-      </c>
-      <c r="E57" s="43">
-        <v>43895</v>
+    <row r="57" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="B57" s="67"/>
+      <c r="C57" s="68" t="s">
+        <v>56</v>
+      </c>
+      <c r="D57" s="69">
+        <v>43892</v>
+      </c>
+      <c r="E57" s="70">
+        <v>43892</v>
       </c>
       <c r="F57" s="42"/>
       <c r="G57" s="43"/>
       <c r="H57" s="49"/>
     </row>
     <row r="58" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="15"/>
-      <c r="B58" s="15"/>
-      <c r="C58" s="38"/>
-      <c r="D58" s="42"/>
-      <c r="E58" s="43"/>
+      <c r="A58" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="B58" s="40"/>
+      <c r="C58" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="D58" s="42">
+        <v>43893</v>
+      </c>
+      <c r="E58" s="43">
+        <v>43895</v>
+      </c>
       <c r="F58" s="42"/>
       <c r="G58" s="43"/>
-      <c r="H58" s="49" t="str">
-        <f>IF(OR(ISBLANK(F58),ISBLANK(G58)),"",G58-F58+1)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="59" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A59" s="15"/>
-      <c r="B59" s="61"/>
-      <c r="C59" s="38"/>
-      <c r="D59" s="42"/>
-      <c r="E59" s="43"/>
+      <c r="H58" s="49"/>
+    </row>
+    <row r="59" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="38" t="s">
+        <v>93</v>
+      </c>
+      <c r="B59" s="40"/>
+      <c r="C59" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D59" s="42">
+        <v>43893</v>
+      </c>
+      <c r="E59" s="43">
+        <v>43895</v>
+      </c>
       <c r="F59" s="42"/>
       <c r="G59" s="43"/>
       <c r="H59" s="49"/>
-      <c r="I59" s="58"/>
-    </row>
-    <row r="60" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="15"/>
-      <c r="B60" s="61"/>
-      <c r="C60" s="38"/>
-      <c r="D60" s="42"/>
-      <c r="E60" s="43"/>
-      <c r="F60" s="42"/>
-      <c r="G60" s="43"/>
-      <c r="H60" s="49"/>
-      <c r="I60" s="58"/>
-    </row>
-    <row r="61" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="40"/>
-      <c r="B61" s="62"/>
-      <c r="C61" s="38"/>
-      <c r="D61" s="42"/>
-      <c r="E61" s="43"/>
-      <c r="F61" s="42"/>
-      <c r="G61" s="43"/>
-      <c r="H61" s="49"/>
-      <c r="I61" s="58"/>
+    </row>
+    <row r="60" spans="1:62" s="58" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B60" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C60" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D60" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E60" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G60" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H60" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I60" s="36"/>
+      <c r="J60" s="36"/>
+      <c r="K60" s="36"/>
+      <c r="L60" s="36"/>
+      <c r="M60" s="36"/>
+      <c r="N60" s="36"/>
+      <c r="O60" s="36"/>
+      <c r="P60" s="36"/>
+      <c r="Q60" s="36"/>
+      <c r="R60" s="36"/>
+      <c r="S60" s="36"/>
+      <c r="T60" s="36"/>
+      <c r="U60" s="36"/>
+      <c r="V60" s="36"/>
+      <c r="W60" s="36"/>
+      <c r="X60" s="36"/>
+      <c r="Y60" s="36"/>
+      <c r="Z60" s="36"/>
+      <c r="AA60" s="36"/>
+      <c r="AB60" s="36"/>
+      <c r="AC60" s="36"/>
+      <c r="AD60" s="36"/>
+      <c r="AE60" s="36"/>
+      <c r="AF60" s="36"/>
+      <c r="AG60" s="36"/>
+      <c r="AH60" s="36"/>
+      <c r="AI60" s="36"/>
+      <c r="AJ60" s="36"/>
+      <c r="AK60" s="36"/>
+      <c r="AL60" s="36"/>
+      <c r="AM60" s="36"/>
+      <c r="AN60" s="36"/>
+      <c r="AO60" s="36"/>
+      <c r="AP60" s="36"/>
+      <c r="AQ60" s="36"/>
+      <c r="AR60" s="36"/>
+      <c r="AS60" s="36"/>
+      <c r="AT60" s="36"/>
+      <c r="AU60" s="36"/>
+      <c r="AV60" s="36"/>
+      <c r="AW60" s="36"/>
+      <c r="AX60" s="36"/>
+      <c r="AY60" s="36"/>
+      <c r="AZ60" s="36"/>
+      <c r="BA60" s="36"/>
+      <c r="BB60" s="36"/>
+      <c r="BC60" s="36"/>
+      <c r="BD60" s="36"/>
+      <c r="BE60" s="36"/>
+      <c r="BF60" s="36"/>
+      <c r="BG60" s="36"/>
+      <c r="BH60" s="36"/>
+      <c r="BI60" s="36"/>
+      <c r="BJ60" s="36"/>
+    </row>
+    <row r="61" spans="1:62" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="63" t="s">
+        <v>95</v>
+      </c>
+      <c r="B61" s="63"/>
+      <c r="C61" s="64"/>
+      <c r="D61" s="65"/>
+      <c r="E61" s="66"/>
+      <c r="F61" s="44"/>
+      <c r="G61" s="45"/>
+      <c r="H61" s="50"/>
     </row>
     <row r="62" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="40"/>
-      <c r="B62" s="40"/>
-      <c r="C62" s="38"/>
-      <c r="D62" s="42"/>
-      <c r="E62" s="43"/>
-      <c r="F62" s="42"/>
-      <c r="G62" s="43"/>
+      <c r="A62" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="B62" s="61" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D62" s="42">
+        <v>43985</v>
+      </c>
+      <c r="E62" s="43">
+        <v>44077</v>
+      </c>
+      <c r="F62" s="42">
+        <v>43985</v>
+      </c>
+      <c r="G62" s="43">
+        <v>44077</v>
+      </c>
       <c r="H62" s="49"/>
       <c r="I62" s="58"/>
     </row>
     <row r="63" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="40"/>
-      <c r="B63" s="40"/>
-      <c r="C63" s="38"/>
-      <c r="D63" s="42"/>
-      <c r="E63" s="43"/>
-      <c r="F63" s="42"/>
-      <c r="G63" s="43"/>
+      <c r="A63" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="B63" s="61" t="s">
+        <v>99</v>
+      </c>
+      <c r="C63" s="38" t="s">
+        <v>100</v>
+      </c>
+      <c r="D63" s="42">
+        <v>43985</v>
+      </c>
+      <c r="E63" s="43">
+        <v>44077</v>
+      </c>
+      <c r="F63" s="42">
+        <v>43985</v>
+      </c>
+      <c r="G63" s="43">
+        <v>44077</v>
+      </c>
       <c r="H63" s="49"/>
       <c r="I63" s="58"/>
     </row>
     <row r="64" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="15"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="38"/>
-      <c r="D64" s="42"/>
-      <c r="E64" s="43"/>
+      <c r="A64" s="72" t="s">
+        <v>92</v>
+      </c>
+      <c r="B64" s="62"/>
+      <c r="C64" s="38" t="s">
+        <v>56</v>
+      </c>
+      <c r="D64" s="42">
+        <v>44077</v>
+      </c>
+      <c r="E64" s="43">
+        <v>44107</v>
+      </c>
       <c r="F64" s="42"/>
       <c r="G64" s="43"/>
       <c r="H64" s="49"/>
       <c r="I64" s="58"/>
     </row>
-    <row r="65" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="15"/>
-      <c r="B65" s="15"/>
-      <c r="C65" s="38"/>
-      <c r="D65" s="42"/>
-      <c r="E65" s="43"/>
-      <c r="F65" s="46"/>
-      <c r="G65" s="47"/>
-      <c r="H65" s="51"/>
+    <row r="65" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="38" t="s">
+        <v>101</v>
+      </c>
+      <c r="B65" s="40"/>
+      <c r="C65" s="38" t="s">
+        <v>39</v>
+      </c>
+      <c r="D65" s="42">
+        <v>44077</v>
+      </c>
+      <c r="E65" s="43">
+        <v>44107</v>
+      </c>
+      <c r="F65" s="42"/>
+      <c r="G65" s="43"/>
+      <c r="H65" s="49"/>
       <c r="I65" s="58"/>
     </row>
-    <row r="66" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="15"/>
-      <c r="B66" s="15"/>
-      <c r="C66" s="38"/>
-      <c r="D66" s="42"/>
-      <c r="E66" s="43"/>
-      <c r="F66" s="63"/>
-      <c r="G66" s="64"/>
-      <c r="H66" s="65"/>
-    </row>
-    <row r="67" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="38" t="s">
+        <v>106</v>
+      </c>
+      <c r="B66" s="40"/>
+      <c r="C66" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="D66" s="42">
+        <v>44138</v>
+      </c>
+      <c r="E66" s="43">
+        <v>44168</v>
+      </c>
+      <c r="F66" s="42"/>
+      <c r="G66" s="43"/>
+      <c r="H66" s="49"/>
+      <c r="I66" s="58"/>
+    </row>
+    <row r="67" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A67" s="15"/>
       <c r="B67" s="15"/>
       <c r="C67" s="38"/>
       <c r="D67" s="42"/>
       <c r="E67" s="43"/>
-      <c r="F67" s="63"/>
-      <c r="G67" s="64"/>
-      <c r="H67" s="65"/>
-    </row>
-    <row r="68" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F67" s="42"/>
+      <c r="G67" s="43"/>
+      <c r="H67" s="49"/>
+      <c r="I67" s="58"/>
+    </row>
+    <row r="68" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A68" s="15"/>
-      <c r="B68" s="61"/>
+      <c r="B68" s="15"/>
       <c r="C68" s="38"/>
       <c r="D68" s="42"/>
       <c r="E68" s="43"/>
-      <c r="F68" s="42"/>
-      <c r="G68" s="43"/>
-      <c r="H68" s="49"/>
-    </row>
-    <row r="69" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="15"/>
-      <c r="B69" s="61"/>
-      <c r="C69" s="38"/>
-      <c r="D69" s="42"/>
-      <c r="E69" s="43"/>
-      <c r="F69" s="42"/>
-      <c r="G69" s="43"/>
-      <c r="H69" s="49"/>
-    </row>
-    <row r="70" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="40"/>
-      <c r="B70" s="62"/>
-      <c r="C70" s="38"/>
-      <c r="D70" s="42"/>
-      <c r="E70" s="43"/>
-      <c r="F70" s="42"/>
-      <c r="G70" s="43"/>
-      <c r="H70" s="49"/>
-    </row>
-    <row r="71" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="40"/>
-      <c r="B71" s="40"/>
-      <c r="C71" s="38"/>
-      <c r="D71" s="42"/>
-      <c r="E71" s="43"/>
-      <c r="F71" s="42"/>
-      <c r="G71" s="43"/>
-      <c r="H71" s="49"/>
-    </row>
-    <row r="72" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="40"/>
-      <c r="B72" s="40"/>
-      <c r="C72" s="38"/>
-      <c r="D72" s="42"/>
-      <c r="E72" s="43"/>
-      <c r="F72" s="42"/>
-      <c r="G72" s="43"/>
-      <c r="H72" s="49"/>
-    </row>
-    <row r="73" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F68" s="46"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="51"/>
+      <c r="I68" s="58"/>
+    </row>
+    <row r="69" spans="1:62" s="8" customFormat="1" ht="22.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="41" t="s">
+        <v>102</v>
+      </c>
+      <c r="B69" s="41"/>
+      <c r="C69" s="39"/>
+      <c r="D69" s="44"/>
+      <c r="E69" s="45"/>
+      <c r="F69" s="44"/>
+      <c r="G69" s="45"/>
+      <c r="H69" s="50" t="str">
+        <f>IF(OR(ISBLANK(F69),ISBLANK(G69)),"",G69-F69+1)</f>
+        <v/>
+      </c>
+      <c r="I69" s="16"/>
+      <c r="J69" s="16"/>
+      <c r="K69" s="16"/>
+      <c r="L69" s="16"/>
+      <c r="M69" s="16"/>
+      <c r="N69" s="16"/>
+      <c r="O69" s="16"/>
+      <c r="P69" s="16"/>
+      <c r="Q69" s="16"/>
+      <c r="R69" s="16"/>
+      <c r="S69" s="16"/>
+      <c r="T69" s="16"/>
+      <c r="U69" s="16"/>
+      <c r="V69" s="16"/>
+      <c r="W69" s="16"/>
+      <c r="X69" s="16"/>
+      <c r="Y69" s="16"/>
+      <c r="Z69" s="16"/>
+      <c r="AA69" s="16"/>
+      <c r="AB69" s="16"/>
+      <c r="AC69" s="16"/>
+      <c r="AD69" s="16"/>
+      <c r="AE69" s="16"/>
+      <c r="AF69" s="16"/>
+      <c r="AG69" s="16"/>
+      <c r="AH69" s="16"/>
+      <c r="AI69" s="16"/>
+      <c r="AJ69" s="16"/>
+      <c r="AK69" s="16"/>
+      <c r="AL69" s="16"/>
+      <c r="AM69" s="16"/>
+      <c r="AN69" s="16"/>
+      <c r="AO69" s="16"/>
+      <c r="AP69" s="16"/>
+      <c r="AQ69" s="16"/>
+      <c r="AR69" s="16"/>
+      <c r="AS69" s="16"/>
+      <c r="AT69" s="16"/>
+      <c r="AU69" s="16"/>
+      <c r="AV69" s="16"/>
+      <c r="AW69" s="16"/>
+      <c r="AX69" s="16"/>
+      <c r="AY69" s="16"/>
+      <c r="AZ69" s="16"/>
+      <c r="BA69" s="16"/>
+      <c r="BB69" s="16"/>
+      <c r="BC69" s="16"/>
+      <c r="BD69" s="16"/>
+      <c r="BE69" s="16"/>
+      <c r="BF69" s="16"/>
+      <c r="BG69" s="16"/>
+      <c r="BH69" s="16"/>
+      <c r="BI69" s="16"/>
+      <c r="BJ69" s="16"/>
+    </row>
+    <row r="70" spans="1:62" s="58" customFormat="1" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B70" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="C70" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="D70" s="56" t="s">
+        <v>7</v>
+      </c>
+      <c r="E70" s="56" t="s">
+        <v>8</v>
+      </c>
+      <c r="F70" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="G70" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="H70" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="I70" s="36"/>
+      <c r="J70" s="36"/>
+      <c r="K70" s="36"/>
+      <c r="L70" s="36"/>
+      <c r="M70" s="36"/>
+      <c r="N70" s="36"/>
+      <c r="O70" s="36"/>
+      <c r="P70" s="36"/>
+      <c r="Q70" s="36"/>
+      <c r="R70" s="36"/>
+      <c r="S70" s="36"/>
+      <c r="T70" s="36"/>
+      <c r="U70" s="36"/>
+      <c r="V70" s="36"/>
+      <c r="W70" s="36"/>
+      <c r="X70" s="36"/>
+      <c r="Y70" s="36"/>
+      <c r="Z70" s="36"/>
+      <c r="AA70" s="36"/>
+      <c r="AB70" s="36"/>
+      <c r="AC70" s="36"/>
+      <c r="AD70" s="36"/>
+      <c r="AE70" s="36"/>
+      <c r="AF70" s="36"/>
+      <c r="AG70" s="36"/>
+      <c r="AH70" s="36"/>
+      <c r="AI70" s="36"/>
+      <c r="AJ70" s="36"/>
+      <c r="AK70" s="36"/>
+      <c r="AL70" s="36"/>
+      <c r="AM70" s="36"/>
+      <c r="AN70" s="36"/>
+      <c r="AO70" s="36"/>
+      <c r="AP70" s="36"/>
+      <c r="AQ70" s="36"/>
+      <c r="AR70" s="36"/>
+      <c r="AS70" s="36"/>
+      <c r="AT70" s="36"/>
+      <c r="AU70" s="36"/>
+      <c r="AV70" s="36"/>
+      <c r="AW70" s="36"/>
+      <c r="AX70" s="36"/>
+      <c r="AY70" s="36"/>
+      <c r="AZ70" s="36"/>
+      <c r="BA70" s="36"/>
+      <c r="BB70" s="36"/>
+      <c r="BC70" s="36"/>
+      <c r="BD70" s="36"/>
+      <c r="BE70" s="36"/>
+      <c r="BF70" s="36"/>
+      <c r="BG70" s="36"/>
+      <c r="BH70" s="36"/>
+      <c r="BI70" s="36"/>
+      <c r="BJ70" s="36"/>
+    </row>
+    <row r="71" spans="1:62" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>105</v>
+      </c>
+      <c r="C71" s="59" t="s">
+        <v>46</v>
+      </c>
+      <c r="D71" s="76">
+        <v>43900</v>
+      </c>
+      <c r="E71" s="77">
+        <v>43901</v>
+      </c>
+    </row>
+    <row r="72" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="15" t="s">
+        <v>104</v>
+      </c>
+      <c r="B72" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="C72" s="38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D72" s="42">
+        <v>43900</v>
+      </c>
+      <c r="E72" s="43">
+        <v>43905</v>
+      </c>
+      <c r="F72" s="46"/>
+      <c r="G72" s="47"/>
+      <c r="H72" s="51"/>
+    </row>
+    <row r="73" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A73" s="15"/>
-      <c r="B73" s="15"/>
+      <c r="B73" s="61"/>
       <c r="C73" s="38"/>
       <c r="D73" s="42"/>
       <c r="E73" s="43"/>
@@ -5264,192 +5888,279 @@
       <c r="G73" s="43"/>
       <c r="H73" s="49"/>
     </row>
-    <row r="74" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="15"/>
-      <c r="B74" s="15"/>
+    <row r="74" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A74" s="40"/>
+      <c r="B74" s="62"/>
       <c r="C74" s="38"/>
       <c r="D74" s="42"/>
       <c r="E74" s="43"/>
-      <c r="F74" s="46"/>
-      <c r="G74" s="47"/>
-      <c r="H74" s="51"/>
-    </row>
-    <row r="75" spans="1:9" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="F74" s="42"/>
+      <c r="G74" s="43"/>
+      <c r="H74" s="49"/>
+    </row>
+    <row r="75" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="40"/>
       <c r="B75" s="40"/>
       <c r="C75" s="38"/>
       <c r="D75" s="42"/>
       <c r="E75" s="43"/>
-      <c r="F75" s="59"/>
+      <c r="F75" s="42"/>
+      <c r="G75" s="43"/>
+      <c r="H75" s="49"/>
+    </row>
+    <row r="76" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="40"/>
+      <c r="B76" s="40"/>
+      <c r="C76" s="38"/>
+      <c r="D76" s="42"/>
+      <c r="E76" s="43"/>
+      <c r="F76" s="42"/>
+      <c r="G76" s="43"/>
+      <c r="H76" s="49"/>
+    </row>
+    <row r="77" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="15"/>
+      <c r="B77" s="15"/>
+      <c r="C77" s="38"/>
+      <c r="D77" s="42"/>
+      <c r="E77" s="43"/>
+      <c r="F77" s="42"/>
+      <c r="G77" s="43"/>
+      <c r="H77" s="49"/>
+    </row>
+    <row r="78" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="15"/>
+      <c r="B78" s="15"/>
+      <c r="C78" s="38"/>
+      <c r="D78" s="42"/>
+      <c r="E78" s="43"/>
+      <c r="F78" s="46"/>
+      <c r="G78" s="47"/>
+      <c r="H78" s="51"/>
+    </row>
+    <row r="79" spans="1:62" s="58" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="40"/>
+      <c r="B79" s="40"/>
+      <c r="C79" s="38"/>
+      <c r="D79" s="42"/>
+      <c r="E79" s="43"/>
+      <c r="F79" s="59"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="D4:E4"/>
   </mergeCells>
   <conditionalFormatting sqref="I7:BJ16 I19:BJ25 I27:BJ36">
-    <cfRule type="expression" dxfId="41" priority="43">
+    <cfRule type="expression" dxfId="52" priority="51">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I18:BJ18">
-    <cfRule type="expression" dxfId="40" priority="38">
+    <cfRule type="expression" dxfId="51" priority="46">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I17:BJ17">
-    <cfRule type="expression" dxfId="39" priority="35">
+    <cfRule type="expression" dxfId="50" priority="43">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I26:BJ26">
-    <cfRule type="expression" dxfId="38" priority="34">
+    <cfRule type="expression" dxfId="49" priority="42">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I9:BJ16 I18:BJ25">
-    <cfRule type="expression" dxfId="37" priority="59" stopIfTrue="1">
+    <cfRule type="expression" dxfId="48" priority="67" stopIfTrue="1">
       <formula>NOT(AND(MAX($G9,$E9)&gt;=I$6,MIN($F9,$D9)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="36" priority="60">
+    <cfRule type="expression" dxfId="47" priority="68">
       <formula>AND($E9&gt;=I$6,$D9&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="35" priority="61" stopIfTrue="1">
+    <cfRule type="expression" dxfId="46" priority="69" stopIfTrue="1">
       <formula>AND($G9&gt;=I$6,$F9&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37:BJ37">
-    <cfRule type="expression" dxfId="34" priority="79" stopIfTrue="1">
-      <formula>NOT(AND(MAX($G44,$E44)&gt;=I$6,MIN($F44,$D44)&lt;J$6))</formula>
+    <cfRule type="expression" dxfId="45" priority="87" stopIfTrue="1">
+      <formula>NOT(AND(MAX($G45,$E45)&gt;=I$6,MIN($F45,$D45)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="33" priority="80">
-      <formula>AND($E44&gt;=I$6,$D44&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="44" priority="88">
+      <formula>AND($E45&gt;=I$6,$D45&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="81" stopIfTrue="1">
-      <formula>AND($G44&gt;=I$6,$F44&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="43" priority="89" stopIfTrue="1">
+      <formula>AND($G45&gt;=I$6,$F45&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I30:BJ30 I27:BJ27">
-    <cfRule type="expression" dxfId="31" priority="82" stopIfTrue="1">
+    <cfRule type="expression" dxfId="42" priority="90" stopIfTrue="1">
       <formula>NOT(AND(MAX(#REF!,#REF!)&gt;=I$6,MIN(#REF!,#REF!)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="30" priority="83">
+    <cfRule type="expression" dxfId="41" priority="91">
       <formula>AND(#REF!&gt;=I$6,#REF!&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="29" priority="84" stopIfTrue="1">
+    <cfRule type="expression" dxfId="40" priority="92" stopIfTrue="1">
       <formula>AND(#REF!&gt;=I$6,#REF!&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I28:BJ29 I36:BJ36 I38:BJ39">
-    <cfRule type="expression" dxfId="28" priority="96" stopIfTrue="1">
+  <conditionalFormatting sqref="I28:BJ29">
+    <cfRule type="expression" dxfId="39" priority="104" stopIfTrue="1">
       <formula>NOT(AND(MAX($G34,$E34)&gt;=I$6,MIN($F34,$D34)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="27" priority="97">
+    <cfRule type="expression" dxfId="38" priority="105">
       <formula>AND($E34&gt;=I$6,$D34&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="26" priority="98" stopIfTrue="1">
+    <cfRule type="expression" dxfId="37" priority="106" stopIfTrue="1">
       <formula>AND($G34&gt;=I$6,$F34&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I37:BJ37">
-    <cfRule type="expression" dxfId="25" priority="25">
+    <cfRule type="expression" dxfId="36" priority="33">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I31:BJ31 I34:BJ35">
-    <cfRule type="expression" dxfId="24" priority="140" stopIfTrue="1">
+    <cfRule type="expression" dxfId="35" priority="148" stopIfTrue="1">
       <formula>NOT(AND(MAX($G36,$E36)&gt;=I$6,MIN($F36,$D36)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="23" priority="141">
+    <cfRule type="expression" dxfId="34" priority="149">
       <formula>AND($E36&gt;=I$6,$D36&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="22" priority="142" stopIfTrue="1">
+    <cfRule type="expression" dxfId="33" priority="150" stopIfTrue="1">
       <formula>AND($G36&gt;=I$6,$F36&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I38:BJ40">
-    <cfRule type="expression" dxfId="21" priority="14">
+    <cfRule type="expression" dxfId="32" priority="22">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:BJ41">
-    <cfRule type="expression" dxfId="20" priority="10">
+    <cfRule type="expression" dxfId="31" priority="18">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I32:BJ32">
-    <cfRule type="expression" dxfId="19" priority="149" stopIfTrue="1">
+    <cfRule type="expression" dxfId="30" priority="157" stopIfTrue="1">
       <formula>NOT(AND(MAX(#REF!,#REF!)&gt;=I$6,MIN(#REF!,#REF!)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="18" priority="150">
+    <cfRule type="expression" dxfId="29" priority="158">
       <formula>AND(#REF!&gt;=I$6,#REF!&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="17" priority="151" stopIfTrue="1">
+    <cfRule type="expression" dxfId="28" priority="159" stopIfTrue="1">
       <formula>AND(#REF!&gt;=I$6,#REF!&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I33:BJ33">
-    <cfRule type="expression" dxfId="16" priority="178" stopIfTrue="1">
+    <cfRule type="expression" dxfId="27" priority="186" stopIfTrue="1">
       <formula>NOT(AND(MAX($G37,$E37)&gt;=I$6,MIN($F37,$D37)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="15" priority="179">
+    <cfRule type="expression" dxfId="26" priority="187">
       <formula>AND($E37&gt;=I$6,$D37&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="14" priority="180" stopIfTrue="1">
+    <cfRule type="expression" dxfId="25" priority="188" stopIfTrue="1">
       <formula>AND($G37&gt;=I$6,$F37&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I42:BJ42">
-    <cfRule type="expression" dxfId="13" priority="6">
+  <conditionalFormatting sqref="I43:BJ43">
+    <cfRule type="expression" dxfId="24" priority="14">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I41:BJ41">
-    <cfRule type="expression" dxfId="12" priority="199" stopIfTrue="1">
-      <formula>NOT(AND(MAX($G47,$E56)&gt;=I$6,MIN($F47,$D56)&lt;J$6))</formula>
+    <cfRule type="expression" dxfId="23" priority="207" stopIfTrue="1">
+      <formula>NOT(AND(MAX($G48,$E58)&gt;=I$6,MIN($F48,$D58)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="11" priority="200">
-      <formula>AND($E56&gt;=I$6,$D56&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="22" priority="208">
+      <formula>AND($E58&gt;=I$6,$D58&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="10" priority="201" stopIfTrue="1">
-      <formula>AND($G47&gt;=I$6,$F47&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="21" priority="209" stopIfTrue="1">
+      <formula>AND($G48&gt;=I$6,$F48&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I40:BJ40">
-    <cfRule type="expression" dxfId="9" priority="202" stopIfTrue="1">
-      <formula>NOT(AND(MAX($G49,$E54)&gt;=I$6,MIN($F49,$D54)&lt;J$6))</formula>
+    <cfRule type="expression" dxfId="20" priority="210" stopIfTrue="1">
+      <formula>NOT(AND(MAX($G50,$E56)&gt;=I$6,MIN($F50,$D56)&lt;J$6))</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="8" priority="203">
-      <formula>AND($E54&gt;=I$6,$D54&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="19" priority="211">
+      <formula>AND($E56&gt;=I$6,$D56&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="7" priority="204" stopIfTrue="1">
-      <formula>AND($G49&gt;=I$6,$F49&lt;J$6)</formula>
+    <cfRule type="expression" dxfId="18" priority="212" stopIfTrue="1">
+      <formula>AND($G50&gt;=I$6,$F50&lt;J$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I43:BJ43">
+    <cfRule type="expression" dxfId="17" priority="222" stopIfTrue="1">
+      <formula>NOT(AND(MAX($G51,$E57)&gt;=I$6,MIN($F51,$D57)&lt;J$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="16" priority="223">
+      <formula>AND($E57&gt;=I$6,$D57&lt;J$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="15" priority="224" stopIfTrue="1">
+      <formula>AND($G51&gt;=I$6,$F51&lt;J$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I53:BJ53">
+    <cfRule type="expression" dxfId="14" priority="9">
+      <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I53:BJ53">
+    <cfRule type="expression" dxfId="13" priority="225" stopIfTrue="1">
+      <formula>NOT(AND(MAX($G63,$E67)&gt;=I$6,MIN($F63,$D67)&lt;J$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="12" priority="226">
+      <formula>AND($E67&gt;=I$6,$D67&lt;J$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="11" priority="227" stopIfTrue="1">
+      <formula>AND($G63&gt;=I$6,$F63&lt;J$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I52:BJ52">
+    <cfRule type="expression" dxfId="10" priority="8">
+      <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I38:BJ39 I36:BJ36">
+    <cfRule type="expression" dxfId="9" priority="228" stopIfTrue="1">
+      <formula>NOT(AND(MAX($G43,$E43)&gt;=I$6,MIN($F43,$D43)&lt;J$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="8" priority="229">
+      <formula>AND($E43&gt;=I$6,$D43&lt;J$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="7" priority="230" stopIfTrue="1">
+      <formula>AND($G43&gt;=I$6,$F43&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I42:BJ42">
-    <cfRule type="expression" dxfId="6" priority="214" stopIfTrue="1">
-      <formula>NOT(AND(MAX($G50,$E55)&gt;=I$6,MIN($F50,$D55)&lt;J$6))</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="5" priority="215">
-      <formula>AND($E55&gt;=I$6,$D55&lt;J$6)</formula>
-    </cfRule>
-    <cfRule type="expression" dxfId="4" priority="216" stopIfTrue="1">
-      <formula>AND($G50&gt;=I$6,$F50&lt;J$6)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="I51:BJ51">
-    <cfRule type="expression" dxfId="3" priority="1">
+    <cfRule type="expression" dxfId="6" priority="7">
       <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="I51:BJ51">
-    <cfRule type="expression" dxfId="2" priority="217" stopIfTrue="1">
-      <formula>NOT(AND(MAX($G60,$E64)&gt;=I$6,MIN($F60,$D64)&lt;J$6))</formula>
+  <conditionalFormatting sqref="I60:BJ60">
+    <cfRule type="expression" dxfId="5" priority="6">
+      <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="218">
-      <formula>AND($E64&gt;=I$6,$D64&lt;J$6)</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I69:BJ69">
+    <cfRule type="expression" dxfId="4" priority="2">
+      <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="219" stopIfTrue="1">
-      <formula>AND($G60&gt;=I$6,$F60&lt;J$6)</formula>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I69:BJ69">
+    <cfRule type="expression" dxfId="3" priority="3" stopIfTrue="1">
+      <formula>NOT(AND(MAX($G69,$E69)&gt;=I$6,MIN($F69,$D69)&lt;J$6))</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="2" priority="4">
+      <formula>AND($E69&gt;=I$6,$D69&lt;J$6)</formula>
+    </cfRule>
+    <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
+      <formula>AND($G69&gt;=I$6,$F69&lt;J$6)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I70:BJ70">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>AND(TODAY()&gt;=I$6,TODAY()&lt;J$6)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations disablePrompts="1" count="1">
@@ -5518,10 +6229,10 @@
       <c r="C1" s="4"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="B2" s="78" t="s">
+      <c r="B2" s="75" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="78"/>
+      <c r="C2" s="75"/>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="C3" s="21" t="s">

</xml_diff>